<commit_message>
modify some mds, start operating system learning md
</commit_message>
<xml_diff>
--- a/学习记录.xlsx
+++ b/学习记录.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\不怕晒的铃铛\Desktop\学习资料（真的）\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\不怕晒的铃铛\Desktop\学习资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA3A680B-4898-4A16-9C5B-71A89F179084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA74DCD-F8B4-4B9B-9474-343B87B3A749}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JavaWeb相关" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="499">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="503">
   <si>
     <t>JavaSE</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2030,6 +2030,22 @@
   </si>
   <si>
     <t>创建者模式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>加油站(反证法)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分发糖果</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>操作系统基本概念</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>操作系统基本特征</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2137,7 +2153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2427,6 +2443,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2754,10 +2773,10 @@
   <dimension ref="A1:M623"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B200" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B203" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C205" sqref="C205"/>
+      <selection pane="bottomRight" activeCell="C213" sqref="C213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
@@ -2821,7 +2840,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="108">
+      <c r="A3" s="109">
         <v>44566</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -2831,7 +2850,7 @@
       <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="109"/>
+      <c r="A4" s="110"/>
       <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
@@ -2839,7 +2858,7 @@
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:13" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="110"/>
+      <c r="A5" s="111"/>
       <c r="B5" s="6" t="s">
         <v>28</v>
       </c>
@@ -2877,7 +2896,7 @@
       <c r="D8" s="12"/>
     </row>
     <row r="9" spans="1:13" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="108">
+      <c r="A9" s="109">
         <v>44572</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -2887,7 +2906,7 @@
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:13" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="110"/>
+      <c r="A10" s="111"/>
       <c r="B10" s="17" t="s">
         <v>38</v>
       </c>
@@ -2895,7 +2914,7 @@
       <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="108">
+      <c r="A11" s="109">
         <v>44573</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2905,7 +2924,7 @@
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="109"/>
+      <c r="A12" s="110"/>
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
@@ -2913,7 +2932,7 @@
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="110"/>
+      <c r="A13" s="111"/>
       <c r="B13" s="18" t="s">
         <v>40</v>
       </c>
@@ -2921,7 +2940,7 @@
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:13" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="108">
+      <c r="A14" s="109">
         <v>44574</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -2931,7 +2950,7 @@
       <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:13" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="110"/>
+      <c r="A15" s="111"/>
       <c r="B15" s="19" t="s">
         <v>42</v>
       </c>
@@ -2941,7 +2960,7 @@
       <c r="D15" s="19"/>
     </row>
     <row r="16" spans="1:13" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="108">
+      <c r="A16" s="109">
         <v>44575</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -2953,7 +2972,7 @@
       <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="109"/>
+      <c r="A17" s="110"/>
       <c r="B17" s="4" t="s">
         <v>47</v>
       </c>
@@ -2964,7 +2983,7 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="109"/>
+      <c r="A18" s="110"/>
       <c r="B18" s="4" t="s">
         <v>48</v>
       </c>
@@ -2975,7 +2994,7 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="110"/>
+      <c r="A19" s="111"/>
       <c r="B19" s="20" t="s">
         <v>49</v>
       </c>
@@ -2984,7 +3003,7 @@
       <c r="E19" s="21"/>
     </row>
     <row r="20" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="108">
+      <c r="A20" s="109">
         <v>44576</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -2997,7 +3016,7 @@
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="109"/>
+      <c r="A21" s="110"/>
       <c r="B21" s="4" t="s">
         <v>59</v>
       </c>
@@ -3008,7 +3027,7 @@
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="109"/>
+      <c r="A22" s="110"/>
       <c r="B22" s="4" t="s">
         <v>60</v>
       </c>
@@ -3019,7 +3038,7 @@
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="110"/>
+      <c r="A23" s="111"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20" t="s">
         <v>57</v>
@@ -3028,7 +3047,7 @@
       <c r="E23" s="21"/>
     </row>
     <row r="24" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="108">
+      <c r="A24" s="109">
         <v>44577</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -3043,7 +3062,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="109"/>
+      <c r="A25" s="110"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
         <v>63</v>
@@ -3054,7 +3073,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="110"/>
+      <c r="A26" s="111"/>
       <c r="B26" s="21"/>
       <c r="C26" s="21" t="s">
         <v>64</v>
@@ -3065,7 +3084,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="108">
+      <c r="A27" s="109">
         <v>44578</v>
       </c>
       <c r="B27" s="8" t="s">
@@ -3076,7 +3095,7 @@
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="109"/>
+      <c r="A28" s="110"/>
       <c r="B28" s="4" t="s">
         <v>69</v>
       </c>
@@ -3085,7 +3104,7 @@
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="109"/>
+      <c r="A29" s="110"/>
       <c r="B29" s="4" t="s">
         <v>70</v>
       </c>
@@ -3094,7 +3113,7 @@
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="110"/>
+      <c r="A30" s="111"/>
       <c r="B30" s="22" t="s">
         <v>71</v>
       </c>
@@ -3103,7 +3122,7 @@
       <c r="E30" s="22"/>
     </row>
     <row r="31" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="108">
+      <c r="A31" s="109">
         <v>44579</v>
       </c>
       <c r="B31" s="8" t="s">
@@ -3118,7 +3137,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="110"/>
+      <c r="A32" s="111"/>
       <c r="B32" s="22" t="s">
         <v>73</v>
       </c>
@@ -3129,7 +3148,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="108">
+      <c r="A33" s="109">
         <v>44580</v>
       </c>
       <c r="B33" s="8" t="s">
@@ -3143,7 +3162,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="110"/>
+      <c r="A34" s="111"/>
       <c r="B34" s="23" t="s">
         <v>83</v>
       </c>
@@ -3152,7 +3171,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="108">
+      <c r="A35" s="109">
         <v>44581</v>
       </c>
       <c r="B35" s="8" t="s">
@@ -3164,7 +3183,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="109"/>
+      <c r="A36" s="110"/>
       <c r="B36" s="4" t="s">
         <v>85</v>
       </c>
@@ -3174,7 +3193,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="109"/>
+      <c r="A37" s="110"/>
       <c r="B37" s="4" t="s">
         <v>86</v>
       </c>
@@ -3182,7 +3201,7 @@
       <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="109"/>
+      <c r="A38" s="110"/>
       <c r="B38" s="4" t="s">
         <v>87</v>
       </c>
@@ -3190,7 +3209,7 @@
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="110"/>
+      <c r="A39" s="111"/>
       <c r="B39" s="23" t="s">
         <v>88</v>
       </c>
@@ -3198,7 +3217,7 @@
       <c r="D39" s="23"/>
     </row>
     <row r="40" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="108">
+      <c r="A40" s="109">
         <v>44582</v>
       </c>
       <c r="B40" s="8" t="s">
@@ -3215,7 +3234,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="111"/>
+      <c r="A41" s="112"/>
       <c r="B41" s="4" t="s">
         <v>91</v>
       </c>
@@ -3227,7 +3246,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="111"/>
+      <c r="A42" s="112"/>
       <c r="B42" s="4" t="s">
         <v>98</v>
       </c>
@@ -3237,7 +3256,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="112"/>
+      <c r="A43" s="113"/>
       <c r="B43" s="24" t="s">
         <v>99</v>
       </c>
@@ -3247,7 +3266,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="108">
+      <c r="A44" s="109">
         <v>44583</v>
       </c>
       <c r="B44" s="8" t="s">
@@ -3257,7 +3276,7 @@
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="109"/>
+      <c r="A45" s="110"/>
       <c r="B45" s="4" t="s">
         <v>101</v>
       </c>
@@ -3265,7 +3284,7 @@
       <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="109"/>
+      <c r="A46" s="110"/>
       <c r="B46" s="4" t="s">
         <v>102</v>
       </c>
@@ -3273,7 +3292,7 @@
       <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="109"/>
+      <c r="A47" s="110"/>
       <c r="B47" s="4" t="s">
         <v>103</v>
       </c>
@@ -3281,7 +3300,7 @@
       <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="109"/>
+      <c r="A48" s="110"/>
       <c r="B48" s="4" t="s">
         <v>104</v>
       </c>
@@ -3289,7 +3308,7 @@
       <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="110"/>
+      <c r="A49" s="111"/>
       <c r="B49" s="25" t="s">
         <v>105</v>
       </c>
@@ -3297,7 +3316,7 @@
       <c r="D49" s="25"/>
     </row>
     <row r="50" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="108">
+      <c r="A50" s="109">
         <v>44584</v>
       </c>
       <c r="B50" s="8" t="s">
@@ -3307,7 +3326,7 @@
       <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="111"/>
+      <c r="A51" s="112"/>
       <c r="B51" s="4" t="s">
         <v>107</v>
       </c>
@@ -3315,7 +3334,7 @@
       <c r="D51" s="4"/>
     </row>
     <row r="52" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="111"/>
+      <c r="A52" s="112"/>
       <c r="B52" s="4" t="s">
         <v>108</v>
       </c>
@@ -3323,7 +3342,7 @@
       <c r="D52" s="4"/>
     </row>
     <row r="53" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="112"/>
+      <c r="A53" s="113"/>
       <c r="B53" s="26" t="s">
         <v>109</v>
       </c>
@@ -3331,7 +3350,7 @@
       <c r="D53" s="26"/>
     </row>
     <row r="54" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="108">
+      <c r="A54" s="109">
         <v>44585</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -3341,7 +3360,7 @@
       <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="110"/>
+      <c r="A55" s="111"/>
       <c r="B55" s="27" t="s">
         <v>111</v>
       </c>
@@ -3349,7 +3368,7 @@
       <c r="D55" s="27"/>
     </row>
     <row r="56" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="108">
+      <c r="A56" s="109">
         <v>44586</v>
       </c>
       <c r="B56" s="8"/>
@@ -3364,7 +3383,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="109"/>
+      <c r="A57" s="110"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4" t="s">
@@ -3373,7 +3392,7 @@
       <c r="E57" s="4"/>
     </row>
     <row r="58" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="110"/>
+      <c r="A58" s="111"/>
       <c r="B58" s="27"/>
       <c r="C58" s="27"/>
       <c r="D58" s="27" t="s">
@@ -3382,7 +3401,7 @@
       <c r="E58" s="27"/>
     </row>
     <row r="59" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="108">
+      <c r="A59" s="109">
         <v>44587</v>
       </c>
       <c r="B59" s="8"/>
@@ -3397,7 +3416,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="109"/>
+      <c r="A60" s="110"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4" t="s">
         <v>120</v>
@@ -3407,7 +3426,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="109"/>
+      <c r="A61" s="110"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4" t="s">
         <v>123</v>
@@ -3418,7 +3437,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="110"/>
+      <c r="A62" s="111"/>
       <c r="B62" s="29"/>
       <c r="C62" s="29" t="s">
         <v>124</v>
@@ -3427,7 +3446,7 @@
       <c r="E62" s="29"/>
     </row>
     <row r="63" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="108">
+      <c r="A63" s="109">
         <v>44588</v>
       </c>
       <c r="B63" s="8"/>
@@ -3442,7 +3461,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="109"/>
+      <c r="A64" s="110"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4" t="s">
         <v>126</v>
@@ -3453,7 +3472,7 @@
       <c r="E64" s="4"/>
     </row>
     <row r="65" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="109"/>
+      <c r="A65" s="110"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4" t="s">
         <v>127</v>
@@ -3464,7 +3483,7 @@
       <c r="E65" s="4"/>
     </row>
     <row r="66" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="110"/>
+      <c r="A66" s="111"/>
       <c r="B66" s="30"/>
       <c r="C66" s="30" t="s">
         <v>128</v>
@@ -3473,7 +3492,7 @@
       <c r="E66" s="30"/>
     </row>
     <row r="67" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="108">
+      <c r="A67" s="109">
         <v>44589</v>
       </c>
       <c r="B67" s="8"/>
@@ -3484,7 +3503,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="109"/>
+      <c r="A68" s="110"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -3493,7 +3512,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="110"/>
+      <c r="A69" s="111"/>
       <c r="B69" s="32"/>
       <c r="C69" s="32"/>
       <c r="D69" s="32"/>
@@ -3526,7 +3545,7 @@
       </c>
     </row>
     <row r="72" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="108">
+      <c r="A72" s="109">
         <v>44594</v>
       </c>
       <c r="B72" s="8"/>
@@ -3537,7 +3556,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="109"/>
+      <c r="A73" s="110"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
@@ -3546,7 +3565,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="109"/>
+      <c r="A74" s="110"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
@@ -3555,7 +3574,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="110"/>
+      <c r="A75" s="111"/>
       <c r="B75" s="37"/>
       <c r="C75" s="37"/>
       <c r="D75" s="37"/>
@@ -3586,7 +3605,7 @@
       </c>
     </row>
     <row r="78" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="108">
+      <c r="A78" s="109">
         <v>44598</v>
       </c>
       <c r="B78" s="8"/>
@@ -3597,7 +3616,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="109"/>
+      <c r="A79" s="110"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
@@ -3606,7 +3625,7 @@
       </c>
     </row>
     <row r="80" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="109"/>
+      <c r="A80" s="110"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -3615,7 +3634,7 @@
       </c>
     </row>
     <row r="81" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="110"/>
+      <c r="A81" s="111"/>
       <c r="B81" s="48"/>
       <c r="C81" s="48"/>
       <c r="D81" s="48"/>
@@ -3624,7 +3643,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="108">
+      <c r="A82" s="109">
         <v>44599</v>
       </c>
       <c r="B82" s="8"/>
@@ -3635,7 +3654,7 @@
       </c>
     </row>
     <row r="83" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="109"/>
+      <c r="A83" s="110"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
@@ -3644,7 +3663,7 @@
       </c>
     </row>
     <row r="84" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="110"/>
+      <c r="A84" s="111"/>
       <c r="B84" s="49"/>
       <c r="C84" s="49"/>
       <c r="D84" s="49"/>
@@ -3653,7 +3672,7 @@
       </c>
     </row>
     <row r="85" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="108">
+      <c r="A85" s="109">
         <v>44600</v>
       </c>
       <c r="B85" s="8"/>
@@ -3671,7 +3690,7 @@
       <c r="J85" s="8"/>
     </row>
     <row r="86" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="110"/>
+      <c r="A86" s="111"/>
       <c r="B86" s="50"/>
       <c r="C86" s="50"/>
       <c r="D86" s="50"/>
@@ -3685,7 +3704,7 @@
       <c r="J86" s="50"/>
     </row>
     <row r="87" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="108">
+      <c r="A87" s="109">
         <v>44601</v>
       </c>
       <c r="B87" s="8"/>
@@ -3703,7 +3722,7 @@
       <c r="J87" s="8"/>
     </row>
     <row r="88" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="109"/>
+      <c r="A88" s="110"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4" t="s">
@@ -3719,7 +3738,7 @@
       <c r="J88" s="4"/>
     </row>
     <row r="89" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="109"/>
+      <c r="A89" s="110"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4" t="s">
@@ -3735,7 +3754,7 @@
       <c r="J89" s="4"/>
     </row>
     <row r="90" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="109"/>
+      <c r="A90" s="110"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4" t="s">
@@ -3749,7 +3768,7 @@
       <c r="J90" s="4"/>
     </row>
     <row r="91" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="109"/>
+      <c r="A91" s="110"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4" t="s">
@@ -3763,7 +3782,7 @@
       <c r="J91" s="4"/>
     </row>
     <row r="92" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="109"/>
+      <c r="A92" s="110"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="52" t="s">
@@ -3777,7 +3796,7 @@
       <c r="J92" s="4"/>
     </row>
     <row r="93" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="109"/>
+      <c r="A93" s="110"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4" t="s">
@@ -3791,7 +3810,7 @@
       <c r="J93" s="4"/>
     </row>
     <row r="94" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="110"/>
+      <c r="A94" s="111"/>
       <c r="B94" s="51"/>
       <c r="C94" s="51"/>
       <c r="D94" s="54" t="s">
@@ -3805,7 +3824,7 @@
       <c r="J94" s="51"/>
     </row>
     <row r="95" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="108">
+      <c r="A95" s="109">
         <v>44602</v>
       </c>
       <c r="B95" s="8"/>
@@ -3823,7 +3842,7 @@
       <c r="J95" s="8"/>
     </row>
     <row r="96" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="109"/>
+      <c r="A96" s="110"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4" t="s">
@@ -3839,7 +3858,7 @@
       <c r="J96" s="4"/>
     </row>
     <row r="97" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="110"/>
+      <c r="A97" s="111"/>
       <c r="B97" s="53"/>
       <c r="C97" s="53"/>
       <c r="D97" s="53"/>
@@ -3853,7 +3872,7 @@
       <c r="J97" s="53"/>
     </row>
     <row r="98" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="108">
+      <c r="A98" s="109">
         <v>44603</v>
       </c>
       <c r="B98" s="8"/>
@@ -3869,7 +3888,7 @@
       <c r="J98" s="8"/>
     </row>
     <row r="99" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="109"/>
+      <c r="A99" s="110"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
@@ -3883,7 +3902,7 @@
       <c r="J99" s="4"/>
     </row>
     <row r="100" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="109"/>
+      <c r="A100" s="110"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
@@ -3897,7 +3916,7 @@
       <c r="J100" s="4"/>
     </row>
     <row r="101" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="109"/>
+      <c r="A101" s="110"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
@@ -3911,7 +3930,7 @@
       <c r="J101" s="4"/>
     </row>
     <row r="102" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="109"/>
+      <c r="A102" s="110"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
@@ -3925,7 +3944,7 @@
       <c r="J102" s="4"/>
     </row>
     <row r="103" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="110"/>
+      <c r="A103" s="111"/>
       <c r="B103" s="55"/>
       <c r="C103" s="55"/>
       <c r="D103" s="55"/>
@@ -3939,7 +3958,7 @@
       <c r="J103" s="55"/>
     </row>
     <row r="104" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="108">
+      <c r="A104" s="109">
         <v>44604</v>
       </c>
       <c r="B104" s="8"/>
@@ -3955,7 +3974,7 @@
       <c r="J104" s="8"/>
     </row>
     <row r="105" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="109"/>
+      <c r="A105" s="110"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
@@ -3969,7 +3988,7 @@
       <c r="J105" s="4"/>
     </row>
     <row r="106" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="109"/>
+      <c r="A106" s="110"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
@@ -3983,7 +4002,7 @@
       <c r="J106" s="4"/>
     </row>
     <row r="107" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="109"/>
+      <c r="A107" s="110"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
@@ -3997,7 +4016,7 @@
       <c r="J107" s="4"/>
     </row>
     <row r="108" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="109"/>
+      <c r="A108" s="110"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
@@ -4011,7 +4030,7 @@
       <c r="J108" s="4"/>
     </row>
     <row r="109" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="109"/>
+      <c r="A109" s="110"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
@@ -4025,7 +4044,7 @@
       <c r="J109" s="4"/>
     </row>
     <row r="110" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="110"/>
+      <c r="A110" s="111"/>
       <c r="B110" s="56"/>
       <c r="C110" s="56"/>
       <c r="D110" s="56"/>
@@ -4039,7 +4058,7 @@
       <c r="J110" s="56"/>
     </row>
     <row r="111" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="108">
+      <c r="A111" s="109">
         <v>44605</v>
       </c>
       <c r="B111" s="8"/>
@@ -4055,7 +4074,7 @@
       <c r="J111" s="8"/>
     </row>
     <row r="112" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="109"/>
+      <c r="A112" s="110"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
@@ -4069,7 +4088,7 @@
       <c r="J112" s="4"/>
     </row>
     <row r="113" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="109"/>
+      <c r="A113" s="110"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
@@ -4083,7 +4102,7 @@
       <c r="J113" s="4"/>
     </row>
     <row r="114" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="109"/>
+      <c r="A114" s="110"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
@@ -4097,7 +4116,7 @@
       <c r="J114" s="4"/>
     </row>
     <row r="115" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="109"/>
+      <c r="A115" s="110"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
@@ -4111,7 +4130,7 @@
       <c r="J115" s="4"/>
     </row>
     <row r="116" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="109"/>
+      <c r="A116" s="110"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
@@ -4125,7 +4144,7 @@
       <c r="J116" s="4"/>
     </row>
     <row r="117" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="110"/>
+      <c r="A117" s="111"/>
       <c r="B117" s="57"/>
       <c r="C117" s="57"/>
       <c r="D117" s="57"/>
@@ -4139,7 +4158,7 @@
       <c r="J117" s="57"/>
     </row>
     <row r="118" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="108">
+      <c r="A118" s="109">
         <v>44606</v>
       </c>
       <c r="B118" s="8"/>
@@ -4155,7 +4174,7 @@
       <c r="J118" s="8"/>
     </row>
     <row r="119" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="110"/>
+      <c r="A119" s="111"/>
       <c r="B119" s="58"/>
       <c r="C119" s="58"/>
       <c r="D119" s="58"/>
@@ -4169,7 +4188,7 @@
       <c r="J119" s="58"/>
     </row>
     <row r="120" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="108">
+      <c r="A120" s="109">
         <v>44607</v>
       </c>
       <c r="B120" s="8"/>
@@ -4185,7 +4204,7 @@
       <c r="J120" s="8"/>
     </row>
     <row r="121" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="110"/>
+      <c r="A121" s="111"/>
       <c r="B121" s="58"/>
       <c r="C121" s="58"/>
       <c r="D121" s="58"/>
@@ -4229,7 +4248,7 @@
       <c r="J123" s="64"/>
     </row>
     <row r="124" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="108">
+      <c r="A124" s="109">
         <v>44609</v>
       </c>
       <c r="B124" s="8"/>
@@ -4245,7 +4264,7 @@
       <c r="J124" s="8"/>
     </row>
     <row r="125" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="109"/>
+      <c r="A125" s="110"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
@@ -4259,7 +4278,7 @@
       <c r="J125" s="4"/>
     </row>
     <row r="126" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="109"/>
+      <c r="A126" s="110"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
@@ -4273,7 +4292,7 @@
       <c r="J126" s="4"/>
     </row>
     <row r="127" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="109"/>
+      <c r="A127" s="110"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
@@ -4287,7 +4306,7 @@
       <c r="J127" s="4"/>
     </row>
     <row r="128" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="109"/>
+      <c r="A128" s="110"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
@@ -4301,7 +4320,7 @@
       <c r="J128" s="4"/>
     </row>
     <row r="129" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="110"/>
+      <c r="A129" s="111"/>
       <c r="B129" s="67"/>
       <c r="C129" s="67"/>
       <c r="D129" s="67"/>
@@ -4315,7 +4334,7 @@
       <c r="J129" s="67"/>
     </row>
     <row r="130" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="108">
+      <c r="A130" s="109">
         <v>44610</v>
       </c>
       <c r="B130" s="8"/>
@@ -4331,7 +4350,7 @@
       <c r="J130" s="8"/>
     </row>
     <row r="131" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="109"/>
+      <c r="A131" s="110"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
@@ -4345,7 +4364,7 @@
       <c r="J131" s="4"/>
     </row>
     <row r="132" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="109"/>
+      <c r="A132" s="110"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
@@ -4359,7 +4378,7 @@
       <c r="J132" s="4"/>
     </row>
     <row r="133" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="110"/>
+      <c r="A133" s="111"/>
       <c r="B133" s="67"/>
       <c r="C133" s="67"/>
       <c r="D133" s="67"/>
@@ -4391,7 +4410,7 @@
       <c r="J134" s="12"/>
     </row>
     <row r="135" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="108">
+      <c r="A135" s="109">
         <v>44612</v>
       </c>
       <c r="B135" s="8"/>
@@ -4407,7 +4426,7 @@
       <c r="J135" s="8"/>
     </row>
     <row r="136" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="110"/>
+      <c r="A136" s="111"/>
       <c r="B136" s="71"/>
       <c r="C136" s="71"/>
       <c r="D136" s="71"/>
@@ -4421,7 +4440,7 @@
       <c r="J136" s="71"/>
     </row>
     <row r="137" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="108">
+      <c r="A137" s="109">
         <v>44613</v>
       </c>
       <c r="B137" s="8"/>
@@ -4439,7 +4458,7 @@
       <c r="J137" s="8"/>
     </row>
     <row r="138" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="109"/>
+      <c r="A138" s="110"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
       <c r="D138" s="4"/>
@@ -4455,7 +4474,7 @@
       <c r="J138" s="4"/>
     </row>
     <row r="139" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="109"/>
+      <c r="A139" s="110"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
@@ -4469,7 +4488,7 @@
       <c r="J139" s="4"/>
     </row>
     <row r="140" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="109"/>
+      <c r="A140" s="110"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
       <c r="D140" s="4"/>
@@ -4483,7 +4502,7 @@
       <c r="J140" s="4"/>
     </row>
     <row r="141" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="109"/>
+      <c r="A141" s="110"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
       <c r="D141" s="4"/>
@@ -4497,7 +4516,7 @@
       <c r="J141" s="4"/>
     </row>
     <row r="142" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="109"/>
+      <c r="A142" s="110"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
@@ -4511,7 +4530,7 @@
       <c r="J142" s="4"/>
     </row>
     <row r="143" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="110"/>
+      <c r="A143" s="111"/>
       <c r="B143" s="72"/>
       <c r="C143" s="72"/>
       <c r="D143" s="72"/>
@@ -4525,7 +4544,7 @@
       <c r="J143" s="72"/>
     </row>
     <row r="144" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="108">
+      <c r="A144" s="109">
         <v>44614</v>
       </c>
       <c r="B144" s="8"/>
@@ -4543,7 +4562,7 @@
       <c r="J144" s="8"/>
     </row>
     <row r="145" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="109"/>
+      <c r="A145" s="110"/>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
       <c r="D145" s="4"/>
@@ -4557,7 +4576,7 @@
       <c r="J145" s="4"/>
     </row>
     <row r="146" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="109"/>
+      <c r="A146" s="110"/>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
       <c r="D146" s="4"/>
@@ -4571,7 +4590,7 @@
       <c r="J146" s="4"/>
     </row>
     <row r="147" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="109"/>
+      <c r="A147" s="110"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
       <c r="D147" s="4"/>
@@ -4585,7 +4604,7 @@
       <c r="J147" s="4"/>
     </row>
     <row r="148" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="110"/>
+      <c r="A148" s="111"/>
       <c r="B148" s="75"/>
       <c r="C148" s="75"/>
       <c r="D148" s="75"/>
@@ -4599,7 +4618,7 @@
       <c r="J148" s="75"/>
     </row>
     <row r="149" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="108">
+      <c r="A149" s="109">
         <v>44615</v>
       </c>
       <c r="B149" s="8"/>
@@ -4617,7 +4636,7 @@
       <c r="J149" s="8"/>
     </row>
     <row r="150" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="110"/>
+      <c r="A150" s="111"/>
       <c r="B150" s="75"/>
       <c r="C150" s="75"/>
       <c r="D150" s="75"/>
@@ -4631,7 +4650,7 @@
       <c r="J150" s="75"/>
     </row>
     <row r="151" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="108">
+      <c r="A151" s="109">
         <v>44616</v>
       </c>
       <c r="B151" s="8"/>
@@ -4649,7 +4668,7 @@
       <c r="J151" s="8"/>
     </row>
     <row r="152" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="109"/>
+      <c r="A152" s="110"/>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
@@ -4663,7 +4682,7 @@
       <c r="J152" s="4"/>
     </row>
     <row r="153" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="110"/>
+      <c r="A153" s="111"/>
       <c r="B153" s="76"/>
       <c r="C153" s="76"/>
       <c r="D153" s="76"/>
@@ -4677,7 +4696,7 @@
       <c r="J153" s="76"/>
     </row>
     <row r="154" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="108">
+      <c r="A154" s="109">
         <v>44617</v>
       </c>
       <c r="B154" s="8"/>
@@ -4695,7 +4714,7 @@
       <c r="J154" s="8"/>
     </row>
     <row r="155" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="109"/>
+      <c r="A155" s="110"/>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
@@ -4709,7 +4728,7 @@
       <c r="J155" s="4"/>
     </row>
     <row r="156" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="110"/>
+      <c r="A156" s="111"/>
       <c r="B156" s="77"/>
       <c r="C156" s="77"/>
       <c r="D156" s="77"/>
@@ -4723,7 +4742,7 @@
       <c r="J156" s="77"/>
     </row>
     <row r="157" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="108">
+      <c r="A157" s="109">
         <v>44618</v>
       </c>
       <c r="B157" s="8"/>
@@ -4743,7 +4762,7 @@
       <c r="J157" s="8"/>
     </row>
     <row r="158" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="110"/>
+      <c r="A158" s="111"/>
       <c r="B158" s="78"/>
       <c r="C158" s="78"/>
       <c r="D158" s="78"/>
@@ -4759,7 +4778,7 @@
       <c r="J158" s="78"/>
     </row>
     <row r="159" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="108">
+      <c r="A159" s="109">
         <v>44619</v>
       </c>
       <c r="B159" s="8"/>
@@ -4777,7 +4796,7 @@
       <c r="J159" s="8"/>
     </row>
     <row r="160" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="109"/>
+      <c r="A160" s="110"/>
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
       <c r="D160" s="4"/>
@@ -4793,7 +4812,7 @@
       <c r="J160" s="4"/>
     </row>
     <row r="161" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="110"/>
+      <c r="A161" s="111"/>
       <c r="B161" s="79"/>
       <c r="C161" s="79"/>
       <c r="D161" s="79"/>
@@ -4809,7 +4828,7 @@
       <c r="J161" s="79"/>
     </row>
     <row r="162" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="108">
+      <c r="A162" s="109">
         <v>44620</v>
       </c>
       <c r="B162" s="8"/>
@@ -4827,7 +4846,7 @@
       <c r="J162" s="8"/>
     </row>
     <row r="163" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="109"/>
+      <c r="A163" s="110"/>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
       <c r="D163" s="4"/>
@@ -4843,7 +4862,7 @@
       <c r="J163" s="4"/>
     </row>
     <row r="164" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="110"/>
+      <c r="A164" s="111"/>
       <c r="B164" s="80"/>
       <c r="C164" s="80"/>
       <c r="D164" s="80"/>
@@ -4857,7 +4876,7 @@
       <c r="J164" s="80"/>
     </row>
     <row r="165" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="108">
+      <c r="A165" s="109">
         <v>44621</v>
       </c>
       <c r="B165" s="8"/>
@@ -4873,7 +4892,7 @@
       <c r="J165" s="8"/>
     </row>
     <row r="166" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="109"/>
+      <c r="A166" s="110"/>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
@@ -4887,7 +4906,7 @@
       <c r="J166" s="4"/>
     </row>
     <row r="167" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="110"/>
+      <c r="A167" s="111"/>
       <c r="B167" s="81"/>
       <c r="C167" s="81"/>
       <c r="D167" s="81"/>
@@ -4901,7 +4920,7 @@
       <c r="J167" s="81"/>
     </row>
     <row r="168" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="108">
+      <c r="A168" s="109">
         <v>44622</v>
       </c>
       <c r="B168" s="8"/>
@@ -4922,7 +4941,7 @@
       </c>
     </row>
     <row r="169" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="109"/>
+      <c r="A169" s="110"/>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
@@ -4937,7 +4956,7 @@
       </c>
     </row>
     <row r="170" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="110"/>
+      <c r="A170" s="111"/>
       <c r="B170" s="82"/>
       <c r="C170" s="82"/>
       <c r="D170" s="82"/>
@@ -4952,7 +4971,7 @@
       </c>
     </row>
     <row r="171" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="108">
+      <c r="A171" s="109">
         <v>44623</v>
       </c>
       <c r="B171" s="8"/>
@@ -4969,7 +4988,7 @@
       <c r="K171" s="8"/>
     </row>
     <row r="172" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="109"/>
+      <c r="A172" s="110"/>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
       <c r="D172" s="4"/>
@@ -4984,7 +5003,7 @@
       <c r="K172" s="4"/>
     </row>
     <row r="173" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="110"/>
+      <c r="A173" s="111"/>
       <c r="B173" s="83"/>
       <c r="C173" s="83"/>
       <c r="D173" s="83"/>
@@ -4999,7 +5018,7 @@
       <c r="K173" s="83"/>
     </row>
     <row r="174" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="108">
+      <c r="A174" s="109">
         <v>44625</v>
       </c>
       <c r="B174" s="8"/>
@@ -5016,7 +5035,7 @@
       <c r="K174" s="8"/>
     </row>
     <row r="175" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="110"/>
+      <c r="A175" s="111"/>
       <c r="B175" s="85"/>
       <c r="C175" s="85"/>
       <c r="D175" s="85"/>
@@ -5031,7 +5050,7 @@
       <c r="K175" s="85"/>
     </row>
     <row r="176" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="108">
+      <c r="A176" s="109">
         <v>44626</v>
       </c>
       <c r="B176" s="8"/>
@@ -5049,7 +5068,7 @@
       </c>
     </row>
     <row r="177" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="109"/>
+      <c r="A177" s="110"/>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
       <c r="D177" s="4"/>
@@ -5065,7 +5084,7 @@
       </c>
     </row>
     <row r="178" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="110"/>
+      <c r="A178" s="111"/>
       <c r="B178" s="86"/>
       <c r="C178" s="86"/>
       <c r="D178" s="86"/>
@@ -5081,7 +5100,7 @@
       </c>
     </row>
     <row r="179" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="108">
+      <c r="A179" s="109">
         <v>44627</v>
       </c>
       <c r="B179" s="8"/>
@@ -5099,7 +5118,7 @@
       </c>
     </row>
     <row r="180" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="109"/>
+      <c r="A180" s="110"/>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
       <c r="D180" s="4"/>
@@ -5115,7 +5134,7 @@
       </c>
     </row>
     <row r="181" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="109"/>
+      <c r="A181" s="110"/>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
       <c r="D181" s="4"/>
@@ -5131,7 +5150,7 @@
       </c>
     </row>
     <row r="182" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A182" s="110"/>
+      <c r="A182" s="111"/>
       <c r="B182" s="88"/>
       <c r="C182" s="88"/>
       <c r="D182" s="88"/>
@@ -5144,7 +5163,7 @@
       <c r="K182" s="88"/>
     </row>
     <row r="183" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="108">
+      <c r="A183" s="109">
         <v>44628</v>
       </c>
       <c r="B183" s="8" t="s">
@@ -5161,7 +5180,7 @@
       <c r="K183" s="8"/>
     </row>
     <row r="184" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="109"/>
+      <c r="A184" s="110"/>
       <c r="B184" s="4" t="s">
         <v>400</v>
       </c>
@@ -5176,7 +5195,7 @@
       <c r="K184" s="4"/>
     </row>
     <row r="185" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="110"/>
+      <c r="A185" s="111"/>
       <c r="B185" s="91" t="s">
         <v>404</v>
       </c>
@@ -5208,7 +5227,7 @@
       <c r="K186" s="12"/>
     </row>
     <row r="187" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="108">
+      <c r="A187" s="109">
         <v>44630</v>
       </c>
       <c r="B187" s="8"/>
@@ -5225,7 +5244,7 @@
       <c r="K187" s="8"/>
     </row>
     <row r="188" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="109"/>
+      <c r="A188" s="110"/>
       <c r="B188" s="4"/>
       <c r="C188" s="4"/>
       <c r="D188" s="4"/>
@@ -5240,7 +5259,7 @@
       <c r="K188" s="4"/>
     </row>
     <row r="189" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="109"/>
+      <c r="A189" s="110"/>
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
       <c r="D189" s="4"/>
@@ -5255,7 +5274,7 @@
       <c r="K189" s="4"/>
     </row>
     <row r="190" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A190" s="109"/>
+      <c r="A190" s="110"/>
       <c r="B190" s="4"/>
       <c r="C190" s="4"/>
       <c r="D190" s="4"/>
@@ -5270,7 +5289,7 @@
       <c r="K190" s="4"/>
     </row>
     <row r="191" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A191" s="110"/>
+      <c r="A191" s="111"/>
       <c r="B191" s="93"/>
       <c r="C191" s="93"/>
       <c r="D191" s="93"/>
@@ -5285,7 +5304,7 @@
       <c r="K191" s="93"/>
     </row>
     <row r="192" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A192" s="108">
+      <c r="A192" s="109">
         <v>44631</v>
       </c>
       <c r="B192" s="8" t="s">
@@ -5302,7 +5321,7 @@
       <c r="K192" s="8"/>
     </row>
     <row r="193" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="109"/>
+      <c r="A193" s="110"/>
       <c r="B193" s="4" t="s">
         <v>423</v>
       </c>
@@ -5317,7 +5336,7 @@
       <c r="K193" s="4"/>
     </row>
     <row r="194" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="110"/>
+      <c r="A194" s="111"/>
       <c r="B194" s="93" t="s">
         <v>424</v>
       </c>
@@ -5332,7 +5351,7 @@
       <c r="K194" s="93"/>
     </row>
     <row r="195" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="108">
+      <c r="A195" s="109">
         <v>44632</v>
       </c>
       <c r="B195" s="8" t="s">
@@ -5349,7 +5368,7 @@
       <c r="K195" s="8"/>
     </row>
     <row r="196" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="109"/>
+      <c r="A196" s="110"/>
       <c r="B196" s="4" t="s">
         <v>427</v>
       </c>
@@ -5364,7 +5383,7 @@
       <c r="K196" s="4"/>
     </row>
     <row r="197" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A197" s="110"/>
+      <c r="A197" s="111"/>
       <c r="B197" s="95" t="s">
         <v>428</v>
       </c>
@@ -5379,7 +5398,7 @@
       <c r="K197" s="95"/>
     </row>
     <row r="198" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="108">
+      <c r="A198" s="109">
         <v>44633</v>
       </c>
       <c r="B198" s="8" t="s">
@@ -5396,7 +5415,7 @@
       <c r="K198" s="8"/>
     </row>
     <row r="199" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="109"/>
+      <c r="A199" s="110"/>
       <c r="B199" s="4" t="s">
         <v>432</v>
       </c>
@@ -5411,7 +5430,7 @@
       <c r="K199" s="4"/>
     </row>
     <row r="200" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A200" s="110"/>
+      <c r="A200" s="111"/>
       <c r="B200" s="96" t="s">
         <v>433</v>
       </c>
@@ -5426,7 +5445,7 @@
       <c r="K200" s="96"/>
     </row>
     <row r="201" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A201" s="108">
+      <c r="A201" s="109">
         <v>44634</v>
       </c>
       <c r="B201" s="8"/>
@@ -5443,7 +5462,7 @@
       <c r="K201" s="8"/>
     </row>
     <row r="202" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A202" s="109"/>
+      <c r="A202" s="110"/>
       <c r="B202" s="4"/>
       <c r="C202" s="4" t="s">
         <v>445</v>
@@ -5458,7 +5477,7 @@
       <c r="K202" s="4"/>
     </row>
     <row r="203" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A203" s="110"/>
+      <c r="A203" s="111"/>
       <c r="B203" s="98"/>
       <c r="C203" s="98" t="s">
         <v>446</v>
@@ -5490,7 +5509,7 @@
       <c r="K204" s="12"/>
     </row>
     <row r="205" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A205" s="108">
+      <c r="A205" s="109">
         <v>44636</v>
       </c>
       <c r="B205" s="8"/>
@@ -5507,7 +5526,7 @@
       <c r="K205" s="8"/>
     </row>
     <row r="206" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A206" s="110"/>
+      <c r="A206" s="111"/>
       <c r="B206" s="101"/>
       <c r="C206" s="101" t="s">
         <v>460</v>
@@ -5522,7 +5541,7 @@
       <c r="K206" s="101"/>
     </row>
     <row r="207" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A207" s="108">
+      <c r="A207" s="109">
         <v>44639</v>
       </c>
       <c r="B207" s="8"/>
@@ -5539,7 +5558,7 @@
       <c r="K207" s="8"/>
     </row>
     <row r="208" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A208" s="109"/>
+      <c r="A208" s="110"/>
       <c r="B208" s="4"/>
       <c r="C208" s="4" t="s">
         <v>475</v>
@@ -5554,7 +5573,7 @@
       <c r="K208" s="4"/>
     </row>
     <row r="209" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A209" s="110"/>
+      <c r="A209" s="111"/>
       <c r="B209" s="105"/>
       <c r="C209" s="105" t="s">
         <v>476</v>
@@ -5569,7 +5588,7 @@
       <c r="K209" s="105"/>
     </row>
     <row r="210" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="108">
+      <c r="A210" s="109">
         <v>44641</v>
       </c>
       <c r="B210" s="8"/>
@@ -5586,7 +5605,7 @@
       <c r="K210" s="8"/>
     </row>
     <row r="211" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A211" s="109"/>
+      <c r="A211" s="110"/>
       <c r="B211" s="4"/>
       <c r="C211" s="4" t="s">
         <v>486</v>
@@ -5601,7 +5620,7 @@
       <c r="K211" s="4"/>
     </row>
     <row r="212" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A212" s="110"/>
+      <c r="A212" s="111"/>
       <c r="B212" s="107"/>
       <c r="C212" s="107" t="s">
         <v>487</v>
@@ -10272,6 +10291,46 @@
     </row>
   </sheetData>
   <mergeCells count="56">
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="A124:A129"/>
+    <mergeCell ref="A179:A182"/>
+    <mergeCell ref="A176:A178"/>
+    <mergeCell ref="A130:A133"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="A162:A164"/>
+    <mergeCell ref="A144:A148"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="A154:A156"/>
+    <mergeCell ref="A159:A161"/>
+    <mergeCell ref="A157:A158"/>
+    <mergeCell ref="A151:A153"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="A87:A94"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="A98:A103"/>
+    <mergeCell ref="A104:A110"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="A111:A117"/>
     <mergeCell ref="A210:A212"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="A63:A66"/>
@@ -10288,46 +10347,6 @@
     <mergeCell ref="A205:A206"/>
     <mergeCell ref="A201:A203"/>
     <mergeCell ref="A192:A194"/>
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="A87:A94"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A98:A103"/>
-    <mergeCell ref="A104:A110"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A39"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="A111:A117"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="A124:A129"/>
-    <mergeCell ref="A179:A182"/>
-    <mergeCell ref="A176:A178"/>
-    <mergeCell ref="A130:A133"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="A162:A164"/>
-    <mergeCell ref="A144:A148"/>
-    <mergeCell ref="A149:A150"/>
-    <mergeCell ref="A154:A156"/>
-    <mergeCell ref="A159:A161"/>
-    <mergeCell ref="A157:A158"/>
-    <mergeCell ref="A151:A153"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10339,11 +10358,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB912B89-085A-45A1-A863-5220D2C774D8}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E38" sqref="E38"/>
+      <selection pane="bottomRight" activeCell="A37" sqref="A37:A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.25"/>
@@ -10402,7 +10421,7 @@
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="108">
+      <c r="A4" s="109">
         <v>44595</v>
       </c>
       <c r="B4" s="38"/>
@@ -10413,7 +10432,7 @@
       <c r="E4" s="38"/>
     </row>
     <row r="5" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="110"/>
+      <c r="A5" s="111"/>
       <c r="B5" s="42"/>
       <c r="C5" s="46" t="s">
         <v>161</v>
@@ -10422,7 +10441,7 @@
       <c r="E5" s="42"/>
     </row>
     <row r="6" spans="1:7" s="39" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="108">
+      <c r="A6" s="109">
         <v>44596</v>
       </c>
       <c r="B6" s="38"/>
@@ -10433,7 +10452,7 @@
       <c r="E6" s="38"/>
     </row>
     <row r="7" spans="1:7" s="43" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="110"/>
+      <c r="A7" s="111"/>
       <c r="B7" s="42"/>
       <c r="C7" s="42" t="s">
         <v>171</v>
@@ -10453,7 +10472,7 @@
       <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="108">
+      <c r="A9" s="109">
         <v>44608</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -10464,7 +10483,7 @@
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="109"/>
+      <c r="A10" s="110"/>
       <c r="B10" s="4" t="s">
         <v>237</v>
       </c>
@@ -10473,7 +10492,7 @@
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="110"/>
+      <c r="A11" s="111"/>
       <c r="B11" s="64" t="s">
         <v>238</v>
       </c>
@@ -10482,7 +10501,7 @@
       <c r="E11" s="64"/>
     </row>
     <row r="12" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="108">
+      <c r="A12" s="109">
         <v>44609</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -10493,7 +10512,7 @@
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="109"/>
+      <c r="A13" s="110"/>
       <c r="B13" s="4" t="s">
         <v>250</v>
       </c>
@@ -10502,7 +10521,7 @@
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="110"/>
+      <c r="A14" s="111"/>
       <c r="B14" s="67" t="s">
         <v>251</v>
       </c>
@@ -10533,7 +10552,7 @@
       <c r="E16" s="12"/>
     </row>
     <row r="17" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="108">
+      <c r="A17" s="109">
         <v>44616</v>
       </c>
       <c r="B17" s="8"/>
@@ -10544,7 +10563,7 @@
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="109"/>
+      <c r="A18" s="110"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
         <v>303</v>
@@ -10553,7 +10572,7 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="110"/>
+      <c r="A19" s="111"/>
       <c r="B19" s="77"/>
       <c r="C19" s="77" t="s">
         <v>304</v>
@@ -10562,7 +10581,7 @@
       <c r="E19" s="77"/>
     </row>
     <row r="20" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="108">
+      <c r="A20" s="109">
         <v>44621</v>
       </c>
       <c r="B20" s="8"/>
@@ -10573,7 +10592,7 @@
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="109"/>
+      <c r="A21" s="110"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
         <v>350</v>
@@ -10582,7 +10601,7 @@
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="110"/>
+      <c r="A22" s="111"/>
       <c r="B22" s="81"/>
       <c r="C22" s="81" t="s">
         <v>351</v>
@@ -10591,7 +10610,7 @@
       <c r="E22" s="81"/>
     </row>
     <row r="23" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="108">
+      <c r="A23" s="109">
         <v>44623</v>
       </c>
       <c r="B23" s="8"/>
@@ -10602,7 +10621,7 @@
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="110"/>
+      <c r="A24" s="111"/>
       <c r="B24" s="83"/>
       <c r="C24" s="83" t="s">
         <v>366</v>
@@ -10611,7 +10630,7 @@
       <c r="E24" s="83"/>
     </row>
     <row r="25" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="108">
+      <c r="A25" s="109">
         <v>44628</v>
       </c>
       <c r="B25" s="8"/>
@@ -10622,7 +10641,7 @@
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="109"/>
+      <c r="A26" s="110"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
         <v>396</v>
@@ -10631,7 +10650,7 @@
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="109"/>
+      <c r="A27" s="110"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
         <v>397</v>
@@ -10640,7 +10659,7 @@
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="110"/>
+      <c r="A28" s="111"/>
       <c r="B28" s="89"/>
       <c r="C28" s="89" t="s">
         <v>398</v>
@@ -10649,7 +10668,7 @@
       <c r="E28" s="89"/>
     </row>
     <row r="29" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="108">
+      <c r="A29" s="109">
         <v>44635</v>
       </c>
       <c r="B29" s="8"/>
@@ -10664,7 +10683,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="109"/>
+      <c r="A30" s="110"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
         <v>455</v>
@@ -10677,7 +10696,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="110"/>
+      <c r="A31" s="111"/>
       <c r="B31" s="99"/>
       <c r="C31" s="99" t="s">
         <v>456</v>
@@ -10705,7 +10724,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="108">
+      <c r="A33" s="109">
         <v>44640</v>
       </c>
       <c r="B33" s="8"/>
@@ -10718,7 +10737,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="110"/>
+      <c r="A34" s="111"/>
       <c r="B34" s="106"/>
       <c r="C34" s="106"/>
       <c r="D34" s="106"/>
@@ -10728,53 +10747,59 @@
         <v>481</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A35" s="100">
+    <row r="35" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="109">
         <v>44642</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3" t="s">
+      <c r="B35" s="8"/>
+      <c r="C35" s="8" t="s">
         <v>493</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3" t="s">
+      <c r="D35" s="8"/>
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+      <c r="G35" s="8" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A36" s="100"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3" t="s">
+    <row r="36" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="111"/>
+      <c r="B36" s="108"/>
+      <c r="C36" s="108" t="s">
         <v>494</v>
       </c>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3" t="s">
+      <c r="D36" s="108"/>
+      <c r="E36" s="108"/>
+      <c r="F36" s="108"/>
+      <c r="G36" s="108" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A37" s="100"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3" t="s">
+    <row r="37" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="109">
+        <v>44643</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8" t="s">
         <v>495</v>
       </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A38" s="100"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
+      <c r="D37" s="8" t="s">
+        <v>501</v>
+      </c>
+      <c r="E37" s="8"/>
+      <c r="F37" s="8"/>
+      <c r="G37" s="8"/>
+    </row>
+    <row r="38" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="111"/>
+      <c r="B38" s="108"/>
+      <c r="C38" s="108"/>
+      <c r="D38" s="108" t="s">
+        <v>502</v>
+      </c>
+      <c r="E38" s="108"/>
+      <c r="F38" s="108"/>
+      <c r="G38" s="108"/>
     </row>
     <row r="39" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A39" s="100"/>
@@ -10972,17 +10997,19 @@
       <c r="A61" s="100"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A25:A28"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="A20:A22"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="A20:A22"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10998,7 +11025,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B128" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B139" sqref="B139:B140"/>
+      <selection pane="bottomRight" activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.4"/>
@@ -11017,7 +11044,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="109">
+      <c r="A2" s="110">
         <v>44563</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -11028,35 +11055,35 @@
       </c>
     </row>
     <row r="3" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="109"/>
+      <c r="A3" s="110"/>
       <c r="B3" s="4"/>
       <c r="C3" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="109"/>
+      <c r="A4" s="110"/>
       <c r="B4" s="4"/>
       <c r="C4" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="109"/>
+      <c r="A5" s="110"/>
       <c r="B5" s="4"/>
       <c r="C5" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="110"/>
+      <c r="A6" s="111"/>
       <c r="B6" s="6"/>
       <c r="C6" s="15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="108">
+      <c r="A7" s="109">
         <v>44564</v>
       </c>
       <c r="B7" s="8"/>
@@ -11065,56 +11092,56 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="109"/>
+      <c r="A8" s="110"/>
       <c r="B8" s="4"/>
       <c r="C8" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="109"/>
+      <c r="A9" s="110"/>
       <c r="B9" s="4"/>
       <c r="C9" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="109"/>
+      <c r="A10" s="110"/>
       <c r="B10" s="4"/>
       <c r="C10" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="109"/>
+      <c r="A11" s="110"/>
       <c r="B11" s="4"/>
       <c r="C11" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="109"/>
+      <c r="A12" s="110"/>
       <c r="B12" s="4"/>
       <c r="C12" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="109"/>
+      <c r="A13" s="110"/>
       <c r="B13" s="4"/>
       <c r="C13" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="110"/>
+      <c r="A14" s="111"/>
       <c r="B14" s="6"/>
       <c r="C14" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="108">
+      <c r="A15" s="109">
         <v>44565</v>
       </c>
       <c r="B15" s="8"/>
@@ -11123,14 +11150,14 @@
       </c>
     </row>
     <row r="16" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="112"/>
+      <c r="A16" s="113"/>
       <c r="B16" s="6"/>
       <c r="C16" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="108">
+      <c r="A17" s="109">
         <v>44570</v>
       </c>
       <c r="B17" s="8"/>
@@ -11139,19 +11166,19 @@
       </c>
     </row>
     <row r="18" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="109"/>
+      <c r="A18" s="110"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="113" t="s">
+      <c r="C18" s="114" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="110"/>
+      <c r="A19" s="111"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="114"/>
+      <c r="C19" s="115"/>
     </row>
     <row r="20" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="108">
+      <c r="A20" s="109">
         <v>44574</v>
       </c>
       <c r="B20" s="8"/>
@@ -11160,21 +11187,21 @@
       </c>
     </row>
     <row r="21" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="109"/>
+      <c r="A21" s="110"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="110"/>
+      <c r="A22" s="111"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="108">
+      <c r="A23" s="109">
         <v>44590</v>
       </c>
       <c r="B23" s="8"/>
@@ -11183,28 +11210,28 @@
       </c>
     </row>
     <row r="24" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="111"/>
+      <c r="A24" s="112"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="111"/>
+      <c r="A25" s="112"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="112"/>
+      <c r="A26" s="113"/>
       <c r="B26" s="33"/>
       <c r="C26" s="33" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A27" s="108">
+      <c r="A27" s="109">
         <v>44591</v>
       </c>
       <c r="B27" s="8"/>
@@ -11213,49 +11240,49 @@
       </c>
     </row>
     <row r="28" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A28" s="109"/>
+      <c r="A28" s="110"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A29" s="109"/>
+      <c r="A29" s="110"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A30" s="109"/>
+      <c r="A30" s="110"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A31" s="109"/>
+      <c r="A31" s="110"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A32" s="109"/>
+      <c r="A32" s="110"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A33" s="110"/>
+      <c r="A33" s="111"/>
       <c r="B33" s="34"/>
       <c r="C33" s="34" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A34" s="108">
+      <c r="A34" s="109">
         <v>44593</v>
       </c>
       <c r="B34" s="8"/>
@@ -11264,14 +11291,14 @@
       </c>
     </row>
     <row r="35" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A35" s="110"/>
+      <c r="A35" s="111"/>
       <c r="B35" s="36"/>
       <c r="C35" s="36" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="39" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A36" s="108">
+      <c r="A36" s="109">
         <v>44594</v>
       </c>
       <c r="B36" s="38" t="s">
@@ -11282,35 +11309,35 @@
       </c>
     </row>
     <row r="37" spans="1:3" s="41" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A37" s="109"/>
+      <c r="A37" s="110"/>
       <c r="B37" s="40" t="s">
         <v>164</v>
       </c>
       <c r="C37" s="40"/>
     </row>
     <row r="38" spans="1:3" s="41" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A38" s="109"/>
+      <c r="A38" s="110"/>
       <c r="B38" s="40" t="s">
         <v>157</v>
       </c>
       <c r="C38" s="40"/>
     </row>
     <row r="39" spans="1:3" s="41" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A39" s="109"/>
+      <c r="A39" s="110"/>
       <c r="B39" s="40" t="s">
         <v>158</v>
       </c>
       <c r="C39" s="40"/>
     </row>
     <row r="40" spans="1:3" s="43" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A40" s="110"/>
+      <c r="A40" s="111"/>
       <c r="B40" s="42" t="s">
         <v>159</v>
       </c>
       <c r="C40" s="42"/>
     </row>
     <row r="41" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A41" s="108">
+      <c r="A41" s="109">
         <v>44595</v>
       </c>
       <c r="B41" s="8" t="s">
@@ -11321,7 +11348,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A42" s="110"/>
+      <c r="A42" s="111"/>
       <c r="B42" s="44" t="s">
         <v>166</v>
       </c>
@@ -11330,7 +11357,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A43" s="108">
+      <c r="A43" s="109">
         <v>44596</v>
       </c>
       <c r="B43" s="8" t="s">
@@ -11341,21 +11368,21 @@
       </c>
     </row>
     <row r="44" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A44" s="109"/>
+      <c r="A44" s="110"/>
       <c r="B44" s="4" t="s">
         <v>169</v>
       </c>
       <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A45" s="109"/>
+      <c r="A45" s="110"/>
       <c r="B45" s="4" t="s">
         <v>172</v>
       </c>
       <c r="C45" s="4"/>
     </row>
     <row r="46" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A46" s="110"/>
+      <c r="A46" s="111"/>
       <c r="B46" s="47" t="s">
         <v>173</v>
       </c>
@@ -11380,7 +11407,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A49" s="108">
+      <c r="A49" s="109">
         <v>44608</v>
       </c>
       <c r="B49" s="8" t="s">
@@ -11389,14 +11416,14 @@
       <c r="C49" s="8"/>
     </row>
     <row r="50" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A50" s="110"/>
+      <c r="A50" s="111"/>
       <c r="B50" s="64" t="s">
         <v>236</v>
       </c>
       <c r="C50" s="64"/>
     </row>
     <row r="51" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A51" s="108">
+      <c r="A51" s="109">
         <v>44609</v>
       </c>
       <c r="B51" s="8" t="s">
@@ -11405,14 +11432,14 @@
       <c r="C51" s="8"/>
     </row>
     <row r="52" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A52" s="110"/>
+      <c r="A52" s="111"/>
       <c r="B52" s="65" t="s">
         <v>248</v>
       </c>
       <c r="C52" s="65"/>
     </row>
     <row r="53" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A53" s="108">
+      <c r="A53" s="109">
         <v>44610</v>
       </c>
       <c r="B53" s="8" t="s">
@@ -11421,28 +11448,28 @@
       <c r="C53" s="8"/>
     </row>
     <row r="54" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A54" s="109"/>
+      <c r="A54" s="110"/>
       <c r="B54" s="4" t="s">
         <v>253</v>
       </c>
       <c r="C54" s="4"/>
     </row>
     <row r="55" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A55" s="109"/>
+      <c r="A55" s="110"/>
       <c r="B55" s="4" t="s">
         <v>258</v>
       </c>
       <c r="C55" s="4"/>
     </row>
     <row r="56" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A56" s="110"/>
+      <c r="A56" s="111"/>
       <c r="B56" s="68" t="s">
         <v>259</v>
       </c>
       <c r="C56" s="68"/>
     </row>
     <row r="57" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A57" s="108">
+      <c r="A57" s="109">
         <v>44611</v>
       </c>
       <c r="B57" s="8" t="s">
@@ -11451,28 +11478,28 @@
       <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A58" s="109"/>
+      <c r="A58" s="110"/>
       <c r="B58" s="4" t="s">
         <v>261</v>
       </c>
       <c r="C58" s="4"/>
     </row>
     <row r="59" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="109"/>
+      <c r="A59" s="110"/>
       <c r="B59" s="4" t="s">
         <v>263</v>
       </c>
       <c r="C59" s="4"/>
     </row>
     <row r="60" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A60" s="110"/>
+      <c r="A60" s="111"/>
       <c r="B60" s="70" t="s">
         <v>264</v>
       </c>
       <c r="C60" s="70"/>
     </row>
     <row r="61" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A61" s="108">
+      <c r="A61" s="109">
         <v>44612</v>
       </c>
       <c r="B61" s="8" t="s">
@@ -11481,21 +11508,21 @@
       <c r="C61" s="8"/>
     </row>
     <row r="62" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A62" s="109"/>
+      <c r="A62" s="110"/>
       <c r="B62" s="4" t="s">
         <v>266</v>
       </c>
       <c r="C62" s="4"/>
     </row>
     <row r="63" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="110"/>
+      <c r="A63" s="111"/>
       <c r="B63" s="71" t="s">
         <v>267</v>
       </c>
       <c r="C63" s="71"/>
     </row>
     <row r="64" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="108">
+      <c r="A64" s="109">
         <v>44613</v>
       </c>
       <c r="B64" s="8" t="s">
@@ -11504,14 +11531,14 @@
       <c r="C64" s="8"/>
     </row>
     <row r="65" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A65" s="110"/>
+      <c r="A65" s="111"/>
       <c r="B65" s="73" t="s">
         <v>281</v>
       </c>
       <c r="C65" s="73"/>
     </row>
     <row r="66" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A66" s="108">
+      <c r="A66" s="109">
         <v>44614</v>
       </c>
       <c r="B66" s="8" t="s">
@@ -11520,28 +11547,28 @@
       <c r="C66" s="8"/>
     </row>
     <row r="67" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A67" s="109"/>
+      <c r="A67" s="110"/>
       <c r="B67" s="4" t="s">
         <v>283</v>
       </c>
       <c r="C67" s="4"/>
     </row>
     <row r="68" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A68" s="109"/>
+      <c r="A68" s="110"/>
       <c r="B68" s="4" t="s">
         <v>291</v>
       </c>
       <c r="C68" s="4"/>
     </row>
     <row r="69" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A69" s="110"/>
+      <c r="A69" s="111"/>
       <c r="B69" s="74" t="s">
         <v>292</v>
       </c>
       <c r="C69" s="74"/>
     </row>
     <row r="70" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A70" s="108">
+      <c r="A70" s="109">
         <v>44615</v>
       </c>
       <c r="B70" s="8" t="s">
@@ -11550,14 +11577,14 @@
       <c r="C70" s="8"/>
     </row>
     <row r="71" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A71" s="109"/>
+      <c r="A71" s="110"/>
       <c r="B71" s="4" t="s">
         <v>294</v>
       </c>
       <c r="C71" s="4"/>
     </row>
     <row r="72" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A72" s="110"/>
+      <c r="A72" s="111"/>
       <c r="B72" s="75" t="s">
         <v>298</v>
       </c>
@@ -11573,7 +11600,7 @@
       <c r="C73" s="12"/>
     </row>
     <row r="74" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A74" s="108">
+      <c r="A74" s="109">
         <v>44617</v>
       </c>
       <c r="B74" s="8" t="s">
@@ -11582,21 +11609,21 @@
       <c r="C74" s="8"/>
     </row>
     <row r="75" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A75" s="109"/>
+      <c r="A75" s="110"/>
       <c r="B75" s="4" t="s">
         <v>309</v>
       </c>
       <c r="C75" s="4"/>
     </row>
     <row r="76" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A76" s="110"/>
+      <c r="A76" s="111"/>
       <c r="B76" s="77" t="s">
         <v>310</v>
       </c>
       <c r="C76" s="77"/>
     </row>
     <row r="77" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A77" s="108">
+      <c r="A77" s="109">
         <v>44618</v>
       </c>
       <c r="B77" s="8" t="s">
@@ -11605,49 +11632,49 @@
       <c r="C77" s="8"/>
     </row>
     <row r="78" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A78" s="109"/>
+      <c r="A78" s="110"/>
       <c r="B78" s="4" t="s">
         <v>315</v>
       </c>
       <c r="C78" s="4"/>
     </row>
     <row r="79" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A79" s="109"/>
+      <c r="A79" s="110"/>
       <c r="B79" s="4" t="s">
         <v>316</v>
       </c>
       <c r="C79" s="4"/>
     </row>
     <row r="80" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A80" s="109"/>
+      <c r="A80" s="110"/>
       <c r="B80" s="4" t="s">
         <v>317</v>
       </c>
       <c r="C80" s="4"/>
     </row>
     <row r="81" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A81" s="109"/>
+      <c r="A81" s="110"/>
       <c r="B81" s="4" t="s">
         <v>325</v>
       </c>
       <c r="C81" s="4"/>
     </row>
     <row r="82" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A82" s="109"/>
+      <c r="A82" s="110"/>
       <c r="B82" s="4" t="s">
         <v>326</v>
       </c>
       <c r="C82" s="4"/>
     </row>
     <row r="83" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A83" s="110"/>
+      <c r="A83" s="111"/>
       <c r="B83" s="78" t="s">
         <v>327</v>
       </c>
       <c r="C83" s="78"/>
     </row>
     <row r="84" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A84" s="108">
+      <c r="A84" s="109">
         <v>44619</v>
       </c>
       <c r="B84" s="8" t="s">
@@ -11656,14 +11683,14 @@
       <c r="C84" s="8"/>
     </row>
     <row r="85" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A85" s="110"/>
+      <c r="A85" s="111"/>
       <c r="B85" s="79" t="s">
         <v>329</v>
       </c>
       <c r="C85" s="79"/>
     </row>
     <row r="86" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A86" s="108">
+      <c r="A86" s="109">
         <v>44620</v>
       </c>
       <c r="B86" s="8" t="s">
@@ -11672,28 +11699,28 @@
       <c r="C86" s="8"/>
     </row>
     <row r="87" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A87" s="109"/>
+      <c r="A87" s="110"/>
       <c r="B87" s="4" t="s">
         <v>337</v>
       </c>
       <c r="C87" s="4"/>
     </row>
     <row r="88" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A88" s="109"/>
+      <c r="A88" s="110"/>
       <c r="B88" s="4" t="s">
         <v>338</v>
       </c>
       <c r="C88" s="4"/>
     </row>
     <row r="89" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A89" s="110"/>
+      <c r="A89" s="111"/>
       <c r="B89" s="80" t="s">
         <v>339</v>
       </c>
       <c r="C89" s="80"/>
     </row>
     <row r="90" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A90" s="108">
+      <c r="A90" s="109">
         <v>44621</v>
       </c>
       <c r="B90" s="8" t="s">
@@ -11702,28 +11729,28 @@
       <c r="C90" s="8"/>
     </row>
     <row r="91" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A91" s="109"/>
+      <c r="A91" s="110"/>
       <c r="B91" s="4" t="s">
         <v>346</v>
       </c>
       <c r="C91" s="4"/>
     </row>
     <row r="92" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A92" s="109"/>
+      <c r="A92" s="110"/>
       <c r="B92" s="4" t="s">
         <v>347</v>
       </c>
       <c r="C92" s="4"/>
     </row>
     <row r="93" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A93" s="110"/>
+      <c r="A93" s="111"/>
       <c r="B93" s="81" t="s">
         <v>348</v>
       </c>
       <c r="C93" s="81"/>
     </row>
     <row r="94" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A94" s="108">
+      <c r="A94" s="109">
         <v>44622</v>
       </c>
       <c r="B94" s="8" t="s">
@@ -11732,14 +11759,14 @@
       <c r="C94" s="8"/>
     </row>
     <row r="95" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A95" s="110"/>
+      <c r="A95" s="111"/>
       <c r="B95" s="82" t="s">
         <v>356</v>
       </c>
       <c r="C95" s="82"/>
     </row>
     <row r="96" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A96" s="108">
+      <c r="A96" s="109">
         <v>44623</v>
       </c>
       <c r="B96" s="8" t="s">
@@ -11748,14 +11775,14 @@
       <c r="C96" s="8"/>
     </row>
     <row r="97" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A97" s="110"/>
+      <c r="A97" s="111"/>
       <c r="B97" s="83" t="s">
         <v>364</v>
       </c>
       <c r="C97" s="83"/>
     </row>
     <row r="98" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A98" s="108">
+      <c r="A98" s="109">
         <v>44624</v>
       </c>
       <c r="B98" s="8" t="s">
@@ -11764,14 +11791,14 @@
       <c r="C98" s="8"/>
     </row>
     <row r="99" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A99" s="110"/>
+      <c r="A99" s="111"/>
       <c r="B99" s="84" t="s">
         <v>375</v>
       </c>
       <c r="C99" s="84"/>
     </row>
     <row r="100" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A100" s="108">
+      <c r="A100" s="109">
         <v>44625</v>
       </c>
       <c r="B100" s="8" t="s">
@@ -11780,14 +11807,14 @@
       <c r="C100" s="8"/>
     </row>
     <row r="101" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A101" s="110"/>
+      <c r="A101" s="111"/>
       <c r="B101" s="85" t="s">
         <v>380</v>
       </c>
       <c r="C101" s="85"/>
     </row>
     <row r="102" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A102" s="108">
+      <c r="A102" s="109">
         <v>44626</v>
       </c>
       <c r="B102" s="8" t="s">
@@ -11796,14 +11823,14 @@
       <c r="C102" s="8"/>
     </row>
     <row r="103" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A103" s="110"/>
+      <c r="A103" s="111"/>
       <c r="B103" s="87" t="s">
         <v>386</v>
       </c>
       <c r="C103" s="87"/>
     </row>
     <row r="104" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A104" s="108">
+      <c r="A104" s="109">
         <v>44627</v>
       </c>
       <c r="B104" s="8" t="s">
@@ -11812,7 +11839,7 @@
       <c r="C104" s="8"/>
     </row>
     <row r="105" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A105" s="110"/>
+      <c r="A105" s="111"/>
       <c r="B105" s="88" t="s">
         <v>391</v>
       </c>
@@ -11828,7 +11855,7 @@
       <c r="C106" s="12"/>
     </row>
     <row r="107" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A107" s="108">
+      <c r="A107" s="109">
         <v>44629</v>
       </c>
       <c r="B107" s="8" t="s">
@@ -11837,14 +11864,14 @@
       <c r="C107" s="8"/>
     </row>
     <row r="108" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A108" s="110"/>
+      <c r="A108" s="111"/>
       <c r="B108" s="91" t="s">
         <v>407</v>
       </c>
       <c r="C108" s="91"/>
     </row>
     <row r="109" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A109" s="108">
+      <c r="A109" s="109">
         <v>44630</v>
       </c>
       <c r="B109" s="8" t="s">
@@ -11853,14 +11880,14 @@
       <c r="C109" s="8"/>
     </row>
     <row r="110" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A110" s="110"/>
+      <c r="A110" s="111"/>
       <c r="B110" s="92" t="s">
         <v>410</v>
       </c>
       <c r="C110" s="92"/>
     </row>
     <row r="111" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A111" s="108">
+      <c r="A111" s="109">
         <v>44631</v>
       </c>
       <c r="B111" s="8" t="s">
@@ -11869,14 +11896,14 @@
       <c r="C111" s="8"/>
     </row>
     <row r="112" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A112" s="110"/>
+      <c r="A112" s="111"/>
       <c r="B112" s="93" t="s">
         <v>420</v>
       </c>
       <c r="C112" s="93"/>
     </row>
     <row r="113" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A113" s="108">
+      <c r="A113" s="109">
         <v>44632</v>
       </c>
       <c r="B113" s="8" t="s">
@@ -11885,14 +11912,14 @@
       <c r="C113" s="8"/>
     </row>
     <row r="114" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A114" s="110"/>
+      <c r="A114" s="111"/>
       <c r="B114" s="94" t="s">
         <v>425</v>
       </c>
       <c r="C114" s="94"/>
     </row>
     <row r="115" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A115" s="108">
+      <c r="A115" s="109">
         <v>44633</v>
       </c>
       <c r="B115" s="8" t="s">
@@ -11901,14 +11928,14 @@
       <c r="C115" s="8"/>
     </row>
     <row r="116" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A116" s="110"/>
+      <c r="A116" s="111"/>
       <c r="B116" s="96" t="s">
         <v>430</v>
       </c>
       <c r="C116" s="96"/>
     </row>
     <row r="117" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A117" s="108">
+      <c r="A117" s="109">
         <v>44634</v>
       </c>
       <c r="B117" s="8" t="s">
@@ -11917,14 +11944,14 @@
       <c r="C117" s="8"/>
     </row>
     <row r="118" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A118" s="110"/>
+      <c r="A118" s="111"/>
       <c r="B118" s="97" t="s">
         <v>439</v>
       </c>
       <c r="C118" s="97"/>
     </row>
     <row r="119" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A119" s="108">
+      <c r="A119" s="109">
         <v>44635</v>
       </c>
       <c r="B119" s="8" t="s">
@@ -11933,14 +11960,14 @@
       <c r="C119" s="8"/>
     </row>
     <row r="120" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A120" s="110"/>
+      <c r="A120" s="111"/>
       <c r="B120" s="98" t="s">
         <v>448</v>
       </c>
       <c r="C120" s="98"/>
     </row>
     <row r="121" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A121" s="108">
+      <c r="A121" s="109">
         <v>44636</v>
       </c>
       <c r="B121" s="8" t="s">
@@ -11949,14 +11976,14 @@
       <c r="C121" s="8"/>
     </row>
     <row r="122" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A122" s="110"/>
+      <c r="A122" s="111"/>
       <c r="B122" s="99" t="s">
         <v>458</v>
       </c>
       <c r="C122" s="99"/>
     </row>
     <row r="123" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A123" s="108">
+      <c r="A123" s="109">
         <v>44637</v>
       </c>
       <c r="B123" s="8" t="s">
@@ -11965,28 +11992,28 @@
       <c r="C123" s="8"/>
     </row>
     <row r="124" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A124" s="109"/>
+      <c r="A124" s="110"/>
       <c r="B124" s="4" t="s">
         <v>464</v>
       </c>
       <c r="C124" s="4"/>
     </row>
     <row r="125" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A125" s="109"/>
+      <c r="A125" s="110"/>
       <c r="B125" s="4" t="s">
         <v>465</v>
       </c>
       <c r="C125" s="4"/>
     </row>
     <row r="126" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A126" s="110"/>
+      <c r="A126" s="111"/>
       <c r="B126" s="102" t="s">
         <v>466</v>
       </c>
       <c r="C126" s="102"/>
     </row>
     <row r="127" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A127" s="108">
+      <c r="A127" s="109">
         <v>44638</v>
       </c>
       <c r="B127" s="8" t="s">
@@ -11995,14 +12022,14 @@
       <c r="C127" s="8"/>
     </row>
     <row r="128" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A128" s="110"/>
+      <c r="A128" s="111"/>
       <c r="B128" s="103" t="s">
         <v>469</v>
       </c>
       <c r="C128" s="103"/>
     </row>
     <row r="129" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A129" s="108">
+      <c r="A129" s="109">
         <v>44639</v>
       </c>
       <c r="B129" s="8" t="s">
@@ -12011,14 +12038,14 @@
       <c r="C129" s="8"/>
     </row>
     <row r="130" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A130" s="110"/>
+      <c r="A130" s="111"/>
       <c r="B130" s="104" t="s">
         <v>471</v>
       </c>
       <c r="C130" s="104"/>
     </row>
     <row r="131" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A131" s="108">
+      <c r="A131" s="109">
         <v>44640</v>
       </c>
       <c r="B131" s="8" t="s">
@@ -12027,21 +12054,21 @@
       <c r="C131" s="8"/>
     </row>
     <row r="132" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A132" s="109"/>
+      <c r="A132" s="110"/>
       <c r="B132" s="4" t="s">
         <v>478</v>
       </c>
       <c r="C132" s="4"/>
     </row>
     <row r="133" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A133" s="110"/>
+      <c r="A133" s="111"/>
       <c r="B133" s="105" t="s">
         <v>479</v>
       </c>
       <c r="C133" s="105"/>
     </row>
     <row r="134" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A134" s="108">
+      <c r="A134" s="109">
         <v>44641</v>
       </c>
       <c r="B134" s="8" t="s">
@@ -12050,44 +12077,50 @@
       <c r="C134" s="8"/>
     </row>
     <row r="135" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A135" s="109"/>
+      <c r="A135" s="110"/>
       <c r="B135" s="4" t="s">
         <v>483</v>
       </c>
       <c r="C135" s="4"/>
     </row>
     <row r="136" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A136" s="110"/>
+      <c r="A136" s="111"/>
       <c r="B136" s="107" t="s">
         <v>484</v>
       </c>
       <c r="C136" s="107"/>
     </row>
-    <row r="137" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A137" s="28">
+    <row r="137" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A137" s="109">
         <v>44642</v>
       </c>
-      <c r="B137" s="3" t="s">
+      <c r="B137" s="8" t="s">
         <v>492</v>
       </c>
-      <c r="C137" s="3"/>
-    </row>
-    <row r="138" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A138" s="28"/>
-      <c r="B138" s="3" t="s">
+      <c r="C137" s="8"/>
+    </row>
+    <row r="138" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A138" s="111"/>
+      <c r="B138" s="108" t="s">
         <v>496</v>
       </c>
-      <c r="C138" s="3"/>
-    </row>
-    <row r="139" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A139" s="28"/>
-      <c r="B139" s="3"/>
-      <c r="C139" s="3"/>
-    </row>
-    <row r="140" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A140" s="28"/>
-      <c r="B140" s="3"/>
-      <c r="C140" s="3"/>
+      <c r="C138" s="108"/>
+    </row>
+    <row r="139" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A139" s="109">
+        <v>44643</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="C139" s="8"/>
+    </row>
+    <row r="140" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A140" s="111"/>
+      <c r="B140" s="108" t="s">
+        <v>500</v>
+      </c>
+      <c r="C140" s="108"/>
     </row>
     <row r="141" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A141" s="28"/>
@@ -12598,39 +12631,9 @@
       <c r="C242" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="A134:A136"/>
-    <mergeCell ref="A119:A120"/>
-    <mergeCell ref="A117:A118"/>
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="A113:A114"/>
-    <mergeCell ref="A131:A133"/>
-    <mergeCell ref="A129:A130"/>
-    <mergeCell ref="A127:A128"/>
-    <mergeCell ref="A123:A126"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A34:A35"/>
+  <mergeCells count="46">
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="A139:A140"/>
     <mergeCell ref="A61:A63"/>
     <mergeCell ref="A57:A60"/>
     <mergeCell ref="A53:A56"/>
@@ -12643,6 +12646,38 @@
     <mergeCell ref="A70:A72"/>
     <mergeCell ref="A66:A69"/>
     <mergeCell ref="A84:A85"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="A134:A136"/>
+    <mergeCell ref="A119:A120"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="A131:A133"/>
+    <mergeCell ref="A129:A130"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="A123:A126"/>
+    <mergeCell ref="A121:A122"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12654,11 +12689,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1FB6486-C5E6-414E-A2BA-E553A6C57EC0}">
   <dimension ref="A1:Q188"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
+      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -12687,7 +12722,7 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:17" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="108">
+      <c r="A2" s="109">
         <v>44623</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -12695,19 +12730,19 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A3" s="109"/>
+      <c r="A3" s="110"/>
       <c r="B3" s="4" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A4" s="110"/>
+      <c r="A4" s="111"/>
       <c r="B4" s="83" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="108">
+      <c r="A5" s="109">
         <v>44624</v>
       </c>
       <c r="B5" s="31" t="s">
@@ -12715,13 +12750,13 @@
       </c>
     </row>
     <row r="6" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="109"/>
+      <c r="A6" s="110"/>
       <c r="B6" s="52" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="110"/>
+      <c r="A7" s="111"/>
       <c r="B7" s="54" t="s">
         <v>378</v>
       </c>
@@ -12735,7 +12770,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="108">
+      <c r="A9" s="109">
         <v>44628</v>
       </c>
       <c r="B9" s="31"/>
@@ -12758,7 +12793,7 @@
       <c r="Q9" s="31"/>
     </row>
     <row r="10" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="110"/>
+      <c r="A10" s="111"/>
       <c r="B10" s="54"/>
       <c r="C10" s="54" t="s">
         <v>403</v>
@@ -12779,7 +12814,7 @@
       <c r="Q10" s="54"/>
     </row>
     <row r="11" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="108">
+      <c r="A11" s="109">
         <v>44630</v>
       </c>
       <c r="B11" s="31"/>
@@ -12802,7 +12837,7 @@
       <c r="Q11" s="31"/>
     </row>
     <row r="12" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="109"/>
+      <c r="A12" s="110"/>
       <c r="B12" s="52"/>
       <c r="C12" s="52" t="s">
         <v>417</v>
@@ -12823,7 +12858,7 @@
       <c r="Q12" s="52"/>
     </row>
     <row r="13" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="110"/>
+      <c r="A13" s="111"/>
       <c r="B13" s="54"/>
       <c r="C13" s="54" t="s">
         <v>418</v>
@@ -12844,7 +12879,7 @@
       <c r="Q13" s="54"/>
     </row>
     <row r="14" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="108">
+      <c r="A14" s="109">
         <v>44633</v>
       </c>
       <c r="B14" s="31"/>
@@ -12867,7 +12902,7 @@
       <c r="Q14" s="31"/>
     </row>
     <row r="15" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="109"/>
+      <c r="A15" s="110"/>
       <c r="B15" s="52"/>
       <c r="C15" s="52" t="s">
         <v>435</v>
@@ -12888,7 +12923,7 @@
       <c r="Q15" s="52"/>
     </row>
     <row r="16" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="109"/>
+      <c r="A16" s="110"/>
       <c r="B16" s="52"/>
       <c r="C16" s="52" t="s">
         <v>436</v>
@@ -12909,7 +12944,7 @@
       <c r="Q16" s="52"/>
     </row>
     <row r="17" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="110"/>
+      <c r="A17" s="111"/>
       <c r="B17" s="54"/>
       <c r="C17" s="54" t="s">
         <v>437</v>
@@ -12930,7 +12965,7 @@
       <c r="Q17" s="54"/>
     </row>
     <row r="18" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="108">
+      <c r="A18" s="109">
         <v>44634</v>
       </c>
       <c r="B18" s="31"/>
@@ -12953,7 +12988,7 @@
       <c r="Q18" s="31"/>
     </row>
     <row r="19" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="109"/>
+      <c r="A19" s="110"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52" t="s">
         <v>441</v>
@@ -12974,7 +13009,7 @@
       <c r="Q19" s="52"/>
     </row>
     <row r="20" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="109"/>
+      <c r="A20" s="110"/>
       <c r="B20" s="52"/>
       <c r="C20" s="52" t="s">
         <v>442</v>
@@ -12995,7 +13030,7 @@
       <c r="Q20" s="52"/>
     </row>
     <row r="21" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="110"/>
+      <c r="A21" s="111"/>
       <c r="B21" s="54"/>
       <c r="C21" s="54" t="s">
         <v>443</v>
@@ -13016,7 +13051,7 @@
       <c r="Q21" s="54"/>
     </row>
     <row r="22" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="108">
+      <c r="A22" s="109">
         <v>44636</v>
       </c>
       <c r="B22" s="31"/>
@@ -13039,7 +13074,7 @@
       <c r="Q22" s="31"/>
     </row>
     <row r="23" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="110"/>
+      <c r="A23" s="111"/>
       <c r="B23" s="54"/>
       <c r="C23" s="54" t="s">
         <v>462</v>
@@ -13060,7 +13095,7 @@
       <c r="Q23" s="54"/>
     </row>
     <row r="24" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="108">
+      <c r="A24" s="109">
         <v>44639</v>
       </c>
       <c r="B24" s="31"/>
@@ -13083,7 +13118,7 @@
       <c r="Q24" s="31"/>
     </row>
     <row r="25" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="110"/>
+      <c r="A25" s="111"/>
       <c r="B25" s="54"/>
       <c r="C25" s="54" t="s">
         <v>473</v>
@@ -13104,7 +13139,7 @@
       <c r="Q25" s="54"/>
     </row>
     <row r="26" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="108">
+      <c r="A26" s="109">
         <v>44641</v>
       </c>
       <c r="B26" s="31" t="s">
@@ -13127,7 +13162,7 @@
       <c r="Q26" s="31"/>
     </row>
     <row r="27" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="109"/>
+      <c r="A27" s="110"/>
       <c r="B27" s="52" t="s">
         <v>489</v>
       </c>
@@ -13148,7 +13183,7 @@
       <c r="Q27" s="52"/>
     </row>
     <row r="28" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="109"/>
+      <c r="A28" s="110"/>
       <c r="B28" s="52" t="s">
         <v>490</v>
       </c>
@@ -13169,7 +13204,7 @@
       <c r="Q28" s="52"/>
     </row>
     <row r="29" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="110"/>
+      <c r="A29" s="111"/>
       <c r="B29" s="54" t="s">
         <v>491</v>
       </c>

</xml_diff>

<commit_message>
I've forgotten what I'd done ...... sounds bad
</commit_message>
<xml_diff>
--- a/学习记录.xlsx
+++ b/学习记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\不怕晒的铃铛\Desktop\学习资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C677D5-EF4C-4CED-BEC7-04D436CB1870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{489C35F1-58B3-4917-B31C-ED4B6D4303CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JavaWeb相关" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="512">
   <si>
     <t>JavaSE</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2074,6 +2074,14 @@
   </si>
   <si>
     <t>用户权限管理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无重叠区间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>划分字母区间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2181,7 +2189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2471,6 +2479,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2806,7 +2817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P623"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="J208" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2880,7 +2891,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="111">
+      <c r="A3" s="112">
         <v>44566</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -2890,7 +2901,7 @@
       <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:16" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="112"/>
+      <c r="A4" s="113"/>
       <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
@@ -2898,7 +2909,7 @@
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:16" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="113"/>
+      <c r="A5" s="114"/>
       <c r="B5" s="6" t="s">
         <v>28</v>
       </c>
@@ -2936,7 +2947,7 @@
       <c r="D8" s="12"/>
     </row>
     <row r="9" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="111">
+      <c r="A9" s="112">
         <v>44572</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -2946,7 +2957,7 @@
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:16" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="113"/>
+      <c r="A10" s="114"/>
       <c r="B10" s="17" t="s">
         <v>38</v>
       </c>
@@ -2954,7 +2965,7 @@
       <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="111">
+      <c r="A11" s="112">
         <v>44573</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -2964,7 +2975,7 @@
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="112"/>
+      <c r="A12" s="113"/>
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
@@ -2972,7 +2983,7 @@
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="113"/>
+      <c r="A13" s="114"/>
       <c r="B13" s="18" t="s">
         <v>40</v>
       </c>
@@ -2980,7 +2991,7 @@
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="111">
+      <c r="A14" s="112">
         <v>44574</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -2990,7 +3001,7 @@
       <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:16" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="113"/>
+      <c r="A15" s="114"/>
       <c r="B15" s="19" t="s">
         <v>42</v>
       </c>
@@ -3000,7 +3011,7 @@
       <c r="D15" s="19"/>
     </row>
     <row r="16" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="111">
+      <c r="A16" s="112">
         <v>44575</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -3012,7 +3023,7 @@
       <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="112"/>
+      <c r="A17" s="113"/>
       <c r="B17" s="4" t="s">
         <v>47</v>
       </c>
@@ -3023,7 +3034,7 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="112"/>
+      <c r="A18" s="113"/>
       <c r="B18" s="4" t="s">
         <v>48</v>
       </c>
@@ -3034,7 +3045,7 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="113"/>
+      <c r="A19" s="114"/>
       <c r="B19" s="20" t="s">
         <v>49</v>
       </c>
@@ -3043,7 +3054,7 @@
       <c r="E19" s="21"/>
     </row>
     <row r="20" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="111">
+      <c r="A20" s="112">
         <v>44576</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -3056,7 +3067,7 @@
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="112"/>
+      <c r="A21" s="113"/>
       <c r="B21" s="4" t="s">
         <v>59</v>
       </c>
@@ -3067,7 +3078,7 @@
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="112"/>
+      <c r="A22" s="113"/>
       <c r="B22" s="4" t="s">
         <v>60</v>
       </c>
@@ -3078,7 +3089,7 @@
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="113"/>
+      <c r="A23" s="114"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20" t="s">
         <v>57</v>
@@ -3087,7 +3098,7 @@
       <c r="E23" s="21"/>
     </row>
     <row r="24" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="111">
+      <c r="A24" s="112">
         <v>44577</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -3102,7 +3113,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="112"/>
+      <c r="A25" s="113"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
         <v>63</v>
@@ -3113,7 +3124,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="113"/>
+      <c r="A26" s="114"/>
       <c r="B26" s="21"/>
       <c r="C26" s="21" t="s">
         <v>64</v>
@@ -3124,7 +3135,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="111">
+      <c r="A27" s="112">
         <v>44578</v>
       </c>
       <c r="B27" s="8" t="s">
@@ -3135,7 +3146,7 @@
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="112"/>
+      <c r="A28" s="113"/>
       <c r="B28" s="4" t="s">
         <v>69</v>
       </c>
@@ -3144,7 +3155,7 @@
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="112"/>
+      <c r="A29" s="113"/>
       <c r="B29" s="4" t="s">
         <v>70</v>
       </c>
@@ -3153,7 +3164,7 @@
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="113"/>
+      <c r="A30" s="114"/>
       <c r="B30" s="22" t="s">
         <v>71</v>
       </c>
@@ -3162,7 +3173,7 @@
       <c r="E30" s="22"/>
     </row>
     <row r="31" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="111">
+      <c r="A31" s="112">
         <v>44579</v>
       </c>
       <c r="B31" s="8" t="s">
@@ -3177,7 +3188,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="113"/>
+      <c r="A32" s="114"/>
       <c r="B32" s="22" t="s">
         <v>73</v>
       </c>
@@ -3188,7 +3199,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="111">
+      <c r="A33" s="112">
         <v>44580</v>
       </c>
       <c r="B33" s="8" t="s">
@@ -3202,7 +3213,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="113"/>
+      <c r="A34" s="114"/>
       <c r="B34" s="23" t="s">
         <v>83</v>
       </c>
@@ -3211,7 +3222,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="111">
+      <c r="A35" s="112">
         <v>44581</v>
       </c>
       <c r="B35" s="8" t="s">
@@ -3223,7 +3234,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="112"/>
+      <c r="A36" s="113"/>
       <c r="B36" s="4" t="s">
         <v>85</v>
       </c>
@@ -3233,7 +3244,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="112"/>
+      <c r="A37" s="113"/>
       <c r="B37" s="4" t="s">
         <v>86</v>
       </c>
@@ -3241,7 +3252,7 @@
       <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="112"/>
+      <c r="A38" s="113"/>
       <c r="B38" s="4" t="s">
         <v>87</v>
       </c>
@@ -3249,7 +3260,7 @@
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="113"/>
+      <c r="A39" s="114"/>
       <c r="B39" s="23" t="s">
         <v>88</v>
       </c>
@@ -3257,7 +3268,7 @@
       <c r="D39" s="23"/>
     </row>
     <row r="40" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="111">
+      <c r="A40" s="112">
         <v>44582</v>
       </c>
       <c r="B40" s="8" t="s">
@@ -3274,7 +3285,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="114"/>
+      <c r="A41" s="115"/>
       <c r="B41" s="4" t="s">
         <v>91</v>
       </c>
@@ -3286,7 +3297,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="114"/>
+      <c r="A42" s="115"/>
       <c r="B42" s="4" t="s">
         <v>98</v>
       </c>
@@ -3296,7 +3307,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="115"/>
+      <c r="A43" s="116"/>
       <c r="B43" s="24" t="s">
         <v>99</v>
       </c>
@@ -3306,7 +3317,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="111">
+      <c r="A44" s="112">
         <v>44583</v>
       </c>
       <c r="B44" s="8" t="s">
@@ -3316,7 +3327,7 @@
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="112"/>
+      <c r="A45" s="113"/>
       <c r="B45" s="4" t="s">
         <v>101</v>
       </c>
@@ -3324,7 +3335,7 @@
       <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="112"/>
+      <c r="A46" s="113"/>
       <c r="B46" s="4" t="s">
         <v>102</v>
       </c>
@@ -3332,7 +3343,7 @@
       <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="112"/>
+      <c r="A47" s="113"/>
       <c r="B47" s="4" t="s">
         <v>103</v>
       </c>
@@ -3340,7 +3351,7 @@
       <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="112"/>
+      <c r="A48" s="113"/>
       <c r="B48" s="4" t="s">
         <v>104</v>
       </c>
@@ -3348,7 +3359,7 @@
       <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="113"/>
+      <c r="A49" s="114"/>
       <c r="B49" s="25" t="s">
         <v>105</v>
       </c>
@@ -3356,7 +3367,7 @@
       <c r="D49" s="25"/>
     </row>
     <row r="50" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="111">
+      <c r="A50" s="112">
         <v>44584</v>
       </c>
       <c r="B50" s="8" t="s">
@@ -3366,7 +3377,7 @@
       <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="114"/>
+      <c r="A51" s="115"/>
       <c r="B51" s="4" t="s">
         <v>107</v>
       </c>
@@ -3374,7 +3385,7 @@
       <c r="D51" s="4"/>
     </row>
     <row r="52" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="114"/>
+      <c r="A52" s="115"/>
       <c r="B52" s="4" t="s">
         <v>108</v>
       </c>
@@ -3382,7 +3393,7 @@
       <c r="D52" s="4"/>
     </row>
     <row r="53" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="115"/>
+      <c r="A53" s="116"/>
       <c r="B53" s="26" t="s">
         <v>109</v>
       </c>
@@ -3390,7 +3401,7 @@
       <c r="D53" s="26"/>
     </row>
     <row r="54" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="111">
+      <c r="A54" s="112">
         <v>44585</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -3400,7 +3411,7 @@
       <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="113"/>
+      <c r="A55" s="114"/>
       <c r="B55" s="27" t="s">
         <v>111</v>
       </c>
@@ -3408,7 +3419,7 @@
       <c r="D55" s="27"/>
     </row>
     <row r="56" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="111">
+      <c r="A56" s="112">
         <v>44586</v>
       </c>
       <c r="B56" s="8"/>
@@ -3423,7 +3434,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="112"/>
+      <c r="A57" s="113"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4" t="s">
@@ -3432,7 +3443,7 @@
       <c r="E57" s="4"/>
     </row>
     <row r="58" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="113"/>
+      <c r="A58" s="114"/>
       <c r="B58" s="27"/>
       <c r="C58" s="27"/>
       <c r="D58" s="27" t="s">
@@ -3441,7 +3452,7 @@
       <c r="E58" s="27"/>
     </row>
     <row r="59" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="111">
+      <c r="A59" s="112">
         <v>44587</v>
       </c>
       <c r="B59" s="8"/>
@@ -3456,7 +3467,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="112"/>
+      <c r="A60" s="113"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4" t="s">
         <v>120</v>
@@ -3466,7 +3477,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="112"/>
+      <c r="A61" s="113"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4" t="s">
         <v>123</v>
@@ -3477,7 +3488,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="113"/>
+      <c r="A62" s="114"/>
       <c r="B62" s="29"/>
       <c r="C62" s="29" t="s">
         <v>124</v>
@@ -3486,7 +3497,7 @@
       <c r="E62" s="29"/>
     </row>
     <row r="63" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="111">
+      <c r="A63" s="112">
         <v>44588</v>
       </c>
       <c r="B63" s="8"/>
@@ -3501,7 +3512,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="112"/>
+      <c r="A64" s="113"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4" t="s">
         <v>126</v>
@@ -3512,7 +3523,7 @@
       <c r="E64" s="4"/>
     </row>
     <row r="65" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="112"/>
+      <c r="A65" s="113"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4" t="s">
         <v>127</v>
@@ -3523,7 +3534,7 @@
       <c r="E65" s="4"/>
     </row>
     <row r="66" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="113"/>
+      <c r="A66" s="114"/>
       <c r="B66" s="30"/>
       <c r="C66" s="30" t="s">
         <v>128</v>
@@ -3532,7 +3543,7 @@
       <c r="E66" s="30"/>
     </row>
     <row r="67" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="111">
+      <c r="A67" s="112">
         <v>44589</v>
       </c>
       <c r="B67" s="8"/>
@@ -3543,7 +3554,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="112"/>
+      <c r="A68" s="113"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -3552,7 +3563,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="113"/>
+      <c r="A69" s="114"/>
       <c r="B69" s="32"/>
       <c r="C69" s="32"/>
       <c r="D69" s="32"/>
@@ -3585,7 +3596,7 @@
       </c>
     </row>
     <row r="72" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="111">
+      <c r="A72" s="112">
         <v>44594</v>
       </c>
       <c r="B72" s="8"/>
@@ -3596,7 +3607,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="112"/>
+      <c r="A73" s="113"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
@@ -3605,7 +3616,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="112"/>
+      <c r="A74" s="113"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
@@ -3614,7 +3625,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="113"/>
+      <c r="A75" s="114"/>
       <c r="B75" s="37"/>
       <c r="C75" s="37"/>
       <c r="D75" s="37"/>
@@ -3645,7 +3656,7 @@
       </c>
     </row>
     <row r="78" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="111">
+      <c r="A78" s="112">
         <v>44598</v>
       </c>
       <c r="B78" s="8"/>
@@ -3656,7 +3667,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="112"/>
+      <c r="A79" s="113"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
@@ -3665,7 +3676,7 @@
       </c>
     </row>
     <row r="80" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="112"/>
+      <c r="A80" s="113"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -3674,7 +3685,7 @@
       </c>
     </row>
     <row r="81" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="113"/>
+      <c r="A81" s="114"/>
       <c r="B81" s="48"/>
       <c r="C81" s="48"/>
       <c r="D81" s="48"/>
@@ -3683,7 +3694,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="111">
+      <c r="A82" s="112">
         <v>44599</v>
       </c>
       <c r="B82" s="8"/>
@@ -3694,7 +3705,7 @@
       </c>
     </row>
     <row r="83" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="112"/>
+      <c r="A83" s="113"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
@@ -3703,7 +3714,7 @@
       </c>
     </row>
     <row r="84" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="113"/>
+      <c r="A84" s="114"/>
       <c r="B84" s="49"/>
       <c r="C84" s="49"/>
       <c r="D84" s="49"/>
@@ -3712,7 +3723,7 @@
       </c>
     </row>
     <row r="85" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="111">
+      <c r="A85" s="112">
         <v>44600</v>
       </c>
       <c r="B85" s="8"/>
@@ -3730,7 +3741,7 @@
       <c r="J85" s="8"/>
     </row>
     <row r="86" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="113"/>
+      <c r="A86" s="114"/>
       <c r="B86" s="50"/>
       <c r="C86" s="50"/>
       <c r="D86" s="50"/>
@@ -3744,7 +3755,7 @@
       <c r="J86" s="50"/>
     </row>
     <row r="87" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="111">
+      <c r="A87" s="112">
         <v>44601</v>
       </c>
       <c r="B87" s="8"/>
@@ -3762,7 +3773,7 @@
       <c r="J87" s="8"/>
     </row>
     <row r="88" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="112"/>
+      <c r="A88" s="113"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4" t="s">
@@ -3778,7 +3789,7 @@
       <c r="J88" s="4"/>
     </row>
     <row r="89" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="112"/>
+      <c r="A89" s="113"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4" t="s">
@@ -3794,7 +3805,7 @@
       <c r="J89" s="4"/>
     </row>
     <row r="90" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="112"/>
+      <c r="A90" s="113"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4" t="s">
@@ -3808,7 +3819,7 @@
       <c r="J90" s="4"/>
     </row>
     <row r="91" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="112"/>
+      <c r="A91" s="113"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4" t="s">
@@ -3822,7 +3833,7 @@
       <c r="J91" s="4"/>
     </row>
     <row r="92" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="112"/>
+      <c r="A92" s="113"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="52" t="s">
@@ -3836,7 +3847,7 @@
       <c r="J92" s="4"/>
     </row>
     <row r="93" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="112"/>
+      <c r="A93" s="113"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4" t="s">
@@ -3850,7 +3861,7 @@
       <c r="J93" s="4"/>
     </row>
     <row r="94" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="113"/>
+      <c r="A94" s="114"/>
       <c r="B94" s="51"/>
       <c r="C94" s="51"/>
       <c r="D94" s="54" t="s">
@@ -3864,7 +3875,7 @@
       <c r="J94" s="51"/>
     </row>
     <row r="95" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="111">
+      <c r="A95" s="112">
         <v>44602</v>
       </c>
       <c r="B95" s="8"/>
@@ -3882,7 +3893,7 @@
       <c r="J95" s="8"/>
     </row>
     <row r="96" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="112"/>
+      <c r="A96" s="113"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4" t="s">
@@ -3898,7 +3909,7 @@
       <c r="J96" s="4"/>
     </row>
     <row r="97" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="113"/>
+      <c r="A97" s="114"/>
       <c r="B97" s="53"/>
       <c r="C97" s="53"/>
       <c r="D97" s="53"/>
@@ -3912,7 +3923,7 @@
       <c r="J97" s="53"/>
     </row>
     <row r="98" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="111">
+      <c r="A98" s="112">
         <v>44603</v>
       </c>
       <c r="B98" s="8"/>
@@ -3928,7 +3939,7 @@
       <c r="J98" s="8"/>
     </row>
     <row r="99" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="112"/>
+      <c r="A99" s="113"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
@@ -3942,7 +3953,7 @@
       <c r="J99" s="4"/>
     </row>
     <row r="100" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="112"/>
+      <c r="A100" s="113"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
@@ -3956,7 +3967,7 @@
       <c r="J100" s="4"/>
     </row>
     <row r="101" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="112"/>
+      <c r="A101" s="113"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
@@ -3970,7 +3981,7 @@
       <c r="J101" s="4"/>
     </row>
     <row r="102" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="112"/>
+      <c r="A102" s="113"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
@@ -3984,7 +3995,7 @@
       <c r="J102" s="4"/>
     </row>
     <row r="103" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="113"/>
+      <c r="A103" s="114"/>
       <c r="B103" s="55"/>
       <c r="C103" s="55"/>
       <c r="D103" s="55"/>
@@ -3998,7 +4009,7 @@
       <c r="J103" s="55"/>
     </row>
     <row r="104" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="111">
+      <c r="A104" s="112">
         <v>44604</v>
       </c>
       <c r="B104" s="8"/>
@@ -4014,7 +4025,7 @@
       <c r="J104" s="8"/>
     </row>
     <row r="105" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="112"/>
+      <c r="A105" s="113"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
@@ -4028,7 +4039,7 @@
       <c r="J105" s="4"/>
     </row>
     <row r="106" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="112"/>
+      <c r="A106" s="113"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
@@ -4042,7 +4053,7 @@
       <c r="J106" s="4"/>
     </row>
     <row r="107" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="112"/>
+      <c r="A107" s="113"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
@@ -4056,7 +4067,7 @@
       <c r="J107" s="4"/>
     </row>
     <row r="108" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="112"/>
+      <c r="A108" s="113"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
@@ -4070,7 +4081,7 @@
       <c r="J108" s="4"/>
     </row>
     <row r="109" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="112"/>
+      <c r="A109" s="113"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
@@ -4084,7 +4095,7 @@
       <c r="J109" s="4"/>
     </row>
     <row r="110" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="113"/>
+      <c r="A110" s="114"/>
       <c r="B110" s="56"/>
       <c r="C110" s="56"/>
       <c r="D110" s="56"/>
@@ -4098,7 +4109,7 @@
       <c r="J110" s="56"/>
     </row>
     <row r="111" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="111">
+      <c r="A111" s="112">
         <v>44605</v>
       </c>
       <c r="B111" s="8"/>
@@ -4114,7 +4125,7 @@
       <c r="J111" s="8"/>
     </row>
     <row r="112" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="112"/>
+      <c r="A112" s="113"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
@@ -4128,7 +4139,7 @@
       <c r="J112" s="4"/>
     </row>
     <row r="113" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="112"/>
+      <c r="A113" s="113"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
@@ -4142,7 +4153,7 @@
       <c r="J113" s="4"/>
     </row>
     <row r="114" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="112"/>
+      <c r="A114" s="113"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
@@ -4156,7 +4167,7 @@
       <c r="J114" s="4"/>
     </row>
     <row r="115" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="112"/>
+      <c r="A115" s="113"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
@@ -4170,7 +4181,7 @@
       <c r="J115" s="4"/>
     </row>
     <row r="116" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="112"/>
+      <c r="A116" s="113"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
@@ -4184,7 +4195,7 @@
       <c r="J116" s="4"/>
     </row>
     <row r="117" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="113"/>
+      <c r="A117" s="114"/>
       <c r="B117" s="57"/>
       <c r="C117" s="57"/>
       <c r="D117" s="57"/>
@@ -4198,7 +4209,7 @@
       <c r="J117" s="57"/>
     </row>
     <row r="118" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="111">
+      <c r="A118" s="112">
         <v>44606</v>
       </c>
       <c r="B118" s="8"/>
@@ -4214,7 +4225,7 @@
       <c r="J118" s="8"/>
     </row>
     <row r="119" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="113"/>
+      <c r="A119" s="114"/>
       <c r="B119" s="58"/>
       <c r="C119" s="58"/>
       <c r="D119" s="58"/>
@@ -4228,7 +4239,7 @@
       <c r="J119" s="58"/>
     </row>
     <row r="120" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="111">
+      <c r="A120" s="112">
         <v>44607</v>
       </c>
       <c r="B120" s="8"/>
@@ -4244,7 +4255,7 @@
       <c r="J120" s="8"/>
     </row>
     <row r="121" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="113"/>
+      <c r="A121" s="114"/>
       <c r="B121" s="58"/>
       <c r="C121" s="58"/>
       <c r="D121" s="58"/>
@@ -4288,7 +4299,7 @@
       <c r="J123" s="64"/>
     </row>
     <row r="124" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="111">
+      <c r="A124" s="112">
         <v>44609</v>
       </c>
       <c r="B124" s="8"/>
@@ -4304,7 +4315,7 @@
       <c r="J124" s="8"/>
     </row>
     <row r="125" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="112"/>
+      <c r="A125" s="113"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
@@ -4318,7 +4329,7 @@
       <c r="J125" s="4"/>
     </row>
     <row r="126" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="112"/>
+      <c r="A126" s="113"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
@@ -4332,7 +4343,7 @@
       <c r="J126" s="4"/>
     </row>
     <row r="127" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="112"/>
+      <c r="A127" s="113"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
@@ -4346,7 +4357,7 @@
       <c r="J127" s="4"/>
     </row>
     <row r="128" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="112"/>
+      <c r="A128" s="113"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
@@ -4360,7 +4371,7 @@
       <c r="J128" s="4"/>
     </row>
     <row r="129" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="113"/>
+      <c r="A129" s="114"/>
       <c r="B129" s="67"/>
       <c r="C129" s="67"/>
       <c r="D129" s="67"/>
@@ -4374,7 +4385,7 @@
       <c r="J129" s="67"/>
     </row>
     <row r="130" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="111">
+      <c r="A130" s="112">
         <v>44610</v>
       </c>
       <c r="B130" s="8"/>
@@ -4390,7 +4401,7 @@
       <c r="J130" s="8"/>
     </row>
     <row r="131" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="112"/>
+      <c r="A131" s="113"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
@@ -4404,7 +4415,7 @@
       <c r="J131" s="4"/>
     </row>
     <row r="132" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="112"/>
+      <c r="A132" s="113"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
@@ -4418,7 +4429,7 @@
       <c r="J132" s="4"/>
     </row>
     <row r="133" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="113"/>
+      <c r="A133" s="114"/>
       <c r="B133" s="67"/>
       <c r="C133" s="67"/>
       <c r="D133" s="67"/>
@@ -4450,7 +4461,7 @@
       <c r="J134" s="12"/>
     </row>
     <row r="135" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="111">
+      <c r="A135" s="112">
         <v>44612</v>
       </c>
       <c r="B135" s="8"/>
@@ -4466,7 +4477,7 @@
       <c r="J135" s="8"/>
     </row>
     <row r="136" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="113"/>
+      <c r="A136" s="114"/>
       <c r="B136" s="71"/>
       <c r="C136" s="71"/>
       <c r="D136" s="71"/>
@@ -4480,7 +4491,7 @@
       <c r="J136" s="71"/>
     </row>
     <row r="137" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="111">
+      <c r="A137" s="112">
         <v>44613</v>
       </c>
       <c r="B137" s="8"/>
@@ -4498,7 +4509,7 @@
       <c r="J137" s="8"/>
     </row>
     <row r="138" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="112"/>
+      <c r="A138" s="113"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
       <c r="D138" s="4"/>
@@ -4514,7 +4525,7 @@
       <c r="J138" s="4"/>
     </row>
     <row r="139" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="112"/>
+      <c r="A139" s="113"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
@@ -4528,7 +4539,7 @@
       <c r="J139" s="4"/>
     </row>
     <row r="140" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="112"/>
+      <c r="A140" s="113"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
       <c r="D140" s="4"/>
@@ -4542,7 +4553,7 @@
       <c r="J140" s="4"/>
     </row>
     <row r="141" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="112"/>
+      <c r="A141" s="113"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
       <c r="D141" s="4"/>
@@ -4556,7 +4567,7 @@
       <c r="J141" s="4"/>
     </row>
     <row r="142" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="112"/>
+      <c r="A142" s="113"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
@@ -4570,7 +4581,7 @@
       <c r="J142" s="4"/>
     </row>
     <row r="143" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="113"/>
+      <c r="A143" s="114"/>
       <c r="B143" s="72"/>
       <c r="C143" s="72"/>
       <c r="D143" s="72"/>
@@ -4584,7 +4595,7 @@
       <c r="J143" s="72"/>
     </row>
     <row r="144" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="111">
+      <c r="A144" s="112">
         <v>44614</v>
       </c>
       <c r="B144" s="8"/>
@@ -4602,7 +4613,7 @@
       <c r="J144" s="8"/>
     </row>
     <row r="145" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="112"/>
+      <c r="A145" s="113"/>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
       <c r="D145" s="4"/>
@@ -4616,7 +4627,7 @@
       <c r="J145" s="4"/>
     </row>
     <row r="146" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="112"/>
+      <c r="A146" s="113"/>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
       <c r="D146" s="4"/>
@@ -4630,7 +4641,7 @@
       <c r="J146" s="4"/>
     </row>
     <row r="147" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="112"/>
+      <c r="A147" s="113"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
       <c r="D147" s="4"/>
@@ -4644,7 +4655,7 @@
       <c r="J147" s="4"/>
     </row>
     <row r="148" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="113"/>
+      <c r="A148" s="114"/>
       <c r="B148" s="75"/>
       <c r="C148" s="75"/>
       <c r="D148" s="75"/>
@@ -4658,7 +4669,7 @@
       <c r="J148" s="75"/>
     </row>
     <row r="149" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="111">
+      <c r="A149" s="112">
         <v>44615</v>
       </c>
       <c r="B149" s="8"/>
@@ -4676,7 +4687,7 @@
       <c r="J149" s="8"/>
     </row>
     <row r="150" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="113"/>
+      <c r="A150" s="114"/>
       <c r="B150" s="75"/>
       <c r="C150" s="75"/>
       <c r="D150" s="75"/>
@@ -4690,7 +4701,7 @@
       <c r="J150" s="75"/>
     </row>
     <row r="151" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="111">
+      <c r="A151" s="112">
         <v>44616</v>
       </c>
       <c r="B151" s="8"/>
@@ -4708,7 +4719,7 @@
       <c r="J151" s="8"/>
     </row>
     <row r="152" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="112"/>
+      <c r="A152" s="113"/>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
@@ -4722,7 +4733,7 @@
       <c r="J152" s="4"/>
     </row>
     <row r="153" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="113"/>
+      <c r="A153" s="114"/>
       <c r="B153" s="76"/>
       <c r="C153" s="76"/>
       <c r="D153" s="76"/>
@@ -4736,7 +4747,7 @@
       <c r="J153" s="76"/>
     </row>
     <row r="154" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="111">
+      <c r="A154" s="112">
         <v>44617</v>
       </c>
       <c r="B154" s="8"/>
@@ -4754,7 +4765,7 @@
       <c r="J154" s="8"/>
     </row>
     <row r="155" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="112"/>
+      <c r="A155" s="113"/>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
@@ -4768,7 +4779,7 @@
       <c r="J155" s="4"/>
     </row>
     <row r="156" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="113"/>
+      <c r="A156" s="114"/>
       <c r="B156" s="77"/>
       <c r="C156" s="77"/>
       <c r="D156" s="77"/>
@@ -4782,7 +4793,7 @@
       <c r="J156" s="77"/>
     </row>
     <row r="157" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="111">
+      <c r="A157" s="112">
         <v>44618</v>
       </c>
       <c r="B157" s="8"/>
@@ -4802,7 +4813,7 @@
       <c r="J157" s="8"/>
     </row>
     <row r="158" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="113"/>
+      <c r="A158" s="114"/>
       <c r="B158" s="78"/>
       <c r="C158" s="78"/>
       <c r="D158" s="78"/>
@@ -4818,7 +4829,7 @@
       <c r="J158" s="78"/>
     </row>
     <row r="159" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="111">
+      <c r="A159" s="112">
         <v>44619</v>
       </c>
       <c r="B159" s="8"/>
@@ -4836,7 +4847,7 @@
       <c r="J159" s="8"/>
     </row>
     <row r="160" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="112"/>
+      <c r="A160" s="113"/>
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
       <c r="D160" s="4"/>
@@ -4852,7 +4863,7 @@
       <c r="J160" s="4"/>
     </row>
     <row r="161" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="113"/>
+      <c r="A161" s="114"/>
       <c r="B161" s="79"/>
       <c r="C161" s="79"/>
       <c r="D161" s="79"/>
@@ -4868,7 +4879,7 @@
       <c r="J161" s="79"/>
     </row>
     <row r="162" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="111">
+      <c r="A162" s="112">
         <v>44620</v>
       </c>
       <c r="B162" s="8"/>
@@ -4886,7 +4897,7 @@
       <c r="J162" s="8"/>
     </row>
     <row r="163" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="112"/>
+      <c r="A163" s="113"/>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
       <c r="D163" s="4"/>
@@ -4902,7 +4913,7 @@
       <c r="J163" s="4"/>
     </row>
     <row r="164" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="113"/>
+      <c r="A164" s="114"/>
       <c r="B164" s="80"/>
       <c r="C164" s="80"/>
       <c r="D164" s="80"/>
@@ -4916,7 +4927,7 @@
       <c r="J164" s="80"/>
     </row>
     <row r="165" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="111">
+      <c r="A165" s="112">
         <v>44621</v>
       </c>
       <c r="B165" s="8"/>
@@ -4932,7 +4943,7 @@
       <c r="J165" s="8"/>
     </row>
     <row r="166" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="112"/>
+      <c r="A166" s="113"/>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
@@ -4946,7 +4957,7 @@
       <c r="J166" s="4"/>
     </row>
     <row r="167" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="113"/>
+      <c r="A167" s="114"/>
       <c r="B167" s="81"/>
       <c r="C167" s="81"/>
       <c r="D167" s="81"/>
@@ -4960,7 +4971,7 @@
       <c r="J167" s="81"/>
     </row>
     <row r="168" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="111">
+      <c r="A168" s="112">
         <v>44622</v>
       </c>
       <c r="B168" s="8"/>
@@ -4981,7 +4992,7 @@
       </c>
     </row>
     <row r="169" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="112"/>
+      <c r="A169" s="113"/>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
@@ -4996,7 +5007,7 @@
       </c>
     </row>
     <row r="170" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="113"/>
+      <c r="A170" s="114"/>
       <c r="B170" s="82"/>
       <c r="C170" s="82"/>
       <c r="D170" s="82"/>
@@ -5011,7 +5022,7 @@
       </c>
     </row>
     <row r="171" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="111">
+      <c r="A171" s="112">
         <v>44623</v>
       </c>
       <c r="B171" s="8"/>
@@ -5028,7 +5039,7 @@
       <c r="K171" s="8"/>
     </row>
     <row r="172" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="112"/>
+      <c r="A172" s="113"/>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
       <c r="D172" s="4"/>
@@ -5043,7 +5054,7 @@
       <c r="K172" s="4"/>
     </row>
     <row r="173" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="113"/>
+      <c r="A173" s="114"/>
       <c r="B173" s="83"/>
       <c r="C173" s="83"/>
       <c r="D173" s="83"/>
@@ -5058,7 +5069,7 @@
       <c r="K173" s="83"/>
     </row>
     <row r="174" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="111">
+      <c r="A174" s="112">
         <v>44625</v>
       </c>
       <c r="B174" s="8"/>
@@ -5075,7 +5086,7 @@
       <c r="K174" s="8"/>
     </row>
     <row r="175" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="113"/>
+      <c r="A175" s="114"/>
       <c r="B175" s="85"/>
       <c r="C175" s="85"/>
       <c r="D175" s="85"/>
@@ -5090,7 +5101,7 @@
       <c r="K175" s="85"/>
     </row>
     <row r="176" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="111">
+      <c r="A176" s="112">
         <v>44626</v>
       </c>
       <c r="B176" s="8"/>
@@ -5108,7 +5119,7 @@
       </c>
     </row>
     <row r="177" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="112"/>
+      <c r="A177" s="113"/>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
       <c r="D177" s="4"/>
@@ -5124,7 +5135,7 @@
       </c>
     </row>
     <row r="178" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="113"/>
+      <c r="A178" s="114"/>
       <c r="B178" s="86"/>
       <c r="C178" s="86"/>
       <c r="D178" s="86"/>
@@ -5140,7 +5151,7 @@
       </c>
     </row>
     <row r="179" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="111">
+      <c r="A179" s="112">
         <v>44627</v>
       </c>
       <c r="B179" s="8"/>
@@ -5158,7 +5169,7 @@
       </c>
     </row>
     <row r="180" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="112"/>
+      <c r="A180" s="113"/>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
       <c r="D180" s="4"/>
@@ -5174,7 +5185,7 @@
       </c>
     </row>
     <row r="181" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="112"/>
+      <c r="A181" s="113"/>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
       <c r="D181" s="4"/>
@@ -5190,7 +5201,7 @@
       </c>
     </row>
     <row r="182" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A182" s="113"/>
+      <c r="A182" s="114"/>
       <c r="B182" s="88"/>
       <c r="C182" s="88"/>
       <c r="D182" s="88"/>
@@ -5203,7 +5214,7 @@
       <c r="K182" s="88"/>
     </row>
     <row r="183" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="111">
+      <c r="A183" s="112">
         <v>44628</v>
       </c>
       <c r="B183" s="8" t="s">
@@ -5220,7 +5231,7 @@
       <c r="K183" s="8"/>
     </row>
     <row r="184" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="112"/>
+      <c r="A184" s="113"/>
       <c r="B184" s="4" t="s">
         <v>400</v>
       </c>
@@ -5235,7 +5246,7 @@
       <c r="K184" s="4"/>
     </row>
     <row r="185" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="113"/>
+      <c r="A185" s="114"/>
       <c r="B185" s="91" t="s">
         <v>404</v>
       </c>
@@ -5267,7 +5278,7 @@
       <c r="K186" s="12"/>
     </row>
     <row r="187" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="111">
+      <c r="A187" s="112">
         <v>44630</v>
       </c>
       <c r="B187" s="8"/>
@@ -5284,7 +5295,7 @@
       <c r="K187" s="8"/>
     </row>
     <row r="188" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="112"/>
+      <c r="A188" s="113"/>
       <c r="B188" s="4"/>
       <c r="C188" s="4"/>
       <c r="D188" s="4"/>
@@ -5299,7 +5310,7 @@
       <c r="K188" s="4"/>
     </row>
     <row r="189" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="112"/>
+      <c r="A189" s="113"/>
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
       <c r="D189" s="4"/>
@@ -5314,7 +5325,7 @@
       <c r="K189" s="4"/>
     </row>
     <row r="190" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A190" s="112"/>
+      <c r="A190" s="113"/>
       <c r="B190" s="4"/>
       <c r="C190" s="4"/>
       <c r="D190" s="4"/>
@@ -5329,7 +5340,7 @@
       <c r="K190" s="4"/>
     </row>
     <row r="191" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A191" s="113"/>
+      <c r="A191" s="114"/>
       <c r="B191" s="93"/>
       <c r="C191" s="93"/>
       <c r="D191" s="93"/>
@@ -5344,7 +5355,7 @@
       <c r="K191" s="93"/>
     </row>
     <row r="192" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A192" s="111">
+      <c r="A192" s="112">
         <v>44631</v>
       </c>
       <c r="B192" s="8" t="s">
@@ -5361,7 +5372,7 @@
       <c r="K192" s="8"/>
     </row>
     <row r="193" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="112"/>
+      <c r="A193" s="113"/>
       <c r="B193" s="4" t="s">
         <v>423</v>
       </c>
@@ -5376,7 +5387,7 @@
       <c r="K193" s="4"/>
     </row>
     <row r="194" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="113"/>
+      <c r="A194" s="114"/>
       <c r="B194" s="93" t="s">
         <v>424</v>
       </c>
@@ -5391,7 +5402,7 @@
       <c r="K194" s="93"/>
     </row>
     <row r="195" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="111">
+      <c r="A195" s="112">
         <v>44632</v>
       </c>
       <c r="B195" s="8" t="s">
@@ -5408,7 +5419,7 @@
       <c r="K195" s="8"/>
     </row>
     <row r="196" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="112"/>
+      <c r="A196" s="113"/>
       <c r="B196" s="4" t="s">
         <v>427</v>
       </c>
@@ -5423,7 +5434,7 @@
       <c r="K196" s="4"/>
     </row>
     <row r="197" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A197" s="113"/>
+      <c r="A197" s="114"/>
       <c r="B197" s="95" t="s">
         <v>428</v>
       </c>
@@ -5438,7 +5449,7 @@
       <c r="K197" s="95"/>
     </row>
     <row r="198" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="111">
+      <c r="A198" s="112">
         <v>44633</v>
       </c>
       <c r="B198" s="8" t="s">
@@ -5455,7 +5466,7 @@
       <c r="K198" s="8"/>
     </row>
     <row r="199" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="112"/>
+      <c r="A199" s="113"/>
       <c r="B199" s="4" t="s">
         <v>432</v>
       </c>
@@ -5470,7 +5481,7 @@
       <c r="K199" s="4"/>
     </row>
     <row r="200" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A200" s="113"/>
+      <c r="A200" s="114"/>
       <c r="B200" s="96" t="s">
         <v>433</v>
       </c>
@@ -5485,7 +5496,7 @@
       <c r="K200" s="96"/>
     </row>
     <row r="201" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A201" s="111">
+      <c r="A201" s="112">
         <v>44634</v>
       </c>
       <c r="B201" s="8"/>
@@ -5502,7 +5513,7 @@
       <c r="K201" s="8"/>
     </row>
     <row r="202" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A202" s="112"/>
+      <c r="A202" s="113"/>
       <c r="B202" s="4"/>
       <c r="C202" s="4" t="s">
         <v>445</v>
@@ -5517,7 +5528,7 @@
       <c r="K202" s="4"/>
     </row>
     <row r="203" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A203" s="113"/>
+      <c r="A203" s="114"/>
       <c r="B203" s="98"/>
       <c r="C203" s="98" t="s">
         <v>446</v>
@@ -5549,7 +5560,7 @@
       <c r="K204" s="12"/>
     </row>
     <row r="205" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A205" s="111">
+      <c r="A205" s="112">
         <v>44636</v>
       </c>
       <c r="B205" s="8"/>
@@ -5566,7 +5577,7 @@
       <c r="K205" s="8"/>
     </row>
     <row r="206" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A206" s="113"/>
+      <c r="A206" s="114"/>
       <c r="B206" s="101"/>
       <c r="C206" s="101" t="s">
         <v>460</v>
@@ -5581,7 +5592,7 @@
       <c r="K206" s="101"/>
     </row>
     <row r="207" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A207" s="111">
+      <c r="A207" s="112">
         <v>44639</v>
       </c>
       <c r="B207" s="8"/>
@@ -5598,7 +5609,7 @@
       <c r="K207" s="8"/>
     </row>
     <row r="208" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A208" s="112"/>
+      <c r="A208" s="113"/>
       <c r="B208" s="4"/>
       <c r="C208" s="4" t="s">
         <v>475</v>
@@ -5613,7 +5624,7 @@
       <c r="K208" s="4"/>
     </row>
     <row r="209" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A209" s="113"/>
+      <c r="A209" s="114"/>
       <c r="B209" s="105"/>
       <c r="C209" s="105" t="s">
         <v>476</v>
@@ -5628,7 +5639,7 @@
       <c r="K209" s="105"/>
     </row>
     <row r="210" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="111">
+      <c r="A210" s="112">
         <v>44641</v>
       </c>
       <c r="B210" s="8"/>
@@ -5645,7 +5656,7 @@
       <c r="K210" s="8"/>
     </row>
     <row r="211" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A211" s="112"/>
+      <c r="A211" s="113"/>
       <c r="B211" s="4"/>
       <c r="C211" s="4" t="s">
         <v>486</v>
@@ -5660,7 +5671,7 @@
       <c r="K211" s="4"/>
     </row>
     <row r="212" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A212" s="113"/>
+      <c r="A212" s="114"/>
       <c r="B212" s="107"/>
       <c r="C212" s="107" t="s">
         <v>487</v>
@@ -5675,7 +5686,7 @@
       <c r="K212" s="107"/>
     </row>
     <row r="213" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A213" s="111">
+      <c r="A213" s="112">
         <v>44644</v>
       </c>
       <c r="B213" s="8"/>
@@ -5693,7 +5704,7 @@
       </c>
     </row>
     <row r="214" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A214" s="112"/>
+      <c r="A214" s="113"/>
       <c r="B214" s="4"/>
       <c r="C214" s="4"/>
       <c r="D214" s="4"/>
@@ -5709,7 +5720,7 @@
       </c>
     </row>
     <row r="215" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A215" s="112"/>
+      <c r="A215" s="113"/>
       <c r="B215" s="4"/>
       <c r="C215" s="4"/>
       <c r="D215" s="4"/>
@@ -5725,7 +5736,7 @@
       </c>
     </row>
     <row r="216" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A216" s="113"/>
+      <c r="A216" s="114"/>
       <c r="B216" s="110"/>
       <c r="C216" s="110"/>
       <c r="D216" s="110"/>
@@ -10721,6 +10732,47 @@
     </row>
   </sheetData>
   <mergeCells count="57">
+    <mergeCell ref="A210:A212"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A207:A209"/>
+    <mergeCell ref="A198:A200"/>
+    <mergeCell ref="A174:A175"/>
+    <mergeCell ref="A171:A173"/>
+    <mergeCell ref="A137:A143"/>
+    <mergeCell ref="A168:A170"/>
+    <mergeCell ref="A165:A167"/>
+    <mergeCell ref="A195:A197"/>
+    <mergeCell ref="A187:A191"/>
+    <mergeCell ref="A205:A206"/>
+    <mergeCell ref="A201:A203"/>
+    <mergeCell ref="A192:A194"/>
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="A87:A94"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="A98:A103"/>
+    <mergeCell ref="A104:A110"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="A111:A117"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A44:A49"/>
     <mergeCell ref="A213:A216"/>
     <mergeCell ref="A56:A58"/>
     <mergeCell ref="A72:A75"/>
@@ -10737,47 +10789,6 @@
     <mergeCell ref="A159:A161"/>
     <mergeCell ref="A157:A158"/>
     <mergeCell ref="A151:A153"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A39"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="A87:A94"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="A98:A103"/>
-    <mergeCell ref="A104:A110"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="A111:A117"/>
-    <mergeCell ref="A210:A212"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A207:A209"/>
-    <mergeCell ref="A198:A200"/>
-    <mergeCell ref="A174:A175"/>
-    <mergeCell ref="A171:A173"/>
-    <mergeCell ref="A137:A143"/>
-    <mergeCell ref="A168:A170"/>
-    <mergeCell ref="A165:A167"/>
-    <mergeCell ref="A195:A197"/>
-    <mergeCell ref="A187:A191"/>
-    <mergeCell ref="A205:A206"/>
-    <mergeCell ref="A201:A203"/>
-    <mergeCell ref="A192:A194"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10852,7 +10863,7 @@
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="111">
+      <c r="A4" s="112">
         <v>44595</v>
       </c>
       <c r="B4" s="38"/>
@@ -10863,7 +10874,7 @@
       <c r="E4" s="38"/>
     </row>
     <row r="5" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="113"/>
+      <c r="A5" s="114"/>
       <c r="B5" s="42"/>
       <c r="C5" s="46" t="s">
         <v>161</v>
@@ -10872,7 +10883,7 @@
       <c r="E5" s="42"/>
     </row>
     <row r="6" spans="1:7" s="39" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="111">
+      <c r="A6" s="112">
         <v>44596</v>
       </c>
       <c r="B6" s="38"/>
@@ -10883,7 +10894,7 @@
       <c r="E6" s="38"/>
     </row>
     <row r="7" spans="1:7" s="43" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="113"/>
+      <c r="A7" s="114"/>
       <c r="B7" s="42"/>
       <c r="C7" s="42" t="s">
         <v>171</v>
@@ -10903,7 +10914,7 @@
       <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="111">
+      <c r="A9" s="112">
         <v>44608</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -10914,7 +10925,7 @@
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="112"/>
+      <c r="A10" s="113"/>
       <c r="B10" s="4" t="s">
         <v>237</v>
       </c>
@@ -10923,7 +10934,7 @@
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="113"/>
+      <c r="A11" s="114"/>
       <c r="B11" s="64" t="s">
         <v>238</v>
       </c>
@@ -10932,7 +10943,7 @@
       <c r="E11" s="64"/>
     </row>
     <row r="12" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="111">
+      <c r="A12" s="112">
         <v>44609</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -10943,7 +10954,7 @@
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="112"/>
+      <c r="A13" s="113"/>
       <c r="B13" s="4" t="s">
         <v>250</v>
       </c>
@@ -10952,7 +10963,7 @@
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="113"/>
+      <c r="A14" s="114"/>
       <c r="B14" s="67" t="s">
         <v>251</v>
       </c>
@@ -10983,7 +10994,7 @@
       <c r="E16" s="12"/>
     </row>
     <row r="17" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="111">
+      <c r="A17" s="112">
         <v>44616</v>
       </c>
       <c r="B17" s="8"/>
@@ -10994,7 +11005,7 @@
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="112"/>
+      <c r="A18" s="113"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
         <v>303</v>
@@ -11003,7 +11014,7 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="113"/>
+      <c r="A19" s="114"/>
       <c r="B19" s="77"/>
       <c r="C19" s="77" t="s">
         <v>304</v>
@@ -11012,7 +11023,7 @@
       <c r="E19" s="77"/>
     </row>
     <row r="20" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="111">
+      <c r="A20" s="112">
         <v>44621</v>
       </c>
       <c r="B20" s="8"/>
@@ -11023,7 +11034,7 @@
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="112"/>
+      <c r="A21" s="113"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
         <v>350</v>
@@ -11032,7 +11043,7 @@
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="113"/>
+      <c r="A22" s="114"/>
       <c r="B22" s="81"/>
       <c r="C22" s="81" t="s">
         <v>351</v>
@@ -11041,7 +11052,7 @@
       <c r="E22" s="81"/>
     </row>
     <row r="23" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="111">
+      <c r="A23" s="112">
         <v>44623</v>
       </c>
       <c r="B23" s="8"/>
@@ -11052,7 +11063,7 @@
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="113"/>
+      <c r="A24" s="114"/>
       <c r="B24" s="83"/>
       <c r="C24" s="83" t="s">
         <v>366</v>
@@ -11061,7 +11072,7 @@
       <c r="E24" s="83"/>
     </row>
     <row r="25" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="111">
+      <c r="A25" s="112">
         <v>44628</v>
       </c>
       <c r="B25" s="8"/>
@@ -11072,7 +11083,7 @@
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="112"/>
+      <c r="A26" s="113"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
         <v>396</v>
@@ -11081,7 +11092,7 @@
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="112"/>
+      <c r="A27" s="113"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
         <v>397</v>
@@ -11090,7 +11101,7 @@
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="113"/>
+      <c r="A28" s="114"/>
       <c r="B28" s="89"/>
       <c r="C28" s="89" t="s">
         <v>398</v>
@@ -11099,7 +11110,7 @@
       <c r="E28" s="89"/>
     </row>
     <row r="29" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="111">
+      <c r="A29" s="112">
         <v>44635</v>
       </c>
       <c r="B29" s="8"/>
@@ -11114,7 +11125,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="112"/>
+      <c r="A30" s="113"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
         <v>455</v>
@@ -11127,7 +11138,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="113"/>
+      <c r="A31" s="114"/>
       <c r="B31" s="99"/>
       <c r="C31" s="99" t="s">
         <v>456</v>
@@ -11155,7 +11166,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="111">
+      <c r="A33" s="112">
         <v>44640</v>
       </c>
       <c r="B33" s="8"/>
@@ -11168,7 +11179,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="113"/>
+      <c r="A34" s="114"/>
       <c r="B34" s="106"/>
       <c r="C34" s="106"/>
       <c r="D34" s="106"/>
@@ -11179,7 +11190,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="111">
+      <c r="A35" s="112">
         <v>44642</v>
       </c>
       <c r="B35" s="8"/>
@@ -11194,7 +11205,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="113"/>
+      <c r="A36" s="114"/>
       <c r="B36" s="108"/>
       <c r="C36" s="108" t="s">
         <v>494</v>
@@ -11207,7 +11218,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="111">
+      <c r="A37" s="112">
         <v>44643</v>
       </c>
       <c r="B37" s="8"/>
@@ -11222,7 +11233,7 @@
       <c r="G37" s="8"/>
     </row>
     <row r="38" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="113"/>
+      <c r="A38" s="114"/>
       <c r="B38" s="108"/>
       <c r="C38" s="108"/>
       <c r="D38" s="108" t="s">
@@ -11429,11 +11440,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A29:A31"/>
-    <mergeCell ref="A25:A28"/>
     <mergeCell ref="A23:A24"/>
     <mergeCell ref="A20:A22"/>
     <mergeCell ref="A4:A5"/>
@@ -11441,6 +11447,11 @@
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A29:A31"/>
+    <mergeCell ref="A25:A28"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11452,11 +11463,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44415538-EB73-4FF7-B2CA-34821DA5346F}">
   <dimension ref="A1:C242"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B137" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C147" sqref="C147"/>
+      <selection pane="bottomRight" activeCell="C144" sqref="C144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.4"/>
@@ -11475,7 +11486,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="112">
+      <c r="A2" s="113">
         <v>44563</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -11486,35 +11497,35 @@
       </c>
     </row>
     <row r="3" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="112"/>
+      <c r="A3" s="113"/>
       <c r="B3" s="4"/>
       <c r="C3" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="112"/>
+      <c r="A4" s="113"/>
       <c r="B4" s="4"/>
       <c r="C4" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="112"/>
+      <c r="A5" s="113"/>
       <c r="B5" s="4"/>
       <c r="C5" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="113"/>
+      <c r="A6" s="114"/>
       <c r="B6" s="6"/>
       <c r="C6" s="15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="111">
+      <c r="A7" s="112">
         <v>44564</v>
       </c>
       <c r="B7" s="8"/>
@@ -11523,56 +11534,56 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="112"/>
+      <c r="A8" s="113"/>
       <c r="B8" s="4"/>
       <c r="C8" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="112"/>
+      <c r="A9" s="113"/>
       <c r="B9" s="4"/>
       <c r="C9" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="112"/>
+      <c r="A10" s="113"/>
       <c r="B10" s="4"/>
       <c r="C10" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="112"/>
+      <c r="A11" s="113"/>
       <c r="B11" s="4"/>
       <c r="C11" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="112"/>
+      <c r="A12" s="113"/>
       <c r="B12" s="4"/>
       <c r="C12" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="112"/>
+      <c r="A13" s="113"/>
       <c r="B13" s="4"/>
       <c r="C13" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="113"/>
+      <c r="A14" s="114"/>
       <c r="B14" s="6"/>
       <c r="C14" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="111">
+      <c r="A15" s="112">
         <v>44565</v>
       </c>
       <c r="B15" s="8"/>
@@ -11581,14 +11592,14 @@
       </c>
     </row>
     <row r="16" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="115"/>
+      <c r="A16" s="116"/>
       <c r="B16" s="6"/>
       <c r="C16" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="111">
+      <c r="A17" s="112">
         <v>44570</v>
       </c>
       <c r="B17" s="8"/>
@@ -11597,19 +11608,19 @@
       </c>
     </row>
     <row r="18" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="112"/>
+      <c r="A18" s="113"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="116" t="s">
+      <c r="C18" s="117" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="113"/>
+      <c r="A19" s="114"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="117"/>
+      <c r="C19" s="118"/>
     </row>
     <row r="20" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="111">
+      <c r="A20" s="112">
         <v>44574</v>
       </c>
       <c r="B20" s="8"/>
@@ -11618,21 +11629,21 @@
       </c>
     </row>
     <row r="21" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="112"/>
+      <c r="A21" s="113"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="113"/>
+      <c r="A22" s="114"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="111">
+      <c r="A23" s="112">
         <v>44590</v>
       </c>
       <c r="B23" s="8"/>
@@ -11641,28 +11652,28 @@
       </c>
     </row>
     <row r="24" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="114"/>
+      <c r="A24" s="115"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="114"/>
+      <c r="A25" s="115"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="115"/>
+      <c r="A26" s="116"/>
       <c r="B26" s="33"/>
       <c r="C26" s="33" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A27" s="111">
+      <c r="A27" s="112">
         <v>44591</v>
       </c>
       <c r="B27" s="8"/>
@@ -11671,49 +11682,49 @@
       </c>
     </row>
     <row r="28" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A28" s="112"/>
+      <c r="A28" s="113"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A29" s="112"/>
+      <c r="A29" s="113"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A30" s="112"/>
+      <c r="A30" s="113"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A31" s="112"/>
+      <c r="A31" s="113"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A32" s="112"/>
+      <c r="A32" s="113"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A33" s="113"/>
+      <c r="A33" s="114"/>
       <c r="B33" s="34"/>
       <c r="C33" s="34" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A34" s="111">
+      <c r="A34" s="112">
         <v>44593</v>
       </c>
       <c r="B34" s="8"/>
@@ -11722,14 +11733,14 @@
       </c>
     </row>
     <row r="35" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A35" s="113"/>
+      <c r="A35" s="114"/>
       <c r="B35" s="36"/>
       <c r="C35" s="36" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="39" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A36" s="111">
+      <c r="A36" s="112">
         <v>44594</v>
       </c>
       <c r="B36" s="38" t="s">
@@ -11740,35 +11751,35 @@
       </c>
     </row>
     <row r="37" spans="1:3" s="41" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A37" s="112"/>
+      <c r="A37" s="113"/>
       <c r="B37" s="40" t="s">
         <v>164</v>
       </c>
       <c r="C37" s="40"/>
     </row>
     <row r="38" spans="1:3" s="41" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A38" s="112"/>
+      <c r="A38" s="113"/>
       <c r="B38" s="40" t="s">
         <v>157</v>
       </c>
       <c r="C38" s="40"/>
     </row>
     <row r="39" spans="1:3" s="41" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A39" s="112"/>
+      <c r="A39" s="113"/>
       <c r="B39" s="40" t="s">
         <v>158</v>
       </c>
       <c r="C39" s="40"/>
     </row>
     <row r="40" spans="1:3" s="43" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A40" s="113"/>
+      <c r="A40" s="114"/>
       <c r="B40" s="42" t="s">
         <v>159</v>
       </c>
       <c r="C40" s="42"/>
     </row>
     <row r="41" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A41" s="111">
+      <c r="A41" s="112">
         <v>44595</v>
       </c>
       <c r="B41" s="8" t="s">
@@ -11779,7 +11790,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A42" s="113"/>
+      <c r="A42" s="114"/>
       <c r="B42" s="44" t="s">
         <v>166</v>
       </c>
@@ -11788,7 +11799,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A43" s="111">
+      <c r="A43" s="112">
         <v>44596</v>
       </c>
       <c r="B43" s="8" t="s">
@@ -11799,21 +11810,21 @@
       </c>
     </row>
     <row r="44" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A44" s="112"/>
+      <c r="A44" s="113"/>
       <c r="B44" s="4" t="s">
         <v>169</v>
       </c>
       <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A45" s="112"/>
+      <c r="A45" s="113"/>
       <c r="B45" s="4" t="s">
         <v>172</v>
       </c>
       <c r="C45" s="4"/>
     </row>
     <row r="46" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A46" s="113"/>
+      <c r="A46" s="114"/>
       <c r="B46" s="47" t="s">
         <v>173</v>
       </c>
@@ -11838,7 +11849,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A49" s="111">
+      <c r="A49" s="112">
         <v>44608</v>
       </c>
       <c r="B49" s="8" t="s">
@@ -11847,14 +11858,14 @@
       <c r="C49" s="8"/>
     </row>
     <row r="50" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A50" s="113"/>
+      <c r="A50" s="114"/>
       <c r="B50" s="64" t="s">
         <v>236</v>
       </c>
       <c r="C50" s="64"/>
     </row>
     <row r="51" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A51" s="111">
+      <c r="A51" s="112">
         <v>44609</v>
       </c>
       <c r="B51" s="8" t="s">
@@ -11863,14 +11874,14 @@
       <c r="C51" s="8"/>
     </row>
     <row r="52" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A52" s="113"/>
+      <c r="A52" s="114"/>
       <c r="B52" s="65" t="s">
         <v>248</v>
       </c>
       <c r="C52" s="65"/>
     </row>
     <row r="53" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A53" s="111">
+      <c r="A53" s="112">
         <v>44610</v>
       </c>
       <c r="B53" s="8" t="s">
@@ -11879,28 +11890,28 @@
       <c r="C53" s="8"/>
     </row>
     <row r="54" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A54" s="112"/>
+      <c r="A54" s="113"/>
       <c r="B54" s="4" t="s">
         <v>253</v>
       </c>
       <c r="C54" s="4"/>
     </row>
     <row r="55" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A55" s="112"/>
+      <c r="A55" s="113"/>
       <c r="B55" s="4" t="s">
         <v>258</v>
       </c>
       <c r="C55" s="4"/>
     </row>
     <row r="56" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A56" s="113"/>
+      <c r="A56" s="114"/>
       <c r="B56" s="68" t="s">
         <v>259</v>
       </c>
       <c r="C56" s="68"/>
     </row>
     <row r="57" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A57" s="111">
+      <c r="A57" s="112">
         <v>44611</v>
       </c>
       <c r="B57" s="8" t="s">
@@ -11909,28 +11920,28 @@
       <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A58" s="112"/>
+      <c r="A58" s="113"/>
       <c r="B58" s="4" t="s">
         <v>261</v>
       </c>
       <c r="C58" s="4"/>
     </row>
     <row r="59" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="112"/>
+      <c r="A59" s="113"/>
       <c r="B59" s="4" t="s">
         <v>263</v>
       </c>
       <c r="C59" s="4"/>
     </row>
     <row r="60" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A60" s="113"/>
+      <c r="A60" s="114"/>
       <c r="B60" s="70" t="s">
         <v>264</v>
       </c>
       <c r="C60" s="70"/>
     </row>
     <row r="61" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A61" s="111">
+      <c r="A61" s="112">
         <v>44612</v>
       </c>
       <c r="B61" s="8" t="s">
@@ -11939,21 +11950,21 @@
       <c r="C61" s="8"/>
     </row>
     <row r="62" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A62" s="112"/>
+      <c r="A62" s="113"/>
       <c r="B62" s="4" t="s">
         <v>266</v>
       </c>
       <c r="C62" s="4"/>
     </row>
     <row r="63" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="113"/>
+      <c r="A63" s="114"/>
       <c r="B63" s="71" t="s">
         <v>267</v>
       </c>
       <c r="C63" s="71"/>
     </row>
     <row r="64" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="111">
+      <c r="A64" s="112">
         <v>44613</v>
       </c>
       <c r="B64" s="8" t="s">
@@ -11962,14 +11973,14 @@
       <c r="C64" s="8"/>
     </row>
     <row r="65" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A65" s="113"/>
+      <c r="A65" s="114"/>
       <c r="B65" s="73" t="s">
         <v>281</v>
       </c>
       <c r="C65" s="73"/>
     </row>
     <row r="66" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A66" s="111">
+      <c r="A66" s="112">
         <v>44614</v>
       </c>
       <c r="B66" s="8" t="s">
@@ -11978,28 +11989,28 @@
       <c r="C66" s="8"/>
     </row>
     <row r="67" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A67" s="112"/>
+      <c r="A67" s="113"/>
       <c r="B67" s="4" t="s">
         <v>283</v>
       </c>
       <c r="C67" s="4"/>
     </row>
     <row r="68" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A68" s="112"/>
+      <c r="A68" s="113"/>
       <c r="B68" s="4" t="s">
         <v>291</v>
       </c>
       <c r="C68" s="4"/>
     </row>
     <row r="69" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A69" s="113"/>
+      <c r="A69" s="114"/>
       <c r="B69" s="74" t="s">
         <v>292</v>
       </c>
       <c r="C69" s="74"/>
     </row>
     <row r="70" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A70" s="111">
+      <c r="A70" s="112">
         <v>44615</v>
       </c>
       <c r="B70" s="8" t="s">
@@ -12008,14 +12019,14 @@
       <c r="C70" s="8"/>
     </row>
     <row r="71" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A71" s="112"/>
+      <c r="A71" s="113"/>
       <c r="B71" s="4" t="s">
         <v>294</v>
       </c>
       <c r="C71" s="4"/>
     </row>
     <row r="72" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A72" s="113"/>
+      <c r="A72" s="114"/>
       <c r="B72" s="75" t="s">
         <v>298</v>
       </c>
@@ -12031,7 +12042,7 @@
       <c r="C73" s="12"/>
     </row>
     <row r="74" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A74" s="111">
+      <c r="A74" s="112">
         <v>44617</v>
       </c>
       <c r="B74" s="8" t="s">
@@ -12040,21 +12051,21 @@
       <c r="C74" s="8"/>
     </row>
     <row r="75" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A75" s="112"/>
+      <c r="A75" s="113"/>
       <c r="B75" s="4" t="s">
         <v>309</v>
       </c>
       <c r="C75" s="4"/>
     </row>
     <row r="76" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A76" s="113"/>
+      <c r="A76" s="114"/>
       <c r="B76" s="77" t="s">
         <v>310</v>
       </c>
       <c r="C76" s="77"/>
     </row>
     <row r="77" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A77" s="111">
+      <c r="A77" s="112">
         <v>44618</v>
       </c>
       <c r="B77" s="8" t="s">
@@ -12063,49 +12074,49 @@
       <c r="C77" s="8"/>
     </row>
     <row r="78" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A78" s="112"/>
+      <c r="A78" s="113"/>
       <c r="B78" s="4" t="s">
         <v>315</v>
       </c>
       <c r="C78" s="4"/>
     </row>
     <row r="79" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A79" s="112"/>
+      <c r="A79" s="113"/>
       <c r="B79" s="4" t="s">
         <v>316</v>
       </c>
       <c r="C79" s="4"/>
     </row>
     <row r="80" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A80" s="112"/>
+      <c r="A80" s="113"/>
       <c r="B80" s="4" t="s">
         <v>317</v>
       </c>
       <c r="C80" s="4"/>
     </row>
     <row r="81" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A81" s="112"/>
+      <c r="A81" s="113"/>
       <c r="B81" s="4" t="s">
         <v>325</v>
       </c>
       <c r="C81" s="4"/>
     </row>
     <row r="82" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A82" s="112"/>
+      <c r="A82" s="113"/>
       <c r="B82" s="4" t="s">
         <v>326</v>
       </c>
       <c r="C82" s="4"/>
     </row>
     <row r="83" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A83" s="113"/>
+      <c r="A83" s="114"/>
       <c r="B83" s="78" t="s">
         <v>327</v>
       </c>
       <c r="C83" s="78"/>
     </row>
     <row r="84" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A84" s="111">
+      <c r="A84" s="112">
         <v>44619</v>
       </c>
       <c r="B84" s="8" t="s">
@@ -12114,14 +12125,14 @@
       <c r="C84" s="8"/>
     </row>
     <row r="85" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A85" s="113"/>
+      <c r="A85" s="114"/>
       <c r="B85" s="79" t="s">
         <v>329</v>
       </c>
       <c r="C85" s="79"/>
     </row>
     <row r="86" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A86" s="111">
+      <c r="A86" s="112">
         <v>44620</v>
       </c>
       <c r="B86" s="8" t="s">
@@ -12130,28 +12141,28 @@
       <c r="C86" s="8"/>
     </row>
     <row r="87" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A87" s="112"/>
+      <c r="A87" s="113"/>
       <c r="B87" s="4" t="s">
         <v>337</v>
       </c>
       <c r="C87" s="4"/>
     </row>
     <row r="88" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A88" s="112"/>
+      <c r="A88" s="113"/>
       <c r="B88" s="4" t="s">
         <v>338</v>
       </c>
       <c r="C88" s="4"/>
     </row>
     <row r="89" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A89" s="113"/>
+      <c r="A89" s="114"/>
       <c r="B89" s="80" t="s">
         <v>339</v>
       </c>
       <c r="C89" s="80"/>
     </row>
     <row r="90" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A90" s="111">
+      <c r="A90" s="112">
         <v>44621</v>
       </c>
       <c r="B90" s="8" t="s">
@@ -12160,28 +12171,28 @@
       <c r="C90" s="8"/>
     </row>
     <row r="91" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A91" s="112"/>
+      <c r="A91" s="113"/>
       <c r="B91" s="4" t="s">
         <v>346</v>
       </c>
       <c r="C91" s="4"/>
     </row>
     <row r="92" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A92" s="112"/>
+      <c r="A92" s="113"/>
       <c r="B92" s="4" t="s">
         <v>347</v>
       </c>
       <c r="C92" s="4"/>
     </row>
     <row r="93" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A93" s="113"/>
+      <c r="A93" s="114"/>
       <c r="B93" s="81" t="s">
         <v>348</v>
       </c>
       <c r="C93" s="81"/>
     </row>
     <row r="94" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A94" s="111">
+      <c r="A94" s="112">
         <v>44622</v>
       </c>
       <c r="B94" s="8" t="s">
@@ -12190,14 +12201,14 @@
       <c r="C94" s="8"/>
     </row>
     <row r="95" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A95" s="113"/>
+      <c r="A95" s="114"/>
       <c r="B95" s="82" t="s">
         <v>356</v>
       </c>
       <c r="C95" s="82"/>
     </row>
     <row r="96" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A96" s="111">
+      <c r="A96" s="112">
         <v>44623</v>
       </c>
       <c r="B96" s="8" t="s">
@@ -12206,14 +12217,14 @@
       <c r="C96" s="8"/>
     </row>
     <row r="97" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A97" s="113"/>
+      <c r="A97" s="114"/>
       <c r="B97" s="83" t="s">
         <v>364</v>
       </c>
       <c r="C97" s="83"/>
     </row>
     <row r="98" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A98" s="111">
+      <c r="A98" s="112">
         <v>44624</v>
       </c>
       <c r="B98" s="8" t="s">
@@ -12222,14 +12233,14 @@
       <c r="C98" s="8"/>
     </row>
     <row r="99" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A99" s="113"/>
+      <c r="A99" s="114"/>
       <c r="B99" s="84" t="s">
         <v>375</v>
       </c>
       <c r="C99" s="84"/>
     </row>
     <row r="100" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A100" s="111">
+      <c r="A100" s="112">
         <v>44625</v>
       </c>
       <c r="B100" s="8" t="s">
@@ -12238,14 +12249,14 @@
       <c r="C100" s="8"/>
     </row>
     <row r="101" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A101" s="113"/>
+      <c r="A101" s="114"/>
       <c r="B101" s="85" t="s">
         <v>380</v>
       </c>
       <c r="C101" s="85"/>
     </row>
     <row r="102" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A102" s="111">
+      <c r="A102" s="112">
         <v>44626</v>
       </c>
       <c r="B102" s="8" t="s">
@@ -12254,14 +12265,14 @@
       <c r="C102" s="8"/>
     </row>
     <row r="103" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A103" s="113"/>
+      <c r="A103" s="114"/>
       <c r="B103" s="87" t="s">
         <v>386</v>
       </c>
       <c r="C103" s="87"/>
     </row>
     <row r="104" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A104" s="111">
+      <c r="A104" s="112">
         <v>44627</v>
       </c>
       <c r="B104" s="8" t="s">
@@ -12270,7 +12281,7 @@
       <c r="C104" s="8"/>
     </row>
     <row r="105" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A105" s="113"/>
+      <c r="A105" s="114"/>
       <c r="B105" s="88" t="s">
         <v>391</v>
       </c>
@@ -12286,7 +12297,7 @@
       <c r="C106" s="12"/>
     </row>
     <row r="107" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A107" s="111">
+      <c r="A107" s="112">
         <v>44629</v>
       </c>
       <c r="B107" s="8" t="s">
@@ -12295,14 +12306,14 @@
       <c r="C107" s="8"/>
     </row>
     <row r="108" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A108" s="113"/>
+      <c r="A108" s="114"/>
       <c r="B108" s="91" t="s">
         <v>407</v>
       </c>
       <c r="C108" s="91"/>
     </row>
     <row r="109" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A109" s="111">
+      <c r="A109" s="112">
         <v>44630</v>
       </c>
       <c r="B109" s="8" t="s">
@@ -12311,14 +12322,14 @@
       <c r="C109" s="8"/>
     </row>
     <row r="110" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A110" s="113"/>
+      <c r="A110" s="114"/>
       <c r="B110" s="92" t="s">
         <v>410</v>
       </c>
       <c r="C110" s="92"/>
     </row>
     <row r="111" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A111" s="111">
+      <c r="A111" s="112">
         <v>44631</v>
       </c>
       <c r="B111" s="8" t="s">
@@ -12327,14 +12338,14 @@
       <c r="C111" s="8"/>
     </row>
     <row r="112" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A112" s="113"/>
+      <c r="A112" s="114"/>
       <c r="B112" s="93" t="s">
         <v>420</v>
       </c>
       <c r="C112" s="93"/>
     </row>
     <row r="113" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A113" s="111">
+      <c r="A113" s="112">
         <v>44632</v>
       </c>
       <c r="B113" s="8" t="s">
@@ -12343,14 +12354,14 @@
       <c r="C113" s="8"/>
     </row>
     <row r="114" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A114" s="113"/>
+      <c r="A114" s="114"/>
       <c r="B114" s="94" t="s">
         <v>425</v>
       </c>
       <c r="C114" s="94"/>
     </row>
     <row r="115" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A115" s="111">
+      <c r="A115" s="112">
         <v>44633</v>
       </c>
       <c r="B115" s="8" t="s">
@@ -12359,14 +12370,14 @@
       <c r="C115" s="8"/>
     </row>
     <row r="116" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A116" s="113"/>
+      <c r="A116" s="114"/>
       <c r="B116" s="96" t="s">
         <v>430</v>
       </c>
       <c r="C116" s="96"/>
     </row>
     <row r="117" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A117" s="111">
+      <c r="A117" s="112">
         <v>44634</v>
       </c>
       <c r="B117" s="8" t="s">
@@ -12375,14 +12386,14 @@
       <c r="C117" s="8"/>
     </row>
     <row r="118" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A118" s="113"/>
+      <c r="A118" s="114"/>
       <c r="B118" s="97" t="s">
         <v>439</v>
       </c>
       <c r="C118" s="97"/>
     </row>
     <row r="119" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A119" s="111">
+      <c r="A119" s="112">
         <v>44635</v>
       </c>
       <c r="B119" s="8" t="s">
@@ -12391,14 +12402,14 @@
       <c r="C119" s="8"/>
     </row>
     <row r="120" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A120" s="113"/>
+      <c r="A120" s="114"/>
       <c r="B120" s="98" t="s">
         <v>448</v>
       </c>
       <c r="C120" s="98"/>
     </row>
     <row r="121" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A121" s="111">
+      <c r="A121" s="112">
         <v>44636</v>
       </c>
       <c r="B121" s="8" t="s">
@@ -12407,14 +12418,14 @@
       <c r="C121" s="8"/>
     </row>
     <row r="122" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A122" s="113"/>
+      <c r="A122" s="114"/>
       <c r="B122" s="99" t="s">
         <v>458</v>
       </c>
       <c r="C122" s="99"/>
     </row>
     <row r="123" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A123" s="111">
+      <c r="A123" s="112">
         <v>44637</v>
       </c>
       <c r="B123" s="8" t="s">
@@ -12423,28 +12434,28 @@
       <c r="C123" s="8"/>
     </row>
     <row r="124" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A124" s="112"/>
+      <c r="A124" s="113"/>
       <c r="B124" s="4" t="s">
         <v>464</v>
       </c>
       <c r="C124" s="4"/>
     </row>
     <row r="125" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A125" s="112"/>
+      <c r="A125" s="113"/>
       <c r="B125" s="4" t="s">
         <v>465</v>
       </c>
       <c r="C125" s="4"/>
     </row>
     <row r="126" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A126" s="113"/>
+      <c r="A126" s="114"/>
       <c r="B126" s="102" t="s">
         <v>466</v>
       </c>
       <c r="C126" s="102"/>
     </row>
     <row r="127" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A127" s="111">
+      <c r="A127" s="112">
         <v>44638</v>
       </c>
       <c r="B127" s="8" t="s">
@@ -12453,14 +12464,14 @@
       <c r="C127" s="8"/>
     </row>
     <row r="128" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A128" s="113"/>
+      <c r="A128" s="114"/>
       <c r="B128" s="103" t="s">
         <v>469</v>
       </c>
       <c r="C128" s="103"/>
     </row>
     <row r="129" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A129" s="111">
+      <c r="A129" s="112">
         <v>44639</v>
       </c>
       <c r="B129" s="8" t="s">
@@ -12469,14 +12480,14 @@
       <c r="C129" s="8"/>
     </row>
     <row r="130" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A130" s="113"/>
+      <c r="A130" s="114"/>
       <c r="B130" s="104" t="s">
         <v>471</v>
       </c>
       <c r="C130" s="104"/>
     </row>
     <row r="131" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A131" s="111">
+      <c r="A131" s="112">
         <v>44640</v>
       </c>
       <c r="B131" s="8" t="s">
@@ -12485,21 +12496,21 @@
       <c r="C131" s="8"/>
     </row>
     <row r="132" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A132" s="112"/>
+      <c r="A132" s="113"/>
       <c r="B132" s="4" t="s">
         <v>478</v>
       </c>
       <c r="C132" s="4"/>
     </row>
     <row r="133" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A133" s="113"/>
+      <c r="A133" s="114"/>
       <c r="B133" s="105" t="s">
         <v>479</v>
       </c>
       <c r="C133" s="105"/>
     </row>
     <row r="134" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A134" s="111">
+      <c r="A134" s="112">
         <v>44641</v>
       </c>
       <c r="B134" s="8" t="s">
@@ -12508,21 +12519,21 @@
       <c r="C134" s="8"/>
     </row>
     <row r="135" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A135" s="112"/>
+      <c r="A135" s="113"/>
       <c r="B135" s="4" t="s">
         <v>483</v>
       </c>
       <c r="C135" s="4"/>
     </row>
     <row r="136" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A136" s="113"/>
+      <c r="A136" s="114"/>
       <c r="B136" s="107" t="s">
         <v>484</v>
       </c>
       <c r="C136" s="107"/>
     </row>
     <row r="137" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A137" s="111">
+      <c r="A137" s="112">
         <v>44642</v>
       </c>
       <c r="B137" s="8" t="s">
@@ -12531,14 +12542,14 @@
       <c r="C137" s="8"/>
     </row>
     <row r="138" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A138" s="113"/>
+      <c r="A138" s="114"/>
       <c r="B138" s="108" t="s">
         <v>496</v>
       </c>
       <c r="C138" s="108"/>
     </row>
     <row r="139" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A139" s="111">
+      <c r="A139" s="112">
         <v>44643</v>
       </c>
       <c r="B139" s="8" t="s">
@@ -12547,14 +12558,14 @@
       <c r="C139" s="8"/>
     </row>
     <row r="140" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A140" s="113"/>
+      <c r="A140" s="114"/>
       <c r="B140" s="108" t="s">
         <v>500</v>
       </c>
       <c r="C140" s="108"/>
     </row>
     <row r="141" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A141" s="111">
+      <c r="A141" s="112">
         <v>44644</v>
       </c>
       <c r="B141" s="8" t="s">
@@ -12563,28 +12574,34 @@
       <c r="C141" s="8"/>
     </row>
     <row r="142" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A142" s="112"/>
+      <c r="A142" s="113"/>
       <c r="B142" s="4" t="s">
         <v>504</v>
       </c>
       <c r="C142" s="4"/>
     </row>
     <row r="143" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A143" s="113"/>
+      <c r="A143" s="114"/>
       <c r="B143" s="109" t="s">
         <v>505</v>
       </c>
       <c r="C143" s="109"/>
     </row>
-    <row r="144" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A144" s="28"/>
-      <c r="B144" s="3"/>
-      <c r="C144" s="3"/>
-    </row>
-    <row r="145" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A145" s="28"/>
-      <c r="B145" s="3"/>
-      <c r="C145" s="3"/>
+    <row r="144" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A144" s="112">
+        <v>44645</v>
+      </c>
+      <c r="B144" s="8" t="s">
+        <v>510</v>
+      </c>
+      <c r="C144" s="8"/>
+    </row>
+    <row r="145" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A145" s="114"/>
+      <c r="B145" s="111" t="s">
+        <v>511</v>
+      </c>
+      <c r="C145" s="111"/>
     </row>
     <row r="146" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A146" s="28"/>
@@ -13070,7 +13087,39 @@
       <c r="C242" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="47">
+  <mergeCells count="48">
+    <mergeCell ref="A144:A145"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="A134:A136"/>
+    <mergeCell ref="A119:A120"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="A131:A133"/>
+    <mergeCell ref="A129:A130"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="A123:A126"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A34:A35"/>
     <mergeCell ref="A137:A138"/>
     <mergeCell ref="A139:A140"/>
     <mergeCell ref="A61:A63"/>
@@ -13087,37 +13136,6 @@
     <mergeCell ref="A84:A85"/>
     <mergeCell ref="A98:A99"/>
     <mergeCell ref="A96:A97"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="A134:A136"/>
-    <mergeCell ref="A119:A120"/>
-    <mergeCell ref="A117:A118"/>
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="A113:A114"/>
-    <mergeCell ref="A131:A133"/>
-    <mergeCell ref="A129:A130"/>
-    <mergeCell ref="A127:A128"/>
-    <mergeCell ref="A123:A126"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A109:A110"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13162,7 +13180,7 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:17" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="111">
+      <c r="A2" s="112">
         <v>44623</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -13170,19 +13188,19 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A3" s="112"/>
+      <c r="A3" s="113"/>
       <c r="B3" s="4" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A4" s="113"/>
+      <c r="A4" s="114"/>
       <c r="B4" s="83" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="111">
+      <c r="A5" s="112">
         <v>44624</v>
       </c>
       <c r="B5" s="31" t="s">
@@ -13190,13 +13208,13 @@
       </c>
     </row>
     <row r="6" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="112"/>
+      <c r="A6" s="113"/>
       <c r="B6" s="52" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="113"/>
+      <c r="A7" s="114"/>
       <c r="B7" s="54" t="s">
         <v>378</v>
       </c>
@@ -13210,7 +13228,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="111">
+      <c r="A9" s="112">
         <v>44628</v>
       </c>
       <c r="B9" s="31"/>
@@ -13233,7 +13251,7 @@
       <c r="Q9" s="31"/>
     </row>
     <row r="10" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="113"/>
+      <c r="A10" s="114"/>
       <c r="B10" s="54"/>
       <c r="C10" s="54" t="s">
         <v>403</v>
@@ -13254,7 +13272,7 @@
       <c r="Q10" s="54"/>
     </row>
     <row r="11" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="111">
+      <c r="A11" s="112">
         <v>44630</v>
       </c>
       <c r="B11" s="31"/>
@@ -13277,7 +13295,7 @@
       <c r="Q11" s="31"/>
     </row>
     <row r="12" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="112"/>
+      <c r="A12" s="113"/>
       <c r="B12" s="52"/>
       <c r="C12" s="52" t="s">
         <v>417</v>
@@ -13298,7 +13316,7 @@
       <c r="Q12" s="52"/>
     </row>
     <row r="13" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="113"/>
+      <c r="A13" s="114"/>
       <c r="B13" s="54"/>
       <c r="C13" s="54" t="s">
         <v>418</v>
@@ -13319,7 +13337,7 @@
       <c r="Q13" s="54"/>
     </row>
     <row r="14" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="111">
+      <c r="A14" s="112">
         <v>44633</v>
       </c>
       <c r="B14" s="31"/>
@@ -13342,7 +13360,7 @@
       <c r="Q14" s="31"/>
     </row>
     <row r="15" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="112"/>
+      <c r="A15" s="113"/>
       <c r="B15" s="52"/>
       <c r="C15" s="52" t="s">
         <v>435</v>
@@ -13363,7 +13381,7 @@
       <c r="Q15" s="52"/>
     </row>
     <row r="16" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="112"/>
+      <c r="A16" s="113"/>
       <c r="B16" s="52"/>
       <c r="C16" s="52" t="s">
         <v>436</v>
@@ -13384,7 +13402,7 @@
       <c r="Q16" s="52"/>
     </row>
     <row r="17" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="113"/>
+      <c r="A17" s="114"/>
       <c r="B17" s="54"/>
       <c r="C17" s="54" t="s">
         <v>437</v>
@@ -13405,7 +13423,7 @@
       <c r="Q17" s="54"/>
     </row>
     <row r="18" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="111">
+      <c r="A18" s="112">
         <v>44634</v>
       </c>
       <c r="B18" s="31"/>
@@ -13428,7 +13446,7 @@
       <c r="Q18" s="31"/>
     </row>
     <row r="19" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="112"/>
+      <c r="A19" s="113"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52" t="s">
         <v>441</v>
@@ -13449,7 +13467,7 @@
       <c r="Q19" s="52"/>
     </row>
     <row r="20" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="112"/>
+      <c r="A20" s="113"/>
       <c r="B20" s="52"/>
       <c r="C20" s="52" t="s">
         <v>442</v>
@@ -13470,7 +13488,7 @@
       <c r="Q20" s="52"/>
     </row>
     <row r="21" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="113"/>
+      <c r="A21" s="114"/>
       <c r="B21" s="54"/>
       <c r="C21" s="54" t="s">
         <v>443</v>
@@ -13491,7 +13509,7 @@
       <c r="Q21" s="54"/>
     </row>
     <row r="22" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="111">
+      <c r="A22" s="112">
         <v>44636</v>
       </c>
       <c r="B22" s="31"/>
@@ -13514,7 +13532,7 @@
       <c r="Q22" s="31"/>
     </row>
     <row r="23" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="113"/>
+      <c r="A23" s="114"/>
       <c r="B23" s="54"/>
       <c r="C23" s="54" t="s">
         <v>462</v>
@@ -13535,7 +13553,7 @@
       <c r="Q23" s="54"/>
     </row>
     <row r="24" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="111">
+      <c r="A24" s="112">
         <v>44639</v>
       </c>
       <c r="B24" s="31"/>
@@ -13558,7 +13576,7 @@
       <c r="Q24" s="31"/>
     </row>
     <row r="25" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="113"/>
+      <c r="A25" s="114"/>
       <c r="B25" s="54"/>
       <c r="C25" s="54" t="s">
         <v>473</v>
@@ -13579,7 +13597,7 @@
       <c r="Q25" s="54"/>
     </row>
     <row r="26" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="111">
+      <c r="A26" s="112">
         <v>44641</v>
       </c>
       <c r="B26" s="31" t="s">
@@ -13602,7 +13620,7 @@
       <c r="Q26" s="31"/>
     </row>
     <row r="27" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="112"/>
+      <c r="A27" s="113"/>
       <c r="B27" s="52" t="s">
         <v>489</v>
       </c>
@@ -13623,7 +13641,7 @@
       <c r="Q27" s="52"/>
     </row>
     <row r="28" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="112"/>
+      <c r="A28" s="113"/>
       <c r="B28" s="52" t="s">
         <v>490</v>
       </c>
@@ -13644,7 +13662,7 @@
       <c r="Q28" s="52"/>
     </row>
     <row r="29" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="113"/>
+      <c r="A29" s="114"/>
       <c r="B29" s="54" t="s">
         <v>491</v>
       </c>

</xml_diff>

<commit_message>
Last day for March ...
</commit_message>
<xml_diff>
--- a/学习记录.xlsx
+++ b/学习记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\不怕晒的铃铛\Desktop\学习资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{918C4458-D9E4-4D6D-B4B7-EBA8B236E2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DBFDA1-031A-44FD-B30E-2D05E2AB135E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JavaWeb相关" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="553">
   <si>
     <t>JavaSE</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2158,6 +2158,94 @@
   </si>
   <si>
     <t>存储过程概述与基本语法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不同路径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不同路径 II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>整数拆分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>操作系统的发展与分类</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>不同的二叉搜索树</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>01背包问题理论</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 分割等和子集</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>存储过程变量</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>存储过程参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>存储过程程序流程控制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最后一块石头的重量 II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>目标和</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一和零</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>定点数的乘法与除法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>存储函数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>synchronized互斥应用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>共享问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>线程安全分析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monitor</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用工厂创建对象</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Bean创建与获取源码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>类适配器模式</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2265,7 +2353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="121">
+  <cellXfs count="124">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2596,13 +2684,22 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2899,11 +2996,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P623"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B211" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B220" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C215" sqref="C215"/>
+      <selection pane="bottomRight" activeCell="B237" sqref="B237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
@@ -2973,7 +3070,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="114">
+      <c r="A3" s="117">
         <v>44566</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -2983,7 +3080,7 @@
       <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:16" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="115"/>
+      <c r="A4" s="119"/>
       <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
@@ -2991,7 +3088,7 @@
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:16" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="116"/>
+      <c r="A5" s="118"/>
       <c r="B5" s="6" t="s">
         <v>28</v>
       </c>
@@ -3029,7 +3126,7 @@
       <c r="D8" s="12"/>
     </row>
     <row r="9" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="114">
+      <c r="A9" s="117">
         <v>44572</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -3039,7 +3136,7 @@
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:16" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="116"/>
+      <c r="A10" s="118"/>
       <c r="B10" s="17" t="s">
         <v>38</v>
       </c>
@@ -3047,7 +3144,7 @@
       <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="114">
+      <c r="A11" s="117">
         <v>44573</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -3057,7 +3154,7 @@
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="115"/>
+      <c r="A12" s="119"/>
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
@@ -3065,7 +3162,7 @@
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="116"/>
+      <c r="A13" s="118"/>
       <c r="B13" s="18" t="s">
         <v>40</v>
       </c>
@@ -3073,7 +3170,7 @@
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="114">
+      <c r="A14" s="117">
         <v>44574</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -3083,7 +3180,7 @@
       <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:16" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="116"/>
+      <c r="A15" s="118"/>
       <c r="B15" s="19" t="s">
         <v>42</v>
       </c>
@@ -3093,7 +3190,7 @@
       <c r="D15" s="19"/>
     </row>
     <row r="16" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="114">
+      <c r="A16" s="117">
         <v>44575</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -3105,7 +3202,7 @@
       <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="115"/>
+      <c r="A17" s="119"/>
       <c r="B17" s="4" t="s">
         <v>47</v>
       </c>
@@ -3116,7 +3213,7 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="115"/>
+      <c r="A18" s="119"/>
       <c r="B18" s="4" t="s">
         <v>48</v>
       </c>
@@ -3127,7 +3224,7 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="116"/>
+      <c r="A19" s="118"/>
       <c r="B19" s="20" t="s">
         <v>49</v>
       </c>
@@ -3136,7 +3233,7 @@
       <c r="E19" s="21"/>
     </row>
     <row r="20" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="114">
+      <c r="A20" s="117">
         <v>44576</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -3149,7 +3246,7 @@
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="115"/>
+      <c r="A21" s="119"/>
       <c r="B21" s="4" t="s">
         <v>59</v>
       </c>
@@ -3160,7 +3257,7 @@
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="115"/>
+      <c r="A22" s="119"/>
       <c r="B22" s="4" t="s">
         <v>60</v>
       </c>
@@ -3171,7 +3268,7 @@
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="116"/>
+      <c r="A23" s="118"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20" t="s">
         <v>57</v>
@@ -3180,7 +3277,7 @@
       <c r="E23" s="21"/>
     </row>
     <row r="24" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="114">
+      <c r="A24" s="117">
         <v>44577</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -3195,7 +3292,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="115"/>
+      <c r="A25" s="119"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
         <v>63</v>
@@ -3206,7 +3303,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="116"/>
+      <c r="A26" s="118"/>
       <c r="B26" s="21"/>
       <c r="C26" s="21" t="s">
         <v>64</v>
@@ -3217,7 +3314,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="114">
+      <c r="A27" s="117">
         <v>44578</v>
       </c>
       <c r="B27" s="8" t="s">
@@ -3228,7 +3325,7 @@
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="115"/>
+      <c r="A28" s="119"/>
       <c r="B28" s="4" t="s">
         <v>69</v>
       </c>
@@ -3237,7 +3334,7 @@
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="115"/>
+      <c r="A29" s="119"/>
       <c r="B29" s="4" t="s">
         <v>70</v>
       </c>
@@ -3246,7 +3343,7 @@
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="116"/>
+      <c r="A30" s="118"/>
       <c r="B30" s="22" t="s">
         <v>71</v>
       </c>
@@ -3255,7 +3352,7 @@
       <c r="E30" s="22"/>
     </row>
     <row r="31" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="114">
+      <c r="A31" s="117">
         <v>44579</v>
       </c>
       <c r="B31" s="8" t="s">
@@ -3270,7 +3367,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="116"/>
+      <c r="A32" s="118"/>
       <c r="B32" s="22" t="s">
         <v>73</v>
       </c>
@@ -3281,7 +3378,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="114">
+      <c r="A33" s="117">
         <v>44580</v>
       </c>
       <c r="B33" s="8" t="s">
@@ -3295,7 +3392,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="116"/>
+      <c r="A34" s="118"/>
       <c r="B34" s="23" t="s">
         <v>83</v>
       </c>
@@ -3304,7 +3401,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="114">
+      <c r="A35" s="117">
         <v>44581</v>
       </c>
       <c r="B35" s="8" t="s">
@@ -3316,7 +3413,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="115"/>
+      <c r="A36" s="119"/>
       <c r="B36" s="4" t="s">
         <v>85</v>
       </c>
@@ -3326,7 +3423,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="115"/>
+      <c r="A37" s="119"/>
       <c r="B37" s="4" t="s">
         <v>86</v>
       </c>
@@ -3334,7 +3431,7 @@
       <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="115"/>
+      <c r="A38" s="119"/>
       <c r="B38" s="4" t="s">
         <v>87</v>
       </c>
@@ -3342,7 +3439,7 @@
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="116"/>
+      <c r="A39" s="118"/>
       <c r="B39" s="23" t="s">
         <v>88</v>
       </c>
@@ -3350,7 +3447,7 @@
       <c r="D39" s="23"/>
     </row>
     <row r="40" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="114">
+      <c r="A40" s="117">
         <v>44582</v>
       </c>
       <c r="B40" s="8" t="s">
@@ -3367,7 +3464,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="117"/>
+      <c r="A41" s="120"/>
       <c r="B41" s="4" t="s">
         <v>91</v>
       </c>
@@ -3379,7 +3476,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="117"/>
+      <c r="A42" s="120"/>
       <c r="B42" s="4" t="s">
         <v>98</v>
       </c>
@@ -3389,7 +3486,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="118"/>
+      <c r="A43" s="121"/>
       <c r="B43" s="24" t="s">
         <v>99</v>
       </c>
@@ -3399,7 +3496,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="114">
+      <c r="A44" s="117">
         <v>44583</v>
       </c>
       <c r="B44" s="8" t="s">
@@ -3409,7 +3506,7 @@
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="115"/>
+      <c r="A45" s="119"/>
       <c r="B45" s="4" t="s">
         <v>101</v>
       </c>
@@ -3417,7 +3514,7 @@
       <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="115"/>
+      <c r="A46" s="119"/>
       <c r="B46" s="4" t="s">
         <v>102</v>
       </c>
@@ -3425,7 +3522,7 @@
       <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="115"/>
+      <c r="A47" s="119"/>
       <c r="B47" s="4" t="s">
         <v>103</v>
       </c>
@@ -3433,7 +3530,7 @@
       <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="115"/>
+      <c r="A48" s="119"/>
       <c r="B48" s="4" t="s">
         <v>104</v>
       </c>
@@ -3441,7 +3538,7 @@
       <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="116"/>
+      <c r="A49" s="118"/>
       <c r="B49" s="25" t="s">
         <v>105</v>
       </c>
@@ -3449,7 +3546,7 @@
       <c r="D49" s="25"/>
     </row>
     <row r="50" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="114">
+      <c r="A50" s="117">
         <v>44584</v>
       </c>
       <c r="B50" s="8" t="s">
@@ -3459,7 +3556,7 @@
       <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="117"/>
+      <c r="A51" s="120"/>
       <c r="B51" s="4" t="s">
         <v>107</v>
       </c>
@@ -3467,7 +3564,7 @@
       <c r="D51" s="4"/>
     </row>
     <row r="52" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="117"/>
+      <c r="A52" s="120"/>
       <c r="B52" s="4" t="s">
         <v>108</v>
       </c>
@@ -3475,7 +3572,7 @@
       <c r="D52" s="4"/>
     </row>
     <row r="53" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="118"/>
+      <c r="A53" s="121"/>
       <c r="B53" s="26" t="s">
         <v>109</v>
       </c>
@@ -3483,7 +3580,7 @@
       <c r="D53" s="26"/>
     </row>
     <row r="54" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="114">
+      <c r="A54" s="117">
         <v>44585</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -3493,7 +3590,7 @@
       <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="116"/>
+      <c r="A55" s="118"/>
       <c r="B55" s="27" t="s">
         <v>111</v>
       </c>
@@ -3501,7 +3598,7 @@
       <c r="D55" s="27"/>
     </row>
     <row r="56" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="114">
+      <c r="A56" s="117">
         <v>44586</v>
       </c>
       <c r="B56" s="8"/>
@@ -3516,7 +3613,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="115"/>
+      <c r="A57" s="119"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4" t="s">
@@ -3525,7 +3622,7 @@
       <c r="E57" s="4"/>
     </row>
     <row r="58" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="116"/>
+      <c r="A58" s="118"/>
       <c r="B58" s="27"/>
       <c r="C58" s="27"/>
       <c r="D58" s="27" t="s">
@@ -3534,7 +3631,7 @@
       <c r="E58" s="27"/>
     </row>
     <row r="59" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="114">
+      <c r="A59" s="117">
         <v>44587</v>
       </c>
       <c r="B59" s="8"/>
@@ -3549,7 +3646,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="115"/>
+      <c r="A60" s="119"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4" t="s">
         <v>120</v>
@@ -3559,7 +3656,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="115"/>
+      <c r="A61" s="119"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4" t="s">
         <v>123</v>
@@ -3570,7 +3667,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="116"/>
+      <c r="A62" s="118"/>
       <c r="B62" s="29"/>
       <c r="C62" s="29" t="s">
         <v>124</v>
@@ -3579,7 +3676,7 @@
       <c r="E62" s="29"/>
     </row>
     <row r="63" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="114">
+      <c r="A63" s="117">
         <v>44588</v>
       </c>
       <c r="B63" s="8"/>
@@ -3594,7 +3691,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="115"/>
+      <c r="A64" s="119"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4" t="s">
         <v>126</v>
@@ -3605,7 +3702,7 @@
       <c r="E64" s="4"/>
     </row>
     <row r="65" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="115"/>
+      <c r="A65" s="119"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4" t="s">
         <v>127</v>
@@ -3616,7 +3713,7 @@
       <c r="E65" s="4"/>
     </row>
     <row r="66" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="116"/>
+      <c r="A66" s="118"/>
       <c r="B66" s="30"/>
       <c r="C66" s="30" t="s">
         <v>128</v>
@@ -3625,7 +3722,7 @@
       <c r="E66" s="30"/>
     </row>
     <row r="67" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="114">
+      <c r="A67" s="117">
         <v>44589</v>
       </c>
       <c r="B67" s="8"/>
@@ -3636,7 +3733,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="115"/>
+      <c r="A68" s="119"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -3645,7 +3742,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="116"/>
+      <c r="A69" s="118"/>
       <c r="B69" s="32"/>
       <c r="C69" s="32"/>
       <c r="D69" s="32"/>
@@ -3678,7 +3775,7 @@
       </c>
     </row>
     <row r="72" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="114">
+      <c r="A72" s="117">
         <v>44594</v>
       </c>
       <c r="B72" s="8"/>
@@ -3689,7 +3786,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="115"/>
+      <c r="A73" s="119"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
@@ -3698,7 +3795,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="115"/>
+      <c r="A74" s="119"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
@@ -3707,7 +3804,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="116"/>
+      <c r="A75" s="118"/>
       <c r="B75" s="37"/>
       <c r="C75" s="37"/>
       <c r="D75" s="37"/>
@@ -3738,7 +3835,7 @@
       </c>
     </row>
     <row r="78" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="114">
+      <c r="A78" s="117">
         <v>44598</v>
       </c>
       <c r="B78" s="8"/>
@@ -3749,7 +3846,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="115"/>
+      <c r="A79" s="119"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
@@ -3758,7 +3855,7 @@
       </c>
     </row>
     <row r="80" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="115"/>
+      <c r="A80" s="119"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -3767,7 +3864,7 @@
       </c>
     </row>
     <row r="81" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="116"/>
+      <c r="A81" s="118"/>
       <c r="B81" s="48"/>
       <c r="C81" s="48"/>
       <c r="D81" s="48"/>
@@ -3776,7 +3873,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="114">
+      <c r="A82" s="117">
         <v>44599</v>
       </c>
       <c r="B82" s="8"/>
@@ -3787,7 +3884,7 @@
       </c>
     </row>
     <row r="83" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="115"/>
+      <c r="A83" s="119"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
@@ -3796,7 +3893,7 @@
       </c>
     </row>
     <row r="84" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="116"/>
+      <c r="A84" s="118"/>
       <c r="B84" s="49"/>
       <c r="C84" s="49"/>
       <c r="D84" s="49"/>
@@ -3805,7 +3902,7 @@
       </c>
     </row>
     <row r="85" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="114">
+      <c r="A85" s="117">
         <v>44600</v>
       </c>
       <c r="B85" s="8"/>
@@ -3823,7 +3920,7 @@
       <c r="J85" s="8"/>
     </row>
     <row r="86" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="116"/>
+      <c r="A86" s="118"/>
       <c r="B86" s="50"/>
       <c r="C86" s="50"/>
       <c r="D86" s="50"/>
@@ -3837,7 +3934,7 @@
       <c r="J86" s="50"/>
     </row>
     <row r="87" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="114">
+      <c r="A87" s="117">
         <v>44601</v>
       </c>
       <c r="B87" s="8"/>
@@ -3855,7 +3952,7 @@
       <c r="J87" s="8"/>
     </row>
     <row r="88" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="115"/>
+      <c r="A88" s="119"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4" t="s">
@@ -3871,7 +3968,7 @@
       <c r="J88" s="4"/>
     </row>
     <row r="89" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="115"/>
+      <c r="A89" s="119"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4" t="s">
@@ -3887,7 +3984,7 @@
       <c r="J89" s="4"/>
     </row>
     <row r="90" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="115"/>
+      <c r="A90" s="119"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4" t="s">
@@ -3901,7 +3998,7 @@
       <c r="J90" s="4"/>
     </row>
     <row r="91" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="115"/>
+      <c r="A91" s="119"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4" t="s">
@@ -3915,7 +4012,7 @@
       <c r="J91" s="4"/>
     </row>
     <row r="92" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="115"/>
+      <c r="A92" s="119"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="52" t="s">
@@ -3929,7 +4026,7 @@
       <c r="J92" s="4"/>
     </row>
     <row r="93" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="115"/>
+      <c r="A93" s="119"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4" t="s">
@@ -3943,7 +4040,7 @@
       <c r="J93" s="4"/>
     </row>
     <row r="94" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="116"/>
+      <c r="A94" s="118"/>
       <c r="B94" s="51"/>
       <c r="C94" s="51"/>
       <c r="D94" s="54" t="s">
@@ -3957,7 +4054,7 @@
       <c r="J94" s="51"/>
     </row>
     <row r="95" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="114">
+      <c r="A95" s="117">
         <v>44602</v>
       </c>
       <c r="B95" s="8"/>
@@ -3975,7 +4072,7 @@
       <c r="J95" s="8"/>
     </row>
     <row r="96" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="115"/>
+      <c r="A96" s="119"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4" t="s">
@@ -3991,7 +4088,7 @@
       <c r="J96" s="4"/>
     </row>
     <row r="97" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="116"/>
+      <c r="A97" s="118"/>
       <c r="B97" s="53"/>
       <c r="C97" s="53"/>
       <c r="D97" s="53"/>
@@ -4005,7 +4102,7 @@
       <c r="J97" s="53"/>
     </row>
     <row r="98" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="114">
+      <c r="A98" s="117">
         <v>44603</v>
       </c>
       <c r="B98" s="8"/>
@@ -4021,7 +4118,7 @@
       <c r="J98" s="8"/>
     </row>
     <row r="99" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="115"/>
+      <c r="A99" s="119"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
@@ -4035,7 +4132,7 @@
       <c r="J99" s="4"/>
     </row>
     <row r="100" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="115"/>
+      <c r="A100" s="119"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
@@ -4049,7 +4146,7 @@
       <c r="J100" s="4"/>
     </row>
     <row r="101" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="115"/>
+      <c r="A101" s="119"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
@@ -4063,7 +4160,7 @@
       <c r="J101" s="4"/>
     </row>
     <row r="102" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="115"/>
+      <c r="A102" s="119"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
@@ -4077,7 +4174,7 @@
       <c r="J102" s="4"/>
     </row>
     <row r="103" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="116"/>
+      <c r="A103" s="118"/>
       <c r="B103" s="55"/>
       <c r="C103" s="55"/>
       <c r="D103" s="55"/>
@@ -4091,7 +4188,7 @@
       <c r="J103" s="55"/>
     </row>
     <row r="104" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="114">
+      <c r="A104" s="117">
         <v>44604</v>
       </c>
       <c r="B104" s="8"/>
@@ -4107,7 +4204,7 @@
       <c r="J104" s="8"/>
     </row>
     <row r="105" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="115"/>
+      <c r="A105" s="119"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
@@ -4121,7 +4218,7 @@
       <c r="J105" s="4"/>
     </row>
     <row r="106" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="115"/>
+      <c r="A106" s="119"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
@@ -4135,7 +4232,7 @@
       <c r="J106" s="4"/>
     </row>
     <row r="107" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="115"/>
+      <c r="A107" s="119"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
@@ -4149,7 +4246,7 @@
       <c r="J107" s="4"/>
     </row>
     <row r="108" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="115"/>
+      <c r="A108" s="119"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
@@ -4163,7 +4260,7 @@
       <c r="J108" s="4"/>
     </row>
     <row r="109" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="115"/>
+      <c r="A109" s="119"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
@@ -4177,7 +4274,7 @@
       <c r="J109" s="4"/>
     </row>
     <row r="110" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="116"/>
+      <c r="A110" s="118"/>
       <c r="B110" s="56"/>
       <c r="C110" s="56"/>
       <c r="D110" s="56"/>
@@ -4191,7 +4288,7 @@
       <c r="J110" s="56"/>
     </row>
     <row r="111" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="114">
+      <c r="A111" s="117">
         <v>44605</v>
       </c>
       <c r="B111" s="8"/>
@@ -4207,7 +4304,7 @@
       <c r="J111" s="8"/>
     </row>
     <row r="112" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="115"/>
+      <c r="A112" s="119"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
@@ -4221,7 +4318,7 @@
       <c r="J112" s="4"/>
     </row>
     <row r="113" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="115"/>
+      <c r="A113" s="119"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
@@ -4235,7 +4332,7 @@
       <c r="J113" s="4"/>
     </row>
     <row r="114" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="115"/>
+      <c r="A114" s="119"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
@@ -4249,7 +4346,7 @@
       <c r="J114" s="4"/>
     </row>
     <row r="115" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="115"/>
+      <c r="A115" s="119"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
@@ -4263,7 +4360,7 @@
       <c r="J115" s="4"/>
     </row>
     <row r="116" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="115"/>
+      <c r="A116" s="119"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
@@ -4277,7 +4374,7 @@
       <c r="J116" s="4"/>
     </row>
     <row r="117" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="116"/>
+      <c r="A117" s="118"/>
       <c r="B117" s="57"/>
       <c r="C117" s="57"/>
       <c r="D117" s="57"/>
@@ -4291,7 +4388,7 @@
       <c r="J117" s="57"/>
     </row>
     <row r="118" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="114">
+      <c r="A118" s="117">
         <v>44606</v>
       </c>
       <c r="B118" s="8"/>
@@ -4307,7 +4404,7 @@
       <c r="J118" s="8"/>
     </row>
     <row r="119" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="116"/>
+      <c r="A119" s="118"/>
       <c r="B119" s="58"/>
       <c r="C119" s="58"/>
       <c r="D119" s="58"/>
@@ -4321,7 +4418,7 @@
       <c r="J119" s="58"/>
     </row>
     <row r="120" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="114">
+      <c r="A120" s="117">
         <v>44607</v>
       </c>
       <c r="B120" s="8"/>
@@ -4337,7 +4434,7 @@
       <c r="J120" s="8"/>
     </row>
     <row r="121" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="116"/>
+      <c r="A121" s="118"/>
       <c r="B121" s="58"/>
       <c r="C121" s="58"/>
       <c r="D121" s="58"/>
@@ -4381,7 +4478,7 @@
       <c r="J123" s="64"/>
     </row>
     <row r="124" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="114">
+      <c r="A124" s="117">
         <v>44609</v>
       </c>
       <c r="B124" s="8"/>
@@ -4397,7 +4494,7 @@
       <c r="J124" s="8"/>
     </row>
     <row r="125" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="115"/>
+      <c r="A125" s="119"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
@@ -4411,7 +4508,7 @@
       <c r="J125" s="4"/>
     </row>
     <row r="126" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="115"/>
+      <c r="A126" s="119"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
@@ -4425,7 +4522,7 @@
       <c r="J126" s="4"/>
     </row>
     <row r="127" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="115"/>
+      <c r="A127" s="119"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
@@ -4439,7 +4536,7 @@
       <c r="J127" s="4"/>
     </row>
     <row r="128" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="115"/>
+      <c r="A128" s="119"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
@@ -4453,7 +4550,7 @@
       <c r="J128" s="4"/>
     </row>
     <row r="129" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="116"/>
+      <c r="A129" s="118"/>
       <c r="B129" s="67"/>
       <c r="C129" s="67"/>
       <c r="D129" s="67"/>
@@ -4467,7 +4564,7 @@
       <c r="J129" s="67"/>
     </row>
     <row r="130" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="114">
+      <c r="A130" s="117">
         <v>44610</v>
       </c>
       <c r="B130" s="8"/>
@@ -4483,7 +4580,7 @@
       <c r="J130" s="8"/>
     </row>
     <row r="131" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="115"/>
+      <c r="A131" s="119"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
@@ -4497,7 +4594,7 @@
       <c r="J131" s="4"/>
     </row>
     <row r="132" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="115"/>
+      <c r="A132" s="119"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
@@ -4511,7 +4608,7 @@
       <c r="J132" s="4"/>
     </row>
     <row r="133" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="116"/>
+      <c r="A133" s="118"/>
       <c r="B133" s="67"/>
       <c r="C133" s="67"/>
       <c r="D133" s="67"/>
@@ -4543,7 +4640,7 @@
       <c r="J134" s="12"/>
     </row>
     <row r="135" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="114">
+      <c r="A135" s="117">
         <v>44612</v>
       </c>
       <c r="B135" s="8"/>
@@ -4559,7 +4656,7 @@
       <c r="J135" s="8"/>
     </row>
     <row r="136" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="116"/>
+      <c r="A136" s="118"/>
       <c r="B136" s="71"/>
       <c r="C136" s="71"/>
       <c r="D136" s="71"/>
@@ -4573,7 +4670,7 @@
       <c r="J136" s="71"/>
     </row>
     <row r="137" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="114">
+      <c r="A137" s="117">
         <v>44613</v>
       </c>
       <c r="B137" s="8"/>
@@ -4591,7 +4688,7 @@
       <c r="J137" s="8"/>
     </row>
     <row r="138" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="115"/>
+      <c r="A138" s="119"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
       <c r="D138" s="4"/>
@@ -4607,7 +4704,7 @@
       <c r="J138" s="4"/>
     </row>
     <row r="139" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="115"/>
+      <c r="A139" s="119"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
@@ -4621,7 +4718,7 @@
       <c r="J139" s="4"/>
     </row>
     <row r="140" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="115"/>
+      <c r="A140" s="119"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
       <c r="D140" s="4"/>
@@ -4635,7 +4732,7 @@
       <c r="J140" s="4"/>
     </row>
     <row r="141" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="115"/>
+      <c r="A141" s="119"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
       <c r="D141" s="4"/>
@@ -4649,7 +4746,7 @@
       <c r="J141" s="4"/>
     </row>
     <row r="142" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="115"/>
+      <c r="A142" s="119"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
@@ -4663,7 +4760,7 @@
       <c r="J142" s="4"/>
     </row>
     <row r="143" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="116"/>
+      <c r="A143" s="118"/>
       <c r="B143" s="72"/>
       <c r="C143" s="72"/>
       <c r="D143" s="72"/>
@@ -4677,7 +4774,7 @@
       <c r="J143" s="72"/>
     </row>
     <row r="144" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="114">
+      <c r="A144" s="117">
         <v>44614</v>
       </c>
       <c r="B144" s="8"/>
@@ -4695,7 +4792,7 @@
       <c r="J144" s="8"/>
     </row>
     <row r="145" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="115"/>
+      <c r="A145" s="119"/>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
       <c r="D145" s="4"/>
@@ -4709,7 +4806,7 @@
       <c r="J145" s="4"/>
     </row>
     <row r="146" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="115"/>
+      <c r="A146" s="119"/>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
       <c r="D146" s="4"/>
@@ -4723,7 +4820,7 @@
       <c r="J146" s="4"/>
     </row>
     <row r="147" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="115"/>
+      <c r="A147" s="119"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
       <c r="D147" s="4"/>
@@ -4737,7 +4834,7 @@
       <c r="J147" s="4"/>
     </row>
     <row r="148" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="116"/>
+      <c r="A148" s="118"/>
       <c r="B148" s="75"/>
       <c r="C148" s="75"/>
       <c r="D148" s="75"/>
@@ -4751,7 +4848,7 @@
       <c r="J148" s="75"/>
     </row>
     <row r="149" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="114">
+      <c r="A149" s="117">
         <v>44615</v>
       </c>
       <c r="B149" s="8"/>
@@ -4769,7 +4866,7 @@
       <c r="J149" s="8"/>
     </row>
     <row r="150" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="116"/>
+      <c r="A150" s="118"/>
       <c r="B150" s="75"/>
       <c r="C150" s="75"/>
       <c r="D150" s="75"/>
@@ -4783,7 +4880,7 @@
       <c r="J150" s="75"/>
     </row>
     <row r="151" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="114">
+      <c r="A151" s="117">
         <v>44616</v>
       </c>
       <c r="B151" s="8"/>
@@ -4801,7 +4898,7 @@
       <c r="J151" s="8"/>
     </row>
     <row r="152" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="115"/>
+      <c r="A152" s="119"/>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
@@ -4815,7 +4912,7 @@
       <c r="J152" s="4"/>
     </row>
     <row r="153" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="116"/>
+      <c r="A153" s="118"/>
       <c r="B153" s="76"/>
       <c r="C153" s="76"/>
       <c r="D153" s="76"/>
@@ -4829,7 +4926,7 @@
       <c r="J153" s="76"/>
     </row>
     <row r="154" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="114">
+      <c r="A154" s="117">
         <v>44617</v>
       </c>
       <c r="B154" s="8"/>
@@ -4847,7 +4944,7 @@
       <c r="J154" s="8"/>
     </row>
     <row r="155" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="115"/>
+      <c r="A155" s="119"/>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
@@ -4861,7 +4958,7 @@
       <c r="J155" s="4"/>
     </row>
     <row r="156" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="116"/>
+      <c r="A156" s="118"/>
       <c r="B156" s="77"/>
       <c r="C156" s="77"/>
       <c r="D156" s="77"/>
@@ -4875,7 +4972,7 @@
       <c r="J156" s="77"/>
     </row>
     <row r="157" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="114">
+      <c r="A157" s="117">
         <v>44618</v>
       </c>
       <c r="B157" s="8"/>
@@ -4895,7 +4992,7 @@
       <c r="J157" s="8"/>
     </row>
     <row r="158" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="116"/>
+      <c r="A158" s="118"/>
       <c r="B158" s="78"/>
       <c r="C158" s="78"/>
       <c r="D158" s="78"/>
@@ -4911,7 +5008,7 @@
       <c r="J158" s="78"/>
     </row>
     <row r="159" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="114">
+      <c r="A159" s="117">
         <v>44619</v>
       </c>
       <c r="B159" s="8"/>
@@ -4929,7 +5026,7 @@
       <c r="J159" s="8"/>
     </row>
     <row r="160" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="115"/>
+      <c r="A160" s="119"/>
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
       <c r="D160" s="4"/>
@@ -4945,7 +5042,7 @@
       <c r="J160" s="4"/>
     </row>
     <row r="161" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="116"/>
+      <c r="A161" s="118"/>
       <c r="B161" s="79"/>
       <c r="C161" s="79"/>
       <c r="D161" s="79"/>
@@ -4961,7 +5058,7 @@
       <c r="J161" s="79"/>
     </row>
     <row r="162" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="114">
+      <c r="A162" s="117">
         <v>44620</v>
       </c>
       <c r="B162" s="8"/>
@@ -4979,7 +5076,7 @@
       <c r="J162" s="8"/>
     </row>
     <row r="163" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="115"/>
+      <c r="A163" s="119"/>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
       <c r="D163" s="4"/>
@@ -4995,7 +5092,7 @@
       <c r="J163" s="4"/>
     </row>
     <row r="164" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="116"/>
+      <c r="A164" s="118"/>
       <c r="B164" s="80"/>
       <c r="C164" s="80"/>
       <c r="D164" s="80"/>
@@ -5009,7 +5106,7 @@
       <c r="J164" s="80"/>
     </row>
     <row r="165" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="114">
+      <c r="A165" s="117">
         <v>44621</v>
       </c>
       <c r="B165" s="8"/>
@@ -5025,7 +5122,7 @@
       <c r="J165" s="8"/>
     </row>
     <row r="166" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="115"/>
+      <c r="A166" s="119"/>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
@@ -5039,7 +5136,7 @@
       <c r="J166" s="4"/>
     </row>
     <row r="167" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="116"/>
+      <c r="A167" s="118"/>
       <c r="B167" s="81"/>
       <c r="C167" s="81"/>
       <c r="D167" s="81"/>
@@ -5053,7 +5150,7 @@
       <c r="J167" s="81"/>
     </row>
     <row r="168" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="114">
+      <c r="A168" s="117">
         <v>44622</v>
       </c>
       <c r="B168" s="8"/>
@@ -5074,7 +5171,7 @@
       </c>
     </row>
     <row r="169" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="115"/>
+      <c r="A169" s="119"/>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
@@ -5089,7 +5186,7 @@
       </c>
     </row>
     <row r="170" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="116"/>
+      <c r="A170" s="118"/>
       <c r="B170" s="82"/>
       <c r="C170" s="82"/>
       <c r="D170" s="82"/>
@@ -5104,7 +5201,7 @@
       </c>
     </row>
     <row r="171" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="114">
+      <c r="A171" s="117">
         <v>44623</v>
       </c>
       <c r="B171" s="8"/>
@@ -5121,7 +5218,7 @@
       <c r="K171" s="8"/>
     </row>
     <row r="172" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="115"/>
+      <c r="A172" s="119"/>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
       <c r="D172" s="4"/>
@@ -5136,7 +5233,7 @@
       <c r="K172" s="4"/>
     </row>
     <row r="173" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="116"/>
+      <c r="A173" s="118"/>
       <c r="B173" s="83"/>
       <c r="C173" s="83"/>
       <c r="D173" s="83"/>
@@ -5151,7 +5248,7 @@
       <c r="K173" s="83"/>
     </row>
     <row r="174" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="114">
+      <c r="A174" s="117">
         <v>44625</v>
       </c>
       <c r="B174" s="8"/>
@@ -5168,7 +5265,7 @@
       <c r="K174" s="8"/>
     </row>
     <row r="175" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="116"/>
+      <c r="A175" s="118"/>
       <c r="B175" s="85"/>
       <c r="C175" s="85"/>
       <c r="D175" s="85"/>
@@ -5183,7 +5280,7 @@
       <c r="K175" s="85"/>
     </row>
     <row r="176" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="114">
+      <c r="A176" s="117">
         <v>44626</v>
       </c>
       <c r="B176" s="8"/>
@@ -5201,7 +5298,7 @@
       </c>
     </row>
     <row r="177" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="115"/>
+      <c r="A177" s="119"/>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
       <c r="D177" s="4"/>
@@ -5217,7 +5314,7 @@
       </c>
     </row>
     <row r="178" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="116"/>
+      <c r="A178" s="118"/>
       <c r="B178" s="86"/>
       <c r="C178" s="86"/>
       <c r="D178" s="86"/>
@@ -5233,7 +5330,7 @@
       </c>
     </row>
     <row r="179" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="114">
+      <c r="A179" s="117">
         <v>44627</v>
       </c>
       <c r="B179" s="8"/>
@@ -5251,7 +5348,7 @@
       </c>
     </row>
     <row r="180" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="115"/>
+      <c r="A180" s="119"/>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
       <c r="D180" s="4"/>
@@ -5267,7 +5364,7 @@
       </c>
     </row>
     <row r="181" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="115"/>
+      <c r="A181" s="119"/>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
       <c r="D181" s="4"/>
@@ -5283,7 +5380,7 @@
       </c>
     </row>
     <row r="182" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A182" s="116"/>
+      <c r="A182" s="118"/>
       <c r="B182" s="88"/>
       <c r="C182" s="88"/>
       <c r="D182" s="88"/>
@@ -5296,7 +5393,7 @@
       <c r="K182" s="88"/>
     </row>
     <row r="183" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="114">
+      <c r="A183" s="117">
         <v>44628</v>
       </c>
       <c r="B183" s="8" t="s">
@@ -5313,7 +5410,7 @@
       <c r="K183" s="8"/>
     </row>
     <row r="184" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="115"/>
+      <c r="A184" s="119"/>
       <c r="B184" s="4" t="s">
         <v>400</v>
       </c>
@@ -5328,7 +5425,7 @@
       <c r="K184" s="4"/>
     </row>
     <row r="185" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="116"/>
+      <c r="A185" s="118"/>
       <c r="B185" s="91" t="s">
         <v>404</v>
       </c>
@@ -5360,7 +5457,7 @@
       <c r="K186" s="12"/>
     </row>
     <row r="187" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="114">
+      <c r="A187" s="117">
         <v>44630</v>
       </c>
       <c r="B187" s="8"/>
@@ -5377,7 +5474,7 @@
       <c r="K187" s="8"/>
     </row>
     <row r="188" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="115"/>
+      <c r="A188" s="119"/>
       <c r="B188" s="4"/>
       <c r="C188" s="4"/>
       <c r="D188" s="4"/>
@@ -5392,7 +5489,7 @@
       <c r="K188" s="4"/>
     </row>
     <row r="189" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="115"/>
+      <c r="A189" s="119"/>
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
       <c r="D189" s="4"/>
@@ -5407,7 +5504,7 @@
       <c r="K189" s="4"/>
     </row>
     <row r="190" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A190" s="115"/>
+      <c r="A190" s="119"/>
       <c r="B190" s="4"/>
       <c r="C190" s="4"/>
       <c r="D190" s="4"/>
@@ -5422,7 +5519,7 @@
       <c r="K190" s="4"/>
     </row>
     <row r="191" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A191" s="116"/>
+      <c r="A191" s="118"/>
       <c r="B191" s="93"/>
       <c r="C191" s="93"/>
       <c r="D191" s="93"/>
@@ -5437,7 +5534,7 @@
       <c r="K191" s="93"/>
     </row>
     <row r="192" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A192" s="114">
+      <c r="A192" s="117">
         <v>44631</v>
       </c>
       <c r="B192" s="8" t="s">
@@ -5454,7 +5551,7 @@
       <c r="K192" s="8"/>
     </row>
     <row r="193" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="115"/>
+      <c r="A193" s="119"/>
       <c r="B193" s="4" t="s">
         <v>423</v>
       </c>
@@ -5469,7 +5566,7 @@
       <c r="K193" s="4"/>
     </row>
     <row r="194" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="116"/>
+      <c r="A194" s="118"/>
       <c r="B194" s="93" t="s">
         <v>424</v>
       </c>
@@ -5484,7 +5581,7 @@
       <c r="K194" s="93"/>
     </row>
     <row r="195" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="114">
+      <c r="A195" s="117">
         <v>44632</v>
       </c>
       <c r="B195" s="8" t="s">
@@ -5501,7 +5598,7 @@
       <c r="K195" s="8"/>
     </row>
     <row r="196" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="115"/>
+      <c r="A196" s="119"/>
       <c r="B196" s="4" t="s">
         <v>427</v>
       </c>
@@ -5516,7 +5613,7 @@
       <c r="K196" s="4"/>
     </row>
     <row r="197" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A197" s="116"/>
+      <c r="A197" s="118"/>
       <c r="B197" s="95" t="s">
         <v>428</v>
       </c>
@@ -5531,7 +5628,7 @@
       <c r="K197" s="95"/>
     </row>
     <row r="198" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="114">
+      <c r="A198" s="117">
         <v>44633</v>
       </c>
       <c r="B198" s="8" t="s">
@@ -5548,7 +5645,7 @@
       <c r="K198" s="8"/>
     </row>
     <row r="199" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="115"/>
+      <c r="A199" s="119"/>
       <c r="B199" s="4" t="s">
         <v>432</v>
       </c>
@@ -5563,7 +5660,7 @@
       <c r="K199" s="4"/>
     </row>
     <row r="200" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A200" s="116"/>
+      <c r="A200" s="118"/>
       <c r="B200" s="96" t="s">
         <v>433</v>
       </c>
@@ -5578,7 +5675,7 @@
       <c r="K200" s="96"/>
     </row>
     <row r="201" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A201" s="114">
+      <c r="A201" s="117">
         <v>44634</v>
       </c>
       <c r="B201" s="8"/>
@@ -5595,7 +5692,7 @@
       <c r="K201" s="8"/>
     </row>
     <row r="202" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A202" s="115"/>
+      <c r="A202" s="119"/>
       <c r="B202" s="4"/>
       <c r="C202" s="4" t="s">
         <v>445</v>
@@ -5610,7 +5707,7 @@
       <c r="K202" s="4"/>
     </row>
     <row r="203" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A203" s="116"/>
+      <c r="A203" s="118"/>
       <c r="B203" s="98"/>
       <c r="C203" s="98" t="s">
         <v>446</v>
@@ -5642,7 +5739,7 @@
       <c r="K204" s="12"/>
     </row>
     <row r="205" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A205" s="114">
+      <c r="A205" s="117">
         <v>44636</v>
       </c>
       <c r="B205" s="8"/>
@@ -5659,7 +5756,7 @@
       <c r="K205" s="8"/>
     </row>
     <row r="206" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A206" s="116"/>
+      <c r="A206" s="118"/>
       <c r="B206" s="101"/>
       <c r="C206" s="101" t="s">
         <v>460</v>
@@ -5674,7 +5771,7 @@
       <c r="K206" s="101"/>
     </row>
     <row r="207" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A207" s="114">
+      <c r="A207" s="117">
         <v>44639</v>
       </c>
       <c r="B207" s="8"/>
@@ -5691,7 +5788,7 @@
       <c r="K207" s="8"/>
     </row>
     <row r="208" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A208" s="115"/>
+      <c r="A208" s="119"/>
       <c r="B208" s="4"/>
       <c r="C208" s="4" t="s">
         <v>475</v>
@@ -5706,7 +5803,7 @@
       <c r="K208" s="4"/>
     </row>
     <row r="209" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A209" s="116"/>
+      <c r="A209" s="118"/>
       <c r="B209" s="105"/>
       <c r="C209" s="105" t="s">
         <v>476</v>
@@ -5721,7 +5818,7 @@
       <c r="K209" s="105"/>
     </row>
     <row r="210" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="114">
+      <c r="A210" s="117">
         <v>44641</v>
       </c>
       <c r="B210" s="8"/>
@@ -5738,7 +5835,7 @@
       <c r="K210" s="8"/>
     </row>
     <row r="211" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A211" s="115"/>
+      <c r="A211" s="119"/>
       <c r="B211" s="4"/>
       <c r="C211" s="4" t="s">
         <v>486</v>
@@ -5753,7 +5850,7 @@
       <c r="K211" s="4"/>
     </row>
     <row r="212" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A212" s="116"/>
+      <c r="A212" s="118"/>
       <c r="B212" s="107"/>
       <c r="C212" s="107" t="s">
         <v>487</v>
@@ -5768,7 +5865,7 @@
       <c r="K212" s="107"/>
     </row>
     <row r="213" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A213" s="114">
+      <c r="A213" s="117">
         <v>44644</v>
       </c>
       <c r="B213" s="8"/>
@@ -5786,7 +5883,7 @@
       </c>
     </row>
     <row r="214" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A214" s="115"/>
+      <c r="A214" s="119"/>
       <c r="B214" s="4"/>
       <c r="C214" s="4"/>
       <c r="D214" s="4"/>
@@ -5802,7 +5899,7 @@
       </c>
     </row>
     <row r="215" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A215" s="115"/>
+      <c r="A215" s="119"/>
       <c r="B215" s="4"/>
       <c r="C215" s="4"/>
       <c r="D215" s="4"/>
@@ -5818,7 +5915,7 @@
       </c>
     </row>
     <row r="216" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A216" s="116"/>
+      <c r="A216" s="118"/>
       <c r="B216" s="110"/>
       <c r="C216" s="110"/>
       <c r="D216" s="110"/>
@@ -5834,7 +5931,7 @@
       </c>
     </row>
     <row r="217" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A217" s="114">
+      <c r="A217" s="117">
         <v>44647</v>
       </c>
       <c r="B217" s="8" t="s">
@@ -5852,7 +5949,7 @@
       <c r="M217" s="8"/>
     </row>
     <row r="218" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A218" s="116"/>
+      <c r="A218" s="118"/>
       <c r="B218" s="113" t="s">
         <v>516</v>
       </c>
@@ -5868,7 +5965,7 @@
       <c r="M218" s="113"/>
     </row>
     <row r="219" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A219" s="114">
+      <c r="A219" s="117">
         <v>44648</v>
       </c>
       <c r="B219" s="8" t="s">
@@ -5888,7 +5985,7 @@
       <c r="M219" s="8"/>
     </row>
     <row r="220" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A220" s="115"/>
+      <c r="A220" s="119"/>
       <c r="B220" s="4" t="s">
         <v>518</v>
       </c>
@@ -5906,7 +6003,7 @@
       <c r="M220" s="4"/>
     </row>
     <row r="221" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A221" s="115"/>
+      <c r="A221" s="119"/>
       <c r="B221" s="4" t="s">
         <v>519</v>
       </c>
@@ -5922,7 +6019,7 @@
       <c r="M221" s="4"/>
     </row>
     <row r="222" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="115"/>
+      <c r="A222" s="119"/>
       <c r="B222" s="4" t="s">
         <v>520</v>
       </c>
@@ -5938,7 +6035,7 @@
       <c r="M222" s="4"/>
     </row>
     <row r="223" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A223" s="115"/>
+      <c r="A223" s="119"/>
       <c r="B223" s="4" t="s">
         <v>521</v>
       </c>
@@ -5954,7 +6051,7 @@
       <c r="M223" s="4"/>
     </row>
     <row r="224" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A224" s="116"/>
+      <c r="A224" s="118"/>
       <c r="B224" s="113" t="s">
         <v>522</v>
       </c>
@@ -5969,38 +6066,56 @@
       <c r="K224" s="113"/>
       <c r="M224" s="113"/>
     </row>
-    <row r="225" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A225" s="28"/>
-      <c r="B225" s="3"/>
-      <c r="C225" s="3"/>
-      <c r="D225" s="4"/>
-      <c r="E225" s="4"/>
-      <c r="F225" s="4"/>
-      <c r="G225" s="4"/>
-      <c r="H225" s="4"/>
-      <c r="I225" s="4"/>
-      <c r="J225" s="4"/>
-      <c r="K225" s="4"/>
-      <c r="M225" s="4"/>
-    </row>
-    <row r="226" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A226" s="28"/>
-      <c r="B226" s="3"/>
-      <c r="C226" s="3"/>
+    <row r="225" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A225" s="117">
+        <v>44650</v>
+      </c>
+      <c r="B225" s="8" t="s">
+        <v>546</v>
+      </c>
+      <c r="C225" s="8" t="s">
+        <v>538</v>
+      </c>
+      <c r="D225" s="8"/>
+      <c r="E225" s="8"/>
+      <c r="F225" s="8"/>
+      <c r="G225" s="8"/>
+      <c r="H225" s="8" t="s">
+        <v>550</v>
+      </c>
+      <c r="I225" s="8"/>
+      <c r="J225" s="8"/>
+      <c r="K225" s="8"/>
+      <c r="M225" s="8"/>
+    </row>
+    <row r="226" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A226" s="119"/>
+      <c r="B226" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="C226" s="4" t="s">
+        <v>539</v>
+      </c>
       <c r="D226" s="4"/>
       <c r="E226" s="4"/>
       <c r="F226" s="4"/>
       <c r="G226" s="4"/>
-      <c r="H226" s="4"/>
+      <c r="H226" s="4" t="s">
+        <v>551</v>
+      </c>
       <c r="I226" s="4"/>
       <c r="J226" s="4"/>
       <c r="K226" s="4"/>
       <c r="M226" s="4"/>
     </row>
-    <row r="227" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A227" s="28"/>
-      <c r="B227" s="3"/>
-      <c r="C227" s="3"/>
+    <row r="227" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A227" s="119"/>
+      <c r="B227" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="C227" s="4" t="s">
+        <v>540</v>
+      </c>
       <c r="D227" s="4"/>
       <c r="E227" s="4"/>
       <c r="F227" s="4"/>
@@ -6011,19 +6126,23 @@
       <c r="K227" s="4"/>
       <c r="M227" s="4"/>
     </row>
-    <row r="228" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A228" s="28"/>
-      <c r="B228" s="3"/>
-      <c r="C228" s="3"/>
-      <c r="D228" s="4"/>
-      <c r="E228" s="4"/>
-      <c r="F228" s="4"/>
-      <c r="G228" s="4"/>
-      <c r="H228" s="4"/>
-      <c r="I228" s="4"/>
-      <c r="J228" s="4"/>
-      <c r="K228" s="4"/>
-      <c r="M228" s="4"/>
+    <row r="228" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A228" s="118"/>
+      <c r="B228" s="116" t="s">
+        <v>549</v>
+      </c>
+      <c r="C228" s="116" t="s">
+        <v>545</v>
+      </c>
+      <c r="D228" s="116"/>
+      <c r="E228" s="116"/>
+      <c r="F228" s="116"/>
+      <c r="G228" s="116"/>
+      <c r="H228" s="116"/>
+      <c r="I228" s="116"/>
+      <c r="J228" s="116"/>
+      <c r="K228" s="116"/>
+      <c r="M228" s="116"/>
     </row>
     <row r="229" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A229" s="28"/>
@@ -10837,7 +10956,51 @@
       <c r="D623" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="59">
+  <mergeCells count="60">
+    <mergeCell ref="A225:A228"/>
+    <mergeCell ref="A213:A216"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="A124:A129"/>
+    <mergeCell ref="A179:A182"/>
+    <mergeCell ref="A176:A178"/>
+    <mergeCell ref="A130:A133"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="A162:A164"/>
+    <mergeCell ref="A144:A148"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="A154:A156"/>
+    <mergeCell ref="A159:A161"/>
+    <mergeCell ref="A157:A158"/>
+    <mergeCell ref="A151:A153"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A201:A203"/>
+    <mergeCell ref="A192:A194"/>
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="A87:A94"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="A98:A103"/>
+    <mergeCell ref="A104:A110"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="A111:A117"/>
     <mergeCell ref="A217:A218"/>
     <mergeCell ref="A219:A224"/>
     <mergeCell ref="A210:A212"/>
@@ -10854,49 +11017,6 @@
     <mergeCell ref="A195:A197"/>
     <mergeCell ref="A187:A191"/>
     <mergeCell ref="A205:A206"/>
-    <mergeCell ref="A201:A203"/>
-    <mergeCell ref="A192:A194"/>
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="A87:A94"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="A98:A103"/>
-    <mergeCell ref="A104:A110"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="A111:A117"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A39"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="A213:A216"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="A124:A129"/>
-    <mergeCell ref="A179:A182"/>
-    <mergeCell ref="A176:A178"/>
-    <mergeCell ref="A130:A133"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="A162:A164"/>
-    <mergeCell ref="A144:A148"/>
-    <mergeCell ref="A149:A150"/>
-    <mergeCell ref="A154:A156"/>
-    <mergeCell ref="A159:A161"/>
-    <mergeCell ref="A157:A158"/>
-    <mergeCell ref="A151:A153"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10909,10 +11029,10 @@
   <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D29" sqref="D29"/>
+      <selection pane="bottomRight" activeCell="C48" sqref="C47:C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.25"/>
@@ -10971,7 +11091,7 @@
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="114">
+      <c r="A4" s="117">
         <v>44595</v>
       </c>
       <c r="B4" s="38"/>
@@ -10982,7 +11102,7 @@
       <c r="E4" s="38"/>
     </row>
     <row r="5" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="116"/>
+      <c r="A5" s="118"/>
       <c r="B5" s="42"/>
       <c r="C5" s="46" t="s">
         <v>161</v>
@@ -10991,7 +11111,7 @@
       <c r="E5" s="42"/>
     </row>
     <row r="6" spans="1:7" s="39" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="114">
+      <c r="A6" s="117">
         <v>44596</v>
       </c>
       <c r="B6" s="38"/>
@@ -11002,7 +11122,7 @@
       <c r="E6" s="38"/>
     </row>
     <row r="7" spans="1:7" s="43" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="116"/>
+      <c r="A7" s="118"/>
       <c r="B7" s="42"/>
       <c r="C7" s="42" t="s">
         <v>171</v>
@@ -11022,7 +11142,7 @@
       <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="114">
+      <c r="A9" s="117">
         <v>44608</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -11033,7 +11153,7 @@
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="115"/>
+      <c r="A10" s="119"/>
       <c r="B10" s="4" t="s">
         <v>237</v>
       </c>
@@ -11042,7 +11162,7 @@
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="116"/>
+      <c r="A11" s="118"/>
       <c r="B11" s="64" t="s">
         <v>238</v>
       </c>
@@ -11051,7 +11171,7 @@
       <c r="E11" s="64"/>
     </row>
     <row r="12" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="114">
+      <c r="A12" s="117">
         <v>44609</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -11062,7 +11182,7 @@
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="115"/>
+      <c r="A13" s="119"/>
       <c r="B13" s="4" t="s">
         <v>250</v>
       </c>
@@ -11071,7 +11191,7 @@
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="116"/>
+      <c r="A14" s="118"/>
       <c r="B14" s="67" t="s">
         <v>251</v>
       </c>
@@ -11102,7 +11222,7 @@
       <c r="E16" s="12"/>
     </row>
     <row r="17" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="114">
+      <c r="A17" s="117">
         <v>44616</v>
       </c>
       <c r="B17" s="8"/>
@@ -11113,7 +11233,7 @@
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="115"/>
+      <c r="A18" s="119"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
         <v>303</v>
@@ -11122,7 +11242,7 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="116"/>
+      <c r="A19" s="118"/>
       <c r="B19" s="77"/>
       <c r="C19" s="77" t="s">
         <v>304</v>
@@ -11131,7 +11251,7 @@
       <c r="E19" s="77"/>
     </row>
     <row r="20" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="114">
+      <c r="A20" s="117">
         <v>44621</v>
       </c>
       <c r="B20" s="8"/>
@@ -11142,7 +11262,7 @@
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="115"/>
+      <c r="A21" s="119"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
         <v>350</v>
@@ -11151,7 +11271,7 @@
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="116"/>
+      <c r="A22" s="118"/>
       <c r="B22" s="81"/>
       <c r="C22" s="81" t="s">
         <v>351</v>
@@ -11160,7 +11280,7 @@
       <c r="E22" s="81"/>
     </row>
     <row r="23" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="114">
+      <c r="A23" s="117">
         <v>44623</v>
       </c>
       <c r="B23" s="8"/>
@@ -11171,7 +11291,7 @@
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="116"/>
+      <c r="A24" s="118"/>
       <c r="B24" s="83"/>
       <c r="C24" s="83" t="s">
         <v>366</v>
@@ -11180,7 +11300,7 @@
       <c r="E24" s="83"/>
     </row>
     <row r="25" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="114">
+      <c r="A25" s="117">
         <v>44628</v>
       </c>
       <c r="B25" s="8"/>
@@ -11191,7 +11311,7 @@
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="115"/>
+      <c r="A26" s="119"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
         <v>396</v>
@@ -11200,7 +11320,7 @@
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="115"/>
+      <c r="A27" s="119"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
         <v>397</v>
@@ -11209,7 +11329,7 @@
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="116"/>
+      <c r="A28" s="118"/>
       <c r="B28" s="89"/>
       <c r="C28" s="89" t="s">
         <v>398</v>
@@ -11218,7 +11338,7 @@
       <c r="E28" s="89"/>
     </row>
     <row r="29" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="114">
+      <c r="A29" s="117">
         <v>44635</v>
       </c>
       <c r="B29" s="8"/>
@@ -11233,7 +11353,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="115"/>
+      <c r="A30" s="119"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
         <v>455</v>
@@ -11246,7 +11366,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="116"/>
+      <c r="A31" s="118"/>
       <c r="B31" s="99"/>
       <c r="C31" s="99" t="s">
         <v>456</v>
@@ -11274,7 +11394,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="114">
+      <c r="A33" s="117">
         <v>44640</v>
       </c>
       <c r="B33" s="8"/>
@@ -11287,7 +11407,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="116"/>
+      <c r="A34" s="118"/>
       <c r="B34" s="106"/>
       <c r="C34" s="106"/>
       <c r="D34" s="106"/>
@@ -11298,7 +11418,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="114">
+      <c r="A35" s="117">
         <v>44642</v>
       </c>
       <c r="B35" s="8"/>
@@ -11313,7 +11433,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="116"/>
+      <c r="A36" s="118"/>
       <c r="B36" s="108"/>
       <c r="C36" s="108" t="s">
         <v>494</v>
@@ -11326,7 +11446,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="114">
+      <c r="A37" s="117">
         <v>44643</v>
       </c>
       <c r="B37" s="8"/>
@@ -11341,7 +11461,7 @@
       <c r="G37" s="8"/>
     </row>
     <row r="38" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="116"/>
+      <c r="A38" s="118"/>
       <c r="B38" s="108"/>
       <c r="C38" s="108"/>
       <c r="D38" s="108" t="s">
@@ -11352,7 +11472,7 @@
       <c r="G38" s="108"/>
     </row>
     <row r="39" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="114">
+      <c r="A39" s="117">
         <v>44648</v>
       </c>
       <c r="B39" s="8"/>
@@ -11365,7 +11485,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="115"/>
+      <c r="A40" s="119"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -11376,7 +11496,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="116"/>
+      <c r="A41" s="118"/>
       <c r="B41" s="113"/>
       <c r="C41" s="113"/>
       <c r="D41" s="113"/>
@@ -11386,23 +11506,33 @@
         <v>529</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A42" s="100"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-    </row>
-    <row r="43" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A43" s="100"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
+    <row r="42" spans="1:7" s="13" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A42" s="11">
+        <v>44649</v>
+      </c>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12" t="s">
+        <v>534</v>
+      </c>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+    </row>
+    <row r="43" spans="1:7" s="13" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A43" s="11">
+        <v>44651</v>
+      </c>
+      <c r="B43" s="12"/>
+      <c r="C43" s="12" t="s">
+        <v>544</v>
+      </c>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12" t="s">
+        <v>552</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A44" s="100"/>
@@ -11581,10 +11711,10 @@
   <dimension ref="A1:C242"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B143" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B155" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B145" sqref="B145"/>
+      <selection pane="bottomRight" activeCell="F151" sqref="F151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.4"/>
@@ -11603,7 +11733,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="115">
+      <c r="A2" s="119">
         <v>44563</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -11614,35 +11744,35 @@
       </c>
     </row>
     <row r="3" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="115"/>
+      <c r="A3" s="119"/>
       <c r="B3" s="4"/>
       <c r="C3" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="115"/>
+      <c r="A4" s="119"/>
       <c r="B4" s="4"/>
       <c r="C4" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="115"/>
+      <c r="A5" s="119"/>
       <c r="B5" s="4"/>
       <c r="C5" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="116"/>
+      <c r="A6" s="118"/>
       <c r="B6" s="6"/>
       <c r="C6" s="15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="114">
+      <c r="A7" s="117">
         <v>44564</v>
       </c>
       <c r="B7" s="8"/>
@@ -11651,56 +11781,56 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="115"/>
+      <c r="A8" s="119"/>
       <c r="B8" s="4"/>
       <c r="C8" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="115"/>
+      <c r="A9" s="119"/>
       <c r="B9" s="4"/>
       <c r="C9" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="115"/>
+      <c r="A10" s="119"/>
       <c r="B10" s="4"/>
       <c r="C10" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="115"/>
+      <c r="A11" s="119"/>
       <c r="B11" s="4"/>
       <c r="C11" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="115"/>
+      <c r="A12" s="119"/>
       <c r="B12" s="4"/>
       <c r="C12" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="115"/>
+      <c r="A13" s="119"/>
       <c r="B13" s="4"/>
       <c r="C13" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="116"/>
+      <c r="A14" s="118"/>
       <c r="B14" s="6"/>
       <c r="C14" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="114">
+      <c r="A15" s="117">
         <v>44565</v>
       </c>
       <c r="B15" s="8"/>
@@ -11709,14 +11839,14 @@
       </c>
     </row>
     <row r="16" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="118"/>
+      <c r="A16" s="121"/>
       <c r="B16" s="6"/>
       <c r="C16" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="114">
+      <c r="A17" s="117">
         <v>44570</v>
       </c>
       <c r="B17" s="8"/>
@@ -11725,19 +11855,19 @@
       </c>
     </row>
     <row r="18" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="115"/>
+      <c r="A18" s="119"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="119" t="s">
+      <c r="C18" s="122" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="116"/>
+      <c r="A19" s="118"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="120"/>
+      <c r="C19" s="123"/>
     </row>
     <row r="20" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="114">
+      <c r="A20" s="117">
         <v>44574</v>
       </c>
       <c r="B20" s="8"/>
@@ -11746,21 +11876,21 @@
       </c>
     </row>
     <row r="21" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="115"/>
+      <c r="A21" s="119"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="116"/>
+      <c r="A22" s="118"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="114">
+      <c r="A23" s="117">
         <v>44590</v>
       </c>
       <c r="B23" s="8"/>
@@ -11769,28 +11899,28 @@
       </c>
     </row>
     <row r="24" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="117"/>
+      <c r="A24" s="120"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="117"/>
+      <c r="A25" s="120"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="118"/>
+      <c r="A26" s="121"/>
       <c r="B26" s="33"/>
       <c r="C26" s="33" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A27" s="114">
+      <c r="A27" s="117">
         <v>44591</v>
       </c>
       <c r="B27" s="8"/>
@@ -11799,49 +11929,49 @@
       </c>
     </row>
     <row r="28" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A28" s="115"/>
+      <c r="A28" s="119"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A29" s="115"/>
+      <c r="A29" s="119"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A30" s="115"/>
+      <c r="A30" s="119"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A31" s="115"/>
+      <c r="A31" s="119"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A32" s="115"/>
+      <c r="A32" s="119"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A33" s="116"/>
+      <c r="A33" s="118"/>
       <c r="B33" s="34"/>
       <c r="C33" s="34" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A34" s="114">
+      <c r="A34" s="117">
         <v>44593</v>
       </c>
       <c r="B34" s="8"/>
@@ -11850,14 +11980,14 @@
       </c>
     </row>
     <row r="35" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A35" s="116"/>
+      <c r="A35" s="118"/>
       <c r="B35" s="36"/>
       <c r="C35" s="36" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="39" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A36" s="114">
+      <c r="A36" s="117">
         <v>44594</v>
       </c>
       <c r="B36" s="38" t="s">
@@ -11868,35 +11998,35 @@
       </c>
     </row>
     <row r="37" spans="1:3" s="41" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A37" s="115"/>
+      <c r="A37" s="119"/>
       <c r="B37" s="40" t="s">
         <v>164</v>
       </c>
       <c r="C37" s="40"/>
     </row>
     <row r="38" spans="1:3" s="41" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A38" s="115"/>
+      <c r="A38" s="119"/>
       <c r="B38" s="40" t="s">
         <v>157</v>
       </c>
       <c r="C38" s="40"/>
     </row>
     <row r="39" spans="1:3" s="41" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A39" s="115"/>
+      <c r="A39" s="119"/>
       <c r="B39" s="40" t="s">
         <v>158</v>
       </c>
       <c r="C39" s="40"/>
     </row>
     <row r="40" spans="1:3" s="43" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A40" s="116"/>
+      <c r="A40" s="118"/>
       <c r="B40" s="42" t="s">
         <v>159</v>
       </c>
       <c r="C40" s="42"/>
     </row>
     <row r="41" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A41" s="114">
+      <c r="A41" s="117">
         <v>44595</v>
       </c>
       <c r="B41" s="8" t="s">
@@ -11907,7 +12037,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A42" s="116"/>
+      <c r="A42" s="118"/>
       <c r="B42" s="44" t="s">
         <v>166</v>
       </c>
@@ -11916,7 +12046,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A43" s="114">
+      <c r="A43" s="117">
         <v>44596</v>
       </c>
       <c r="B43" s="8" t="s">
@@ -11927,21 +12057,21 @@
       </c>
     </row>
     <row r="44" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A44" s="115"/>
+      <c r="A44" s="119"/>
       <c r="B44" s="4" t="s">
         <v>169</v>
       </c>
       <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A45" s="115"/>
+      <c r="A45" s="119"/>
       <c r="B45" s="4" t="s">
         <v>172</v>
       </c>
       <c r="C45" s="4"/>
     </row>
     <row r="46" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A46" s="116"/>
+      <c r="A46" s="118"/>
       <c r="B46" s="47" t="s">
         <v>173</v>
       </c>
@@ -11966,7 +12096,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A49" s="114">
+      <c r="A49" s="117">
         <v>44608</v>
       </c>
       <c r="B49" s="8" t="s">
@@ -11975,14 +12105,14 @@
       <c r="C49" s="8"/>
     </row>
     <row r="50" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A50" s="116"/>
+      <c r="A50" s="118"/>
       <c r="B50" s="64" t="s">
         <v>236</v>
       </c>
       <c r="C50" s="64"/>
     </row>
     <row r="51" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A51" s="114">
+      <c r="A51" s="117">
         <v>44609</v>
       </c>
       <c r="B51" s="8" t="s">
@@ -11991,14 +12121,14 @@
       <c r="C51" s="8"/>
     </row>
     <row r="52" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A52" s="116"/>
+      <c r="A52" s="118"/>
       <c r="B52" s="65" t="s">
         <v>248</v>
       </c>
       <c r="C52" s="65"/>
     </row>
     <row r="53" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A53" s="114">
+      <c r="A53" s="117">
         <v>44610</v>
       </c>
       <c r="B53" s="8" t="s">
@@ -12007,28 +12137,28 @@
       <c r="C53" s="8"/>
     </row>
     <row r="54" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A54" s="115"/>
+      <c r="A54" s="119"/>
       <c r="B54" s="4" t="s">
         <v>253</v>
       </c>
       <c r="C54" s="4"/>
     </row>
     <row r="55" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A55" s="115"/>
+      <c r="A55" s="119"/>
       <c r="B55" s="4" t="s">
         <v>258</v>
       </c>
       <c r="C55" s="4"/>
     </row>
     <row r="56" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A56" s="116"/>
+      <c r="A56" s="118"/>
       <c r="B56" s="68" t="s">
         <v>259</v>
       </c>
       <c r="C56" s="68"/>
     </row>
     <row r="57" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A57" s="114">
+      <c r="A57" s="117">
         <v>44611</v>
       </c>
       <c r="B57" s="8" t="s">
@@ -12037,28 +12167,28 @@
       <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A58" s="115"/>
+      <c r="A58" s="119"/>
       <c r="B58" s="4" t="s">
         <v>261</v>
       </c>
       <c r="C58" s="4"/>
     </row>
     <row r="59" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="115"/>
+      <c r="A59" s="119"/>
       <c r="B59" s="4" t="s">
         <v>263</v>
       </c>
       <c r="C59" s="4"/>
     </row>
     <row r="60" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A60" s="116"/>
+      <c r="A60" s="118"/>
       <c r="B60" s="70" t="s">
         <v>264</v>
       </c>
       <c r="C60" s="70"/>
     </row>
     <row r="61" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A61" s="114">
+      <c r="A61" s="117">
         <v>44612</v>
       </c>
       <c r="B61" s="8" t="s">
@@ -12067,21 +12197,21 @@
       <c r="C61" s="8"/>
     </row>
     <row r="62" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A62" s="115"/>
+      <c r="A62" s="119"/>
       <c r="B62" s="4" t="s">
         <v>266</v>
       </c>
       <c r="C62" s="4"/>
     </row>
     <row r="63" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="116"/>
+      <c r="A63" s="118"/>
       <c r="B63" s="71" t="s">
         <v>267</v>
       </c>
       <c r="C63" s="71"/>
     </row>
     <row r="64" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="114">
+      <c r="A64" s="117">
         <v>44613</v>
       </c>
       <c r="B64" s="8" t="s">
@@ -12090,14 +12220,14 @@
       <c r="C64" s="8"/>
     </row>
     <row r="65" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A65" s="116"/>
+      <c r="A65" s="118"/>
       <c r="B65" s="73" t="s">
         <v>281</v>
       </c>
       <c r="C65" s="73"/>
     </row>
     <row r="66" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A66" s="114">
+      <c r="A66" s="117">
         <v>44614</v>
       </c>
       <c r="B66" s="8" t="s">
@@ -12106,28 +12236,28 @@
       <c r="C66" s="8"/>
     </row>
     <row r="67" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A67" s="115"/>
+      <c r="A67" s="119"/>
       <c r="B67" s="4" t="s">
         <v>283</v>
       </c>
       <c r="C67" s="4"/>
     </row>
     <row r="68" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A68" s="115"/>
+      <c r="A68" s="119"/>
       <c r="B68" s="4" t="s">
         <v>291</v>
       </c>
       <c r="C68" s="4"/>
     </row>
     <row r="69" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A69" s="116"/>
+      <c r="A69" s="118"/>
       <c r="B69" s="74" t="s">
         <v>292</v>
       </c>
       <c r="C69" s="74"/>
     </row>
     <row r="70" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A70" s="114">
+      <c r="A70" s="117">
         <v>44615</v>
       </c>
       <c r="B70" s="8" t="s">
@@ -12136,14 +12266,14 @@
       <c r="C70" s="8"/>
     </row>
     <row r="71" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A71" s="115"/>
+      <c r="A71" s="119"/>
       <c r="B71" s="4" t="s">
         <v>294</v>
       </c>
       <c r="C71" s="4"/>
     </row>
     <row r="72" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A72" s="116"/>
+      <c r="A72" s="118"/>
       <c r="B72" s="75" t="s">
         <v>298</v>
       </c>
@@ -12159,7 +12289,7 @@
       <c r="C73" s="12"/>
     </row>
     <row r="74" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A74" s="114">
+      <c r="A74" s="117">
         <v>44617</v>
       </c>
       <c r="B74" s="8" t="s">
@@ -12168,21 +12298,21 @@
       <c r="C74" s="8"/>
     </row>
     <row r="75" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A75" s="115"/>
+      <c r="A75" s="119"/>
       <c r="B75" s="4" t="s">
         <v>309</v>
       </c>
       <c r="C75" s="4"/>
     </row>
     <row r="76" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A76" s="116"/>
+      <c r="A76" s="118"/>
       <c r="B76" s="77" t="s">
         <v>310</v>
       </c>
       <c r="C76" s="77"/>
     </row>
     <row r="77" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A77" s="114">
+      <c r="A77" s="117">
         <v>44618</v>
       </c>
       <c r="B77" s="8" t="s">
@@ -12191,49 +12321,49 @@
       <c r="C77" s="8"/>
     </row>
     <row r="78" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A78" s="115"/>
+      <c r="A78" s="119"/>
       <c r="B78" s="4" t="s">
         <v>315</v>
       </c>
       <c r="C78" s="4"/>
     </row>
     <row r="79" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A79" s="115"/>
+      <c r="A79" s="119"/>
       <c r="B79" s="4" t="s">
         <v>316</v>
       </c>
       <c r="C79" s="4"/>
     </row>
     <row r="80" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A80" s="115"/>
+      <c r="A80" s="119"/>
       <c r="B80" s="4" t="s">
         <v>317</v>
       </c>
       <c r="C80" s="4"/>
     </row>
     <row r="81" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A81" s="115"/>
+      <c r="A81" s="119"/>
       <c r="B81" s="4" t="s">
         <v>325</v>
       </c>
       <c r="C81" s="4"/>
     </row>
     <row r="82" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A82" s="115"/>
+      <c r="A82" s="119"/>
       <c r="B82" s="4" t="s">
         <v>326</v>
       </c>
       <c r="C82" s="4"/>
     </row>
     <row r="83" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A83" s="116"/>
+      <c r="A83" s="118"/>
       <c r="B83" s="78" t="s">
         <v>327</v>
       </c>
       <c r="C83" s="78"/>
     </row>
     <row r="84" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A84" s="114">
+      <c r="A84" s="117">
         <v>44619</v>
       </c>
       <c r="B84" s="8" t="s">
@@ -12242,14 +12372,14 @@
       <c r="C84" s="8"/>
     </row>
     <row r="85" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A85" s="116"/>
+      <c r="A85" s="118"/>
       <c r="B85" s="79" t="s">
         <v>329</v>
       </c>
       <c r="C85" s="79"/>
     </row>
     <row r="86" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A86" s="114">
+      <c r="A86" s="117">
         <v>44620</v>
       </c>
       <c r="B86" s="8" t="s">
@@ -12258,28 +12388,28 @@
       <c r="C86" s="8"/>
     </row>
     <row r="87" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A87" s="115"/>
+      <c r="A87" s="119"/>
       <c r="B87" s="4" t="s">
         <v>337</v>
       </c>
       <c r="C87" s="4"/>
     </row>
     <row r="88" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A88" s="115"/>
+      <c r="A88" s="119"/>
       <c r="B88" s="4" t="s">
         <v>338</v>
       </c>
       <c r="C88" s="4"/>
     </row>
     <row r="89" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A89" s="116"/>
+      <c r="A89" s="118"/>
       <c r="B89" s="80" t="s">
         <v>339</v>
       </c>
       <c r="C89" s="80"/>
     </row>
     <row r="90" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A90" s="114">
+      <c r="A90" s="117">
         <v>44621</v>
       </c>
       <c r="B90" s="8" t="s">
@@ -12288,28 +12418,28 @@
       <c r="C90" s="8"/>
     </row>
     <row r="91" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A91" s="115"/>
+      <c r="A91" s="119"/>
       <c r="B91" s="4" t="s">
         <v>346</v>
       </c>
       <c r="C91" s="4"/>
     </row>
     <row r="92" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A92" s="115"/>
+      <c r="A92" s="119"/>
       <c r="B92" s="4" t="s">
         <v>347</v>
       </c>
       <c r="C92" s="4"/>
     </row>
     <row r="93" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A93" s="116"/>
+      <c r="A93" s="118"/>
       <c r="B93" s="81" t="s">
         <v>348</v>
       </c>
       <c r="C93" s="81"/>
     </row>
     <row r="94" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A94" s="114">
+      <c r="A94" s="117">
         <v>44622</v>
       </c>
       <c r="B94" s="8" t="s">
@@ -12318,14 +12448,14 @@
       <c r="C94" s="8"/>
     </row>
     <row r="95" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A95" s="116"/>
+      <c r="A95" s="118"/>
       <c r="B95" s="82" t="s">
         <v>356</v>
       </c>
       <c r="C95" s="82"/>
     </row>
     <row r="96" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A96" s="114">
+      <c r="A96" s="117">
         <v>44623</v>
       </c>
       <c r="B96" s="8" t="s">
@@ -12334,14 +12464,14 @@
       <c r="C96" s="8"/>
     </row>
     <row r="97" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A97" s="116"/>
+      <c r="A97" s="118"/>
       <c r="B97" s="83" t="s">
         <v>364</v>
       </c>
       <c r="C97" s="83"/>
     </row>
     <row r="98" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A98" s="114">
+      <c r="A98" s="117">
         <v>44624</v>
       </c>
       <c r="B98" s="8" t="s">
@@ -12350,14 +12480,14 @@
       <c r="C98" s="8"/>
     </row>
     <row r="99" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A99" s="116"/>
+      <c r="A99" s="118"/>
       <c r="B99" s="84" t="s">
         <v>375</v>
       </c>
       <c r="C99" s="84"/>
     </row>
     <row r="100" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A100" s="114">
+      <c r="A100" s="117">
         <v>44625</v>
       </c>
       <c r="B100" s="8" t="s">
@@ -12366,14 +12496,14 @@
       <c r="C100" s="8"/>
     </row>
     <row r="101" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A101" s="116"/>
+      <c r="A101" s="118"/>
       <c r="B101" s="85" t="s">
         <v>380</v>
       </c>
       <c r="C101" s="85"/>
     </row>
     <row r="102" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A102" s="114">
+      <c r="A102" s="117">
         <v>44626</v>
       </c>
       <c r="B102" s="8" t="s">
@@ -12382,14 +12512,14 @@
       <c r="C102" s="8"/>
     </row>
     <row r="103" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A103" s="116"/>
+      <c r="A103" s="118"/>
       <c r="B103" s="87" t="s">
         <v>386</v>
       </c>
       <c r="C103" s="87"/>
     </row>
     <row r="104" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A104" s="114">
+      <c r="A104" s="117">
         <v>44627</v>
       </c>
       <c r="B104" s="8" t="s">
@@ -12398,7 +12528,7 @@
       <c r="C104" s="8"/>
     </row>
     <row r="105" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A105" s="116"/>
+      <c r="A105" s="118"/>
       <c r="B105" s="88" t="s">
         <v>391</v>
       </c>
@@ -12414,7 +12544,7 @@
       <c r="C106" s="12"/>
     </row>
     <row r="107" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A107" s="114">
+      <c r="A107" s="117">
         <v>44629</v>
       </c>
       <c r="B107" s="8" t="s">
@@ -12423,14 +12553,14 @@
       <c r="C107" s="8"/>
     </row>
     <row r="108" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A108" s="116"/>
+      <c r="A108" s="118"/>
       <c r="B108" s="91" t="s">
         <v>407</v>
       </c>
       <c r="C108" s="91"/>
     </row>
     <row r="109" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A109" s="114">
+      <c r="A109" s="117">
         <v>44630</v>
       </c>
       <c r="B109" s="8" t="s">
@@ -12439,14 +12569,14 @@
       <c r="C109" s="8"/>
     </row>
     <row r="110" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A110" s="116"/>
+      <c r="A110" s="118"/>
       <c r="B110" s="92" t="s">
         <v>410</v>
       </c>
       <c r="C110" s="92"/>
     </row>
     <row r="111" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A111" s="114">
+      <c r="A111" s="117">
         <v>44631</v>
       </c>
       <c r="B111" s="8" t="s">
@@ -12455,14 +12585,14 @@
       <c r="C111" s="8"/>
     </row>
     <row r="112" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A112" s="116"/>
+      <c r="A112" s="118"/>
       <c r="B112" s="93" t="s">
         <v>420</v>
       </c>
       <c r="C112" s="93"/>
     </row>
     <row r="113" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A113" s="114">
+      <c r="A113" s="117">
         <v>44632</v>
       </c>
       <c r="B113" s="8" t="s">
@@ -12471,14 +12601,14 @@
       <c r="C113" s="8"/>
     </row>
     <row r="114" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A114" s="116"/>
+      <c r="A114" s="118"/>
       <c r="B114" s="94" t="s">
         <v>425</v>
       </c>
       <c r="C114" s="94"/>
     </row>
     <row r="115" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A115" s="114">
+      <c r="A115" s="117">
         <v>44633</v>
       </c>
       <c r="B115" s="8" t="s">
@@ -12487,14 +12617,14 @@
       <c r="C115" s="8"/>
     </row>
     <row r="116" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A116" s="116"/>
+      <c r="A116" s="118"/>
       <c r="B116" s="96" t="s">
         <v>430</v>
       </c>
       <c r="C116" s="96"/>
     </row>
     <row r="117" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A117" s="114">
+      <c r="A117" s="117">
         <v>44634</v>
       </c>
       <c r="B117" s="8" t="s">
@@ -12503,14 +12633,14 @@
       <c r="C117" s="8"/>
     </row>
     <row r="118" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A118" s="116"/>
+      <c r="A118" s="118"/>
       <c r="B118" s="97" t="s">
         <v>439</v>
       </c>
       <c r="C118" s="97"/>
     </row>
     <row r="119" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A119" s="114">
+      <c r="A119" s="117">
         <v>44635</v>
       </c>
       <c r="B119" s="8" t="s">
@@ -12519,14 +12649,14 @@
       <c r="C119" s="8"/>
     </row>
     <row r="120" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A120" s="116"/>
+      <c r="A120" s="118"/>
       <c r="B120" s="98" t="s">
         <v>448</v>
       </c>
       <c r="C120" s="98"/>
     </row>
     <row r="121" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A121" s="114">
+      <c r="A121" s="117">
         <v>44636</v>
       </c>
       <c r="B121" s="8" t="s">
@@ -12535,14 +12665,14 @@
       <c r="C121" s="8"/>
     </row>
     <row r="122" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A122" s="116"/>
+      <c r="A122" s="118"/>
       <c r="B122" s="99" t="s">
         <v>458</v>
       </c>
       <c r="C122" s="99"/>
     </row>
     <row r="123" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A123" s="114">
+      <c r="A123" s="117">
         <v>44637</v>
       </c>
       <c r="B123" s="8" t="s">
@@ -12551,28 +12681,28 @@
       <c r="C123" s="8"/>
     </row>
     <row r="124" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A124" s="115"/>
+      <c r="A124" s="119"/>
       <c r="B124" s="4" t="s">
         <v>464</v>
       </c>
       <c r="C124" s="4"/>
     </row>
     <row r="125" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A125" s="115"/>
+      <c r="A125" s="119"/>
       <c r="B125" s="4" t="s">
         <v>465</v>
       </c>
       <c r="C125" s="4"/>
     </row>
     <row r="126" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A126" s="116"/>
+      <c r="A126" s="118"/>
       <c r="B126" s="102" t="s">
         <v>466</v>
       </c>
       <c r="C126" s="102"/>
     </row>
     <row r="127" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A127" s="114">
+      <c r="A127" s="117">
         <v>44638</v>
       </c>
       <c r="B127" s="8" t="s">
@@ -12581,14 +12711,14 @@
       <c r="C127" s="8"/>
     </row>
     <row r="128" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A128" s="116"/>
+      <c r="A128" s="118"/>
       <c r="B128" s="103" t="s">
         <v>469</v>
       </c>
       <c r="C128" s="103"/>
     </row>
     <row r="129" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A129" s="114">
+      <c r="A129" s="117">
         <v>44639</v>
       </c>
       <c r="B129" s="8" t="s">
@@ -12597,14 +12727,14 @@
       <c r="C129" s="8"/>
     </row>
     <row r="130" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A130" s="116"/>
+      <c r="A130" s="118"/>
       <c r="B130" s="104" t="s">
         <v>471</v>
       </c>
       <c r="C130" s="104"/>
     </row>
     <row r="131" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A131" s="114">
+      <c r="A131" s="117">
         <v>44640</v>
       </c>
       <c r="B131" s="8" t="s">
@@ -12613,21 +12743,21 @@
       <c r="C131" s="8"/>
     </row>
     <row r="132" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A132" s="115"/>
+      <c r="A132" s="119"/>
       <c r="B132" s="4" t="s">
         <v>478</v>
       </c>
       <c r="C132" s="4"/>
     </row>
     <row r="133" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A133" s="116"/>
+      <c r="A133" s="118"/>
       <c r="B133" s="105" t="s">
         <v>479</v>
       </c>
       <c r="C133" s="105"/>
     </row>
     <row r="134" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A134" s="114">
+      <c r="A134" s="117">
         <v>44641</v>
       </c>
       <c r="B134" s="8" t="s">
@@ -12636,21 +12766,21 @@
       <c r="C134" s="8"/>
     </row>
     <row r="135" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A135" s="115"/>
+      <c r="A135" s="119"/>
       <c r="B135" s="4" t="s">
         <v>483</v>
       </c>
       <c r="C135" s="4"/>
     </row>
     <row r="136" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A136" s="116"/>
+      <c r="A136" s="118"/>
       <c r="B136" s="107" t="s">
         <v>484</v>
       </c>
       <c r="C136" s="107"/>
     </row>
     <row r="137" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A137" s="114">
+      <c r="A137" s="117">
         <v>44642</v>
       </c>
       <c r="B137" s="8" t="s">
@@ -12659,14 +12789,14 @@
       <c r="C137" s="8"/>
     </row>
     <row r="138" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A138" s="116"/>
+      <c r="A138" s="118"/>
       <c r="B138" s="108" t="s">
         <v>496</v>
       </c>
       <c r="C138" s="108"/>
     </row>
     <row r="139" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A139" s="114">
+      <c r="A139" s="117">
         <v>44643</v>
       </c>
       <c r="B139" s="8" t="s">
@@ -12675,14 +12805,14 @@
       <c r="C139" s="8"/>
     </row>
     <row r="140" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A140" s="116"/>
+      <c r="A140" s="118"/>
       <c r="B140" s="108" t="s">
         <v>500</v>
       </c>
       <c r="C140" s="108"/>
     </row>
     <row r="141" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A141" s="114">
+      <c r="A141" s="117">
         <v>44644</v>
       </c>
       <c r="B141" s="8" t="s">
@@ -12691,21 +12821,21 @@
       <c r="C141" s="8"/>
     </row>
     <row r="142" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A142" s="115"/>
+      <c r="A142" s="119"/>
       <c r="B142" s="4" t="s">
         <v>504</v>
       </c>
       <c r="C142" s="4"/>
     </row>
     <row r="143" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A143" s="116"/>
+      <c r="A143" s="118"/>
       <c r="B143" s="109" t="s">
         <v>505</v>
       </c>
       <c r="C143" s="109"/>
     </row>
     <row r="144" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A144" s="114">
+      <c r="A144" s="117">
         <v>44645</v>
       </c>
       <c r="B144" s="8" t="s">
@@ -12714,7 +12844,7 @@
       <c r="C144" s="8"/>
     </row>
     <row r="145" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A145" s="116"/>
+      <c r="A145" s="118"/>
       <c r="B145" s="111" t="s">
         <v>511</v>
       </c>
@@ -12730,7 +12860,7 @@
       <c r="C146" s="12"/>
     </row>
     <row r="147" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A147" s="114">
+      <c r="A147" s="117">
         <v>44647</v>
       </c>
       <c r="B147" s="8" t="s">
@@ -12739,14 +12869,14 @@
       <c r="C147" s="8"/>
     </row>
     <row r="148" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A148" s="116"/>
+      <c r="A148" s="118"/>
       <c r="B148" s="112" t="s">
         <v>514</v>
       </c>
       <c r="C148" s="112"/>
     </row>
     <row r="149" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A149" s="114">
+      <c r="A149" s="117">
         <v>44648</v>
       </c>
       <c r="B149" s="8" t="s">
@@ -12755,70 +12885,94 @@
       <c r="C149" s="8"/>
     </row>
     <row r="150" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A150" s="115"/>
+      <c r="A150" s="119"/>
       <c r="B150" s="4" t="s">
         <v>523</v>
       </c>
       <c r="C150" s="4"/>
     </row>
     <row r="151" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A151" s="115"/>
+      <c r="A151" s="119"/>
       <c r="B151" s="4" t="s">
         <v>525</v>
       </c>
       <c r="C151" s="4"/>
     </row>
     <row r="152" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A152" s="116"/>
+      <c r="A152" s="118"/>
       <c r="B152" s="113" t="s">
         <v>526</v>
       </c>
       <c r="C152" s="113"/>
     </row>
-    <row r="153" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A153" s="28"/>
-      <c r="B153" s="3"/>
-      <c r="C153" s="3"/>
-    </row>
-    <row r="154" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A154" s="28"/>
-      <c r="B154" s="3"/>
-      <c r="C154" s="3"/>
-    </row>
-    <row r="155" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A155" s="28"/>
-      <c r="B155" s="3"/>
-      <c r="C155" s="3"/>
-    </row>
-    <row r="156" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A156" s="28"/>
-      <c r="B156" s="3"/>
-      <c r="C156" s="3"/>
-    </row>
-    <row r="157" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A157" s="28"/>
-      <c r="B157" s="3"/>
-      <c r="C157" s="3"/>
-    </row>
-    <row r="158" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A158" s="28"/>
-      <c r="B158" s="3"/>
-      <c r="C158" s="3"/>
-    </row>
-    <row r="159" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A159" s="28"/>
-      <c r="B159" s="3"/>
-      <c r="C159" s="3"/>
-    </row>
-    <row r="160" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A160" s="28"/>
-      <c r="B160" s="3"/>
-      <c r="C160" s="3"/>
-    </row>
-    <row r="161" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A161" s="28"/>
-      <c r="B161" s="3"/>
-      <c r="C161" s="3"/>
+    <row r="153" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A153" s="117">
+        <v>44649</v>
+      </c>
+      <c r="B153" s="8" t="s">
+        <v>531</v>
+      </c>
+      <c r="C153" s="8"/>
+    </row>
+    <row r="154" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A154" s="119"/>
+      <c r="B154" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="C154" s="4"/>
+    </row>
+    <row r="155" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A155" s="118"/>
+      <c r="B155" s="114" t="s">
+        <v>533</v>
+      </c>
+      <c r="C155" s="114"/>
+    </row>
+    <row r="156" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A156" s="117">
+        <v>44650</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>535</v>
+      </c>
+      <c r="C156" s="8"/>
+    </row>
+    <row r="157" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A157" s="119"/>
+      <c r="B157" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="C157" s="4"/>
+    </row>
+    <row r="158" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A158" s="118"/>
+      <c r="B158" s="114" t="s">
+        <v>537</v>
+      </c>
+      <c r="C158" s="114"/>
+    </row>
+    <row r="159" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A159" s="117">
+        <v>44651</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>541</v>
+      </c>
+      <c r="C159" s="8"/>
+    </row>
+    <row r="160" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A160" s="119"/>
+      <c r="B160" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="C160" s="4"/>
+    </row>
+    <row r="161" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A161" s="118"/>
+      <c r="B161" s="115" t="s">
+        <v>543</v>
+      </c>
+      <c r="C161" s="115"/>
     </row>
     <row r="162" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A162" s="28"/>
@@ -13224,46 +13378,7 @@
       <c r="C242" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="50">
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A149:A152"/>
-    <mergeCell ref="A113:A114"/>
-    <mergeCell ref="A131:A133"/>
-    <mergeCell ref="A129:A130"/>
-    <mergeCell ref="A127:A128"/>
-    <mergeCell ref="A123:A126"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="A90:A93"/>
-    <mergeCell ref="A86:A89"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="A77:A83"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="A57:A60"/>
+  <mergeCells count="53">
     <mergeCell ref="A98:A99"/>
     <mergeCell ref="A96:A97"/>
     <mergeCell ref="A109:A110"/>
@@ -13275,6 +13390,48 @@
     <mergeCell ref="A119:A120"/>
     <mergeCell ref="A117:A118"/>
     <mergeCell ref="A115:A116"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A90:A93"/>
+    <mergeCell ref="A86:A89"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="A77:A83"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A159:A161"/>
+    <mergeCell ref="A149:A152"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="A131:A133"/>
+    <mergeCell ref="A129:A130"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="A123:A126"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="A153:A155"/>
+    <mergeCell ref="A156:A158"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13319,7 +13476,7 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:17" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="114">
+      <c r="A2" s="117">
         <v>44623</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -13327,19 +13484,19 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A3" s="115"/>
+      <c r="A3" s="119"/>
       <c r="B3" s="4" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A4" s="116"/>
+      <c r="A4" s="118"/>
       <c r="B4" s="83" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="114">
+      <c r="A5" s="117">
         <v>44624</v>
       </c>
       <c r="B5" s="31" t="s">
@@ -13347,13 +13504,13 @@
       </c>
     </row>
     <row r="6" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="115"/>
+      <c r="A6" s="119"/>
       <c r="B6" s="52" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="116"/>
+      <c r="A7" s="118"/>
       <c r="B7" s="54" t="s">
         <v>378</v>
       </c>
@@ -13367,7 +13524,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="114">
+      <c r="A9" s="117">
         <v>44628</v>
       </c>
       <c r="B9" s="31"/>
@@ -13390,7 +13547,7 @@
       <c r="Q9" s="31"/>
     </row>
     <row r="10" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="116"/>
+      <c r="A10" s="118"/>
       <c r="B10" s="54"/>
       <c r="C10" s="54" t="s">
         <v>403</v>
@@ -13411,7 +13568,7 @@
       <c r="Q10" s="54"/>
     </row>
     <row r="11" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="114">
+      <c r="A11" s="117">
         <v>44630</v>
       </c>
       <c r="B11" s="31"/>
@@ -13434,7 +13591,7 @@
       <c r="Q11" s="31"/>
     </row>
     <row r="12" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="115"/>
+      <c r="A12" s="119"/>
       <c r="B12" s="52"/>
       <c r="C12" s="52" t="s">
         <v>417</v>
@@ -13455,7 +13612,7 @@
       <c r="Q12" s="52"/>
     </row>
     <row r="13" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="116"/>
+      <c r="A13" s="118"/>
       <c r="B13" s="54"/>
       <c r="C13" s="54" t="s">
         <v>418</v>
@@ -13476,7 +13633,7 @@
       <c r="Q13" s="54"/>
     </row>
     <row r="14" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="114">
+      <c r="A14" s="117">
         <v>44633</v>
       </c>
       <c r="B14" s="31"/>
@@ -13499,7 +13656,7 @@
       <c r="Q14" s="31"/>
     </row>
     <row r="15" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="115"/>
+      <c r="A15" s="119"/>
       <c r="B15" s="52"/>
       <c r="C15" s="52" t="s">
         <v>435</v>
@@ -13520,7 +13677,7 @@
       <c r="Q15" s="52"/>
     </row>
     <row r="16" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="115"/>
+      <c r="A16" s="119"/>
       <c r="B16" s="52"/>
       <c r="C16" s="52" t="s">
         <v>436</v>
@@ -13541,7 +13698,7 @@
       <c r="Q16" s="52"/>
     </row>
     <row r="17" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="116"/>
+      <c r="A17" s="118"/>
       <c r="B17" s="54"/>
       <c r="C17" s="54" t="s">
         <v>437</v>
@@ -13562,7 +13719,7 @@
       <c r="Q17" s="54"/>
     </row>
     <row r="18" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="114">
+      <c r="A18" s="117">
         <v>44634</v>
       </c>
       <c r="B18" s="31"/>
@@ -13585,7 +13742,7 @@
       <c r="Q18" s="31"/>
     </row>
     <row r="19" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="115"/>
+      <c r="A19" s="119"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52" t="s">
         <v>441</v>
@@ -13606,7 +13763,7 @@
       <c r="Q19" s="52"/>
     </row>
     <row r="20" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="115"/>
+      <c r="A20" s="119"/>
       <c r="B20" s="52"/>
       <c r="C20" s="52" t="s">
         <v>442</v>
@@ -13627,7 +13784,7 @@
       <c r="Q20" s="52"/>
     </row>
     <row r="21" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="116"/>
+      <c r="A21" s="118"/>
       <c r="B21" s="54"/>
       <c r="C21" s="54" t="s">
         <v>443</v>
@@ -13648,7 +13805,7 @@
       <c r="Q21" s="54"/>
     </row>
     <row r="22" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="114">
+      <c r="A22" s="117">
         <v>44636</v>
       </c>
       <c r="B22" s="31"/>
@@ -13671,7 +13828,7 @@
       <c r="Q22" s="31"/>
     </row>
     <row r="23" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="116"/>
+      <c r="A23" s="118"/>
       <c r="B23" s="54"/>
       <c r="C23" s="54" t="s">
         <v>462</v>
@@ -13692,7 +13849,7 @@
       <c r="Q23" s="54"/>
     </row>
     <row r="24" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="114">
+      <c r="A24" s="117">
         <v>44639</v>
       </c>
       <c r="B24" s="31"/>
@@ -13715,7 +13872,7 @@
       <c r="Q24" s="31"/>
     </row>
     <row r="25" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="116"/>
+      <c r="A25" s="118"/>
       <c r="B25" s="54"/>
       <c r="C25" s="54" t="s">
         <v>473</v>
@@ -13736,7 +13893,7 @@
       <c r="Q25" s="54"/>
     </row>
     <row r="26" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="114">
+      <c r="A26" s="117">
         <v>44641</v>
       </c>
       <c r="B26" s="31" t="s">
@@ -13759,7 +13916,7 @@
       <c r="Q26" s="31"/>
     </row>
     <row r="27" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="115"/>
+      <c r="A27" s="119"/>
       <c r="B27" s="52" t="s">
         <v>489</v>
       </c>
@@ -13780,7 +13937,7 @@
       <c r="Q27" s="52"/>
     </row>
     <row r="28" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="115"/>
+      <c r="A28" s="119"/>
       <c r="B28" s="52" t="s">
         <v>490</v>
       </c>
@@ -13801,7 +13958,7 @@
       <c r="Q28" s="52"/>
     </row>
     <row r="29" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="116"/>
+      <c r="A29" s="118"/>
       <c r="B29" s="54" t="s">
         <v>491</v>
       </c>
@@ -16741,7 +16898,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C434693-A01C-4220-BD8E-CE7EBA29C799}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
First update for April
</commit_message>
<xml_diff>
--- a/学习记录.xlsx
+++ b/学习记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\不怕晒的铃铛\Desktop\学习资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DBFDA1-031A-44FD-B30E-2D05E2AB135E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43DDC2C8-3CFB-4F31-8F37-D332C0EDDAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JavaWeb相关" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="577">
   <si>
     <t>JavaSE</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2246,6 +2246,102 @@
   </si>
   <si>
     <t>类适配器模式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>零钱兑换 II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>组合总和 Ⅳ（排列总和）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>爬楼梯(1-m)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>零钱兑换</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>轻量级锁</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完全平方数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单词拆分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>KMP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>偏向锁概述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>偏向锁hashCode撤销</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打家劫舍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打家劫舍 II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>打家劫舍 III</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>偏向锁撤销</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>偏向锁批量重偏向</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>偏向锁批量撤销</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>锁消除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wait和notify的原理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>wait和notify相关API介绍</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>买卖股票的最佳时机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>买卖股票的最佳时机 III</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>适配器模式</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>买卖股票的最佳时机 IV</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最佳买卖股票时机含冷冻期</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2353,7 +2449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="130">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2693,13 +2789,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2997,10 +3111,10 @@
   <dimension ref="A1:P623"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B220" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B224" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B237" sqref="B237"/>
+      <selection pane="bottomRight" activeCell="B227" sqref="B227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.35"/>
@@ -3070,7 +3184,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="117">
+      <c r="A3" s="123">
         <v>44566</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -3080,7 +3194,7 @@
       <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:16" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="119"/>
+      <c r="A4" s="124"/>
       <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
@@ -3088,7 +3202,7 @@
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:16" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="118"/>
+      <c r="A5" s="125"/>
       <c r="B5" s="6" t="s">
         <v>28</v>
       </c>
@@ -3126,7 +3240,7 @@
       <c r="D8" s="12"/>
     </row>
     <row r="9" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="117">
+      <c r="A9" s="123">
         <v>44572</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -3136,7 +3250,7 @@
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:16" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="118"/>
+      <c r="A10" s="125"/>
       <c r="B10" s="17" t="s">
         <v>38</v>
       </c>
@@ -3144,7 +3258,7 @@
       <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="117">
+      <c r="A11" s="123">
         <v>44573</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -3154,7 +3268,7 @@
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="119"/>
+      <c r="A12" s="124"/>
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
@@ -3162,7 +3276,7 @@
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="118"/>
+      <c r="A13" s="125"/>
       <c r="B13" s="18" t="s">
         <v>40</v>
       </c>
@@ -3170,7 +3284,7 @@
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="117">
+      <c r="A14" s="123">
         <v>44574</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -3180,7 +3294,7 @@
       <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:16" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="118"/>
+      <c r="A15" s="125"/>
       <c r="B15" s="19" t="s">
         <v>42</v>
       </c>
@@ -3190,7 +3304,7 @@
       <c r="D15" s="19"/>
     </row>
     <row r="16" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="117">
+      <c r="A16" s="123">
         <v>44575</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -3202,7 +3316,7 @@
       <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="119"/>
+      <c r="A17" s="124"/>
       <c r="B17" s="4" t="s">
         <v>47</v>
       </c>
@@ -3213,7 +3327,7 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="119"/>
+      <c r="A18" s="124"/>
       <c r="B18" s="4" t="s">
         <v>48</v>
       </c>
@@ -3224,7 +3338,7 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="118"/>
+      <c r="A19" s="125"/>
       <c r="B19" s="20" t="s">
         <v>49</v>
       </c>
@@ -3233,7 +3347,7 @@
       <c r="E19" s="21"/>
     </row>
     <row r="20" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="117">
+      <c r="A20" s="123">
         <v>44576</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -3246,7 +3360,7 @@
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="119"/>
+      <c r="A21" s="124"/>
       <c r="B21" s="4" t="s">
         <v>59</v>
       </c>
@@ -3257,7 +3371,7 @@
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="119"/>
+      <c r="A22" s="124"/>
       <c r="B22" s="4" t="s">
         <v>60</v>
       </c>
@@ -3268,7 +3382,7 @@
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="118"/>
+      <c r="A23" s="125"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20" t="s">
         <v>57</v>
@@ -3277,7 +3391,7 @@
       <c r="E23" s="21"/>
     </row>
     <row r="24" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="117">
+      <c r="A24" s="123">
         <v>44577</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -3292,7 +3406,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="119"/>
+      <c r="A25" s="124"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
         <v>63</v>
@@ -3303,7 +3417,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="118"/>
+      <c r="A26" s="125"/>
       <c r="B26" s="21"/>
       <c r="C26" s="21" t="s">
         <v>64</v>
@@ -3314,7 +3428,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="117">
+      <c r="A27" s="123">
         <v>44578</v>
       </c>
       <c r="B27" s="8" t="s">
@@ -3325,7 +3439,7 @@
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="119"/>
+      <c r="A28" s="124"/>
       <c r="B28" s="4" t="s">
         <v>69</v>
       </c>
@@ -3334,7 +3448,7 @@
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="119"/>
+      <c r="A29" s="124"/>
       <c r="B29" s="4" t="s">
         <v>70</v>
       </c>
@@ -3343,7 +3457,7 @@
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="118"/>
+      <c r="A30" s="125"/>
       <c r="B30" s="22" t="s">
         <v>71</v>
       </c>
@@ -3352,7 +3466,7 @@
       <c r="E30" s="22"/>
     </row>
     <row r="31" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="117">
+      <c r="A31" s="123">
         <v>44579</v>
       </c>
       <c r="B31" s="8" t="s">
@@ -3367,7 +3481,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="118"/>
+      <c r="A32" s="125"/>
       <c r="B32" s="22" t="s">
         <v>73</v>
       </c>
@@ -3378,7 +3492,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="117">
+      <c r="A33" s="123">
         <v>44580</v>
       </c>
       <c r="B33" s="8" t="s">
@@ -3392,7 +3506,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="118"/>
+      <c r="A34" s="125"/>
       <c r="B34" s="23" t="s">
         <v>83</v>
       </c>
@@ -3401,7 +3515,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="117">
+      <c r="A35" s="123">
         <v>44581</v>
       </c>
       <c r="B35" s="8" t="s">
@@ -3413,7 +3527,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="119"/>
+      <c r="A36" s="124"/>
       <c r="B36" s="4" t="s">
         <v>85</v>
       </c>
@@ -3423,7 +3537,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="119"/>
+      <c r="A37" s="124"/>
       <c r="B37" s="4" t="s">
         <v>86</v>
       </c>
@@ -3431,7 +3545,7 @@
       <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="119"/>
+      <c r="A38" s="124"/>
       <c r="B38" s="4" t="s">
         <v>87</v>
       </c>
@@ -3439,7 +3553,7 @@
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="118"/>
+      <c r="A39" s="125"/>
       <c r="B39" s="23" t="s">
         <v>88</v>
       </c>
@@ -3447,7 +3561,7 @@
       <c r="D39" s="23"/>
     </row>
     <row r="40" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="117">
+      <c r="A40" s="123">
         <v>44582</v>
       </c>
       <c r="B40" s="8" t="s">
@@ -3464,7 +3578,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="120"/>
+      <c r="A41" s="126"/>
       <c r="B41" s="4" t="s">
         <v>91</v>
       </c>
@@ -3476,7 +3590,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="120"/>
+      <c r="A42" s="126"/>
       <c r="B42" s="4" t="s">
         <v>98</v>
       </c>
@@ -3486,7 +3600,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="121"/>
+      <c r="A43" s="127"/>
       <c r="B43" s="24" t="s">
         <v>99</v>
       </c>
@@ -3496,7 +3610,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="117">
+      <c r="A44" s="123">
         <v>44583</v>
       </c>
       <c r="B44" s="8" t="s">
@@ -3506,7 +3620,7 @@
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="119"/>
+      <c r="A45" s="124"/>
       <c r="B45" s="4" t="s">
         <v>101</v>
       </c>
@@ -3514,7 +3628,7 @@
       <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="119"/>
+      <c r="A46" s="124"/>
       <c r="B46" s="4" t="s">
         <v>102</v>
       </c>
@@ -3522,7 +3636,7 @@
       <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="119"/>
+      <c r="A47" s="124"/>
       <c r="B47" s="4" t="s">
         <v>103</v>
       </c>
@@ -3530,7 +3644,7 @@
       <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="119"/>
+      <c r="A48" s="124"/>
       <c r="B48" s="4" t="s">
         <v>104</v>
       </c>
@@ -3538,7 +3652,7 @@
       <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="118"/>
+      <c r="A49" s="125"/>
       <c r="B49" s="25" t="s">
         <v>105</v>
       </c>
@@ -3546,7 +3660,7 @@
       <c r="D49" s="25"/>
     </row>
     <row r="50" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="117">
+      <c r="A50" s="123">
         <v>44584</v>
       </c>
       <c r="B50" s="8" t="s">
@@ -3556,7 +3670,7 @@
       <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="120"/>
+      <c r="A51" s="126"/>
       <c r="B51" s="4" t="s">
         <v>107</v>
       </c>
@@ -3564,7 +3678,7 @@
       <c r="D51" s="4"/>
     </row>
     <row r="52" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="120"/>
+      <c r="A52" s="126"/>
       <c r="B52" s="4" t="s">
         <v>108</v>
       </c>
@@ -3572,7 +3686,7 @@
       <c r="D52" s="4"/>
     </row>
     <row r="53" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="121"/>
+      <c r="A53" s="127"/>
       <c r="B53" s="26" t="s">
         <v>109</v>
       </c>
@@ -3580,7 +3694,7 @@
       <c r="D53" s="26"/>
     </row>
     <row r="54" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="117">
+      <c r="A54" s="123">
         <v>44585</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -3590,7 +3704,7 @@
       <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="118"/>
+      <c r="A55" s="125"/>
       <c r="B55" s="27" t="s">
         <v>111</v>
       </c>
@@ -3598,7 +3712,7 @@
       <c r="D55" s="27"/>
     </row>
     <row r="56" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="117">
+      <c r="A56" s="123">
         <v>44586</v>
       </c>
       <c r="B56" s="8"/>
@@ -3613,7 +3727,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="119"/>
+      <c r="A57" s="124"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4" t="s">
@@ -3622,7 +3736,7 @@
       <c r="E57" s="4"/>
     </row>
     <row r="58" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="118"/>
+      <c r="A58" s="125"/>
       <c r="B58" s="27"/>
       <c r="C58" s="27"/>
       <c r="D58" s="27" t="s">
@@ -3631,7 +3745,7 @@
       <c r="E58" s="27"/>
     </row>
     <row r="59" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="117">
+      <c r="A59" s="123">
         <v>44587</v>
       </c>
       <c r="B59" s="8"/>
@@ -3646,7 +3760,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="119"/>
+      <c r="A60" s="124"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4" t="s">
         <v>120</v>
@@ -3656,7 +3770,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="119"/>
+      <c r="A61" s="124"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4" t="s">
         <v>123</v>
@@ -3667,7 +3781,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="118"/>
+      <c r="A62" s="125"/>
       <c r="B62" s="29"/>
       <c r="C62" s="29" t="s">
         <v>124</v>
@@ -3676,7 +3790,7 @@
       <c r="E62" s="29"/>
     </row>
     <row r="63" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="117">
+      <c r="A63" s="123">
         <v>44588</v>
       </c>
       <c r="B63" s="8"/>
@@ -3691,7 +3805,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="119"/>
+      <c r="A64" s="124"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4" t="s">
         <v>126</v>
@@ -3702,7 +3816,7 @@
       <c r="E64" s="4"/>
     </row>
     <row r="65" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="119"/>
+      <c r="A65" s="124"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4" t="s">
         <v>127</v>
@@ -3713,7 +3827,7 @@
       <c r="E65" s="4"/>
     </row>
     <row r="66" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="118"/>
+      <c r="A66" s="125"/>
       <c r="B66" s="30"/>
       <c r="C66" s="30" t="s">
         <v>128</v>
@@ -3722,7 +3836,7 @@
       <c r="E66" s="30"/>
     </row>
     <row r="67" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="117">
+      <c r="A67" s="123">
         <v>44589</v>
       </c>
       <c r="B67" s="8"/>
@@ -3733,7 +3847,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="119"/>
+      <c r="A68" s="124"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -3742,7 +3856,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="118"/>
+      <c r="A69" s="125"/>
       <c r="B69" s="32"/>
       <c r="C69" s="32"/>
       <c r="D69" s="32"/>
@@ -3775,7 +3889,7 @@
       </c>
     </row>
     <row r="72" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="117">
+      <c r="A72" s="123">
         <v>44594</v>
       </c>
       <c r="B72" s="8"/>
@@ -3786,7 +3900,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="119"/>
+      <c r="A73" s="124"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
@@ -3795,7 +3909,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="119"/>
+      <c r="A74" s="124"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
@@ -3804,7 +3918,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="118"/>
+      <c r="A75" s="125"/>
       <c r="B75" s="37"/>
       <c r="C75" s="37"/>
       <c r="D75" s="37"/>
@@ -3835,7 +3949,7 @@
       </c>
     </row>
     <row r="78" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="117">
+      <c r="A78" s="123">
         <v>44598</v>
       </c>
       <c r="B78" s="8"/>
@@ -3846,7 +3960,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="119"/>
+      <c r="A79" s="124"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
@@ -3855,7 +3969,7 @@
       </c>
     </row>
     <row r="80" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="119"/>
+      <c r="A80" s="124"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -3864,7 +3978,7 @@
       </c>
     </row>
     <row r="81" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="118"/>
+      <c r="A81" s="125"/>
       <c r="B81" s="48"/>
       <c r="C81" s="48"/>
       <c r="D81" s="48"/>
@@ -3873,7 +3987,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="117">
+      <c r="A82" s="123">
         <v>44599</v>
       </c>
       <c r="B82" s="8"/>
@@ -3884,7 +3998,7 @@
       </c>
     </row>
     <row r="83" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="119"/>
+      <c r="A83" s="124"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
@@ -3893,7 +4007,7 @@
       </c>
     </row>
     <row r="84" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="118"/>
+      <c r="A84" s="125"/>
       <c r="B84" s="49"/>
       <c r="C84" s="49"/>
       <c r="D84" s="49"/>
@@ -3902,7 +4016,7 @@
       </c>
     </row>
     <row r="85" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="117">
+      <c r="A85" s="123">
         <v>44600</v>
       </c>
       <c r="B85" s="8"/>
@@ -3920,7 +4034,7 @@
       <c r="J85" s="8"/>
     </row>
     <row r="86" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="118"/>
+      <c r="A86" s="125"/>
       <c r="B86" s="50"/>
       <c r="C86" s="50"/>
       <c r="D86" s="50"/>
@@ -3934,7 +4048,7 @@
       <c r="J86" s="50"/>
     </row>
     <row r="87" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="117">
+      <c r="A87" s="123">
         <v>44601</v>
       </c>
       <c r="B87" s="8"/>
@@ -3952,7 +4066,7 @@
       <c r="J87" s="8"/>
     </row>
     <row r="88" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="119"/>
+      <c r="A88" s="124"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4" t="s">
@@ -3968,7 +4082,7 @@
       <c r="J88" s="4"/>
     </row>
     <row r="89" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="119"/>
+      <c r="A89" s="124"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4" t="s">
@@ -3984,7 +4098,7 @@
       <c r="J89" s="4"/>
     </row>
     <row r="90" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="119"/>
+      <c r="A90" s="124"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4" t="s">
@@ -3998,7 +4112,7 @@
       <c r="J90" s="4"/>
     </row>
     <row r="91" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="119"/>
+      <c r="A91" s="124"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4" t="s">
@@ -4012,7 +4126,7 @@
       <c r="J91" s="4"/>
     </row>
     <row r="92" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="119"/>
+      <c r="A92" s="124"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="52" t="s">
@@ -4026,7 +4140,7 @@
       <c r="J92" s="4"/>
     </row>
     <row r="93" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="119"/>
+      <c r="A93" s="124"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4" t="s">
@@ -4040,7 +4154,7 @@
       <c r="J93" s="4"/>
     </row>
     <row r="94" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="118"/>
+      <c r="A94" s="125"/>
       <c r="B94" s="51"/>
       <c r="C94" s="51"/>
       <c r="D94" s="54" t="s">
@@ -4054,7 +4168,7 @@
       <c r="J94" s="51"/>
     </row>
     <row r="95" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="117">
+      <c r="A95" s="123">
         <v>44602</v>
       </c>
       <c r="B95" s="8"/>
@@ -4072,7 +4186,7 @@
       <c r="J95" s="8"/>
     </row>
     <row r="96" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="119"/>
+      <c r="A96" s="124"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4" t="s">
@@ -4088,7 +4202,7 @@
       <c r="J96" s="4"/>
     </row>
     <row r="97" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="118"/>
+      <c r="A97" s="125"/>
       <c r="B97" s="53"/>
       <c r="C97" s="53"/>
       <c r="D97" s="53"/>
@@ -4102,7 +4216,7 @@
       <c r="J97" s="53"/>
     </row>
     <row r="98" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="117">
+      <c r="A98" s="123">
         <v>44603</v>
       </c>
       <c r="B98" s="8"/>
@@ -4118,7 +4232,7 @@
       <c r="J98" s="8"/>
     </row>
     <row r="99" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="119"/>
+      <c r="A99" s="124"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
@@ -4132,7 +4246,7 @@
       <c r="J99" s="4"/>
     </row>
     <row r="100" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="119"/>
+      <c r="A100" s="124"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
@@ -4146,7 +4260,7 @@
       <c r="J100" s="4"/>
     </row>
     <row r="101" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="119"/>
+      <c r="A101" s="124"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
@@ -4160,7 +4274,7 @@
       <c r="J101" s="4"/>
     </row>
     <row r="102" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="119"/>
+      <c r="A102" s="124"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
@@ -4174,7 +4288,7 @@
       <c r="J102" s="4"/>
     </row>
     <row r="103" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="118"/>
+      <c r="A103" s="125"/>
       <c r="B103" s="55"/>
       <c r="C103" s="55"/>
       <c r="D103" s="55"/>
@@ -4188,7 +4302,7 @@
       <c r="J103" s="55"/>
     </row>
     <row r="104" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="117">
+      <c r="A104" s="123">
         <v>44604</v>
       </c>
       <c r="B104" s="8"/>
@@ -4204,7 +4318,7 @@
       <c r="J104" s="8"/>
     </row>
     <row r="105" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="119"/>
+      <c r="A105" s="124"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
@@ -4218,7 +4332,7 @@
       <c r="J105" s="4"/>
     </row>
     <row r="106" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="119"/>
+      <c r="A106" s="124"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
@@ -4232,7 +4346,7 @@
       <c r="J106" s="4"/>
     </row>
     <row r="107" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="119"/>
+      <c r="A107" s="124"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
@@ -4246,7 +4360,7 @@
       <c r="J107" s="4"/>
     </row>
     <row r="108" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="119"/>
+      <c r="A108" s="124"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
@@ -4260,7 +4374,7 @@
       <c r="J108" s="4"/>
     </row>
     <row r="109" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="119"/>
+      <c r="A109" s="124"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
@@ -4274,7 +4388,7 @@
       <c r="J109" s="4"/>
     </row>
     <row r="110" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="118"/>
+      <c r="A110" s="125"/>
       <c r="B110" s="56"/>
       <c r="C110" s="56"/>
       <c r="D110" s="56"/>
@@ -4288,7 +4402,7 @@
       <c r="J110" s="56"/>
     </row>
     <row r="111" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="117">
+      <c r="A111" s="123">
         <v>44605</v>
       </c>
       <c r="B111" s="8"/>
@@ -4304,7 +4418,7 @@
       <c r="J111" s="8"/>
     </row>
     <row r="112" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="119"/>
+      <c r="A112" s="124"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
@@ -4318,7 +4432,7 @@
       <c r="J112" s="4"/>
     </row>
     <row r="113" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="119"/>
+      <c r="A113" s="124"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
@@ -4332,7 +4446,7 @@
       <c r="J113" s="4"/>
     </row>
     <row r="114" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="119"/>
+      <c r="A114" s="124"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
@@ -4346,7 +4460,7 @@
       <c r="J114" s="4"/>
     </row>
     <row r="115" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="119"/>
+      <c r="A115" s="124"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
@@ -4360,7 +4474,7 @@
       <c r="J115" s="4"/>
     </row>
     <row r="116" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="119"/>
+      <c r="A116" s="124"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
@@ -4374,7 +4488,7 @@
       <c r="J116" s="4"/>
     </row>
     <row r="117" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="118"/>
+      <c r="A117" s="125"/>
       <c r="B117" s="57"/>
       <c r="C117" s="57"/>
       <c r="D117" s="57"/>
@@ -4388,7 +4502,7 @@
       <c r="J117" s="57"/>
     </row>
     <row r="118" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="117">
+      <c r="A118" s="123">
         <v>44606</v>
       </c>
       <c r="B118" s="8"/>
@@ -4404,7 +4518,7 @@
       <c r="J118" s="8"/>
     </row>
     <row r="119" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="118"/>
+      <c r="A119" s="125"/>
       <c r="B119" s="58"/>
       <c r="C119" s="58"/>
       <c r="D119" s="58"/>
@@ -4418,7 +4532,7 @@
       <c r="J119" s="58"/>
     </row>
     <row r="120" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="117">
+      <c r="A120" s="123">
         <v>44607</v>
       </c>
       <c r="B120" s="8"/>
@@ -4434,7 +4548,7 @@
       <c r="J120" s="8"/>
     </row>
     <row r="121" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="118"/>
+      <c r="A121" s="125"/>
       <c r="B121" s="58"/>
       <c r="C121" s="58"/>
       <c r="D121" s="58"/>
@@ -4478,7 +4592,7 @@
       <c r="J123" s="64"/>
     </row>
     <row r="124" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="117">
+      <c r="A124" s="123">
         <v>44609</v>
       </c>
       <c r="B124" s="8"/>
@@ -4494,7 +4608,7 @@
       <c r="J124" s="8"/>
     </row>
     <row r="125" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="119"/>
+      <c r="A125" s="124"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
@@ -4508,7 +4622,7 @@
       <c r="J125" s="4"/>
     </row>
     <row r="126" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="119"/>
+      <c r="A126" s="124"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
@@ -4522,7 +4636,7 @@
       <c r="J126" s="4"/>
     </row>
     <row r="127" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="119"/>
+      <c r="A127" s="124"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
@@ -4536,7 +4650,7 @@
       <c r="J127" s="4"/>
     </row>
     <row r="128" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="119"/>
+      <c r="A128" s="124"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
@@ -4550,7 +4664,7 @@
       <c r="J128" s="4"/>
     </row>
     <row r="129" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="118"/>
+      <c r="A129" s="125"/>
       <c r="B129" s="67"/>
       <c r="C129" s="67"/>
       <c r="D129" s="67"/>
@@ -4564,7 +4678,7 @@
       <c r="J129" s="67"/>
     </row>
     <row r="130" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="117">
+      <c r="A130" s="123">
         <v>44610</v>
       </c>
       <c r="B130" s="8"/>
@@ -4580,7 +4694,7 @@
       <c r="J130" s="8"/>
     </row>
     <row r="131" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="119"/>
+      <c r="A131" s="124"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
@@ -4594,7 +4708,7 @@
       <c r="J131" s="4"/>
     </row>
     <row r="132" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="119"/>
+      <c r="A132" s="124"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
@@ -4608,7 +4722,7 @@
       <c r="J132" s="4"/>
     </row>
     <row r="133" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="118"/>
+      <c r="A133" s="125"/>
       <c r="B133" s="67"/>
       <c r="C133" s="67"/>
       <c r="D133" s="67"/>
@@ -4640,7 +4754,7 @@
       <c r="J134" s="12"/>
     </row>
     <row r="135" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="117">
+      <c r="A135" s="123">
         <v>44612</v>
       </c>
       <c r="B135" s="8"/>
@@ -4656,7 +4770,7 @@
       <c r="J135" s="8"/>
     </row>
     <row r="136" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="118"/>
+      <c r="A136" s="125"/>
       <c r="B136" s="71"/>
       <c r="C136" s="71"/>
       <c r="D136" s="71"/>
@@ -4670,7 +4784,7 @@
       <c r="J136" s="71"/>
     </row>
     <row r="137" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="117">
+      <c r="A137" s="123">
         <v>44613</v>
       </c>
       <c r="B137" s="8"/>
@@ -4688,7 +4802,7 @@
       <c r="J137" s="8"/>
     </row>
     <row r="138" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="119"/>
+      <c r="A138" s="124"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
       <c r="D138" s="4"/>
@@ -4704,7 +4818,7 @@
       <c r="J138" s="4"/>
     </row>
     <row r="139" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="119"/>
+      <c r="A139" s="124"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
@@ -4718,7 +4832,7 @@
       <c r="J139" s="4"/>
     </row>
     <row r="140" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="119"/>
+      <c r="A140" s="124"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
       <c r="D140" s="4"/>
@@ -4732,7 +4846,7 @@
       <c r="J140" s="4"/>
     </row>
     <row r="141" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="119"/>
+      <c r="A141" s="124"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
       <c r="D141" s="4"/>
@@ -4746,7 +4860,7 @@
       <c r="J141" s="4"/>
     </row>
     <row r="142" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="119"/>
+      <c r="A142" s="124"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
@@ -4760,7 +4874,7 @@
       <c r="J142" s="4"/>
     </row>
     <row r="143" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="118"/>
+      <c r="A143" s="125"/>
       <c r="B143" s="72"/>
       <c r="C143" s="72"/>
       <c r="D143" s="72"/>
@@ -4774,7 +4888,7 @@
       <c r="J143" s="72"/>
     </row>
     <row r="144" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="117">
+      <c r="A144" s="123">
         <v>44614</v>
       </c>
       <c r="B144" s="8"/>
@@ -4792,7 +4906,7 @@
       <c r="J144" s="8"/>
     </row>
     <row r="145" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="119"/>
+      <c r="A145" s="124"/>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
       <c r="D145" s="4"/>
@@ -4806,7 +4920,7 @@
       <c r="J145" s="4"/>
     </row>
     <row r="146" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="119"/>
+      <c r="A146" s="124"/>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
       <c r="D146" s="4"/>
@@ -4820,7 +4934,7 @@
       <c r="J146" s="4"/>
     </row>
     <row r="147" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="119"/>
+      <c r="A147" s="124"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
       <c r="D147" s="4"/>
@@ -4834,7 +4948,7 @@
       <c r="J147" s="4"/>
     </row>
     <row r="148" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="118"/>
+      <c r="A148" s="125"/>
       <c r="B148" s="75"/>
       <c r="C148" s="75"/>
       <c r="D148" s="75"/>
@@ -4848,7 +4962,7 @@
       <c r="J148" s="75"/>
     </row>
     <row r="149" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="117">
+      <c r="A149" s="123">
         <v>44615</v>
       </c>
       <c r="B149" s="8"/>
@@ -4866,7 +4980,7 @@
       <c r="J149" s="8"/>
     </row>
     <row r="150" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="118"/>
+      <c r="A150" s="125"/>
       <c r="B150" s="75"/>
       <c r="C150" s="75"/>
       <c r="D150" s="75"/>
@@ -4880,7 +4994,7 @@
       <c r="J150" s="75"/>
     </row>
     <row r="151" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="117">
+      <c r="A151" s="123">
         <v>44616</v>
       </c>
       <c r="B151" s="8"/>
@@ -4898,7 +5012,7 @@
       <c r="J151" s="8"/>
     </row>
     <row r="152" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="119"/>
+      <c r="A152" s="124"/>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
@@ -4912,7 +5026,7 @@
       <c r="J152" s="4"/>
     </row>
     <row r="153" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="118"/>
+      <c r="A153" s="125"/>
       <c r="B153" s="76"/>
       <c r="C153" s="76"/>
       <c r="D153" s="76"/>
@@ -4926,7 +5040,7 @@
       <c r="J153" s="76"/>
     </row>
     <row r="154" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="117">
+      <c r="A154" s="123">
         <v>44617</v>
       </c>
       <c r="B154" s="8"/>
@@ -4944,7 +5058,7 @@
       <c r="J154" s="8"/>
     </row>
     <row r="155" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="119"/>
+      <c r="A155" s="124"/>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
@@ -4958,7 +5072,7 @@
       <c r="J155" s="4"/>
     </row>
     <row r="156" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="118"/>
+      <c r="A156" s="125"/>
       <c r="B156" s="77"/>
       <c r="C156" s="77"/>
       <c r="D156" s="77"/>
@@ -4972,7 +5086,7 @@
       <c r="J156" s="77"/>
     </row>
     <row r="157" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="117">
+      <c r="A157" s="123">
         <v>44618</v>
       </c>
       <c r="B157" s="8"/>
@@ -4992,7 +5106,7 @@
       <c r="J157" s="8"/>
     </row>
     <row r="158" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="118"/>
+      <c r="A158" s="125"/>
       <c r="B158" s="78"/>
       <c r="C158" s="78"/>
       <c r="D158" s="78"/>
@@ -5008,7 +5122,7 @@
       <c r="J158" s="78"/>
     </row>
     <row r="159" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="117">
+      <c r="A159" s="123">
         <v>44619</v>
       </c>
       <c r="B159" s="8"/>
@@ -5026,7 +5140,7 @@
       <c r="J159" s="8"/>
     </row>
     <row r="160" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="119"/>
+      <c r="A160" s="124"/>
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
       <c r="D160" s="4"/>
@@ -5042,7 +5156,7 @@
       <c r="J160" s="4"/>
     </row>
     <row r="161" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="118"/>
+      <c r="A161" s="125"/>
       <c r="B161" s="79"/>
       <c r="C161" s="79"/>
       <c r="D161" s="79"/>
@@ -5058,7 +5172,7 @@
       <c r="J161" s="79"/>
     </row>
     <row r="162" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="117">
+      <c r="A162" s="123">
         <v>44620</v>
       </c>
       <c r="B162" s="8"/>
@@ -5076,7 +5190,7 @@
       <c r="J162" s="8"/>
     </row>
     <row r="163" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="119"/>
+      <c r="A163" s="124"/>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
       <c r="D163" s="4"/>
@@ -5092,7 +5206,7 @@
       <c r="J163" s="4"/>
     </row>
     <row r="164" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="118"/>
+      <c r="A164" s="125"/>
       <c r="B164" s="80"/>
       <c r="C164" s="80"/>
       <c r="D164" s="80"/>
@@ -5106,7 +5220,7 @@
       <c r="J164" s="80"/>
     </row>
     <row r="165" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="117">
+      <c r="A165" s="123">
         <v>44621</v>
       </c>
       <c r="B165" s="8"/>
@@ -5122,7 +5236,7 @@
       <c r="J165" s="8"/>
     </row>
     <row r="166" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="119"/>
+      <c r="A166" s="124"/>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
@@ -5136,7 +5250,7 @@
       <c r="J166" s="4"/>
     </row>
     <row r="167" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="118"/>
+      <c r="A167" s="125"/>
       <c r="B167" s="81"/>
       <c r="C167" s="81"/>
       <c r="D167" s="81"/>
@@ -5150,7 +5264,7 @@
       <c r="J167" s="81"/>
     </row>
     <row r="168" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="117">
+      <c r="A168" s="123">
         <v>44622</v>
       </c>
       <c r="B168" s="8"/>
@@ -5171,7 +5285,7 @@
       </c>
     </row>
     <row r="169" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="119"/>
+      <c r="A169" s="124"/>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
@@ -5186,7 +5300,7 @@
       </c>
     </row>
     <row r="170" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="118"/>
+      <c r="A170" s="125"/>
       <c r="B170" s="82"/>
       <c r="C170" s="82"/>
       <c r="D170" s="82"/>
@@ -5201,7 +5315,7 @@
       </c>
     </row>
     <row r="171" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="117">
+      <c r="A171" s="123">
         <v>44623</v>
       </c>
       <c r="B171" s="8"/>
@@ -5218,7 +5332,7 @@
       <c r="K171" s="8"/>
     </row>
     <row r="172" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="119"/>
+      <c r="A172" s="124"/>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
       <c r="D172" s="4"/>
@@ -5233,7 +5347,7 @@
       <c r="K172" s="4"/>
     </row>
     <row r="173" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="118"/>
+      <c r="A173" s="125"/>
       <c r="B173" s="83"/>
       <c r="C173" s="83"/>
       <c r="D173" s="83"/>
@@ -5248,7 +5362,7 @@
       <c r="K173" s="83"/>
     </row>
     <row r="174" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="117">
+      <c r="A174" s="123">
         <v>44625</v>
       </c>
       <c r="B174" s="8"/>
@@ -5265,7 +5379,7 @@
       <c r="K174" s="8"/>
     </row>
     <row r="175" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="118"/>
+      <c r="A175" s="125"/>
       <c r="B175" s="85"/>
       <c r="C175" s="85"/>
       <c r="D175" s="85"/>
@@ -5280,7 +5394,7 @@
       <c r="K175" s="85"/>
     </row>
     <row r="176" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="117">
+      <c r="A176" s="123">
         <v>44626</v>
       </c>
       <c r="B176" s="8"/>
@@ -5298,7 +5412,7 @@
       </c>
     </row>
     <row r="177" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="119"/>
+      <c r="A177" s="124"/>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
       <c r="D177" s="4"/>
@@ -5314,7 +5428,7 @@
       </c>
     </row>
     <row r="178" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="118"/>
+      <c r="A178" s="125"/>
       <c r="B178" s="86"/>
       <c r="C178" s="86"/>
       <c r="D178" s="86"/>
@@ -5330,7 +5444,7 @@
       </c>
     </row>
     <row r="179" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="117">
+      <c r="A179" s="123">
         <v>44627</v>
       </c>
       <c r="B179" s="8"/>
@@ -5348,7 +5462,7 @@
       </c>
     </row>
     <row r="180" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="119"/>
+      <c r="A180" s="124"/>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
       <c r="D180" s="4"/>
@@ -5364,7 +5478,7 @@
       </c>
     </row>
     <row r="181" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="119"/>
+      <c r="A181" s="124"/>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
       <c r="D181" s="4"/>
@@ -5380,7 +5494,7 @@
       </c>
     </row>
     <row r="182" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A182" s="118"/>
+      <c r="A182" s="125"/>
       <c r="B182" s="88"/>
       <c r="C182" s="88"/>
       <c r="D182" s="88"/>
@@ -5393,7 +5507,7 @@
       <c r="K182" s="88"/>
     </row>
     <row r="183" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="117">
+      <c r="A183" s="123">
         <v>44628</v>
       </c>
       <c r="B183" s="8" t="s">
@@ -5410,7 +5524,7 @@
       <c r="K183" s="8"/>
     </row>
     <row r="184" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="119"/>
+      <c r="A184" s="124"/>
       <c r="B184" s="4" t="s">
         <v>400</v>
       </c>
@@ -5425,7 +5539,7 @@
       <c r="K184" s="4"/>
     </row>
     <row r="185" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="118"/>
+      <c r="A185" s="125"/>
       <c r="B185" s="91" t="s">
         <v>404</v>
       </c>
@@ -5457,7 +5571,7 @@
       <c r="K186" s="12"/>
     </row>
     <row r="187" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="117">
+      <c r="A187" s="123">
         <v>44630</v>
       </c>
       <c r="B187" s="8"/>
@@ -5474,7 +5588,7 @@
       <c r="K187" s="8"/>
     </row>
     <row r="188" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="119"/>
+      <c r="A188" s="124"/>
       <c r="B188" s="4"/>
       <c r="C188" s="4"/>
       <c r="D188" s="4"/>
@@ -5489,7 +5603,7 @@
       <c r="K188" s="4"/>
     </row>
     <row r="189" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="119"/>
+      <c r="A189" s="124"/>
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
       <c r="D189" s="4"/>
@@ -5504,7 +5618,7 @@
       <c r="K189" s="4"/>
     </row>
     <row r="190" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A190" s="119"/>
+      <c r="A190" s="124"/>
       <c r="B190" s="4"/>
       <c r="C190" s="4"/>
       <c r="D190" s="4"/>
@@ -5519,7 +5633,7 @@
       <c r="K190" s="4"/>
     </row>
     <row r="191" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A191" s="118"/>
+      <c r="A191" s="125"/>
       <c r="B191" s="93"/>
       <c r="C191" s="93"/>
       <c r="D191" s="93"/>
@@ -5534,7 +5648,7 @@
       <c r="K191" s="93"/>
     </row>
     <row r="192" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A192" s="117">
+      <c r="A192" s="123">
         <v>44631</v>
       </c>
       <c r="B192" s="8" t="s">
@@ -5551,7 +5665,7 @@
       <c r="K192" s="8"/>
     </row>
     <row r="193" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="119"/>
+      <c r="A193" s="124"/>
       <c r="B193" s="4" t="s">
         <v>423</v>
       </c>
@@ -5566,7 +5680,7 @@
       <c r="K193" s="4"/>
     </row>
     <row r="194" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="118"/>
+      <c r="A194" s="125"/>
       <c r="B194" s="93" t="s">
         <v>424</v>
       </c>
@@ -5581,7 +5695,7 @@
       <c r="K194" s="93"/>
     </row>
     <row r="195" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="117">
+      <c r="A195" s="123">
         <v>44632</v>
       </c>
       <c r="B195" s="8" t="s">
@@ -5598,7 +5712,7 @@
       <c r="K195" s="8"/>
     </row>
     <row r="196" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="119"/>
+      <c r="A196" s="124"/>
       <c r="B196" s="4" t="s">
         <v>427</v>
       </c>
@@ -5613,7 +5727,7 @@
       <c r="K196" s="4"/>
     </row>
     <row r="197" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A197" s="118"/>
+      <c r="A197" s="125"/>
       <c r="B197" s="95" t="s">
         <v>428</v>
       </c>
@@ -5628,7 +5742,7 @@
       <c r="K197" s="95"/>
     </row>
     <row r="198" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="117">
+      <c r="A198" s="123">
         <v>44633</v>
       </c>
       <c r="B198" s="8" t="s">
@@ -5645,7 +5759,7 @@
       <c r="K198" s="8"/>
     </row>
     <row r="199" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="119"/>
+      <c r="A199" s="124"/>
       <c r="B199" s="4" t="s">
         <v>432</v>
       </c>
@@ -5660,7 +5774,7 @@
       <c r="K199" s="4"/>
     </row>
     <row r="200" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A200" s="118"/>
+      <c r="A200" s="125"/>
       <c r="B200" s="96" t="s">
         <v>433</v>
       </c>
@@ -5675,7 +5789,7 @@
       <c r="K200" s="96"/>
     </row>
     <row r="201" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A201" s="117">
+      <c r="A201" s="123">
         <v>44634</v>
       </c>
       <c r="B201" s="8"/>
@@ -5692,7 +5806,7 @@
       <c r="K201" s="8"/>
     </row>
     <row r="202" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A202" s="119"/>
+      <c r="A202" s="124"/>
       <c r="B202" s="4"/>
       <c r="C202" s="4" t="s">
         <v>445</v>
@@ -5707,7 +5821,7 @@
       <c r="K202" s="4"/>
     </row>
     <row r="203" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A203" s="118"/>
+      <c r="A203" s="125"/>
       <c r="B203" s="98"/>
       <c r="C203" s="98" t="s">
         <v>446</v>
@@ -5739,7 +5853,7 @@
       <c r="K204" s="12"/>
     </row>
     <row r="205" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A205" s="117">
+      <c r="A205" s="123">
         <v>44636</v>
       </c>
       <c r="B205" s="8"/>
@@ -5756,7 +5870,7 @@
       <c r="K205" s="8"/>
     </row>
     <row r="206" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A206" s="118"/>
+      <c r="A206" s="125"/>
       <c r="B206" s="101"/>
       <c r="C206" s="101" t="s">
         <v>460</v>
@@ -5771,7 +5885,7 @@
       <c r="K206" s="101"/>
     </row>
     <row r="207" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A207" s="117">
+      <c r="A207" s="123">
         <v>44639</v>
       </c>
       <c r="B207" s="8"/>
@@ -5788,7 +5902,7 @@
       <c r="K207" s="8"/>
     </row>
     <row r="208" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A208" s="119"/>
+      <c r="A208" s="124"/>
       <c r="B208" s="4"/>
       <c r="C208" s="4" t="s">
         <v>475</v>
@@ -5803,7 +5917,7 @@
       <c r="K208" s="4"/>
     </row>
     <row r="209" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A209" s="118"/>
+      <c r="A209" s="125"/>
       <c r="B209" s="105"/>
       <c r="C209" s="105" t="s">
         <v>476</v>
@@ -5818,7 +5932,7 @@
       <c r="K209" s="105"/>
     </row>
     <row r="210" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="117">
+      <c r="A210" s="123">
         <v>44641</v>
       </c>
       <c r="B210" s="8"/>
@@ -5835,7 +5949,7 @@
       <c r="K210" s="8"/>
     </row>
     <row r="211" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A211" s="119"/>
+      <c r="A211" s="124"/>
       <c r="B211" s="4"/>
       <c r="C211" s="4" t="s">
         <v>486</v>
@@ -5850,7 +5964,7 @@
       <c r="K211" s="4"/>
     </row>
     <row r="212" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A212" s="118"/>
+      <c r="A212" s="125"/>
       <c r="B212" s="107"/>
       <c r="C212" s="107" t="s">
         <v>487</v>
@@ -5865,7 +5979,7 @@
       <c r="K212" s="107"/>
     </row>
     <row r="213" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A213" s="117">
+      <c r="A213" s="123">
         <v>44644</v>
       </c>
       <c r="B213" s="8"/>
@@ -5883,7 +5997,7 @@
       </c>
     </row>
     <row r="214" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A214" s="119"/>
+      <c r="A214" s="124"/>
       <c r="B214" s="4"/>
       <c r="C214" s="4"/>
       <c r="D214" s="4"/>
@@ -5899,7 +6013,7 @@
       </c>
     </row>
     <row r="215" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A215" s="119"/>
+      <c r="A215" s="124"/>
       <c r="B215" s="4"/>
       <c r="C215" s="4"/>
       <c r="D215" s="4"/>
@@ -5915,7 +6029,7 @@
       </c>
     </row>
     <row r="216" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A216" s="118"/>
+      <c r="A216" s="125"/>
       <c r="B216" s="110"/>
       <c r="C216" s="110"/>
       <c r="D216" s="110"/>
@@ -5931,7 +6045,7 @@
       </c>
     </row>
     <row r="217" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A217" s="117">
+      <c r="A217" s="123">
         <v>44647</v>
       </c>
       <c r="B217" s="8" t="s">
@@ -5949,7 +6063,7 @@
       <c r="M217" s="8"/>
     </row>
     <row r="218" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A218" s="118"/>
+      <c r="A218" s="125"/>
       <c r="B218" s="113" t="s">
         <v>516</v>
       </c>
@@ -5965,7 +6079,7 @@
       <c r="M218" s="113"/>
     </row>
     <row r="219" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A219" s="117">
+      <c r="A219" s="123">
         <v>44648</v>
       </c>
       <c r="B219" s="8" t="s">
@@ -5985,7 +6099,7 @@
       <c r="M219" s="8"/>
     </row>
     <row r="220" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A220" s="119"/>
+      <c r="A220" s="124"/>
       <c r="B220" s="4" t="s">
         <v>518</v>
       </c>
@@ -6003,7 +6117,7 @@
       <c r="M220" s="4"/>
     </row>
     <row r="221" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A221" s="119"/>
+      <c r="A221" s="124"/>
       <c r="B221" s="4" t="s">
         <v>519</v>
       </c>
@@ -6019,7 +6133,7 @@
       <c r="M221" s="4"/>
     </row>
     <row r="222" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="119"/>
+      <c r="A222" s="124"/>
       <c r="B222" s="4" t="s">
         <v>520</v>
       </c>
@@ -6035,7 +6149,7 @@
       <c r="M222" s="4"/>
     </row>
     <row r="223" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A223" s="119"/>
+      <c r="A223" s="124"/>
       <c r="B223" s="4" t="s">
         <v>521</v>
       </c>
@@ -6051,7 +6165,7 @@
       <c r="M223" s="4"/>
     </row>
     <row r="224" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A224" s="118"/>
+      <c r="A224" s="125"/>
       <c r="B224" s="113" t="s">
         <v>522</v>
       </c>
@@ -6067,7 +6181,7 @@
       <c r="M224" s="113"/>
     </row>
     <row r="225" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="117">
+      <c r="A225" s="123">
         <v>44650</v>
       </c>
       <c r="B225" s="8" t="s">
@@ -6089,7 +6203,7 @@
       <c r="M225" s="8"/>
     </row>
     <row r="226" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A226" s="119"/>
+      <c r="A226" s="124"/>
       <c r="B226" s="4" t="s">
         <v>547</v>
       </c>
@@ -6109,7 +6223,7 @@
       <c r="M226" s="4"/>
     </row>
     <row r="227" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A227" s="119"/>
+      <c r="A227" s="124"/>
       <c r="B227" s="4" t="s">
         <v>548</v>
       </c>
@@ -6127,7 +6241,7 @@
       <c r="M227" s="4"/>
     </row>
     <row r="228" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A228" s="118"/>
+      <c r="A228" s="125"/>
       <c r="B228" s="116" t="s">
         <v>549</v>
       </c>
@@ -6144,66 +6258,82 @@
       <c r="K228" s="116"/>
       <c r="M228" s="116"/>
     </row>
-    <row r="229" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A229" s="28"/>
-      <c r="B229" s="3"/>
-      <c r="C229" s="3"/>
-      <c r="D229" s="4"/>
-      <c r="E229" s="4"/>
-      <c r="F229" s="4"/>
-      <c r="G229" s="4"/>
-      <c r="H229" s="4"/>
-      <c r="I229" s="4"/>
-      <c r="J229" s="4"/>
-      <c r="K229" s="4"/>
-      <c r="M229" s="4"/>
-    </row>
-    <row r="230" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A230" s="28"/>
-      <c r="B230" s="3"/>
-      <c r="C230" s="3"/>
-      <c r="D230" s="4"/>
-      <c r="E230" s="4"/>
-      <c r="F230" s="4"/>
-      <c r="G230" s="4"/>
-      <c r="H230" s="4"/>
-      <c r="I230" s="4"/>
-      <c r="J230" s="4"/>
-      <c r="K230" s="4"/>
-      <c r="M230" s="4"/>
-    </row>
-    <row r="231" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A231" s="28"/>
-      <c r="B231" s="3"/>
-      <c r="C231" s="3"/>
-      <c r="D231" s="4"/>
-      <c r="E231" s="4"/>
-      <c r="F231" s="4"/>
-      <c r="G231" s="4"/>
-      <c r="H231" s="4"/>
-      <c r="I231" s="4"/>
-      <c r="J231" s="4"/>
-      <c r="K231" s="4"/>
-      <c r="M231" s="4"/>
-    </row>
-    <row r="232" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A232" s="28"/>
-      <c r="B232" s="3"/>
-      <c r="C232" s="3"/>
-      <c r="D232" s="4"/>
-      <c r="E232" s="4"/>
-      <c r="F232" s="4"/>
-      <c r="G232" s="4"/>
-      <c r="H232" s="4"/>
-      <c r="I232" s="4"/>
-      <c r="J232" s="4"/>
-      <c r="K232" s="4"/>
-      <c r="M232" s="4"/>
-    </row>
-    <row r="233" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A233" s="28"/>
-      <c r="B233" s="3"/>
-      <c r="C233" s="3"/>
+    <row r="229" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A229" s="123">
+        <v>44652</v>
+      </c>
+      <c r="B229" s="8" t="s">
+        <v>557</v>
+      </c>
+      <c r="C229" s="8"/>
+      <c r="D229" s="8"/>
+      <c r="E229" s="8"/>
+      <c r="F229" s="8"/>
+      <c r="G229" s="8"/>
+      <c r="H229" s="8"/>
+      <c r="I229" s="8"/>
+      <c r="J229" s="8"/>
+      <c r="K229" s="8"/>
+      <c r="M229" s="8"/>
+    </row>
+    <row r="230" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A230" s="125"/>
+      <c r="B230" s="118" t="s">
+        <v>561</v>
+      </c>
+      <c r="C230" s="118"/>
+      <c r="D230" s="118"/>
+      <c r="E230" s="118"/>
+      <c r="F230" s="118"/>
+      <c r="G230" s="118"/>
+      <c r="H230" s="118"/>
+      <c r="I230" s="118"/>
+      <c r="J230" s="118"/>
+      <c r="K230" s="118"/>
+      <c r="M230" s="118"/>
+    </row>
+    <row r="231" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A231" s="35">
+        <v>44653</v>
+      </c>
+      <c r="B231" s="12" t="s">
+        <v>562</v>
+      </c>
+      <c r="C231" s="12"/>
+      <c r="D231" s="12"/>
+      <c r="E231" s="12"/>
+      <c r="F231" s="12"/>
+      <c r="G231" s="12"/>
+      <c r="H231" s="12"/>
+      <c r="I231" s="12"/>
+      <c r="J231" s="12"/>
+      <c r="K231" s="12"/>
+      <c r="M231" s="12"/>
+    </row>
+    <row r="232" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A232" s="123">
+        <v>44654</v>
+      </c>
+      <c r="B232" s="8" t="s">
+        <v>566</v>
+      </c>
+      <c r="C232" s="8"/>
+      <c r="D232" s="8"/>
+      <c r="E232" s="8"/>
+      <c r="F232" s="8"/>
+      <c r="G232" s="8"/>
+      <c r="H232" s="8"/>
+      <c r="I232" s="8"/>
+      <c r="J232" s="8"/>
+      <c r="K232" s="8"/>
+      <c r="M232" s="8"/>
+    </row>
+    <row r="233" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A233" s="124"/>
+      <c r="B233" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="C233" s="4"/>
       <c r="D233" s="4"/>
       <c r="E233" s="4"/>
       <c r="F233" s="4"/>
@@ -6214,10 +6344,12 @@
       <c r="K233" s="4"/>
       <c r="M233" s="4"/>
     </row>
-    <row r="234" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A234" s="28"/>
-      <c r="B234" s="3"/>
-      <c r="C234" s="3"/>
+    <row r="234" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A234" s="124"/>
+      <c r="B234" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="C234" s="4"/>
       <c r="D234" s="4"/>
       <c r="E234" s="4"/>
       <c r="F234" s="4"/>
@@ -6228,10 +6360,12 @@
       <c r="K234" s="4"/>
       <c r="M234" s="4"/>
     </row>
-    <row r="235" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A235" s="28"/>
-      <c r="B235" s="3"/>
-      <c r="C235" s="3"/>
+    <row r="235" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A235" s="124"/>
+      <c r="B235" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="C235" s="4"/>
       <c r="D235" s="4"/>
       <c r="E235" s="4"/>
       <c r="F235" s="4"/>
@@ -6242,10 +6376,12 @@
       <c r="K235" s="4"/>
       <c r="M235" s="4"/>
     </row>
-    <row r="236" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A236" s="28"/>
-      <c r="B236" s="3"/>
-      <c r="C236" s="3"/>
+    <row r="236" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A236" s="124"/>
+      <c r="B236" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="C236" s="4"/>
       <c r="D236" s="4"/>
       <c r="E236" s="4"/>
       <c r="F236" s="4"/>
@@ -6256,33 +6392,39 @@
       <c r="K236" s="4"/>
       <c r="M236" s="4"/>
     </row>
-    <row r="237" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A237" s="28"/>
-      <c r="B237" s="3"/>
-      <c r="C237" s="3"/>
-      <c r="D237" s="4"/>
-      <c r="E237" s="4"/>
-      <c r="F237" s="4"/>
-      <c r="G237" s="4"/>
-      <c r="H237" s="4"/>
-      <c r="I237" s="4"/>
-      <c r="J237" s="4"/>
-      <c r="K237" s="4"/>
-      <c r="M237" s="4"/>
-    </row>
-    <row r="238" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A238" s="28"/>
-      <c r="B238" s="3"/>
-      <c r="C238" s="3"/>
-      <c r="D238" s="4"/>
-      <c r="E238" s="4"/>
-      <c r="F238" s="4"/>
-      <c r="G238" s="4"/>
-      <c r="H238" s="4"/>
-      <c r="I238" s="4"/>
-      <c r="J238" s="4"/>
-      <c r="K238" s="4"/>
-      <c r="M238" s="4"/>
+    <row r="237" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A237" s="125"/>
+      <c r="B237" s="121" t="s">
+        <v>571</v>
+      </c>
+      <c r="C237" s="121"/>
+      <c r="D237" s="121"/>
+      <c r="E237" s="121"/>
+      <c r="F237" s="121"/>
+      <c r="G237" s="121"/>
+      <c r="H237" s="121"/>
+      <c r="I237" s="121"/>
+      <c r="J237" s="121"/>
+      <c r="K237" s="121"/>
+      <c r="M237" s="121"/>
+    </row>
+    <row r="238" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A238" s="35">
+        <v>44655</v>
+      </c>
+      <c r="B238" s="12"/>
+      <c r="C238" s="12" t="s">
+        <v>574</v>
+      </c>
+      <c r="D238" s="12"/>
+      <c r="E238" s="12"/>
+      <c r="F238" s="12"/>
+      <c r="G238" s="12"/>
+      <c r="H238" s="12"/>
+      <c r="I238" s="12"/>
+      <c r="J238" s="12"/>
+      <c r="K238" s="12"/>
+      <c r="M238" s="12"/>
     </row>
     <row r="239" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A239" s="28"/>
@@ -10956,51 +11098,7 @@
       <c r="D623" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="60">
-    <mergeCell ref="A225:A228"/>
-    <mergeCell ref="A213:A216"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="A124:A129"/>
-    <mergeCell ref="A179:A182"/>
-    <mergeCell ref="A176:A178"/>
-    <mergeCell ref="A130:A133"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="A162:A164"/>
-    <mergeCell ref="A144:A148"/>
-    <mergeCell ref="A149:A150"/>
-    <mergeCell ref="A154:A156"/>
-    <mergeCell ref="A159:A161"/>
-    <mergeCell ref="A157:A158"/>
-    <mergeCell ref="A151:A153"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A39"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="A201:A203"/>
-    <mergeCell ref="A192:A194"/>
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="A87:A94"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="A98:A103"/>
-    <mergeCell ref="A104:A110"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="A111:A117"/>
+  <mergeCells count="62">
     <mergeCell ref="A217:A218"/>
     <mergeCell ref="A219:A224"/>
     <mergeCell ref="A210:A212"/>
@@ -11017,6 +11115,52 @@
     <mergeCell ref="A195:A197"/>
     <mergeCell ref="A187:A191"/>
     <mergeCell ref="A205:A206"/>
+    <mergeCell ref="A201:A203"/>
+    <mergeCell ref="A192:A194"/>
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="A87:A94"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="A98:A103"/>
+    <mergeCell ref="A104:A110"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="A111:A117"/>
+    <mergeCell ref="A151:A153"/>
+    <mergeCell ref="A157:A158"/>
+    <mergeCell ref="A159:A161"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A232:A237"/>
+    <mergeCell ref="A229:A230"/>
+    <mergeCell ref="A225:A228"/>
+    <mergeCell ref="A213:A216"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="A124:A129"/>
+    <mergeCell ref="A179:A182"/>
+    <mergeCell ref="A176:A178"/>
+    <mergeCell ref="A130:A133"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="A162:A164"/>
+    <mergeCell ref="A144:A148"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="A154:A156"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11032,7 +11176,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B34" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C48" sqref="C47:C48"/>
+      <selection pane="bottomRight" activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.25"/>
@@ -11091,7 +11235,7 @@
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="117">
+      <c r="A4" s="123">
         <v>44595</v>
       </c>
       <c r="B4" s="38"/>
@@ -11102,7 +11246,7 @@
       <c r="E4" s="38"/>
     </row>
     <row r="5" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="118"/>
+      <c r="A5" s="125"/>
       <c r="B5" s="42"/>
       <c r="C5" s="46" t="s">
         <v>161</v>
@@ -11111,7 +11255,7 @@
       <c r="E5" s="42"/>
     </row>
     <row r="6" spans="1:7" s="39" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="117">
+      <c r="A6" s="123">
         <v>44596</v>
       </c>
       <c r="B6" s="38"/>
@@ -11122,7 +11266,7 @@
       <c r="E6" s="38"/>
     </row>
     <row r="7" spans="1:7" s="43" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="118"/>
+      <c r="A7" s="125"/>
       <c r="B7" s="42"/>
       <c r="C7" s="42" t="s">
         <v>171</v>
@@ -11142,7 +11286,7 @@
       <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="117">
+      <c r="A9" s="123">
         <v>44608</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -11153,7 +11297,7 @@
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="119"/>
+      <c r="A10" s="124"/>
       <c r="B10" s="4" t="s">
         <v>237</v>
       </c>
@@ -11162,7 +11306,7 @@
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="118"/>
+      <c r="A11" s="125"/>
       <c r="B11" s="64" t="s">
         <v>238</v>
       </c>
@@ -11171,7 +11315,7 @@
       <c r="E11" s="64"/>
     </row>
     <row r="12" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="117">
+      <c r="A12" s="123">
         <v>44609</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -11182,7 +11326,7 @@
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="119"/>
+      <c r="A13" s="124"/>
       <c r="B13" s="4" t="s">
         <v>250</v>
       </c>
@@ -11191,7 +11335,7 @@
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="118"/>
+      <c r="A14" s="125"/>
       <c r="B14" s="67" t="s">
         <v>251</v>
       </c>
@@ -11222,7 +11366,7 @@
       <c r="E16" s="12"/>
     </row>
     <row r="17" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="117">
+      <c r="A17" s="123">
         <v>44616</v>
       </c>
       <c r="B17" s="8"/>
@@ -11233,7 +11377,7 @@
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="119"/>
+      <c r="A18" s="124"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
         <v>303</v>
@@ -11242,7 +11386,7 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="118"/>
+      <c r="A19" s="125"/>
       <c r="B19" s="77"/>
       <c r="C19" s="77" t="s">
         <v>304</v>
@@ -11251,7 +11395,7 @@
       <c r="E19" s="77"/>
     </row>
     <row r="20" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="117">
+      <c r="A20" s="123">
         <v>44621</v>
       </c>
       <c r="B20" s="8"/>
@@ -11262,7 +11406,7 @@
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="119"/>
+      <c r="A21" s="124"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
         <v>350</v>
@@ -11271,7 +11415,7 @@
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="118"/>
+      <c r="A22" s="125"/>
       <c r="B22" s="81"/>
       <c r="C22" s="81" t="s">
         <v>351</v>
@@ -11280,7 +11424,7 @@
       <c r="E22" s="81"/>
     </row>
     <row r="23" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="117">
+      <c r="A23" s="123">
         <v>44623</v>
       </c>
       <c r="B23" s="8"/>
@@ -11291,7 +11435,7 @@
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="118"/>
+      <c r="A24" s="125"/>
       <c r="B24" s="83"/>
       <c r="C24" s="83" t="s">
         <v>366</v>
@@ -11300,7 +11444,7 @@
       <c r="E24" s="83"/>
     </row>
     <row r="25" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="117">
+      <c r="A25" s="123">
         <v>44628</v>
       </c>
       <c r="B25" s="8"/>
@@ -11311,7 +11455,7 @@
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="119"/>
+      <c r="A26" s="124"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
         <v>396</v>
@@ -11320,7 +11464,7 @@
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="119"/>
+      <c r="A27" s="124"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
         <v>397</v>
@@ -11329,7 +11473,7 @@
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="118"/>
+      <c r="A28" s="125"/>
       <c r="B28" s="89"/>
       <c r="C28" s="89" t="s">
         <v>398</v>
@@ -11338,7 +11482,7 @@
       <c r="E28" s="89"/>
     </row>
     <row r="29" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="117">
+      <c r="A29" s="123">
         <v>44635</v>
       </c>
       <c r="B29" s="8"/>
@@ -11353,7 +11497,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="119"/>
+      <c r="A30" s="124"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
         <v>455</v>
@@ -11366,7 +11510,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="118"/>
+      <c r="A31" s="125"/>
       <c r="B31" s="99"/>
       <c r="C31" s="99" t="s">
         <v>456</v>
@@ -11394,7 +11538,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="117">
+      <c r="A33" s="123">
         <v>44640</v>
       </c>
       <c r="B33" s="8"/>
@@ -11407,7 +11551,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="118"/>
+      <c r="A34" s="125"/>
       <c r="B34" s="106"/>
       <c r="C34" s="106"/>
       <c r="D34" s="106"/>
@@ -11418,7 +11562,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="117">
+      <c r="A35" s="123">
         <v>44642</v>
       </c>
       <c r="B35" s="8"/>
@@ -11433,7 +11577,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="118"/>
+      <c r="A36" s="125"/>
       <c r="B36" s="108"/>
       <c r="C36" s="108" t="s">
         <v>494</v>
@@ -11446,7 +11590,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="117">
+      <c r="A37" s="123">
         <v>44643</v>
       </c>
       <c r="B37" s="8"/>
@@ -11461,7 +11605,7 @@
       <c r="G37" s="8"/>
     </row>
     <row r="38" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="118"/>
+      <c r="A38" s="125"/>
       <c r="B38" s="108"/>
       <c r="C38" s="108"/>
       <c r="D38" s="108" t="s">
@@ -11472,7 +11616,7 @@
       <c r="G38" s="108"/>
     </row>
     <row r="39" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="117">
+      <c r="A39" s="123">
         <v>44648</v>
       </c>
       <c r="B39" s="8"/>
@@ -11485,7 +11629,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="119"/>
+      <c r="A40" s="124"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -11496,7 +11640,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="118"/>
+      <c r="A41" s="125"/>
       <c r="B41" s="113"/>
       <c r="C41" s="113"/>
       <c r="D41" s="113"/>
@@ -11541,7 +11685,9 @@
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
+      <c r="G44" s="3" t="s">
+        <v>574</v>
+      </c>
     </row>
     <row r="45" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A45" s="100"/>
@@ -11710,11 +11856,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44415538-EB73-4FF7-B2CA-34821DA5346F}">
   <dimension ref="A1:C242"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B155" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B164" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F151" sqref="F151"/>
+      <selection pane="bottomRight" activeCell="C170" sqref="C170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.4"/>
@@ -11733,7 +11879,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="119">
+      <c r="A2" s="124">
         <v>44563</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -11744,35 +11890,35 @@
       </c>
     </row>
     <row r="3" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="119"/>
+      <c r="A3" s="124"/>
       <c r="B3" s="4"/>
       <c r="C3" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="119"/>
+      <c r="A4" s="124"/>
       <c r="B4" s="4"/>
       <c r="C4" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="119"/>
+      <c r="A5" s="124"/>
       <c r="B5" s="4"/>
       <c r="C5" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="118"/>
+      <c r="A6" s="125"/>
       <c r="B6" s="6"/>
       <c r="C6" s="15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="117">
+      <c r="A7" s="123">
         <v>44564</v>
       </c>
       <c r="B7" s="8"/>
@@ -11781,56 +11927,56 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="119"/>
+      <c r="A8" s="124"/>
       <c r="B8" s="4"/>
       <c r="C8" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="119"/>
+      <c r="A9" s="124"/>
       <c r="B9" s="4"/>
       <c r="C9" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="119"/>
+      <c r="A10" s="124"/>
       <c r="B10" s="4"/>
       <c r="C10" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="119"/>
+      <c r="A11" s="124"/>
       <c r="B11" s="4"/>
       <c r="C11" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="119"/>
+      <c r="A12" s="124"/>
       <c r="B12" s="4"/>
       <c r="C12" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="119"/>
+      <c r="A13" s="124"/>
       <c r="B13" s="4"/>
       <c r="C13" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="118"/>
+      <c r="A14" s="125"/>
       <c r="B14" s="6"/>
       <c r="C14" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="117">
+      <c r="A15" s="123">
         <v>44565</v>
       </c>
       <c r="B15" s="8"/>
@@ -11839,14 +11985,14 @@
       </c>
     </row>
     <row r="16" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="121"/>
+      <c r="A16" s="127"/>
       <c r="B16" s="6"/>
       <c r="C16" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="117">
+      <c r="A17" s="123">
         <v>44570</v>
       </c>
       <c r="B17" s="8"/>
@@ -11855,19 +12001,19 @@
       </c>
     </row>
     <row r="18" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="119"/>
+      <c r="A18" s="124"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="122" t="s">
+      <c r="C18" s="128" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="118"/>
+      <c r="A19" s="125"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="123"/>
+      <c r="C19" s="129"/>
     </row>
     <row r="20" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="117">
+      <c r="A20" s="123">
         <v>44574</v>
       </c>
       <c r="B20" s="8"/>
@@ -11876,21 +12022,21 @@
       </c>
     </row>
     <row r="21" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="119"/>
+      <c r="A21" s="124"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="118"/>
+      <c r="A22" s="125"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="117">
+      <c r="A23" s="123">
         <v>44590</v>
       </c>
       <c r="B23" s="8"/>
@@ -11899,28 +12045,28 @@
       </c>
     </row>
     <row r="24" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="120"/>
+      <c r="A24" s="126"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="120"/>
+      <c r="A25" s="126"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="121"/>
+      <c r="A26" s="127"/>
       <c r="B26" s="33"/>
       <c r="C26" s="33" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A27" s="117">
+      <c r="A27" s="123">
         <v>44591</v>
       </c>
       <c r="B27" s="8"/>
@@ -11929,49 +12075,49 @@
       </c>
     </row>
     <row r="28" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A28" s="119"/>
+      <c r="A28" s="124"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A29" s="119"/>
+      <c r="A29" s="124"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A30" s="119"/>
+      <c r="A30" s="124"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A31" s="119"/>
+      <c r="A31" s="124"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A32" s="119"/>
+      <c r="A32" s="124"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A33" s="118"/>
+      <c r="A33" s="125"/>
       <c r="B33" s="34"/>
       <c r="C33" s="34" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A34" s="117">
+      <c r="A34" s="123">
         <v>44593</v>
       </c>
       <c r="B34" s="8"/>
@@ -11980,14 +12126,14 @@
       </c>
     </row>
     <row r="35" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A35" s="118"/>
+      <c r="A35" s="125"/>
       <c r="B35" s="36"/>
       <c r="C35" s="36" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="39" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A36" s="117">
+      <c r="A36" s="123">
         <v>44594</v>
       </c>
       <c r="B36" s="38" t="s">
@@ -11998,35 +12144,35 @@
       </c>
     </row>
     <row r="37" spans="1:3" s="41" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A37" s="119"/>
+      <c r="A37" s="124"/>
       <c r="B37" s="40" t="s">
         <v>164</v>
       </c>
       <c r="C37" s="40"/>
     </row>
     <row r="38" spans="1:3" s="41" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A38" s="119"/>
+      <c r="A38" s="124"/>
       <c r="B38" s="40" t="s">
         <v>157</v>
       </c>
       <c r="C38" s="40"/>
     </row>
     <row r="39" spans="1:3" s="41" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A39" s="119"/>
+      <c r="A39" s="124"/>
       <c r="B39" s="40" t="s">
         <v>158</v>
       </c>
       <c r="C39" s="40"/>
     </row>
     <row r="40" spans="1:3" s="43" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A40" s="118"/>
+      <c r="A40" s="125"/>
       <c r="B40" s="42" t="s">
         <v>159</v>
       </c>
       <c r="C40" s="42"/>
     </row>
     <row r="41" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A41" s="117">
+      <c r="A41" s="123">
         <v>44595</v>
       </c>
       <c r="B41" s="8" t="s">
@@ -12037,7 +12183,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A42" s="118"/>
+      <c r="A42" s="125"/>
       <c r="B42" s="44" t="s">
         <v>166</v>
       </c>
@@ -12046,7 +12192,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A43" s="117">
+      <c r="A43" s="123">
         <v>44596</v>
       </c>
       <c r="B43" s="8" t="s">
@@ -12057,21 +12203,21 @@
       </c>
     </row>
     <row r="44" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A44" s="119"/>
+      <c r="A44" s="124"/>
       <c r="B44" s="4" t="s">
         <v>169</v>
       </c>
       <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A45" s="119"/>
+      <c r="A45" s="124"/>
       <c r="B45" s="4" t="s">
         <v>172</v>
       </c>
       <c r="C45" s="4"/>
     </row>
     <row r="46" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A46" s="118"/>
+      <c r="A46" s="125"/>
       <c r="B46" s="47" t="s">
         <v>173</v>
       </c>
@@ -12096,7 +12242,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A49" s="117">
+      <c r="A49" s="123">
         <v>44608</v>
       </c>
       <c r="B49" s="8" t="s">
@@ -12105,14 +12251,14 @@
       <c r="C49" s="8"/>
     </row>
     <row r="50" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A50" s="118"/>
+      <c r="A50" s="125"/>
       <c r="B50" s="64" t="s">
         <v>236</v>
       </c>
       <c r="C50" s="64"/>
     </row>
     <row r="51" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A51" s="117">
+      <c r="A51" s="123">
         <v>44609</v>
       </c>
       <c r="B51" s="8" t="s">
@@ -12121,14 +12267,14 @@
       <c r="C51" s="8"/>
     </row>
     <row r="52" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A52" s="118"/>
+      <c r="A52" s="125"/>
       <c r="B52" s="65" t="s">
         <v>248</v>
       </c>
       <c r="C52" s="65"/>
     </row>
     <row r="53" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A53" s="117">
+      <c r="A53" s="123">
         <v>44610</v>
       </c>
       <c r="B53" s="8" t="s">
@@ -12137,28 +12283,28 @@
       <c r="C53" s="8"/>
     </row>
     <row r="54" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A54" s="119"/>
+      <c r="A54" s="124"/>
       <c r="B54" s="4" t="s">
         <v>253</v>
       </c>
       <c r="C54" s="4"/>
     </row>
     <row r="55" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A55" s="119"/>
+      <c r="A55" s="124"/>
       <c r="B55" s="4" t="s">
         <v>258</v>
       </c>
       <c r="C55" s="4"/>
     </row>
     <row r="56" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A56" s="118"/>
+      <c r="A56" s="125"/>
       <c r="B56" s="68" t="s">
         <v>259</v>
       </c>
       <c r="C56" s="68"/>
     </row>
     <row r="57" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A57" s="117">
+      <c r="A57" s="123">
         <v>44611</v>
       </c>
       <c r="B57" s="8" t="s">
@@ -12167,28 +12313,28 @@
       <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A58" s="119"/>
+      <c r="A58" s="124"/>
       <c r="B58" s="4" t="s">
         <v>261</v>
       </c>
       <c r="C58" s="4"/>
     </row>
     <row r="59" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="119"/>
+      <c r="A59" s="124"/>
       <c r="B59" s="4" t="s">
         <v>263</v>
       </c>
       <c r="C59" s="4"/>
     </row>
     <row r="60" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A60" s="118"/>
+      <c r="A60" s="125"/>
       <c r="B60" s="70" t="s">
         <v>264</v>
       </c>
       <c r="C60" s="70"/>
     </row>
     <row r="61" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A61" s="117">
+      <c r="A61" s="123">
         <v>44612</v>
       </c>
       <c r="B61" s="8" t="s">
@@ -12197,21 +12343,21 @@
       <c r="C61" s="8"/>
     </row>
     <row r="62" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A62" s="119"/>
+      <c r="A62" s="124"/>
       <c r="B62" s="4" t="s">
         <v>266</v>
       </c>
       <c r="C62" s="4"/>
     </row>
     <row r="63" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="118"/>
+      <c r="A63" s="125"/>
       <c r="B63" s="71" t="s">
         <v>267</v>
       </c>
       <c r="C63" s="71"/>
     </row>
     <row r="64" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="117">
+      <c r="A64" s="123">
         <v>44613</v>
       </c>
       <c r="B64" s="8" t="s">
@@ -12220,14 +12366,14 @@
       <c r="C64" s="8"/>
     </row>
     <row r="65" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A65" s="118"/>
+      <c r="A65" s="125"/>
       <c r="B65" s="73" t="s">
         <v>281</v>
       </c>
       <c r="C65" s="73"/>
     </row>
     <row r="66" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A66" s="117">
+      <c r="A66" s="123">
         <v>44614</v>
       </c>
       <c r="B66" s="8" t="s">
@@ -12236,28 +12382,28 @@
       <c r="C66" s="8"/>
     </row>
     <row r="67" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A67" s="119"/>
+      <c r="A67" s="124"/>
       <c r="B67" s="4" t="s">
         <v>283</v>
       </c>
       <c r="C67" s="4"/>
     </row>
     <row r="68" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A68" s="119"/>
+      <c r="A68" s="124"/>
       <c r="B68" s="4" t="s">
         <v>291</v>
       </c>
       <c r="C68" s="4"/>
     </row>
     <row r="69" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A69" s="118"/>
+      <c r="A69" s="125"/>
       <c r="B69" s="74" t="s">
         <v>292</v>
       </c>
       <c r="C69" s="74"/>
     </row>
     <row r="70" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A70" s="117">
+      <c r="A70" s="123">
         <v>44615</v>
       </c>
       <c r="B70" s="8" t="s">
@@ -12266,14 +12412,14 @@
       <c r="C70" s="8"/>
     </row>
     <row r="71" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A71" s="119"/>
+      <c r="A71" s="124"/>
       <c r="B71" s="4" t="s">
         <v>294</v>
       </c>
       <c r="C71" s="4"/>
     </row>
     <row r="72" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A72" s="118"/>
+      <c r="A72" s="125"/>
       <c r="B72" s="75" t="s">
         <v>298</v>
       </c>
@@ -12289,7 +12435,7 @@
       <c r="C73" s="12"/>
     </row>
     <row r="74" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A74" s="117">
+      <c r="A74" s="123">
         <v>44617</v>
       </c>
       <c r="B74" s="8" t="s">
@@ -12298,21 +12444,21 @@
       <c r="C74" s="8"/>
     </row>
     <row r="75" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A75" s="119"/>
+      <c r="A75" s="124"/>
       <c r="B75" s="4" t="s">
         <v>309</v>
       </c>
       <c r="C75" s="4"/>
     </row>
     <row r="76" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A76" s="118"/>
+      <c r="A76" s="125"/>
       <c r="B76" s="77" t="s">
         <v>310</v>
       </c>
       <c r="C76" s="77"/>
     </row>
     <row r="77" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A77" s="117">
+      <c r="A77" s="123">
         <v>44618</v>
       </c>
       <c r="B77" s="8" t="s">
@@ -12321,49 +12467,49 @@
       <c r="C77" s="8"/>
     </row>
     <row r="78" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A78" s="119"/>
+      <c r="A78" s="124"/>
       <c r="B78" s="4" t="s">
         <v>315</v>
       </c>
       <c r="C78" s="4"/>
     </row>
     <row r="79" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A79" s="119"/>
+      <c r="A79" s="124"/>
       <c r="B79" s="4" t="s">
         <v>316</v>
       </c>
       <c r="C79" s="4"/>
     </row>
     <row r="80" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A80" s="119"/>
+      <c r="A80" s="124"/>
       <c r="B80" s="4" t="s">
         <v>317</v>
       </c>
       <c r="C80" s="4"/>
     </row>
     <row r="81" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A81" s="119"/>
+      <c r="A81" s="124"/>
       <c r="B81" s="4" t="s">
         <v>325</v>
       </c>
       <c r="C81" s="4"/>
     </row>
     <row r="82" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A82" s="119"/>
+      <c r="A82" s="124"/>
       <c r="B82" s="4" t="s">
         <v>326</v>
       </c>
       <c r="C82" s="4"/>
     </row>
     <row r="83" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A83" s="118"/>
+      <c r="A83" s="125"/>
       <c r="B83" s="78" t="s">
         <v>327</v>
       </c>
       <c r="C83" s="78"/>
     </row>
     <row r="84" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A84" s="117">
+      <c r="A84" s="123">
         <v>44619</v>
       </c>
       <c r="B84" s="8" t="s">
@@ -12372,14 +12518,14 @@
       <c r="C84" s="8"/>
     </row>
     <row r="85" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A85" s="118"/>
+      <c r="A85" s="125"/>
       <c r="B85" s="79" t="s">
         <v>329</v>
       </c>
       <c r="C85" s="79"/>
     </row>
     <row r="86" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A86" s="117">
+      <c r="A86" s="123">
         <v>44620</v>
       </c>
       <c r="B86" s="8" t="s">
@@ -12388,28 +12534,28 @@
       <c r="C86" s="8"/>
     </row>
     <row r="87" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A87" s="119"/>
+      <c r="A87" s="124"/>
       <c r="B87" s="4" t="s">
         <v>337</v>
       </c>
       <c r="C87" s="4"/>
     </row>
     <row r="88" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A88" s="119"/>
+      <c r="A88" s="124"/>
       <c r="B88" s="4" t="s">
         <v>338</v>
       </c>
       <c r="C88" s="4"/>
     </row>
     <row r="89" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A89" s="118"/>
+      <c r="A89" s="125"/>
       <c r="B89" s="80" t="s">
         <v>339</v>
       </c>
       <c r="C89" s="80"/>
     </row>
     <row r="90" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A90" s="117">
+      <c r="A90" s="123">
         <v>44621</v>
       </c>
       <c r="B90" s="8" t="s">
@@ -12418,28 +12564,28 @@
       <c r="C90" s="8"/>
     </row>
     <row r="91" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A91" s="119"/>
+      <c r="A91" s="124"/>
       <c r="B91" s="4" t="s">
         <v>346</v>
       </c>
       <c r="C91" s="4"/>
     </row>
     <row r="92" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A92" s="119"/>
+      <c r="A92" s="124"/>
       <c r="B92" s="4" t="s">
         <v>347</v>
       </c>
       <c r="C92" s="4"/>
     </row>
     <row r="93" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A93" s="118"/>
+      <c r="A93" s="125"/>
       <c r="B93" s="81" t="s">
         <v>348</v>
       </c>
       <c r="C93" s="81"/>
     </row>
     <row r="94" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A94" s="117">
+      <c r="A94" s="123">
         <v>44622</v>
       </c>
       <c r="B94" s="8" t="s">
@@ -12448,14 +12594,14 @@
       <c r="C94" s="8"/>
     </row>
     <row r="95" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A95" s="118"/>
+      <c r="A95" s="125"/>
       <c r="B95" s="82" t="s">
         <v>356</v>
       </c>
       <c r="C95" s="82"/>
     </row>
     <row r="96" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A96" s="117">
+      <c r="A96" s="123">
         <v>44623</v>
       </c>
       <c r="B96" s="8" t="s">
@@ -12464,14 +12610,14 @@
       <c r="C96" s="8"/>
     </row>
     <row r="97" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A97" s="118"/>
+      <c r="A97" s="125"/>
       <c r="B97" s="83" t="s">
         <v>364</v>
       </c>
       <c r="C97" s="83"/>
     </row>
     <row r="98" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A98" s="117">
+      <c r="A98" s="123">
         <v>44624</v>
       </c>
       <c r="B98" s="8" t="s">
@@ -12480,14 +12626,14 @@
       <c r="C98" s="8"/>
     </row>
     <row r="99" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A99" s="118"/>
+      <c r="A99" s="125"/>
       <c r="B99" s="84" t="s">
         <v>375</v>
       </c>
       <c r="C99" s="84"/>
     </row>
     <row r="100" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A100" s="117">
+      <c r="A100" s="123">
         <v>44625</v>
       </c>
       <c r="B100" s="8" t="s">
@@ -12496,14 +12642,14 @@
       <c r="C100" s="8"/>
     </row>
     <row r="101" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A101" s="118"/>
+      <c r="A101" s="125"/>
       <c r="B101" s="85" t="s">
         <v>380</v>
       </c>
       <c r="C101" s="85"/>
     </row>
     <row r="102" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A102" s="117">
+      <c r="A102" s="123">
         <v>44626</v>
       </c>
       <c r="B102" s="8" t="s">
@@ -12512,14 +12658,14 @@
       <c r="C102" s="8"/>
     </row>
     <row r="103" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A103" s="118"/>
+      <c r="A103" s="125"/>
       <c r="B103" s="87" t="s">
         <v>386</v>
       </c>
       <c r="C103" s="87"/>
     </row>
     <row r="104" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A104" s="117">
+      <c r="A104" s="123">
         <v>44627</v>
       </c>
       <c r="B104" s="8" t="s">
@@ -12528,7 +12674,7 @@
       <c r="C104" s="8"/>
     </row>
     <row r="105" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A105" s="118"/>
+      <c r="A105" s="125"/>
       <c r="B105" s="88" t="s">
         <v>391</v>
       </c>
@@ -12544,7 +12690,7 @@
       <c r="C106" s="12"/>
     </row>
     <row r="107" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A107" s="117">
+      <c r="A107" s="123">
         <v>44629</v>
       </c>
       <c r="B107" s="8" t="s">
@@ -12553,14 +12699,14 @@
       <c r="C107" s="8"/>
     </row>
     <row r="108" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A108" s="118"/>
+      <c r="A108" s="125"/>
       <c r="B108" s="91" t="s">
         <v>407</v>
       </c>
       <c r="C108" s="91"/>
     </row>
     <row r="109" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A109" s="117">
+      <c r="A109" s="123">
         <v>44630</v>
       </c>
       <c r="B109" s="8" t="s">
@@ -12569,14 +12715,14 @@
       <c r="C109" s="8"/>
     </row>
     <row r="110" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A110" s="118"/>
+      <c r="A110" s="125"/>
       <c r="B110" s="92" t="s">
         <v>410</v>
       </c>
       <c r="C110" s="92"/>
     </row>
     <row r="111" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A111" s="117">
+      <c r="A111" s="123">
         <v>44631</v>
       </c>
       <c r="B111" s="8" t="s">
@@ -12585,14 +12731,14 @@
       <c r="C111" s="8"/>
     </row>
     <row r="112" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A112" s="118"/>
+      <c r="A112" s="125"/>
       <c r="B112" s="93" t="s">
         <v>420</v>
       </c>
       <c r="C112" s="93"/>
     </row>
     <row r="113" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A113" s="117">
+      <c r="A113" s="123">
         <v>44632</v>
       </c>
       <c r="B113" s="8" t="s">
@@ -12601,14 +12747,14 @@
       <c r="C113" s="8"/>
     </row>
     <row r="114" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A114" s="118"/>
+      <c r="A114" s="125"/>
       <c r="B114" s="94" t="s">
         <v>425</v>
       </c>
       <c r="C114" s="94"/>
     </row>
     <row r="115" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A115" s="117">
+      <c r="A115" s="123">
         <v>44633</v>
       </c>
       <c r="B115" s="8" t="s">
@@ -12617,14 +12763,14 @@
       <c r="C115" s="8"/>
     </row>
     <row r="116" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A116" s="118"/>
+      <c r="A116" s="125"/>
       <c r="B116" s="96" t="s">
         <v>430</v>
       </c>
       <c r="C116" s="96"/>
     </row>
     <row r="117" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A117" s="117">
+      <c r="A117" s="123">
         <v>44634</v>
       </c>
       <c r="B117" s="8" t="s">
@@ -12633,14 +12779,14 @@
       <c r="C117" s="8"/>
     </row>
     <row r="118" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A118" s="118"/>
+      <c r="A118" s="125"/>
       <c r="B118" s="97" t="s">
         <v>439</v>
       </c>
       <c r="C118" s="97"/>
     </row>
     <row r="119" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A119" s="117">
+      <c r="A119" s="123">
         <v>44635</v>
       </c>
       <c r="B119" s="8" t="s">
@@ -12649,14 +12795,14 @@
       <c r="C119" s="8"/>
     </row>
     <row r="120" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A120" s="118"/>
+      <c r="A120" s="125"/>
       <c r="B120" s="98" t="s">
         <v>448</v>
       </c>
       <c r="C120" s="98"/>
     </row>
     <row r="121" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A121" s="117">
+      <c r="A121" s="123">
         <v>44636</v>
       </c>
       <c r="B121" s="8" t="s">
@@ -12665,14 +12811,14 @@
       <c r="C121" s="8"/>
     </row>
     <row r="122" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A122" s="118"/>
+      <c r="A122" s="125"/>
       <c r="B122" s="99" t="s">
         <v>458</v>
       </c>
       <c r="C122" s="99"/>
     </row>
     <row r="123" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A123" s="117">
+      <c r="A123" s="123">
         <v>44637</v>
       </c>
       <c r="B123" s="8" t="s">
@@ -12681,28 +12827,28 @@
       <c r="C123" s="8"/>
     </row>
     <row r="124" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A124" s="119"/>
+      <c r="A124" s="124"/>
       <c r="B124" s="4" t="s">
         <v>464</v>
       </c>
       <c r="C124" s="4"/>
     </row>
     <row r="125" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A125" s="119"/>
+      <c r="A125" s="124"/>
       <c r="B125" s="4" t="s">
         <v>465</v>
       </c>
       <c r="C125" s="4"/>
     </row>
     <row r="126" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A126" s="118"/>
+      <c r="A126" s="125"/>
       <c r="B126" s="102" t="s">
         <v>466</v>
       </c>
       <c r="C126" s="102"/>
     </row>
     <row r="127" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A127" s="117">
+      <c r="A127" s="123">
         <v>44638</v>
       </c>
       <c r="B127" s="8" t="s">
@@ -12711,14 +12857,14 @@
       <c r="C127" s="8"/>
     </row>
     <row r="128" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A128" s="118"/>
+      <c r="A128" s="125"/>
       <c r="B128" s="103" t="s">
         <v>469</v>
       </c>
       <c r="C128" s="103"/>
     </row>
     <row r="129" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A129" s="117">
+      <c r="A129" s="123">
         <v>44639</v>
       </c>
       <c r="B129" s="8" t="s">
@@ -12727,14 +12873,14 @@
       <c r="C129" s="8"/>
     </row>
     <row r="130" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A130" s="118"/>
+      <c r="A130" s="125"/>
       <c r="B130" s="104" t="s">
         <v>471</v>
       </c>
       <c r="C130" s="104"/>
     </row>
     <row r="131" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A131" s="117">
+      <c r="A131" s="123">
         <v>44640</v>
       </c>
       <c r="B131" s="8" t="s">
@@ -12743,21 +12889,21 @@
       <c r="C131" s="8"/>
     </row>
     <row r="132" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A132" s="119"/>
+      <c r="A132" s="124"/>
       <c r="B132" s="4" t="s">
         <v>478</v>
       </c>
       <c r="C132" s="4"/>
     </row>
     <row r="133" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A133" s="118"/>
+      <c r="A133" s="125"/>
       <c r="B133" s="105" t="s">
         <v>479</v>
       </c>
       <c r="C133" s="105"/>
     </row>
     <row r="134" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A134" s="117">
+      <c r="A134" s="123">
         <v>44641</v>
       </c>
       <c r="B134" s="8" t="s">
@@ -12766,21 +12912,21 @@
       <c r="C134" s="8"/>
     </row>
     <row r="135" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A135" s="119"/>
+      <c r="A135" s="124"/>
       <c r="B135" s="4" t="s">
         <v>483</v>
       </c>
       <c r="C135" s="4"/>
     </row>
     <row r="136" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A136" s="118"/>
+      <c r="A136" s="125"/>
       <c r="B136" s="107" t="s">
         <v>484</v>
       </c>
       <c r="C136" s="107"/>
     </row>
     <row r="137" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A137" s="117">
+      <c r="A137" s="123">
         <v>44642</v>
       </c>
       <c r="B137" s="8" t="s">
@@ -12789,14 +12935,14 @@
       <c r="C137" s="8"/>
     </row>
     <row r="138" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A138" s="118"/>
+      <c r="A138" s="125"/>
       <c r="B138" s="108" t="s">
         <v>496</v>
       </c>
       <c r="C138" s="108"/>
     </row>
     <row r="139" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A139" s="117">
+      <c r="A139" s="123">
         <v>44643</v>
       </c>
       <c r="B139" s="8" t="s">
@@ -12805,14 +12951,14 @@
       <c r="C139" s="8"/>
     </row>
     <row r="140" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A140" s="118"/>
+      <c r="A140" s="125"/>
       <c r="B140" s="108" t="s">
         <v>500</v>
       </c>
       <c r="C140" s="108"/>
     </row>
     <row r="141" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A141" s="117">
+      <c r="A141" s="123">
         <v>44644</v>
       </c>
       <c r="B141" s="8" t="s">
@@ -12821,21 +12967,21 @@
       <c r="C141" s="8"/>
     </row>
     <row r="142" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A142" s="119"/>
+      <c r="A142" s="124"/>
       <c r="B142" s="4" t="s">
         <v>504</v>
       </c>
       <c r="C142" s="4"/>
     </row>
     <row r="143" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A143" s="118"/>
+      <c r="A143" s="125"/>
       <c r="B143" s="109" t="s">
         <v>505</v>
       </c>
       <c r="C143" s="109"/>
     </row>
     <row r="144" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A144" s="117">
+      <c r="A144" s="123">
         <v>44645</v>
       </c>
       <c r="B144" s="8" t="s">
@@ -12844,7 +12990,7 @@
       <c r="C144" s="8"/>
     </row>
     <row r="145" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A145" s="118"/>
+      <c r="A145" s="125"/>
       <c r="B145" s="111" t="s">
         <v>511</v>
       </c>
@@ -12860,7 +13006,7 @@
       <c r="C146" s="12"/>
     </row>
     <row r="147" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A147" s="117">
+      <c r="A147" s="123">
         <v>44647</v>
       </c>
       <c r="B147" s="8" t="s">
@@ -12869,14 +13015,14 @@
       <c r="C147" s="8"/>
     </row>
     <row r="148" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A148" s="118"/>
+      <c r="A148" s="125"/>
       <c r="B148" s="112" t="s">
         <v>514</v>
       </c>
       <c r="C148" s="112"/>
     </row>
     <row r="149" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A149" s="117">
+      <c r="A149" s="123">
         <v>44648</v>
       </c>
       <c r="B149" s="8" t="s">
@@ -12885,28 +13031,28 @@
       <c r="C149" s="8"/>
     </row>
     <row r="150" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A150" s="119"/>
+      <c r="A150" s="124"/>
       <c r="B150" s="4" t="s">
         <v>523</v>
       </c>
       <c r="C150" s="4"/>
     </row>
     <row r="151" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A151" s="119"/>
+      <c r="A151" s="124"/>
       <c r="B151" s="4" t="s">
         <v>525</v>
       </c>
       <c r="C151" s="4"/>
     </row>
     <row r="152" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A152" s="118"/>
+      <c r="A152" s="125"/>
       <c r="B152" s="113" t="s">
         <v>526</v>
       </c>
       <c r="C152" s="113"/>
     </row>
     <row r="153" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A153" s="117">
+      <c r="A153" s="123">
         <v>44649</v>
       </c>
       <c r="B153" s="8" t="s">
@@ -12915,21 +13061,21 @@
       <c r="C153" s="8"/>
     </row>
     <row r="154" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A154" s="119"/>
+      <c r="A154" s="124"/>
       <c r="B154" s="4" t="s">
         <v>532</v>
       </c>
       <c r="C154" s="4"/>
     </row>
     <row r="155" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A155" s="118"/>
+      <c r="A155" s="125"/>
       <c r="B155" s="114" t="s">
         <v>533</v>
       </c>
       <c r="C155" s="114"/>
     </row>
     <row r="156" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A156" s="117">
+      <c r="A156" s="123">
         <v>44650</v>
       </c>
       <c r="B156" s="8" t="s">
@@ -12938,21 +13084,21 @@
       <c r="C156" s="8"/>
     </row>
     <row r="157" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A157" s="119"/>
+      <c r="A157" s="124"/>
       <c r="B157" s="4" t="s">
         <v>536</v>
       </c>
       <c r="C157" s="4"/>
     </row>
     <row r="158" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A158" s="118"/>
+      <c r="A158" s="125"/>
       <c r="B158" s="114" t="s">
         <v>537</v>
       </c>
       <c r="C158" s="114"/>
     </row>
     <row r="159" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A159" s="117">
+      <c r="A159" s="123">
         <v>44651</v>
       </c>
       <c r="B159" s="8" t="s">
@@ -12961,98 +13107,140 @@
       <c r="C159" s="8"/>
     </row>
     <row r="160" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A160" s="119"/>
+      <c r="A160" s="124"/>
       <c r="B160" s="4" t="s">
         <v>542</v>
       </c>
       <c r="C160" s="4"/>
     </row>
     <row r="161" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A161" s="118"/>
+      <c r="A161" s="125"/>
       <c r="B161" s="115" t="s">
         <v>543</v>
       </c>
       <c r="C161" s="115"/>
     </row>
-    <row r="162" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A162" s="28"/>
-      <c r="B162" s="3"/>
-      <c r="C162" s="3"/>
-    </row>
-    <row r="163" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A163" s="28"/>
-      <c r="B163" s="3"/>
-      <c r="C163" s="3"/>
-    </row>
-    <row r="164" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A164" s="28"/>
-      <c r="B164" s="3"/>
-      <c r="C164" s="3"/>
-    </row>
-    <row r="165" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A165" s="28"/>
-      <c r="B165" s="3"/>
-      <c r="C165" s="3"/>
-    </row>
-    <row r="166" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A166" s="28"/>
-      <c r="B166" s="3"/>
-      <c r="C166" s="3"/>
-    </row>
-    <row r="167" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A167" s="28"/>
-      <c r="B167" s="3"/>
-      <c r="C167" s="3"/>
-    </row>
-    <row r="168" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A168" s="28"/>
-      <c r="B168" s="3"/>
-      <c r="C168" s="3"/>
-    </row>
-    <row r="169" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A169" s="28"/>
-      <c r="B169" s="3"/>
-      <c r="C169" s="3"/>
-    </row>
-    <row r="170" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A170" s="28"/>
-      <c r="B170" s="3"/>
-      <c r="C170" s="3"/>
-    </row>
-    <row r="171" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A171" s="28"/>
-      <c r="B171" s="3"/>
-      <c r="C171" s="3"/>
-    </row>
-    <row r="172" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A172" s="28"/>
-      <c r="B172" s="3"/>
-      <c r="C172" s="3"/>
-    </row>
-    <row r="173" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A173" s="28"/>
-      <c r="B173" s="3"/>
-      <c r="C173" s="3"/>
-    </row>
-    <row r="174" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A174" s="28"/>
-      <c r="B174" s="3"/>
-      <c r="C174" s="3"/>
-    </row>
-    <row r="175" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A175" s="28"/>
-      <c r="B175" s="3"/>
-      <c r="C175" s="3"/>
-    </row>
-    <row r="176" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A176" s="28"/>
-      <c r="B176" s="3"/>
-      <c r="C176" s="3"/>
-    </row>
-    <row r="177" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A177" s="28"/>
-      <c r="B177" s="3"/>
-      <c r="C177" s="3"/>
+    <row r="162" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A162" s="123">
+        <v>44652</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>553</v>
+      </c>
+      <c r="C162" s="8"/>
+    </row>
+    <row r="163" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A163" s="124"/>
+      <c r="B163" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="C163" s="4"/>
+    </row>
+    <row r="164" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A164" s="124"/>
+      <c r="B164" s="4" t="s">
+        <v>555</v>
+      </c>
+      <c r="C164" s="4"/>
+    </row>
+    <row r="165" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A165" s="125"/>
+      <c r="B165" s="117" t="s">
+        <v>556</v>
+      </c>
+      <c r="C165" s="117"/>
+    </row>
+    <row r="166" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A166" s="123">
+        <v>44653</v>
+      </c>
+      <c r="B166" s="8" t="s">
+        <v>558</v>
+      </c>
+      <c r="C166" s="8"/>
+    </row>
+    <row r="167" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A167" s="124"/>
+      <c r="B167" s="4" t="s">
+        <v>559</v>
+      </c>
+      <c r="C167" s="4"/>
+    </row>
+    <row r="168" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A168" s="125"/>
+      <c r="B168" s="119" t="s">
+        <v>560</v>
+      </c>
+      <c r="C168" s="119"/>
+    </row>
+    <row r="169" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A169" s="123">
+        <v>44654</v>
+      </c>
+      <c r="B169" s="8" t="s">
+        <v>563</v>
+      </c>
+      <c r="C169" s="8"/>
+    </row>
+    <row r="170" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A170" s="124"/>
+      <c r="B170" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="C170" s="4"/>
+    </row>
+    <row r="171" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A171" s="125"/>
+      <c r="B171" s="120" t="s">
+        <v>565</v>
+      </c>
+      <c r="C171" s="120"/>
+    </row>
+    <row r="172" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A172" s="123">
+        <v>44655</v>
+      </c>
+      <c r="B172" s="8" t="s">
+        <v>572</v>
+      </c>
+      <c r="C172" s="8"/>
+    </row>
+    <row r="173" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A173" s="124"/>
+      <c r="B173" s="4" t="s">
+        <v>483</v>
+      </c>
+      <c r="C173" s="4"/>
+    </row>
+    <row r="174" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A174" s="125"/>
+      <c r="B174" s="121" t="s">
+        <v>573</v>
+      </c>
+      <c r="C174" s="121"/>
+    </row>
+    <row r="175" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A175" s="123">
+        <v>44656</v>
+      </c>
+      <c r="B175" s="8" t="s">
+        <v>575</v>
+      </c>
+      <c r="C175" s="8"/>
+    </row>
+    <row r="176" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A176" s="124"/>
+      <c r="B176" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="C176" s="4"/>
+    </row>
+    <row r="177" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A177" s="125"/>
+      <c r="B177" s="122" t="s">
+        <v>514</v>
+      </c>
+      <c r="C177" s="122"/>
     </row>
     <row r="178" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A178" s="28"/>
@@ -13378,7 +13566,51 @@
       <c r="C242" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="53">
+  <mergeCells count="58">
+    <mergeCell ref="A175:A177"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="A153:A155"/>
+    <mergeCell ref="A156:A158"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="A131:A133"/>
+    <mergeCell ref="A129:A130"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="A123:A126"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A166:A168"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A90:A93"/>
+    <mergeCell ref="A86:A89"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="A77:A83"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A162:A165"/>
+    <mergeCell ref="A159:A161"/>
+    <mergeCell ref="A149:A152"/>
+    <mergeCell ref="A172:A174"/>
+    <mergeCell ref="A169:A171"/>
     <mergeCell ref="A98:A99"/>
     <mergeCell ref="A96:A97"/>
     <mergeCell ref="A109:A110"/>
@@ -13393,45 +13625,6 @@
     <mergeCell ref="A107:A108"/>
     <mergeCell ref="A104:A105"/>
     <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="A90:A93"/>
-    <mergeCell ref="A86:A89"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="A77:A83"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A159:A161"/>
-    <mergeCell ref="A149:A152"/>
-    <mergeCell ref="A113:A114"/>
-    <mergeCell ref="A131:A133"/>
-    <mergeCell ref="A129:A130"/>
-    <mergeCell ref="A127:A128"/>
-    <mergeCell ref="A123:A126"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="A153:A155"/>
-    <mergeCell ref="A156:A158"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13476,7 +13669,7 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:17" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="117">
+      <c r="A2" s="123">
         <v>44623</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -13484,19 +13677,19 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A3" s="119"/>
+      <c r="A3" s="124"/>
       <c r="B3" s="4" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A4" s="118"/>
+      <c r="A4" s="125"/>
       <c r="B4" s="83" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="117">
+      <c r="A5" s="123">
         <v>44624</v>
       </c>
       <c r="B5" s="31" t="s">
@@ -13504,13 +13697,13 @@
       </c>
     </row>
     <row r="6" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="119"/>
+      <c r="A6" s="124"/>
       <c r="B6" s="52" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="118"/>
+      <c r="A7" s="125"/>
       <c r="B7" s="54" t="s">
         <v>378</v>
       </c>
@@ -13524,7 +13717,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="117">
+      <c r="A9" s="123">
         <v>44628</v>
       </c>
       <c r="B9" s="31"/>
@@ -13547,7 +13740,7 @@
       <c r="Q9" s="31"/>
     </row>
     <row r="10" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="118"/>
+      <c r="A10" s="125"/>
       <c r="B10" s="54"/>
       <c r="C10" s="54" t="s">
         <v>403</v>
@@ -13568,7 +13761,7 @@
       <c r="Q10" s="54"/>
     </row>
     <row r="11" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="117">
+      <c r="A11" s="123">
         <v>44630</v>
       </c>
       <c r="B11" s="31"/>
@@ -13591,7 +13784,7 @@
       <c r="Q11" s="31"/>
     </row>
     <row r="12" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="119"/>
+      <c r="A12" s="124"/>
       <c r="B12" s="52"/>
       <c r="C12" s="52" t="s">
         <v>417</v>
@@ -13612,7 +13805,7 @@
       <c r="Q12" s="52"/>
     </row>
     <row r="13" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="118"/>
+      <c r="A13" s="125"/>
       <c r="B13" s="54"/>
       <c r="C13" s="54" t="s">
         <v>418</v>
@@ -13633,7 +13826,7 @@
       <c r="Q13" s="54"/>
     </row>
     <row r="14" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="117">
+      <c r="A14" s="123">
         <v>44633</v>
       </c>
       <c r="B14" s="31"/>
@@ -13656,7 +13849,7 @@
       <c r="Q14" s="31"/>
     </row>
     <row r="15" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="119"/>
+      <c r="A15" s="124"/>
       <c r="B15" s="52"/>
       <c r="C15" s="52" t="s">
         <v>435</v>
@@ -13677,7 +13870,7 @@
       <c r="Q15" s="52"/>
     </row>
     <row r="16" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="119"/>
+      <c r="A16" s="124"/>
       <c r="B16" s="52"/>
       <c r="C16" s="52" t="s">
         <v>436</v>
@@ -13698,7 +13891,7 @@
       <c r="Q16" s="52"/>
     </row>
     <row r="17" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="118"/>
+      <c r="A17" s="125"/>
       <c r="B17" s="54"/>
       <c r="C17" s="54" t="s">
         <v>437</v>
@@ -13719,7 +13912,7 @@
       <c r="Q17" s="54"/>
     </row>
     <row r="18" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="117">
+      <c r="A18" s="123">
         <v>44634</v>
       </c>
       <c r="B18" s="31"/>
@@ -13742,7 +13935,7 @@
       <c r="Q18" s="31"/>
     </row>
     <row r="19" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="119"/>
+      <c r="A19" s="124"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52" t="s">
         <v>441</v>
@@ -13763,7 +13956,7 @@
       <c r="Q19" s="52"/>
     </row>
     <row r="20" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="119"/>
+      <c r="A20" s="124"/>
       <c r="B20" s="52"/>
       <c r="C20" s="52" t="s">
         <v>442</v>
@@ -13784,7 +13977,7 @@
       <c r="Q20" s="52"/>
     </row>
     <row r="21" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="118"/>
+      <c r="A21" s="125"/>
       <c r="B21" s="54"/>
       <c r="C21" s="54" t="s">
         <v>443</v>
@@ -13805,7 +13998,7 @@
       <c r="Q21" s="54"/>
     </row>
     <row r="22" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="117">
+      <c r="A22" s="123">
         <v>44636</v>
       </c>
       <c r="B22" s="31"/>
@@ -13828,7 +14021,7 @@
       <c r="Q22" s="31"/>
     </row>
     <row r="23" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="118"/>
+      <c r="A23" s="125"/>
       <c r="B23" s="54"/>
       <c r="C23" s="54" t="s">
         <v>462</v>
@@ -13849,7 +14042,7 @@
       <c r="Q23" s="54"/>
     </row>
     <row r="24" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="117">
+      <c r="A24" s="123">
         <v>44639</v>
       </c>
       <c r="B24" s="31"/>
@@ -13872,7 +14065,7 @@
       <c r="Q24" s="31"/>
     </row>
     <row r="25" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="118"/>
+      <c r="A25" s="125"/>
       <c r="B25" s="54"/>
       <c r="C25" s="54" t="s">
         <v>473</v>
@@ -13893,7 +14086,7 @@
       <c r="Q25" s="54"/>
     </row>
     <row r="26" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="117">
+      <c r="A26" s="123">
         <v>44641</v>
       </c>
       <c r="B26" s="31" t="s">
@@ -13916,7 +14109,7 @@
       <c r="Q26" s="31"/>
     </row>
     <row r="27" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="119"/>
+      <c r="A27" s="124"/>
       <c r="B27" s="52" t="s">
         <v>489</v>
       </c>
@@ -13937,7 +14130,7 @@
       <c r="Q27" s="52"/>
     </row>
     <row r="28" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="119"/>
+      <c r="A28" s="124"/>
       <c r="B28" s="52" t="s">
         <v>490</v>
       </c>
@@ -13958,7 +14151,7 @@
       <c r="Q28" s="52"/>
     </row>
     <row r="29" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="118"/>
+      <c r="A29" s="125"/>
       <c r="B29" s="54" t="s">
         <v>491</v>
       </c>
@@ -16898,7 +17091,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C434693-A01C-4220-BD8E-CE7EBA29C799}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
The last commit before returning school .
</commit_message>
<xml_diff>
--- a/学习记录.xlsx
+++ b/学习记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\不怕晒的铃铛\Desktop\学习资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9097E22-77C1-4B20-9CE2-2A61546E7D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D751527A-25FD-4A24-88FA-2E56F586270E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="612">
   <si>
     <t>JavaSE</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2474,6 +2474,14 @@
   </si>
   <si>
     <t>下一个更大元素 I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下一个更大元素II</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接雨水</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2581,7 +2589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2966,6 +2974,15 @@
     <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3340,7 +3357,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="131">
+      <c r="A3" s="134">
         <v>44566</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -3350,7 +3367,7 @@
       <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:16" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="132"/>
+      <c r="A4" s="135"/>
       <c r="B4" s="4" t="s">
         <v>27</v>
       </c>
@@ -3358,7 +3375,7 @@
       <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:16" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="133"/>
+      <c r="A5" s="136"/>
       <c r="B5" s="6" t="s">
         <v>28</v>
       </c>
@@ -3396,7 +3413,7 @@
       <c r="D8" s="12"/>
     </row>
     <row r="9" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="131">
+      <c r="A9" s="134">
         <v>44572</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -3406,7 +3423,7 @@
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:16" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="133"/>
+      <c r="A10" s="136"/>
       <c r="B10" s="17" t="s">
         <v>38</v>
       </c>
@@ -3414,7 +3431,7 @@
       <c r="D10" s="17"/>
     </row>
     <row r="11" spans="1:16" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="131">
+      <c r="A11" s="134">
         <v>44573</v>
       </c>
       <c r="B11" s="8" t="s">
@@ -3424,7 +3441,7 @@
       <c r="D11" s="8"/>
     </row>
     <row r="12" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="132"/>
+      <c r="A12" s="135"/>
       <c r="B12" s="4" t="s">
         <v>18</v>
       </c>
@@ -3432,7 +3449,7 @@
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:16" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="133"/>
+      <c r="A13" s="136"/>
       <c r="B13" s="18" t="s">
         <v>40</v>
       </c>
@@ -3440,7 +3457,7 @@
       <c r="D13" s="18"/>
     </row>
     <row r="14" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="131">
+      <c r="A14" s="134">
         <v>44574</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -3450,7 +3467,7 @@
       <c r="D14" s="8"/>
     </row>
     <row r="15" spans="1:16" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="133"/>
+      <c r="A15" s="136"/>
       <c r="B15" s="19" t="s">
         <v>42</v>
       </c>
@@ -3460,7 +3477,7 @@
       <c r="D15" s="19"/>
     </row>
     <row r="16" spans="1:16" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="131">
+      <c r="A16" s="134">
         <v>44575</v>
       </c>
       <c r="B16" s="8" t="s">
@@ -3472,7 +3489,7 @@
       <c r="D16" s="8"/>
     </row>
     <row r="17" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="132"/>
+      <c r="A17" s="135"/>
       <c r="B17" s="4" t="s">
         <v>47</v>
       </c>
@@ -3483,7 +3500,7 @@
       <c r="E17" s="4"/>
     </row>
     <row r="18" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="132"/>
+      <c r="A18" s="135"/>
       <c r="B18" s="4" t="s">
         <v>48</v>
       </c>
@@ -3494,7 +3511,7 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="133"/>
+      <c r="A19" s="136"/>
       <c r="B19" s="20" t="s">
         <v>49</v>
       </c>
@@ -3503,7 +3520,7 @@
       <c r="E19" s="21"/>
     </row>
     <row r="20" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="131">
+      <c r="A20" s="134">
         <v>44576</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -3516,7 +3533,7 @@
       <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="132"/>
+      <c r="A21" s="135"/>
       <c r="B21" s="4" t="s">
         <v>59</v>
       </c>
@@ -3527,7 +3544,7 @@
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="132"/>
+      <c r="A22" s="135"/>
       <c r="B22" s="4" t="s">
         <v>60</v>
       </c>
@@ -3538,7 +3555,7 @@
       <c r="E22" s="4"/>
     </row>
     <row r="23" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="133"/>
+      <c r="A23" s="136"/>
       <c r="B23" s="20"/>
       <c r="C23" s="20" t="s">
         <v>57</v>
@@ -3547,7 +3564,7 @@
       <c r="E23" s="21"/>
     </row>
     <row r="24" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="131">
+      <c r="A24" s="134">
         <v>44577</v>
       </c>
       <c r="B24" s="8" t="s">
@@ -3562,7 +3579,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="132"/>
+      <c r="A25" s="135"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
         <v>63</v>
@@ -3573,7 +3590,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="133"/>
+      <c r="A26" s="136"/>
       <c r="B26" s="21"/>
       <c r="C26" s="21" t="s">
         <v>64</v>
@@ -3584,7 +3601,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="131">
+      <c r="A27" s="134">
         <v>44578</v>
       </c>
       <c r="B27" s="8" t="s">
@@ -3595,7 +3612,7 @@
       <c r="E27" s="8"/>
     </row>
     <row r="28" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="132"/>
+      <c r="A28" s="135"/>
       <c r="B28" s="4" t="s">
         <v>69</v>
       </c>
@@ -3604,7 +3621,7 @@
       <c r="E28" s="4"/>
     </row>
     <row r="29" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="132"/>
+      <c r="A29" s="135"/>
       <c r="B29" s="4" t="s">
         <v>70</v>
       </c>
@@ -3613,7 +3630,7 @@
       <c r="E29" s="4"/>
     </row>
     <row r="30" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="133"/>
+      <c r="A30" s="136"/>
       <c r="B30" s="22" t="s">
         <v>71</v>
       </c>
@@ -3622,7 +3639,7 @@
       <c r="E30" s="22"/>
     </row>
     <row r="31" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="131">
+      <c r="A31" s="134">
         <v>44579</v>
       </c>
       <c r="B31" s="8" t="s">
@@ -3637,7 +3654,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="133"/>
+      <c r="A32" s="136"/>
       <c r="B32" s="22" t="s">
         <v>73</v>
       </c>
@@ -3648,7 +3665,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="131">
+      <c r="A33" s="134">
         <v>44580</v>
       </c>
       <c r="B33" s="8" t="s">
@@ -3662,7 +3679,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="133"/>
+      <c r="A34" s="136"/>
       <c r="B34" s="23" t="s">
         <v>83</v>
       </c>
@@ -3671,7 +3688,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="131">
+      <c r="A35" s="134">
         <v>44581</v>
       </c>
       <c r="B35" s="8" t="s">
@@ -3683,7 +3700,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="132"/>
+      <c r="A36" s="135"/>
       <c r="B36" s="4" t="s">
         <v>85</v>
       </c>
@@ -3693,7 +3710,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="132"/>
+      <c r="A37" s="135"/>
       <c r="B37" s="4" t="s">
         <v>86</v>
       </c>
@@ -3701,7 +3718,7 @@
       <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="132"/>
+      <c r="A38" s="135"/>
       <c r="B38" s="4" t="s">
         <v>87</v>
       </c>
@@ -3709,7 +3726,7 @@
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="133"/>
+      <c r="A39" s="136"/>
       <c r="B39" s="23" t="s">
         <v>88</v>
       </c>
@@ -3717,7 +3734,7 @@
       <c r="D39" s="23"/>
     </row>
     <row r="40" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="131">
+      <c r="A40" s="134">
         <v>44582</v>
       </c>
       <c r="B40" s="8" t="s">
@@ -3734,7 +3751,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="134"/>
+      <c r="A41" s="137"/>
       <c r="B41" s="4" t="s">
         <v>91</v>
       </c>
@@ -3746,7 +3763,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="134"/>
+      <c r="A42" s="137"/>
       <c r="B42" s="4" t="s">
         <v>98</v>
       </c>
@@ -3756,7 +3773,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="135"/>
+      <c r="A43" s="138"/>
       <c r="B43" s="24" t="s">
         <v>99</v>
       </c>
@@ -3766,7 +3783,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="131">
+      <c r="A44" s="134">
         <v>44583</v>
       </c>
       <c r="B44" s="8" t="s">
@@ -3776,7 +3793,7 @@
       <c r="D44" s="8"/>
     </row>
     <row r="45" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="132"/>
+      <c r="A45" s="135"/>
       <c r="B45" s="4" t="s">
         <v>101</v>
       </c>
@@ -3784,7 +3801,7 @@
       <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="132"/>
+      <c r="A46" s="135"/>
       <c r="B46" s="4" t="s">
         <v>102</v>
       </c>
@@ -3792,7 +3809,7 @@
       <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="132"/>
+      <c r="A47" s="135"/>
       <c r="B47" s="4" t="s">
         <v>103</v>
       </c>
@@ -3800,7 +3817,7 @@
       <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:5" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="132"/>
+      <c r="A48" s="135"/>
       <c r="B48" s="4" t="s">
         <v>104</v>
       </c>
@@ -3808,7 +3825,7 @@
       <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="133"/>
+      <c r="A49" s="136"/>
       <c r="B49" s="25" t="s">
         <v>105</v>
       </c>
@@ -3816,7 +3833,7 @@
       <c r="D49" s="25"/>
     </row>
     <row r="50" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="131">
+      <c r="A50" s="134">
         <v>44584</v>
       </c>
       <c r="B50" s="8" t="s">
@@ -3826,7 +3843,7 @@
       <c r="D50" s="8"/>
     </row>
     <row r="51" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="134"/>
+      <c r="A51" s="137"/>
       <c r="B51" s="4" t="s">
         <v>107</v>
       </c>
@@ -3834,7 +3851,7 @@
       <c r="D51" s="4"/>
     </row>
     <row r="52" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="134"/>
+      <c r="A52" s="137"/>
       <c r="B52" s="4" t="s">
         <v>108</v>
       </c>
@@ -3842,7 +3859,7 @@
       <c r="D52" s="4"/>
     </row>
     <row r="53" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="135"/>
+      <c r="A53" s="138"/>
       <c r="B53" s="26" t="s">
         <v>109</v>
       </c>
@@ -3850,7 +3867,7 @@
       <c r="D53" s="26"/>
     </row>
     <row r="54" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="131">
+      <c r="A54" s="134">
         <v>44585</v>
       </c>
       <c r="B54" s="8" t="s">
@@ -3860,7 +3877,7 @@
       <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:5" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="133"/>
+      <c r="A55" s="136"/>
       <c r="B55" s="27" t="s">
         <v>111</v>
       </c>
@@ -3868,7 +3885,7 @@
       <c r="D55" s="27"/>
     </row>
     <row r="56" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="131">
+      <c r="A56" s="134">
         <v>44586</v>
       </c>
       <c r="B56" s="8"/>
@@ -3883,7 +3900,7 @@
       </c>
     </row>
     <row r="57" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="132"/>
+      <c r="A57" s="135"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4" t="s">
@@ -3892,7 +3909,7 @@
       <c r="E57" s="4"/>
     </row>
     <row r="58" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="133"/>
+      <c r="A58" s="136"/>
       <c r="B58" s="27"/>
       <c r="C58" s="27"/>
       <c r="D58" s="27" t="s">
@@ -3901,7 +3918,7 @@
       <c r="E58" s="27"/>
     </row>
     <row r="59" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="131">
+      <c r="A59" s="134">
         <v>44587</v>
       </c>
       <c r="B59" s="8"/>
@@ -3916,7 +3933,7 @@
       </c>
     </row>
     <row r="60" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="132"/>
+      <c r="A60" s="135"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4" t="s">
         <v>120</v>
@@ -3926,7 +3943,7 @@
       </c>
     </row>
     <row r="61" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="132"/>
+      <c r="A61" s="135"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4" t="s">
         <v>123</v>
@@ -3937,7 +3954,7 @@
       </c>
     </row>
     <row r="62" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="133"/>
+      <c r="A62" s="136"/>
       <c r="B62" s="29"/>
       <c r="C62" s="29" t="s">
         <v>124</v>
@@ -3946,7 +3963,7 @@
       <c r="E62" s="29"/>
     </row>
     <row r="63" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="131">
+      <c r="A63" s="134">
         <v>44588</v>
       </c>
       <c r="B63" s="8"/>
@@ -3961,7 +3978,7 @@
       </c>
     </row>
     <row r="64" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="132"/>
+      <c r="A64" s="135"/>
       <c r="B64" s="4"/>
       <c r="C64" s="4" t="s">
         <v>126</v>
@@ -3972,7 +3989,7 @@
       <c r="E64" s="4"/>
     </row>
     <row r="65" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="132"/>
+      <c r="A65" s="135"/>
       <c r="B65" s="4"/>
       <c r="C65" s="4" t="s">
         <v>127</v>
@@ -3983,7 +4000,7 @@
       <c r="E65" s="4"/>
     </row>
     <row r="66" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="133"/>
+      <c r="A66" s="136"/>
       <c r="B66" s="30"/>
       <c r="C66" s="30" t="s">
         <v>128</v>
@@ -3992,7 +4009,7 @@
       <c r="E66" s="30"/>
     </row>
     <row r="67" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="131">
+      <c r="A67" s="134">
         <v>44589</v>
       </c>
       <c r="B67" s="8"/>
@@ -4003,7 +4020,7 @@
       </c>
     </row>
     <row r="68" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="132"/>
+      <c r="A68" s="135"/>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -4012,7 +4029,7 @@
       </c>
     </row>
     <row r="69" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="133"/>
+      <c r="A69" s="136"/>
       <c r="B69" s="32"/>
       <c r="C69" s="32"/>
       <c r="D69" s="32"/>
@@ -4045,7 +4062,7 @@
       </c>
     </row>
     <row r="72" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="131">
+      <c r="A72" s="134">
         <v>44594</v>
       </c>
       <c r="B72" s="8"/>
@@ -4056,7 +4073,7 @@
       </c>
     </row>
     <row r="73" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="132"/>
+      <c r="A73" s="135"/>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
@@ -4065,7 +4082,7 @@
       </c>
     </row>
     <row r="74" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="132"/>
+      <c r="A74" s="135"/>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
@@ -4074,7 +4091,7 @@
       </c>
     </row>
     <row r="75" spans="1:5" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="133"/>
+      <c r="A75" s="136"/>
       <c r="B75" s="37"/>
       <c r="C75" s="37"/>
       <c r="D75" s="37"/>
@@ -4105,7 +4122,7 @@
       </c>
     </row>
     <row r="78" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="131">
+      <c r="A78" s="134">
         <v>44598</v>
       </c>
       <c r="B78" s="8"/>
@@ -4116,7 +4133,7 @@
       </c>
     </row>
     <row r="79" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="132"/>
+      <c r="A79" s="135"/>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
@@ -4125,7 +4142,7 @@
       </c>
     </row>
     <row r="80" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="132"/>
+      <c r="A80" s="135"/>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
@@ -4134,7 +4151,7 @@
       </c>
     </row>
     <row r="81" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="133"/>
+      <c r="A81" s="136"/>
       <c r="B81" s="48"/>
       <c r="C81" s="48"/>
       <c r="D81" s="48"/>
@@ -4143,7 +4160,7 @@
       </c>
     </row>
     <row r="82" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="131">
+      <c r="A82" s="134">
         <v>44599</v>
       </c>
       <c r="B82" s="8"/>
@@ -4154,7 +4171,7 @@
       </c>
     </row>
     <row r="83" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="132"/>
+      <c r="A83" s="135"/>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
@@ -4163,7 +4180,7 @@
       </c>
     </row>
     <row r="84" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="133"/>
+      <c r="A84" s="136"/>
       <c r="B84" s="49"/>
       <c r="C84" s="49"/>
       <c r="D84" s="49"/>
@@ -4172,7 +4189,7 @@
       </c>
     </row>
     <row r="85" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="131">
+      <c r="A85" s="134">
         <v>44600</v>
       </c>
       <c r="B85" s="8"/>
@@ -4190,7 +4207,7 @@
       <c r="J85" s="8"/>
     </row>
     <row r="86" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="133"/>
+      <c r="A86" s="136"/>
       <c r="B86" s="50"/>
       <c r="C86" s="50"/>
       <c r="D86" s="50"/>
@@ -4204,7 +4221,7 @@
       <c r="J86" s="50"/>
     </row>
     <row r="87" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="131">
+      <c r="A87" s="134">
         <v>44601</v>
       </c>
       <c r="B87" s="8"/>
@@ -4222,7 +4239,7 @@
       <c r="J87" s="8"/>
     </row>
     <row r="88" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="132"/>
+      <c r="A88" s="135"/>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4" t="s">
@@ -4238,7 +4255,7 @@
       <c r="J88" s="4"/>
     </row>
     <row r="89" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="132"/>
+      <c r="A89" s="135"/>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4" t="s">
@@ -4254,7 +4271,7 @@
       <c r="J89" s="4"/>
     </row>
     <row r="90" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="132"/>
+      <c r="A90" s="135"/>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4" t="s">
@@ -4268,7 +4285,7 @@
       <c r="J90" s="4"/>
     </row>
     <row r="91" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="132"/>
+      <c r="A91" s="135"/>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4" t="s">
@@ -4282,7 +4299,7 @@
       <c r="J91" s="4"/>
     </row>
     <row r="92" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="132"/>
+      <c r="A92" s="135"/>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="52" t="s">
@@ -4296,7 +4313,7 @@
       <c r="J92" s="4"/>
     </row>
     <row r="93" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="132"/>
+      <c r="A93" s="135"/>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4" t="s">
@@ -4310,7 +4327,7 @@
       <c r="J93" s="4"/>
     </row>
     <row r="94" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="133"/>
+      <c r="A94" s="136"/>
       <c r="B94" s="51"/>
       <c r="C94" s="51"/>
       <c r="D94" s="54" t="s">
@@ -4324,7 +4341,7 @@
       <c r="J94" s="51"/>
     </row>
     <row r="95" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="131">
+      <c r="A95" s="134">
         <v>44602</v>
       </c>
       <c r="B95" s="8"/>
@@ -4342,7 +4359,7 @@
       <c r="J95" s="8"/>
     </row>
     <row r="96" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="132"/>
+      <c r="A96" s="135"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4" t="s">
@@ -4358,7 +4375,7 @@
       <c r="J96" s="4"/>
     </row>
     <row r="97" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="133"/>
+      <c r="A97" s="136"/>
       <c r="B97" s="53"/>
       <c r="C97" s="53"/>
       <c r="D97" s="53"/>
@@ -4372,7 +4389,7 @@
       <c r="J97" s="53"/>
     </row>
     <row r="98" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="131">
+      <c r="A98" s="134">
         <v>44603</v>
       </c>
       <c r="B98" s="8"/>
@@ -4388,7 +4405,7 @@
       <c r="J98" s="8"/>
     </row>
     <row r="99" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="132"/>
+      <c r="A99" s="135"/>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
@@ -4402,7 +4419,7 @@
       <c r="J99" s="4"/>
     </row>
     <row r="100" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="132"/>
+      <c r="A100" s="135"/>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
@@ -4416,7 +4433,7 @@
       <c r="J100" s="4"/>
     </row>
     <row r="101" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="132"/>
+      <c r="A101" s="135"/>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
@@ -4430,7 +4447,7 @@
       <c r="J101" s="4"/>
     </row>
     <row r="102" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="132"/>
+      <c r="A102" s="135"/>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
@@ -4444,7 +4461,7 @@
       <c r="J102" s="4"/>
     </row>
     <row r="103" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="133"/>
+      <c r="A103" s="136"/>
       <c r="B103" s="55"/>
       <c r="C103" s="55"/>
       <c r="D103" s="55"/>
@@ -4458,7 +4475,7 @@
       <c r="J103" s="55"/>
     </row>
     <row r="104" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="131">
+      <c r="A104" s="134">
         <v>44604</v>
       </c>
       <c r="B104" s="8"/>
@@ -4474,7 +4491,7 @@
       <c r="J104" s="8"/>
     </row>
     <row r="105" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="132"/>
+      <c r="A105" s="135"/>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
@@ -4488,7 +4505,7 @@
       <c r="J105" s="4"/>
     </row>
     <row r="106" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="132"/>
+      <c r="A106" s="135"/>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
@@ -4502,7 +4519,7 @@
       <c r="J106" s="4"/>
     </row>
     <row r="107" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A107" s="132"/>
+      <c r="A107" s="135"/>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
@@ -4516,7 +4533,7 @@
       <c r="J107" s="4"/>
     </row>
     <row r="108" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A108" s="132"/>
+      <c r="A108" s="135"/>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
@@ -4530,7 +4547,7 @@
       <c r="J108" s="4"/>
     </row>
     <row r="109" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="132"/>
+      <c r="A109" s="135"/>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
@@ -4544,7 +4561,7 @@
       <c r="J109" s="4"/>
     </row>
     <row r="110" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A110" s="133"/>
+      <c r="A110" s="136"/>
       <c r="B110" s="56"/>
       <c r="C110" s="56"/>
       <c r="D110" s="56"/>
@@ -4558,7 +4575,7 @@
       <c r="J110" s="56"/>
     </row>
     <row r="111" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="131">
+      <c r="A111" s="134">
         <v>44605</v>
       </c>
       <c r="B111" s="8"/>
@@ -4574,7 +4591,7 @@
       <c r="J111" s="8"/>
     </row>
     <row r="112" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="132"/>
+      <c r="A112" s="135"/>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
@@ -4588,7 +4605,7 @@
       <c r="J112" s="4"/>
     </row>
     <row r="113" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="132"/>
+      <c r="A113" s="135"/>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
@@ -4602,7 +4619,7 @@
       <c r="J113" s="4"/>
     </row>
     <row r="114" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="132"/>
+      <c r="A114" s="135"/>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
@@ -4616,7 +4633,7 @@
       <c r="J114" s="4"/>
     </row>
     <row r="115" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="132"/>
+      <c r="A115" s="135"/>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
@@ -4630,7 +4647,7 @@
       <c r="J115" s="4"/>
     </row>
     <row r="116" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="132"/>
+      <c r="A116" s="135"/>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
@@ -4644,7 +4661,7 @@
       <c r="J116" s="4"/>
     </row>
     <row r="117" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="133"/>
+      <c r="A117" s="136"/>
       <c r="B117" s="57"/>
       <c r="C117" s="57"/>
       <c r="D117" s="57"/>
@@ -4658,7 +4675,7 @@
       <c r="J117" s="57"/>
     </row>
     <row r="118" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A118" s="131">
+      <c r="A118" s="134">
         <v>44606</v>
       </c>
       <c r="B118" s="8"/>
@@ -4674,7 +4691,7 @@
       <c r="J118" s="8"/>
     </row>
     <row r="119" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="133"/>
+      <c r="A119" s="136"/>
       <c r="B119" s="58"/>
       <c r="C119" s="58"/>
       <c r="D119" s="58"/>
@@ -4688,7 +4705,7 @@
       <c r="J119" s="58"/>
     </row>
     <row r="120" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A120" s="131">
+      <c r="A120" s="134">
         <v>44607</v>
       </c>
       <c r="B120" s="8"/>
@@ -4704,7 +4721,7 @@
       <c r="J120" s="8"/>
     </row>
     <row r="121" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="133"/>
+      <c r="A121" s="136"/>
       <c r="B121" s="58"/>
       <c r="C121" s="58"/>
       <c r="D121" s="58"/>
@@ -4748,7 +4765,7 @@
       <c r="J123" s="64"/>
     </row>
     <row r="124" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="131">
+      <c r="A124" s="134">
         <v>44609</v>
       </c>
       <c r="B124" s="8"/>
@@ -4764,7 +4781,7 @@
       <c r="J124" s="8"/>
     </row>
     <row r="125" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="132"/>
+      <c r="A125" s="135"/>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
@@ -4778,7 +4795,7 @@
       <c r="J125" s="4"/>
     </row>
     <row r="126" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="132"/>
+      <c r="A126" s="135"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
@@ -4792,7 +4809,7 @@
       <c r="J126" s="4"/>
     </row>
     <row r="127" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="132"/>
+      <c r="A127" s="135"/>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
@@ -4806,7 +4823,7 @@
       <c r="J127" s="4"/>
     </row>
     <row r="128" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="132"/>
+      <c r="A128" s="135"/>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
@@ -4820,7 +4837,7 @@
       <c r="J128" s="4"/>
     </row>
     <row r="129" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="133"/>
+      <c r="A129" s="136"/>
       <c r="B129" s="67"/>
       <c r="C129" s="67"/>
       <c r="D129" s="67"/>
@@ -4834,7 +4851,7 @@
       <c r="J129" s="67"/>
     </row>
     <row r="130" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="131">
+      <c r="A130" s="134">
         <v>44610</v>
       </c>
       <c r="B130" s="8"/>
@@ -4850,7 +4867,7 @@
       <c r="J130" s="8"/>
     </row>
     <row r="131" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="132"/>
+      <c r="A131" s="135"/>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
@@ -4864,7 +4881,7 @@
       <c r="J131" s="4"/>
     </row>
     <row r="132" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="132"/>
+      <c r="A132" s="135"/>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
@@ -4878,7 +4895,7 @@
       <c r="J132" s="4"/>
     </row>
     <row r="133" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="133"/>
+      <c r="A133" s="136"/>
       <c r="B133" s="67"/>
       <c r="C133" s="67"/>
       <c r="D133" s="67"/>
@@ -4910,7 +4927,7 @@
       <c r="J134" s="12"/>
     </row>
     <row r="135" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="131">
+      <c r="A135" s="134">
         <v>44612</v>
       </c>
       <c r="B135" s="8"/>
@@ -4926,7 +4943,7 @@
       <c r="J135" s="8"/>
     </row>
     <row r="136" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A136" s="133"/>
+      <c r="A136" s="136"/>
       <c r="B136" s="71"/>
       <c r="C136" s="71"/>
       <c r="D136" s="71"/>
@@ -4940,7 +4957,7 @@
       <c r="J136" s="71"/>
     </row>
     <row r="137" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="131">
+      <c r="A137" s="134">
         <v>44613</v>
       </c>
       <c r="B137" s="8"/>
@@ -4958,7 +4975,7 @@
       <c r="J137" s="8"/>
     </row>
     <row r="138" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="132"/>
+      <c r="A138" s="135"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
       <c r="D138" s="4"/>
@@ -4974,7 +4991,7 @@
       <c r="J138" s="4"/>
     </row>
     <row r="139" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="132"/>
+      <c r="A139" s="135"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
@@ -4988,7 +5005,7 @@
       <c r="J139" s="4"/>
     </row>
     <row r="140" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="132"/>
+      <c r="A140" s="135"/>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
       <c r="D140" s="4"/>
@@ -5002,7 +5019,7 @@
       <c r="J140" s="4"/>
     </row>
     <row r="141" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="132"/>
+      <c r="A141" s="135"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
       <c r="D141" s="4"/>
@@ -5016,7 +5033,7 @@
       <c r="J141" s="4"/>
     </row>
     <row r="142" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="132"/>
+      <c r="A142" s="135"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
@@ -5030,7 +5047,7 @@
       <c r="J142" s="4"/>
     </row>
     <row r="143" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="133"/>
+      <c r="A143" s="136"/>
       <c r="B143" s="72"/>
       <c r="C143" s="72"/>
       <c r="D143" s="72"/>
@@ -5044,7 +5061,7 @@
       <c r="J143" s="72"/>
     </row>
     <row r="144" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="131">
+      <c r="A144" s="134">
         <v>44614</v>
       </c>
       <c r="B144" s="8"/>
@@ -5062,7 +5079,7 @@
       <c r="J144" s="8"/>
     </row>
     <row r="145" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="132"/>
+      <c r="A145" s="135"/>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
       <c r="D145" s="4"/>
@@ -5076,7 +5093,7 @@
       <c r="J145" s="4"/>
     </row>
     <row r="146" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="132"/>
+      <c r="A146" s="135"/>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
       <c r="D146" s="4"/>
@@ -5090,7 +5107,7 @@
       <c r="J146" s="4"/>
     </row>
     <row r="147" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="132"/>
+      <c r="A147" s="135"/>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
       <c r="D147" s="4"/>
@@ -5104,7 +5121,7 @@
       <c r="J147" s="4"/>
     </row>
     <row r="148" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="133"/>
+      <c r="A148" s="136"/>
       <c r="B148" s="75"/>
       <c r="C148" s="75"/>
       <c r="D148" s="75"/>
@@ -5118,7 +5135,7 @@
       <c r="J148" s="75"/>
     </row>
     <row r="149" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="131">
+      <c r="A149" s="134">
         <v>44615</v>
       </c>
       <c r="B149" s="8"/>
@@ -5136,7 +5153,7 @@
       <c r="J149" s="8"/>
     </row>
     <row r="150" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="133"/>
+      <c r="A150" s="136"/>
       <c r="B150" s="75"/>
       <c r="C150" s="75"/>
       <c r="D150" s="75"/>
@@ -5150,7 +5167,7 @@
       <c r="J150" s="75"/>
     </row>
     <row r="151" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="131">
+      <c r="A151" s="134">
         <v>44616</v>
       </c>
       <c r="B151" s="8"/>
@@ -5168,7 +5185,7 @@
       <c r="J151" s="8"/>
     </row>
     <row r="152" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="132"/>
+      <c r="A152" s="135"/>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
@@ -5182,7 +5199,7 @@
       <c r="J152" s="4"/>
     </row>
     <row r="153" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A153" s="133"/>
+      <c r="A153" s="136"/>
       <c r="B153" s="76"/>
       <c r="C153" s="76"/>
       <c r="D153" s="76"/>
@@ -5196,7 +5213,7 @@
       <c r="J153" s="76"/>
     </row>
     <row r="154" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A154" s="131">
+      <c r="A154" s="134">
         <v>44617</v>
       </c>
       <c r="B154" s="8"/>
@@ -5214,7 +5231,7 @@
       <c r="J154" s="8"/>
     </row>
     <row r="155" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A155" s="132"/>
+      <c r="A155" s="135"/>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
@@ -5228,7 +5245,7 @@
       <c r="J155" s="4"/>
     </row>
     <row r="156" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="133"/>
+      <c r="A156" s="136"/>
       <c r="B156" s="77"/>
       <c r="C156" s="77"/>
       <c r="D156" s="77"/>
@@ -5242,7 +5259,7 @@
       <c r="J156" s="77"/>
     </row>
     <row r="157" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="131">
+      <c r="A157" s="134">
         <v>44618</v>
       </c>
       <c r="B157" s="8"/>
@@ -5262,7 +5279,7 @@
       <c r="J157" s="8"/>
     </row>
     <row r="158" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="133"/>
+      <c r="A158" s="136"/>
       <c r="B158" s="78"/>
       <c r="C158" s="78"/>
       <c r="D158" s="78"/>
@@ -5278,7 +5295,7 @@
       <c r="J158" s="78"/>
     </row>
     <row r="159" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="131">
+      <c r="A159" s="134">
         <v>44619</v>
       </c>
       <c r="B159" s="8"/>
@@ -5296,7 +5313,7 @@
       <c r="J159" s="8"/>
     </row>
     <row r="160" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="132"/>
+      <c r="A160" s="135"/>
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
       <c r="D160" s="4"/>
@@ -5312,7 +5329,7 @@
       <c r="J160" s="4"/>
     </row>
     <row r="161" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="133"/>
+      <c r="A161" s="136"/>
       <c r="B161" s="79"/>
       <c r="C161" s="79"/>
       <c r="D161" s="79"/>
@@ -5328,7 +5345,7 @@
       <c r="J161" s="79"/>
     </row>
     <row r="162" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="131">
+      <c r="A162" s="134">
         <v>44620</v>
       </c>
       <c r="B162" s="8"/>
@@ -5346,7 +5363,7 @@
       <c r="J162" s="8"/>
     </row>
     <row r="163" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="132"/>
+      <c r="A163" s="135"/>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
       <c r="D163" s="4"/>
@@ -5362,7 +5379,7 @@
       <c r="J163" s="4"/>
     </row>
     <row r="164" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="133"/>
+      <c r="A164" s="136"/>
       <c r="B164" s="80"/>
       <c r="C164" s="80"/>
       <c r="D164" s="80"/>
@@ -5376,7 +5393,7 @@
       <c r="J164" s="80"/>
     </row>
     <row r="165" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="131">
+      <c r="A165" s="134">
         <v>44621</v>
       </c>
       <c r="B165" s="8"/>
@@ -5392,7 +5409,7 @@
       <c r="J165" s="8"/>
     </row>
     <row r="166" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="132"/>
+      <c r="A166" s="135"/>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
@@ -5406,7 +5423,7 @@
       <c r="J166" s="4"/>
     </row>
     <row r="167" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="133"/>
+      <c r="A167" s="136"/>
       <c r="B167" s="81"/>
       <c r="C167" s="81"/>
       <c r="D167" s="81"/>
@@ -5420,7 +5437,7 @@
       <c r="J167" s="81"/>
     </row>
     <row r="168" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="131">
+      <c r="A168" s="134">
         <v>44622</v>
       </c>
       <c r="B168" s="8"/>
@@ -5441,7 +5458,7 @@
       </c>
     </row>
     <row r="169" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="132"/>
+      <c r="A169" s="135"/>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
@@ -5456,7 +5473,7 @@
       </c>
     </row>
     <row r="170" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="133"/>
+      <c r="A170" s="136"/>
       <c r="B170" s="82"/>
       <c r="C170" s="82"/>
       <c r="D170" s="82"/>
@@ -5471,7 +5488,7 @@
       </c>
     </row>
     <row r="171" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="131">
+      <c r="A171" s="134">
         <v>44623</v>
       </c>
       <c r="B171" s="8"/>
@@ -5488,7 +5505,7 @@
       <c r="K171" s="8"/>
     </row>
     <row r="172" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="132"/>
+      <c r="A172" s="135"/>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
       <c r="D172" s="4"/>
@@ -5503,7 +5520,7 @@
       <c r="K172" s="4"/>
     </row>
     <row r="173" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="133"/>
+      <c r="A173" s="136"/>
       <c r="B173" s="83"/>
       <c r="C173" s="83"/>
       <c r="D173" s="83"/>
@@ -5518,7 +5535,7 @@
       <c r="K173" s="83"/>
     </row>
     <row r="174" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="131">
+      <c r="A174" s="134">
         <v>44625</v>
       </c>
       <c r="B174" s="8"/>
@@ -5535,7 +5552,7 @@
       <c r="K174" s="8"/>
     </row>
     <row r="175" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="133"/>
+      <c r="A175" s="136"/>
       <c r="B175" s="85"/>
       <c r="C175" s="85"/>
       <c r="D175" s="85"/>
@@ -5550,7 +5567,7 @@
       <c r="K175" s="85"/>
     </row>
     <row r="176" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="131">
+      <c r="A176" s="134">
         <v>44626</v>
       </c>
       <c r="B176" s="8"/>
@@ -5568,7 +5585,7 @@
       </c>
     </row>
     <row r="177" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="132"/>
+      <c r="A177" s="135"/>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
       <c r="D177" s="4"/>
@@ -5584,7 +5601,7 @@
       </c>
     </row>
     <row r="178" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="133"/>
+      <c r="A178" s="136"/>
       <c r="B178" s="86"/>
       <c r="C178" s="86"/>
       <c r="D178" s="86"/>
@@ -5600,7 +5617,7 @@
       </c>
     </row>
     <row r="179" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="131">
+      <c r="A179" s="134">
         <v>44627</v>
       </c>
       <c r="B179" s="8"/>
@@ -5618,7 +5635,7 @@
       </c>
     </row>
     <row r="180" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="132"/>
+      <c r="A180" s="135"/>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
       <c r="D180" s="4"/>
@@ -5634,7 +5651,7 @@
       </c>
     </row>
     <row r="181" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="132"/>
+      <c r="A181" s="135"/>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
       <c r="D181" s="4"/>
@@ -5650,7 +5667,7 @@
       </c>
     </row>
     <row r="182" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A182" s="133"/>
+      <c r="A182" s="136"/>
       <c r="B182" s="88"/>
       <c r="C182" s="88"/>
       <c r="D182" s="88"/>
@@ -5663,7 +5680,7 @@
       <c r="K182" s="88"/>
     </row>
     <row r="183" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="131">
+      <c r="A183" s="134">
         <v>44628</v>
       </c>
       <c r="B183" s="8" t="s">
@@ -5680,7 +5697,7 @@
       <c r="K183" s="8"/>
     </row>
     <row r="184" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="132"/>
+      <c r="A184" s="135"/>
       <c r="B184" s="4" t="s">
         <v>400</v>
       </c>
@@ -5695,7 +5712,7 @@
       <c r="K184" s="4"/>
     </row>
     <row r="185" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="133"/>
+      <c r="A185" s="136"/>
       <c r="B185" s="91" t="s">
         <v>404</v>
       </c>
@@ -5727,7 +5744,7 @@
       <c r="K186" s="12"/>
     </row>
     <row r="187" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="131">
+      <c r="A187" s="134">
         <v>44630</v>
       </c>
       <c r="B187" s="8"/>
@@ -5744,7 +5761,7 @@
       <c r="K187" s="8"/>
     </row>
     <row r="188" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="132"/>
+      <c r="A188" s="135"/>
       <c r="B188" s="4"/>
       <c r="C188" s="4"/>
       <c r="D188" s="4"/>
@@ -5759,7 +5776,7 @@
       <c r="K188" s="4"/>
     </row>
     <row r="189" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="132"/>
+      <c r="A189" s="135"/>
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
       <c r="D189" s="4"/>
@@ -5774,7 +5791,7 @@
       <c r="K189" s="4"/>
     </row>
     <row r="190" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A190" s="132"/>
+      <c r="A190" s="135"/>
       <c r="B190" s="4"/>
       <c r="C190" s="4"/>
       <c r="D190" s="4"/>
@@ -5789,7 +5806,7 @@
       <c r="K190" s="4"/>
     </row>
     <row r="191" spans="1:12" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A191" s="133"/>
+      <c r="A191" s="136"/>
       <c r="B191" s="93"/>
       <c r="C191" s="93"/>
       <c r="D191" s="93"/>
@@ -5804,7 +5821,7 @@
       <c r="K191" s="93"/>
     </row>
     <row r="192" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A192" s="131">
+      <c r="A192" s="134">
         <v>44631</v>
       </c>
       <c r="B192" s="8" t="s">
@@ -5821,7 +5838,7 @@
       <c r="K192" s="8"/>
     </row>
     <row r="193" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="132"/>
+      <c r="A193" s="135"/>
       <c r="B193" s="4" t="s">
         <v>423</v>
       </c>
@@ -5836,7 +5853,7 @@
       <c r="K193" s="4"/>
     </row>
     <row r="194" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="133"/>
+      <c r="A194" s="136"/>
       <c r="B194" s="93" t="s">
         <v>424</v>
       </c>
@@ -5851,7 +5868,7 @@
       <c r="K194" s="93"/>
     </row>
     <row r="195" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="131">
+      <c r="A195" s="134">
         <v>44632</v>
       </c>
       <c r="B195" s="8" t="s">
@@ -5868,7 +5885,7 @@
       <c r="K195" s="8"/>
     </row>
     <row r="196" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="132"/>
+      <c r="A196" s="135"/>
       <c r="B196" s="4" t="s">
         <v>427</v>
       </c>
@@ -5883,7 +5900,7 @@
       <c r="K196" s="4"/>
     </row>
     <row r="197" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A197" s="133"/>
+      <c r="A197" s="136"/>
       <c r="B197" s="95" t="s">
         <v>428</v>
       </c>
@@ -5898,7 +5915,7 @@
       <c r="K197" s="95"/>
     </row>
     <row r="198" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="131">
+      <c r="A198" s="134">
         <v>44633</v>
       </c>
       <c r="B198" s="8" t="s">
@@ -5915,7 +5932,7 @@
       <c r="K198" s="8"/>
     </row>
     <row r="199" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="132"/>
+      <c r="A199" s="135"/>
       <c r="B199" s="4" t="s">
         <v>432</v>
       </c>
@@ -5930,7 +5947,7 @@
       <c r="K199" s="4"/>
     </row>
     <row r="200" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A200" s="133"/>
+      <c r="A200" s="136"/>
       <c r="B200" s="96" t="s">
         <v>433</v>
       </c>
@@ -5945,7 +5962,7 @@
       <c r="K200" s="96"/>
     </row>
     <row r="201" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A201" s="131">
+      <c r="A201" s="134">
         <v>44634</v>
       </c>
       <c r="B201" s="8"/>
@@ -5962,7 +5979,7 @@
       <c r="K201" s="8"/>
     </row>
     <row r="202" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A202" s="132"/>
+      <c r="A202" s="135"/>
       <c r="B202" s="4"/>
       <c r="C202" s="4" t="s">
         <v>445</v>
@@ -5977,7 +5994,7 @@
       <c r="K202" s="4"/>
     </row>
     <row r="203" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A203" s="133"/>
+      <c r="A203" s="136"/>
       <c r="B203" s="98"/>
       <c r="C203" s="98" t="s">
         <v>446</v>
@@ -6009,7 +6026,7 @@
       <c r="K204" s="12"/>
     </row>
     <row r="205" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A205" s="131">
+      <c r="A205" s="134">
         <v>44636</v>
       </c>
       <c r="B205" s="8"/>
@@ -6026,7 +6043,7 @@
       <c r="K205" s="8"/>
     </row>
     <row r="206" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A206" s="133"/>
+      <c r="A206" s="136"/>
       <c r="B206" s="101"/>
       <c r="C206" s="101" t="s">
         <v>460</v>
@@ -6041,7 +6058,7 @@
       <c r="K206" s="101"/>
     </row>
     <row r="207" spans="1:11" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A207" s="131">
+      <c r="A207" s="134">
         <v>44639</v>
       </c>
       <c r="B207" s="8"/>
@@ -6058,7 +6075,7 @@
       <c r="K207" s="8"/>
     </row>
     <row r="208" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A208" s="132"/>
+      <c r="A208" s="135"/>
       <c r="B208" s="4"/>
       <c r="C208" s="4" t="s">
         <v>475</v>
@@ -6073,7 +6090,7 @@
       <c r="K208" s="4"/>
     </row>
     <row r="209" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A209" s="133"/>
+      <c r="A209" s="136"/>
       <c r="B209" s="105"/>
       <c r="C209" s="105" t="s">
         <v>476</v>
@@ -6088,7 +6105,7 @@
       <c r="K209" s="105"/>
     </row>
     <row r="210" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="131">
+      <c r="A210" s="134">
         <v>44641</v>
       </c>
       <c r="B210" s="8"/>
@@ -6105,7 +6122,7 @@
       <c r="K210" s="8"/>
     </row>
     <row r="211" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A211" s="132"/>
+      <c r="A211" s="135"/>
       <c r="B211" s="4"/>
       <c r="C211" s="4" t="s">
         <v>486</v>
@@ -6120,7 +6137,7 @@
       <c r="K211" s="4"/>
     </row>
     <row r="212" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A212" s="133"/>
+      <c r="A212" s="136"/>
       <c r="B212" s="107"/>
       <c r="C212" s="107" t="s">
         <v>487</v>
@@ -6135,7 +6152,7 @@
       <c r="K212" s="107"/>
     </row>
     <row r="213" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A213" s="131">
+      <c r="A213" s="134">
         <v>44644</v>
       </c>
       <c r="B213" s="8"/>
@@ -6153,7 +6170,7 @@
       </c>
     </row>
     <row r="214" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A214" s="132"/>
+      <c r="A214" s="135"/>
       <c r="B214" s="4"/>
       <c r="C214" s="4"/>
       <c r="D214" s="4"/>
@@ -6169,7 +6186,7 @@
       </c>
     </row>
     <row r="215" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A215" s="132"/>
+      <c r="A215" s="135"/>
       <c r="B215" s="4"/>
       <c r="C215" s="4"/>
       <c r="D215" s="4"/>
@@ -6185,7 +6202,7 @@
       </c>
     </row>
     <row r="216" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A216" s="133"/>
+      <c r="A216" s="136"/>
       <c r="B216" s="110"/>
       <c r="C216" s="110"/>
       <c r="D216" s="110"/>
@@ -6201,7 +6218,7 @@
       </c>
     </row>
     <row r="217" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A217" s="131">
+      <c r="A217" s="134">
         <v>44647</v>
       </c>
       <c r="B217" s="8" t="s">
@@ -6219,7 +6236,7 @@
       <c r="M217" s="8"/>
     </row>
     <row r="218" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A218" s="133"/>
+      <c r="A218" s="136"/>
       <c r="B218" s="113" t="s">
         <v>516</v>
       </c>
@@ -6235,7 +6252,7 @@
       <c r="M218" s="113"/>
     </row>
     <row r="219" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A219" s="131">
+      <c r="A219" s="134">
         <v>44648</v>
       </c>
       <c r="B219" s="8" t="s">
@@ -6255,7 +6272,7 @@
       <c r="M219" s="8"/>
     </row>
     <row r="220" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A220" s="132"/>
+      <c r="A220" s="135"/>
       <c r="B220" s="4" t="s">
         <v>518</v>
       </c>
@@ -6273,7 +6290,7 @@
       <c r="M220" s="4"/>
     </row>
     <row r="221" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A221" s="132"/>
+      <c r="A221" s="135"/>
       <c r="B221" s="4" t="s">
         <v>519</v>
       </c>
@@ -6289,7 +6306,7 @@
       <c r="M221" s="4"/>
     </row>
     <row r="222" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="132"/>
+      <c r="A222" s="135"/>
       <c r="B222" s="4" t="s">
         <v>520</v>
       </c>
@@ -6305,7 +6322,7 @@
       <c r="M222" s="4"/>
     </row>
     <row r="223" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A223" s="132"/>
+      <c r="A223" s="135"/>
       <c r="B223" s="4" t="s">
         <v>521</v>
       </c>
@@ -6321,7 +6338,7 @@
       <c r="M223" s="4"/>
     </row>
     <row r="224" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A224" s="133"/>
+      <c r="A224" s="136"/>
       <c r="B224" s="113" t="s">
         <v>522</v>
       </c>
@@ -6337,7 +6354,7 @@
       <c r="M224" s="113"/>
     </row>
     <row r="225" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="131">
+      <c r="A225" s="134">
         <v>44650</v>
       </c>
       <c r="B225" s="8" t="s">
@@ -6359,7 +6376,7 @@
       <c r="M225" s="8"/>
     </row>
     <row r="226" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A226" s="132"/>
+      <c r="A226" s="135"/>
       <c r="B226" s="4" t="s">
         <v>547</v>
       </c>
@@ -6379,7 +6396,7 @@
       <c r="M226" s="4"/>
     </row>
     <row r="227" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A227" s="132"/>
+      <c r="A227" s="135"/>
       <c r="B227" s="4" t="s">
         <v>548</v>
       </c>
@@ -6397,7 +6414,7 @@
       <c r="M227" s="4"/>
     </row>
     <row r="228" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A228" s="133"/>
+      <c r="A228" s="136"/>
       <c r="B228" s="116" t="s">
         <v>549</v>
       </c>
@@ -6415,7 +6432,7 @@
       <c r="M228" s="116"/>
     </row>
     <row r="229" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A229" s="131">
+      <c r="A229" s="134">
         <v>44652</v>
       </c>
       <c r="B229" s="8" t="s">
@@ -6433,7 +6450,7 @@
       <c r="M229" s="8"/>
     </row>
     <row r="230" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A230" s="133"/>
+      <c r="A230" s="136"/>
       <c r="B230" s="118" t="s">
         <v>561</v>
       </c>
@@ -6467,7 +6484,7 @@
       <c r="M231" s="12"/>
     </row>
     <row r="232" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A232" s="131">
+      <c r="A232" s="134">
         <v>44654</v>
       </c>
       <c r="B232" s="8" t="s">
@@ -6485,7 +6502,7 @@
       <c r="M232" s="8"/>
     </row>
     <row r="233" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A233" s="132"/>
+      <c r="A233" s="135"/>
       <c r="B233" s="4" t="s">
         <v>567</v>
       </c>
@@ -6501,7 +6518,7 @@
       <c r="M233" s="4"/>
     </row>
     <row r="234" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="132"/>
+      <c r="A234" s="135"/>
       <c r="B234" s="4" t="s">
         <v>568</v>
       </c>
@@ -6517,7 +6534,7 @@
       <c r="M234" s="4"/>
     </row>
     <row r="235" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A235" s="132"/>
+      <c r="A235" s="135"/>
       <c r="B235" s="4" t="s">
         <v>569</v>
       </c>
@@ -6533,7 +6550,7 @@
       <c r="M235" s="4"/>
     </row>
     <row r="236" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A236" s="132"/>
+      <c r="A236" s="135"/>
       <c r="B236" s="4" t="s">
         <v>570</v>
       </c>
@@ -6549,7 +6566,7 @@
       <c r="M236" s="4"/>
     </row>
     <row r="237" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A237" s="133"/>
+      <c r="A237" s="136"/>
       <c r="B237" s="121" t="s">
         <v>571</v>
       </c>
@@ -6583,7 +6600,7 @@
       <c r="M238" s="12"/>
     </row>
     <row r="239" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A239" s="131">
+      <c r="A239" s="134">
         <v>44659</v>
       </c>
       <c r="B239" s="8"/>
@@ -6601,7 +6618,7 @@
       <c r="M239" s="8"/>
     </row>
     <row r="240" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A240" s="132"/>
+      <c r="A240" s="135"/>
       <c r="B240" s="4"/>
       <c r="C240" s="4"/>
       <c r="D240" s="4"/>
@@ -6617,7 +6634,7 @@
       <c r="M240" s="4"/>
     </row>
     <row r="241" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A241" s="132"/>
+      <c r="A241" s="135"/>
       <c r="B241" s="4"/>
       <c r="C241" s="4"/>
       <c r="D241" s="4"/>
@@ -6633,7 +6650,7 @@
       <c r="M241" s="4"/>
     </row>
     <row r="242" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A242" s="133"/>
+      <c r="A242" s="136"/>
       <c r="B242" s="127"/>
       <c r="C242" s="127"/>
       <c r="D242" s="127"/>
@@ -6649,7 +6666,7 @@
       <c r="M242" s="127"/>
     </row>
     <row r="243" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A243" s="131">
+      <c r="A243" s="134">
         <v>44660</v>
       </c>
       <c r="B243" s="8" t="s">
@@ -6666,7 +6683,7 @@
       <c r="M243" s="8"/>
     </row>
     <row r="244" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A244" s="133"/>
+      <c r="A244" s="136"/>
       <c r="B244" s="128" t="s">
         <v>599</v>
       </c>
@@ -6682,7 +6699,7 @@
       <c r="M244" s="128"/>
     </row>
     <row r="245" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A245" s="131">
+      <c r="A245" s="134">
         <v>44663</v>
       </c>
       <c r="B245" s="8" t="s">
@@ -6700,7 +6717,7 @@
       <c r="M245" s="8"/>
     </row>
     <row r="246" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A246" s="132"/>
+      <c r="A246" s="135"/>
       <c r="B246" s="4" t="s">
         <v>603</v>
       </c>
@@ -6716,7 +6733,7 @@
       <c r="M246" s="4"/>
     </row>
     <row r="247" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A247" s="133"/>
+      <c r="A247" s="136"/>
       <c r="B247" s="129" t="s">
         <v>604</v>
       </c>
@@ -11278,6 +11295,55 @@
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="A245:A247"/>
+    <mergeCell ref="A243:A244"/>
+    <mergeCell ref="A239:A242"/>
+    <mergeCell ref="A217:A218"/>
+    <mergeCell ref="A219:A224"/>
+    <mergeCell ref="A210:A212"/>
+    <mergeCell ref="A50:A53"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="A59:A62"/>
+    <mergeCell ref="A207:A209"/>
+    <mergeCell ref="A198:A200"/>
+    <mergeCell ref="A174:A175"/>
+    <mergeCell ref="A171:A173"/>
+    <mergeCell ref="A137:A143"/>
+    <mergeCell ref="A168:A170"/>
+    <mergeCell ref="A165:A167"/>
+    <mergeCell ref="A195:A197"/>
+    <mergeCell ref="A187:A191"/>
+    <mergeCell ref="A205:A206"/>
+    <mergeCell ref="A201:A203"/>
+    <mergeCell ref="A192:A194"/>
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="A151:A153"/>
+    <mergeCell ref="A157:A158"/>
+    <mergeCell ref="A159:A161"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A104:A110"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="A118:A119"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="A111:A117"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="A87:A94"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="A98:A103"/>
     <mergeCell ref="A154:A156"/>
     <mergeCell ref="A44:A49"/>
     <mergeCell ref="A232:A237"/>
@@ -11294,55 +11360,6 @@
     <mergeCell ref="A135:A136"/>
     <mergeCell ref="A162:A164"/>
     <mergeCell ref="A144:A148"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="A111:A117"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="A87:A94"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="A98:A103"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A39"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A149:A150"/>
-    <mergeCell ref="A151:A153"/>
-    <mergeCell ref="A157:A158"/>
-    <mergeCell ref="A159:A161"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A104:A110"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A210:A212"/>
-    <mergeCell ref="A50:A53"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="A59:A62"/>
-    <mergeCell ref="A207:A209"/>
-    <mergeCell ref="A198:A200"/>
-    <mergeCell ref="A174:A175"/>
-    <mergeCell ref="A171:A173"/>
-    <mergeCell ref="A137:A143"/>
-    <mergeCell ref="A168:A170"/>
-    <mergeCell ref="A165:A167"/>
-    <mergeCell ref="A195:A197"/>
-    <mergeCell ref="A187:A191"/>
-    <mergeCell ref="A205:A206"/>
-    <mergeCell ref="A201:A203"/>
-    <mergeCell ref="A192:A194"/>
-    <mergeCell ref="A245:A247"/>
-    <mergeCell ref="A243:A244"/>
-    <mergeCell ref="A239:A242"/>
-    <mergeCell ref="A217:A218"/>
-    <mergeCell ref="A219:A224"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11417,7 +11434,7 @@
       <c r="E3" s="12"/>
     </row>
     <row r="4" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="131">
+      <c r="A4" s="134">
         <v>44595</v>
       </c>
       <c r="B4" s="38"/>
@@ -11428,7 +11445,7 @@
       <c r="E4" s="38"/>
     </row>
     <row r="5" spans="1:7" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="133"/>
+      <c r="A5" s="136"/>
       <c r="B5" s="42"/>
       <c r="C5" s="46" t="s">
         <v>161</v>
@@ -11437,7 +11454,7 @@
       <c r="E5" s="42"/>
     </row>
     <row r="6" spans="1:7" s="39" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="131">
+      <c r="A6" s="134">
         <v>44596</v>
       </c>
       <c r="B6" s="38"/>
@@ -11448,7 +11465,7 @@
       <c r="E6" s="38"/>
     </row>
     <row r="7" spans="1:7" s="43" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="133"/>
+      <c r="A7" s="136"/>
       <c r="B7" s="42"/>
       <c r="C7" s="42" t="s">
         <v>171</v>
@@ -11468,7 +11485,7 @@
       <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="131">
+      <c r="A9" s="134">
         <v>44608</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -11479,7 +11496,7 @@
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="132"/>
+      <c r="A10" s="135"/>
       <c r="B10" s="4" t="s">
         <v>237</v>
       </c>
@@ -11488,7 +11505,7 @@
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="133"/>
+      <c r="A11" s="136"/>
       <c r="B11" s="64" t="s">
         <v>238</v>
       </c>
@@ -11497,7 +11514,7 @@
       <c r="E11" s="64"/>
     </row>
     <row r="12" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="131">
+      <c r="A12" s="134">
         <v>44609</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -11508,7 +11525,7 @@
       <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="132"/>
+      <c r="A13" s="135"/>
       <c r="B13" s="4" t="s">
         <v>250</v>
       </c>
@@ -11517,7 +11534,7 @@
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="133"/>
+      <c r="A14" s="136"/>
       <c r="B14" s="67" t="s">
         <v>251</v>
       </c>
@@ -11548,7 +11565,7 @@
       <c r="E16" s="12"/>
     </row>
     <row r="17" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="131">
+      <c r="A17" s="134">
         <v>44616</v>
       </c>
       <c r="B17" s="8"/>
@@ -11559,7 +11576,7 @@
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="132"/>
+      <c r="A18" s="135"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
         <v>303</v>
@@ -11568,7 +11585,7 @@
       <c r="E18" s="4"/>
     </row>
     <row r="19" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="133"/>
+      <c r="A19" s="136"/>
       <c r="B19" s="77"/>
       <c r="C19" s="77" t="s">
         <v>304</v>
@@ -11577,7 +11594,7 @@
       <c r="E19" s="77"/>
     </row>
     <row r="20" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="131">
+      <c r="A20" s="134">
         <v>44621</v>
       </c>
       <c r="B20" s="8"/>
@@ -11588,7 +11605,7 @@
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="132"/>
+      <c r="A21" s="135"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
         <v>350</v>
@@ -11597,7 +11614,7 @@
       <c r="E21" s="4"/>
     </row>
     <row r="22" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="133"/>
+      <c r="A22" s="136"/>
       <c r="B22" s="81"/>
       <c r="C22" s="81" t="s">
         <v>351</v>
@@ -11606,7 +11623,7 @@
       <c r="E22" s="81"/>
     </row>
     <row r="23" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="131">
+      <c r="A23" s="134">
         <v>44623</v>
       </c>
       <c r="B23" s="8"/>
@@ -11617,7 +11634,7 @@
       <c r="E23" s="8"/>
     </row>
     <row r="24" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="133"/>
+      <c r="A24" s="136"/>
       <c r="B24" s="83"/>
       <c r="C24" s="83" t="s">
         <v>366</v>
@@ -11626,7 +11643,7 @@
       <c r="E24" s="83"/>
     </row>
     <row r="25" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="131">
+      <c r="A25" s="134">
         <v>44628</v>
       </c>
       <c r="B25" s="8"/>
@@ -11637,7 +11654,7 @@
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="132"/>
+      <c r="A26" s="135"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4" t="s">
         <v>396</v>
@@ -11646,7 +11663,7 @@
       <c r="E26" s="4"/>
     </row>
     <row r="27" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="132"/>
+      <c r="A27" s="135"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4" t="s">
         <v>397</v>
@@ -11655,7 +11672,7 @@
       <c r="E27" s="4"/>
     </row>
     <row r="28" spans="1:7" s="7" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="133"/>
+      <c r="A28" s="136"/>
       <c r="B28" s="89"/>
       <c r="C28" s="89" t="s">
         <v>398</v>
@@ -11664,7 +11681,7 @@
       <c r="E28" s="89"/>
     </row>
     <row r="29" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="131">
+      <c r="A29" s="134">
         <v>44635</v>
       </c>
       <c r="B29" s="8"/>
@@ -11679,7 +11696,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="132"/>
+      <c r="A30" s="135"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
         <v>455</v>
@@ -11692,7 +11709,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="133"/>
+      <c r="A31" s="136"/>
       <c r="B31" s="99"/>
       <c r="C31" s="99" t="s">
         <v>456</v>
@@ -11720,7 +11737,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="131">
+      <c r="A33" s="134">
         <v>44640</v>
       </c>
       <c r="B33" s="8"/>
@@ -11733,7 +11750,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="133"/>
+      <c r="A34" s="136"/>
       <c r="B34" s="106"/>
       <c r="C34" s="106"/>
       <c r="D34" s="106"/>
@@ -11744,7 +11761,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="131">
+      <c r="A35" s="134">
         <v>44642</v>
       </c>
       <c r="B35" s="8"/>
@@ -11759,7 +11776,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="133"/>
+      <c r="A36" s="136"/>
       <c r="B36" s="108"/>
       <c r="C36" s="108" t="s">
         <v>494</v>
@@ -11772,7 +11789,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="131">
+      <c r="A37" s="134">
         <v>44643</v>
       </c>
       <c r="B37" s="8"/>
@@ -11787,7 +11804,7 @@
       <c r="G37" s="8"/>
     </row>
     <row r="38" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="133"/>
+      <c r="A38" s="136"/>
       <c r="B38" s="108"/>
       <c r="C38" s="108"/>
       <c r="D38" s="108" t="s">
@@ -11798,7 +11815,7 @@
       <c r="G38" s="108"/>
     </row>
     <row r="39" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="131">
+      <c r="A39" s="134">
         <v>44648</v>
       </c>
       <c r="B39" s="8"/>
@@ -11811,7 +11828,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="132"/>
+      <c r="A40" s="135"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
@@ -11822,7 +11839,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="133"/>
+      <c r="A41" s="136"/>
       <c r="B41" s="113"/>
       <c r="C41" s="113"/>
       <c r="D41" s="113"/>
@@ -11861,7 +11878,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="131">
+      <c r="A44" s="134">
         <v>44658</v>
       </c>
       <c r="B44" s="8"/>
@@ -11876,7 +11893,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="133"/>
+      <c r="A45" s="136"/>
       <c r="B45" s="125"/>
       <c r="C45" s="125" t="s">
         <v>587</v>
@@ -12053,7 +12070,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B191" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C198" sqref="C198"/>
+      <selection pane="bottomRight" activeCell="B196" sqref="B196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.4"/>
@@ -12072,7 +12089,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="132">
+      <c r="A2" s="135">
         <v>44563</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -12083,35 +12100,35 @@
       </c>
     </row>
     <row r="3" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="132"/>
+      <c r="A3" s="135"/>
       <c r="B3" s="4"/>
       <c r="C3" s="14" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="132"/>
+      <c r="A4" s="135"/>
       <c r="B4" s="4"/>
       <c r="C4" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="132"/>
+      <c r="A5" s="135"/>
       <c r="B5" s="4"/>
       <c r="C5" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="133"/>
+      <c r="A6" s="136"/>
       <c r="B6" s="6"/>
       <c r="C6" s="15" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="131">
+      <c r="A7" s="134">
         <v>44564</v>
       </c>
       <c r="B7" s="8"/>
@@ -12120,56 +12137,56 @@
       </c>
     </row>
     <row r="8" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="132"/>
+      <c r="A8" s="135"/>
       <c r="B8" s="4"/>
       <c r="C8" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="132"/>
+      <c r="A9" s="135"/>
       <c r="B9" s="4"/>
       <c r="C9" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="132"/>
+      <c r="A10" s="135"/>
       <c r="B10" s="4"/>
       <c r="C10" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="132"/>
+      <c r="A11" s="135"/>
       <c r="B11" s="4"/>
       <c r="C11" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="132"/>
+      <c r="A12" s="135"/>
       <c r="B12" s="4"/>
       <c r="C12" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="132"/>
+      <c r="A13" s="135"/>
       <c r="B13" s="4"/>
       <c r="C13" s="14" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="133"/>
+      <c r="A14" s="136"/>
       <c r="B14" s="6"/>
       <c r="C14" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="131">
+      <c r="A15" s="134">
         <v>44565</v>
       </c>
       <c r="B15" s="8"/>
@@ -12178,14 +12195,14 @@
       </c>
     </row>
     <row r="16" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="135"/>
+      <c r="A16" s="138"/>
       <c r="B16" s="6"/>
       <c r="C16" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="131">
+      <c r="A17" s="134">
         <v>44570</v>
       </c>
       <c r="B17" s="8"/>
@@ -12194,19 +12211,19 @@
       </c>
     </row>
     <row r="18" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="132"/>
+      <c r="A18" s="135"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="136" t="s">
+      <c r="C18" s="139" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="133"/>
+      <c r="A19" s="136"/>
       <c r="B19" s="6"/>
-      <c r="C19" s="137"/>
+      <c r="C19" s="140"/>
     </row>
     <row r="20" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="131">
+      <c r="A20" s="134">
         <v>44574</v>
       </c>
       <c r="B20" s="8"/>
@@ -12215,21 +12232,21 @@
       </c>
     </row>
     <row r="21" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="132"/>
+      <c r="A21" s="135"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="133"/>
+      <c r="A22" s="136"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" s="9" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="131">
+      <c r="A23" s="134">
         <v>44590</v>
       </c>
       <c r="B23" s="8"/>
@@ -12238,28 +12255,28 @@
       </c>
     </row>
     <row r="24" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="134"/>
+      <c r="A24" s="137"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="5" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="134"/>
+      <c r="A25" s="137"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:3" s="7" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="135"/>
+      <c r="A26" s="138"/>
       <c r="B26" s="33"/>
       <c r="C26" s="33" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A27" s="131">
+      <c r="A27" s="134">
         <v>44591</v>
       </c>
       <c r="B27" s="8"/>
@@ -12268,49 +12285,49 @@
       </c>
     </row>
     <row r="28" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A28" s="132"/>
+      <c r="A28" s="135"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A29" s="132"/>
+      <c r="A29" s="135"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="30" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A30" s="132"/>
+      <c r="A30" s="135"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A31" s="132"/>
+      <c r="A31" s="135"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A32" s="132"/>
+      <c r="A32" s="135"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A33" s="133"/>
+      <c r="A33" s="136"/>
       <c r="B33" s="34"/>
       <c r="C33" s="34" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A34" s="131">
+      <c r="A34" s="134">
         <v>44593</v>
       </c>
       <c r="B34" s="8"/>
@@ -12319,14 +12336,14 @@
       </c>
     </row>
     <row r="35" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A35" s="133"/>
+      <c r="A35" s="136"/>
       <c r="B35" s="36"/>
       <c r="C35" s="36" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="36" spans="1:3" s="39" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A36" s="131">
+      <c r="A36" s="134">
         <v>44594</v>
       </c>
       <c r="B36" s="38" t="s">
@@ -12337,35 +12354,35 @@
       </c>
     </row>
     <row r="37" spans="1:3" s="41" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A37" s="132"/>
+      <c r="A37" s="135"/>
       <c r="B37" s="40" t="s">
         <v>164</v>
       </c>
       <c r="C37" s="40"/>
     </row>
     <row r="38" spans="1:3" s="41" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A38" s="132"/>
+      <c r="A38" s="135"/>
       <c r="B38" s="40" t="s">
         <v>157</v>
       </c>
       <c r="C38" s="40"/>
     </row>
     <row r="39" spans="1:3" s="41" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A39" s="132"/>
+      <c r="A39" s="135"/>
       <c r="B39" s="40" t="s">
         <v>158</v>
       </c>
       <c r="C39" s="40"/>
     </row>
     <row r="40" spans="1:3" s="43" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A40" s="133"/>
+      <c r="A40" s="136"/>
       <c r="B40" s="42" t="s">
         <v>159</v>
       </c>
       <c r="C40" s="42"/>
     </row>
     <row r="41" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A41" s="131">
+      <c r="A41" s="134">
         <v>44595</v>
       </c>
       <c r="B41" s="8" t="s">
@@ -12376,7 +12393,7 @@
       </c>
     </row>
     <row r="42" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A42" s="133"/>
+      <c r="A42" s="136"/>
       <c r="B42" s="44" t="s">
         <v>166</v>
       </c>
@@ -12385,7 +12402,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A43" s="131">
+      <c r="A43" s="134">
         <v>44596</v>
       </c>
       <c r="B43" s="8" t="s">
@@ -12396,21 +12413,21 @@
       </c>
     </row>
     <row r="44" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A44" s="132"/>
+      <c r="A44" s="135"/>
       <c r="B44" s="4" t="s">
         <v>169</v>
       </c>
       <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A45" s="132"/>
+      <c r="A45" s="135"/>
       <c r="B45" s="4" t="s">
         <v>172</v>
       </c>
       <c r="C45" s="4"/>
     </row>
     <row r="46" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A46" s="133"/>
+      <c r="A46" s="136"/>
       <c r="B46" s="47" t="s">
         <v>173</v>
       </c>
@@ -12435,7 +12452,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A49" s="131">
+      <c r="A49" s="134">
         <v>44608</v>
       </c>
       <c r="B49" s="8" t="s">
@@ -12444,14 +12461,14 @@
       <c r="C49" s="8"/>
     </row>
     <row r="50" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A50" s="133"/>
+      <c r="A50" s="136"/>
       <c r="B50" s="64" t="s">
         <v>236</v>
       </c>
       <c r="C50" s="64"/>
     </row>
     <row r="51" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A51" s="131">
+      <c r="A51" s="134">
         <v>44609</v>
       </c>
       <c r="B51" s="8" t="s">
@@ -12460,14 +12477,14 @@
       <c r="C51" s="8"/>
     </row>
     <row r="52" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A52" s="133"/>
+      <c r="A52" s="136"/>
       <c r="B52" s="65" t="s">
         <v>248</v>
       </c>
       <c r="C52" s="65"/>
     </row>
     <row r="53" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A53" s="131">
+      <c r="A53" s="134">
         <v>44610</v>
       </c>
       <c r="B53" s="8" t="s">
@@ -12476,28 +12493,28 @@
       <c r="C53" s="8"/>
     </row>
     <row r="54" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A54" s="132"/>
+      <c r="A54" s="135"/>
       <c r="B54" s="4" t="s">
         <v>253</v>
       </c>
       <c r="C54" s="4"/>
     </row>
     <row r="55" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A55" s="132"/>
+      <c r="A55" s="135"/>
       <c r="B55" s="4" t="s">
         <v>258</v>
       </c>
       <c r="C55" s="4"/>
     </row>
     <row r="56" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A56" s="133"/>
+      <c r="A56" s="136"/>
       <c r="B56" s="68" t="s">
         <v>259</v>
       </c>
       <c r="C56" s="68"/>
     </row>
     <row r="57" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A57" s="131">
+      <c r="A57" s="134">
         <v>44611</v>
       </c>
       <c r="B57" s="8" t="s">
@@ -12506,28 +12523,28 @@
       <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A58" s="132"/>
+      <c r="A58" s="135"/>
       <c r="B58" s="4" t="s">
         <v>261</v>
       </c>
       <c r="C58" s="4"/>
     </row>
     <row r="59" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A59" s="132"/>
+      <c r="A59" s="135"/>
       <c r="B59" s="4" t="s">
         <v>263</v>
       </c>
       <c r="C59" s="4"/>
     </row>
     <row r="60" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A60" s="133"/>
+      <c r="A60" s="136"/>
       <c r="B60" s="70" t="s">
         <v>264</v>
       </c>
       <c r="C60" s="70"/>
     </row>
     <row r="61" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A61" s="131">
+      <c r="A61" s="134">
         <v>44612</v>
       </c>
       <c r="B61" s="8" t="s">
@@ -12536,21 +12553,21 @@
       <c r="C61" s="8"/>
     </row>
     <row r="62" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A62" s="132"/>
+      <c r="A62" s="135"/>
       <c r="B62" s="4" t="s">
         <v>266</v>
       </c>
       <c r="C62" s="4"/>
     </row>
     <row r="63" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A63" s="133"/>
+      <c r="A63" s="136"/>
       <c r="B63" s="71" t="s">
         <v>267</v>
       </c>
       <c r="C63" s="71"/>
     </row>
     <row r="64" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A64" s="131">
+      <c r="A64" s="134">
         <v>44613</v>
       </c>
       <c r="B64" s="8" t="s">
@@ -12559,14 +12576,14 @@
       <c r="C64" s="8"/>
     </row>
     <row r="65" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A65" s="133"/>
+      <c r="A65" s="136"/>
       <c r="B65" s="73" t="s">
         <v>281</v>
       </c>
       <c r="C65" s="73"/>
     </row>
     <row r="66" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A66" s="131">
+      <c r="A66" s="134">
         <v>44614</v>
       </c>
       <c r="B66" s="8" t="s">
@@ -12575,28 +12592,28 @@
       <c r="C66" s="8"/>
     </row>
     <row r="67" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A67" s="132"/>
+      <c r="A67" s="135"/>
       <c r="B67" s="4" t="s">
         <v>283</v>
       </c>
       <c r="C67" s="4"/>
     </row>
     <row r="68" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A68" s="132"/>
+      <c r="A68" s="135"/>
       <c r="B68" s="4" t="s">
         <v>291</v>
       </c>
       <c r="C68" s="4"/>
     </row>
     <row r="69" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A69" s="133"/>
+      <c r="A69" s="136"/>
       <c r="B69" s="74" t="s">
         <v>292</v>
       </c>
       <c r="C69" s="74"/>
     </row>
     <row r="70" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A70" s="131">
+      <c r="A70" s="134">
         <v>44615</v>
       </c>
       <c r="B70" s="8" t="s">
@@ -12605,14 +12622,14 @@
       <c r="C70" s="8"/>
     </row>
     <row r="71" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A71" s="132"/>
+      <c r="A71" s="135"/>
       <c r="B71" s="4" t="s">
         <v>294</v>
       </c>
       <c r="C71" s="4"/>
     </row>
     <row r="72" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A72" s="133"/>
+      <c r="A72" s="136"/>
       <c r="B72" s="75" t="s">
         <v>298</v>
       </c>
@@ -12628,7 +12645,7 @@
       <c r="C73" s="12"/>
     </row>
     <row r="74" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A74" s="131">
+      <c r="A74" s="134">
         <v>44617</v>
       </c>
       <c r="B74" s="8" t="s">
@@ -12637,21 +12654,21 @@
       <c r="C74" s="8"/>
     </row>
     <row r="75" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A75" s="132"/>
+      <c r="A75" s="135"/>
       <c r="B75" s="4" t="s">
         <v>309</v>
       </c>
       <c r="C75" s="4"/>
     </row>
     <row r="76" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A76" s="133"/>
+      <c r="A76" s="136"/>
       <c r="B76" s="77" t="s">
         <v>310</v>
       </c>
       <c r="C76" s="77"/>
     </row>
     <row r="77" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A77" s="131">
+      <c r="A77" s="134">
         <v>44618</v>
       </c>
       <c r="B77" s="8" t="s">
@@ -12660,49 +12677,49 @@
       <c r="C77" s="8"/>
     </row>
     <row r="78" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A78" s="132"/>
+      <c r="A78" s="135"/>
       <c r="B78" s="4" t="s">
         <v>315</v>
       </c>
       <c r="C78" s="4"/>
     </row>
     <row r="79" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A79" s="132"/>
+      <c r="A79" s="135"/>
       <c r="B79" s="4" t="s">
         <v>316</v>
       </c>
       <c r="C79" s="4"/>
     </row>
     <row r="80" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A80" s="132"/>
+      <c r="A80" s="135"/>
       <c r="B80" s="4" t="s">
         <v>317</v>
       </c>
       <c r="C80" s="4"/>
     </row>
     <row r="81" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A81" s="132"/>
+      <c r="A81" s="135"/>
       <c r="B81" s="4" t="s">
         <v>325</v>
       </c>
       <c r="C81" s="4"/>
     </row>
     <row r="82" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A82" s="132"/>
+      <c r="A82" s="135"/>
       <c r="B82" s="4" t="s">
         <v>326</v>
       </c>
       <c r="C82" s="4"/>
     </row>
     <row r="83" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A83" s="133"/>
+      <c r="A83" s="136"/>
       <c r="B83" s="78" t="s">
         <v>327</v>
       </c>
       <c r="C83" s="78"/>
     </row>
     <row r="84" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A84" s="131">
+      <c r="A84" s="134">
         <v>44619</v>
       </c>
       <c r="B84" s="8" t="s">
@@ -12711,14 +12728,14 @@
       <c r="C84" s="8"/>
     </row>
     <row r="85" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A85" s="133"/>
+      <c r="A85" s="136"/>
       <c r="B85" s="79" t="s">
         <v>329</v>
       </c>
       <c r="C85" s="79"/>
     </row>
     <row r="86" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A86" s="131">
+      <c r="A86" s="134">
         <v>44620</v>
       </c>
       <c r="B86" s="8" t="s">
@@ -12727,28 +12744,28 @@
       <c r="C86" s="8"/>
     </row>
     <row r="87" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A87" s="132"/>
+      <c r="A87" s="135"/>
       <c r="B87" s="4" t="s">
         <v>337</v>
       </c>
       <c r="C87" s="4"/>
     </row>
     <row r="88" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A88" s="132"/>
+      <c r="A88" s="135"/>
       <c r="B88" s="4" t="s">
         <v>338</v>
       </c>
       <c r="C88" s="4"/>
     </row>
     <row r="89" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A89" s="133"/>
+      <c r="A89" s="136"/>
       <c r="B89" s="80" t="s">
         <v>339</v>
       </c>
       <c r="C89" s="80"/>
     </row>
     <row r="90" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A90" s="131">
+      <c r="A90" s="134">
         <v>44621</v>
       </c>
       <c r="B90" s="8" t="s">
@@ -12757,28 +12774,28 @@
       <c r="C90" s="8"/>
     </row>
     <row r="91" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A91" s="132"/>
+      <c r="A91" s="135"/>
       <c r="B91" s="4" t="s">
         <v>346</v>
       </c>
       <c r="C91" s="4"/>
     </row>
     <row r="92" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A92" s="132"/>
+      <c r="A92" s="135"/>
       <c r="B92" s="4" t="s">
         <v>347</v>
       </c>
       <c r="C92" s="4"/>
     </row>
     <row r="93" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A93" s="133"/>
+      <c r="A93" s="136"/>
       <c r="B93" s="81" t="s">
         <v>348</v>
       </c>
       <c r="C93" s="81"/>
     </row>
     <row r="94" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A94" s="131">
+      <c r="A94" s="134">
         <v>44622</v>
       </c>
       <c r="B94" s="8" t="s">
@@ -12787,14 +12804,14 @@
       <c r="C94" s="8"/>
     </row>
     <row r="95" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A95" s="133"/>
+      <c r="A95" s="136"/>
       <c r="B95" s="82" t="s">
         <v>356</v>
       </c>
       <c r="C95" s="82"/>
     </row>
     <row r="96" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A96" s="131">
+      <c r="A96" s="134">
         <v>44623</v>
       </c>
       <c r="B96" s="8" t="s">
@@ -12803,14 +12820,14 @@
       <c r="C96" s="8"/>
     </row>
     <row r="97" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A97" s="133"/>
+      <c r="A97" s="136"/>
       <c r="B97" s="83" t="s">
         <v>364</v>
       </c>
       <c r="C97" s="83"/>
     </row>
     <row r="98" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A98" s="131">
+      <c r="A98" s="134">
         <v>44624</v>
       </c>
       <c r="B98" s="8" t="s">
@@ -12819,14 +12836,14 @@
       <c r="C98" s="8"/>
     </row>
     <row r="99" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A99" s="133"/>
+      <c r="A99" s="136"/>
       <c r="B99" s="84" t="s">
         <v>375</v>
       </c>
       <c r="C99" s="84"/>
     </row>
     <row r="100" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A100" s="131">
+      <c r="A100" s="134">
         <v>44625</v>
       </c>
       <c r="B100" s="8" t="s">
@@ -12835,14 +12852,14 @@
       <c r="C100" s="8"/>
     </row>
     <row r="101" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A101" s="133"/>
+      <c r="A101" s="136"/>
       <c r="B101" s="85" t="s">
         <v>380</v>
       </c>
       <c r="C101" s="85"/>
     </row>
     <row r="102" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A102" s="131">
+      <c r="A102" s="134">
         <v>44626</v>
       </c>
       <c r="B102" s="8" t="s">
@@ -12851,14 +12868,14 @@
       <c r="C102" s="8"/>
     </row>
     <row r="103" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A103" s="133"/>
+      <c r="A103" s="136"/>
       <c r="B103" s="87" t="s">
         <v>386</v>
       </c>
       <c r="C103" s="87"/>
     </row>
     <row r="104" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A104" s="131">
+      <c r="A104" s="134">
         <v>44627</v>
       </c>
       <c r="B104" s="8" t="s">
@@ -12867,7 +12884,7 @@
       <c r="C104" s="8"/>
     </row>
     <row r="105" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A105" s="133"/>
+      <c r="A105" s="136"/>
       <c r="B105" s="88" t="s">
         <v>391</v>
       </c>
@@ -12883,7 +12900,7 @@
       <c r="C106" s="12"/>
     </row>
     <row r="107" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A107" s="131">
+      <c r="A107" s="134">
         <v>44629</v>
       </c>
       <c r="B107" s="8" t="s">
@@ -12892,14 +12909,14 @@
       <c r="C107" s="8"/>
     </row>
     <row r="108" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A108" s="133"/>
+      <c r="A108" s="136"/>
       <c r="B108" s="91" t="s">
         <v>407</v>
       </c>
       <c r="C108" s="91"/>
     </row>
     <row r="109" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A109" s="131">
+      <c r="A109" s="134">
         <v>44630</v>
       </c>
       <c r="B109" s="8" t="s">
@@ -12908,14 +12925,14 @@
       <c r="C109" s="8"/>
     </row>
     <row r="110" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A110" s="133"/>
+      <c r="A110" s="136"/>
       <c r="B110" s="92" t="s">
         <v>410</v>
       </c>
       <c r="C110" s="92"/>
     </row>
     <row r="111" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A111" s="131">
+      <c r="A111" s="134">
         <v>44631</v>
       </c>
       <c r="B111" s="8" t="s">
@@ -12924,14 +12941,14 @@
       <c r="C111" s="8"/>
     </row>
     <row r="112" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A112" s="133"/>
+      <c r="A112" s="136"/>
       <c r="B112" s="93" t="s">
         <v>420</v>
       </c>
       <c r="C112" s="93"/>
     </row>
     <row r="113" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A113" s="131">
+      <c r="A113" s="134">
         <v>44632</v>
       </c>
       <c r="B113" s="8" t="s">
@@ -12940,14 +12957,14 @@
       <c r="C113" s="8"/>
     </row>
     <row r="114" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A114" s="133"/>
+      <c r="A114" s="136"/>
       <c r="B114" s="94" t="s">
         <v>425</v>
       </c>
       <c r="C114" s="94"/>
     </row>
     <row r="115" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A115" s="131">
+      <c r="A115" s="134">
         <v>44633</v>
       </c>
       <c r="B115" s="8" t="s">
@@ -12956,14 +12973,14 @@
       <c r="C115" s="8"/>
     </row>
     <row r="116" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A116" s="133"/>
+      <c r="A116" s="136"/>
       <c r="B116" s="96" t="s">
         <v>430</v>
       </c>
       <c r="C116" s="96"/>
     </row>
     <row r="117" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A117" s="131">
+      <c r="A117" s="134">
         <v>44634</v>
       </c>
       <c r="B117" s="8" t="s">
@@ -12972,14 +12989,14 @@
       <c r="C117" s="8"/>
     </row>
     <row r="118" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A118" s="133"/>
+      <c r="A118" s="136"/>
       <c r="B118" s="97" t="s">
         <v>439</v>
       </c>
       <c r="C118" s="97"/>
     </row>
     <row r="119" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A119" s="131">
+      <c r="A119" s="134">
         <v>44635</v>
       </c>
       <c r="B119" s="8" t="s">
@@ -12988,14 +13005,14 @@
       <c r="C119" s="8"/>
     </row>
     <row r="120" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A120" s="133"/>
+      <c r="A120" s="136"/>
       <c r="B120" s="98" t="s">
         <v>448</v>
       </c>
       <c r="C120" s="98"/>
     </row>
     <row r="121" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A121" s="131">
+      <c r="A121" s="134">
         <v>44636</v>
       </c>
       <c r="B121" s="8" t="s">
@@ -13004,14 +13021,14 @@
       <c r="C121" s="8"/>
     </row>
     <row r="122" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A122" s="133"/>
+      <c r="A122" s="136"/>
       <c r="B122" s="99" t="s">
         <v>458</v>
       </c>
       <c r="C122" s="99"/>
     </row>
     <row r="123" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A123" s="131">
+      <c r="A123" s="134">
         <v>44637</v>
       </c>
       <c r="B123" s="8" t="s">
@@ -13020,28 +13037,28 @@
       <c r="C123" s="8"/>
     </row>
     <row r="124" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A124" s="132"/>
+      <c r="A124" s="135"/>
       <c r="B124" s="4" t="s">
         <v>464</v>
       </c>
       <c r="C124" s="4"/>
     </row>
     <row r="125" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A125" s="132"/>
+      <c r="A125" s="135"/>
       <c r="B125" s="4" t="s">
         <v>465</v>
       </c>
       <c r="C125" s="4"/>
     </row>
     <row r="126" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A126" s="133"/>
+      <c r="A126" s="136"/>
       <c r="B126" s="102" t="s">
         <v>466</v>
       </c>
       <c r="C126" s="102"/>
     </row>
     <row r="127" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A127" s="131">
+      <c r="A127" s="134">
         <v>44638</v>
       </c>
       <c r="B127" s="8" t="s">
@@ -13050,14 +13067,14 @@
       <c r="C127" s="8"/>
     </row>
     <row r="128" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A128" s="133"/>
+      <c r="A128" s="136"/>
       <c r="B128" s="103" t="s">
         <v>469</v>
       </c>
       <c r="C128" s="103"/>
     </row>
     <row r="129" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A129" s="131">
+      <c r="A129" s="134">
         <v>44639</v>
       </c>
       <c r="B129" s="8" t="s">
@@ -13066,14 +13083,14 @@
       <c r="C129" s="8"/>
     </row>
     <row r="130" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A130" s="133"/>
+      <c r="A130" s="136"/>
       <c r="B130" s="104" t="s">
         <v>471</v>
       </c>
       <c r="C130" s="104"/>
     </row>
     <row r="131" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A131" s="131">
+      <c r="A131" s="134">
         <v>44640</v>
       </c>
       <c r="B131" s="8" t="s">
@@ -13082,21 +13099,21 @@
       <c r="C131" s="8"/>
     </row>
     <row r="132" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A132" s="132"/>
+      <c r="A132" s="135"/>
       <c r="B132" s="4" t="s">
         <v>478</v>
       </c>
       <c r="C132" s="4"/>
     </row>
     <row r="133" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A133" s="133"/>
+      <c r="A133" s="136"/>
       <c r="B133" s="105" t="s">
         <v>479</v>
       </c>
       <c r="C133" s="105"/>
     </row>
     <row r="134" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A134" s="131">
+      <c r="A134" s="134">
         <v>44641</v>
       </c>
       <c r="B134" s="8" t="s">
@@ -13105,21 +13122,21 @@
       <c r="C134" s="8"/>
     </row>
     <row r="135" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A135" s="132"/>
+      <c r="A135" s="135"/>
       <c r="B135" s="4" t="s">
         <v>483</v>
       </c>
       <c r="C135" s="4"/>
     </row>
     <row r="136" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A136" s="133"/>
+      <c r="A136" s="136"/>
       <c r="B136" s="107" t="s">
         <v>484</v>
       </c>
       <c r="C136" s="107"/>
     </row>
     <row r="137" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A137" s="131">
+      <c r="A137" s="134">
         <v>44642</v>
       </c>
       <c r="B137" s="8" t="s">
@@ -13128,14 +13145,14 @@
       <c r="C137" s="8"/>
     </row>
     <row r="138" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A138" s="133"/>
+      <c r="A138" s="136"/>
       <c r="B138" s="108" t="s">
         <v>496</v>
       </c>
       <c r="C138" s="108"/>
     </row>
     <row r="139" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A139" s="131">
+      <c r="A139" s="134">
         <v>44643</v>
       </c>
       <c r="B139" s="8" t="s">
@@ -13144,14 +13161,14 @@
       <c r="C139" s="8"/>
     </row>
     <row r="140" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A140" s="133"/>
+      <c r="A140" s="136"/>
       <c r="B140" s="108" t="s">
         <v>500</v>
       </c>
       <c r="C140" s="108"/>
     </row>
     <row r="141" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A141" s="131">
+      <c r="A141" s="134">
         <v>44644</v>
       </c>
       <c r="B141" s="8" t="s">
@@ -13160,21 +13177,21 @@
       <c r="C141" s="8"/>
     </row>
     <row r="142" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A142" s="132"/>
+      <c r="A142" s="135"/>
       <c r="B142" s="4" t="s">
         <v>504</v>
       </c>
       <c r="C142" s="4"/>
     </row>
     <row r="143" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A143" s="133"/>
+      <c r="A143" s="136"/>
       <c r="B143" s="109" t="s">
         <v>505</v>
       </c>
       <c r="C143" s="109"/>
     </row>
     <row r="144" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A144" s="131">
+      <c r="A144" s="134">
         <v>44645</v>
       </c>
       <c r="B144" s="8" t="s">
@@ -13183,7 +13200,7 @@
       <c r="C144" s="8"/>
     </row>
     <row r="145" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A145" s="133"/>
+      <c r="A145" s="136"/>
       <c r="B145" s="111" t="s">
         <v>511</v>
       </c>
@@ -13199,7 +13216,7 @@
       <c r="C146" s="12"/>
     </row>
     <row r="147" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A147" s="131">
+      <c r="A147" s="134">
         <v>44647</v>
       </c>
       <c r="B147" s="8" t="s">
@@ -13208,14 +13225,14 @@
       <c r="C147" s="8"/>
     </row>
     <row r="148" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A148" s="133"/>
+      <c r="A148" s="136"/>
       <c r="B148" s="112" t="s">
         <v>514</v>
       </c>
       <c r="C148" s="112"/>
     </row>
     <row r="149" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A149" s="131">
+      <c r="A149" s="134">
         <v>44648</v>
       </c>
       <c r="B149" s="8" t="s">
@@ -13224,28 +13241,28 @@
       <c r="C149" s="8"/>
     </row>
     <row r="150" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A150" s="132"/>
+      <c r="A150" s="135"/>
       <c r="B150" s="4" t="s">
         <v>523</v>
       </c>
       <c r="C150" s="4"/>
     </row>
     <row r="151" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A151" s="132"/>
+      <c r="A151" s="135"/>
       <c r="B151" s="4" t="s">
         <v>525</v>
       </c>
       <c r="C151" s="4"/>
     </row>
     <row r="152" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A152" s="133"/>
+      <c r="A152" s="136"/>
       <c r="B152" s="113" t="s">
         <v>526</v>
       </c>
       <c r="C152" s="113"/>
     </row>
     <row r="153" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A153" s="131">
+      <c r="A153" s="134">
         <v>44649</v>
       </c>
       <c r="B153" s="8" t="s">
@@ -13254,21 +13271,21 @@
       <c r="C153" s="8"/>
     </row>
     <row r="154" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A154" s="132"/>
+      <c r="A154" s="135"/>
       <c r="B154" s="4" t="s">
         <v>532</v>
       </c>
       <c r="C154" s="4"/>
     </row>
     <row r="155" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A155" s="133"/>
+      <c r="A155" s="136"/>
       <c r="B155" s="114" t="s">
         <v>533</v>
       </c>
       <c r="C155" s="114"/>
     </row>
     <row r="156" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A156" s="131">
+      <c r="A156" s="134">
         <v>44650</v>
       </c>
       <c r="B156" s="8" t="s">
@@ -13277,21 +13294,21 @@
       <c r="C156" s="8"/>
     </row>
     <row r="157" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A157" s="132"/>
+      <c r="A157" s="135"/>
       <c r="B157" s="4" t="s">
         <v>536</v>
       </c>
       <c r="C157" s="4"/>
     </row>
     <row r="158" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A158" s="133"/>
+      <c r="A158" s="136"/>
       <c r="B158" s="114" t="s">
         <v>537</v>
       </c>
       <c r="C158" s="114"/>
     </row>
     <row r="159" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A159" s="131">
+      <c r="A159" s="134">
         <v>44651</v>
       </c>
       <c r="B159" s="8" t="s">
@@ -13300,21 +13317,21 @@
       <c r="C159" s="8"/>
     </row>
     <row r="160" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A160" s="132"/>
+      <c r="A160" s="135"/>
       <c r="B160" s="4" t="s">
         <v>542</v>
       </c>
       <c r="C160" s="4"/>
     </row>
     <row r="161" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A161" s="133"/>
+      <c r="A161" s="136"/>
       <c r="B161" s="115" t="s">
         <v>543</v>
       </c>
       <c r="C161" s="115"/>
     </row>
     <row r="162" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A162" s="131">
+      <c r="A162" s="134">
         <v>44652</v>
       </c>
       <c r="B162" s="8" t="s">
@@ -13323,28 +13340,28 @@
       <c r="C162" s="8"/>
     </row>
     <row r="163" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A163" s="132"/>
+      <c r="A163" s="135"/>
       <c r="B163" s="4" t="s">
         <v>554</v>
       </c>
       <c r="C163" s="4"/>
     </row>
     <row r="164" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A164" s="132"/>
+      <c r="A164" s="135"/>
       <c r="B164" s="4" t="s">
         <v>555</v>
       </c>
       <c r="C164" s="4"/>
     </row>
     <row r="165" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A165" s="133"/>
+      <c r="A165" s="136"/>
       <c r="B165" s="117" t="s">
         <v>556</v>
       </c>
       <c r="C165" s="117"/>
     </row>
     <row r="166" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A166" s="131">
+      <c r="A166" s="134">
         <v>44653</v>
       </c>
       <c r="B166" s="8" t="s">
@@ -13353,21 +13370,21 @@
       <c r="C166" s="8"/>
     </row>
     <row r="167" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A167" s="132"/>
+      <c r="A167" s="135"/>
       <c r="B167" s="4" t="s">
         <v>559</v>
       </c>
       <c r="C167" s="4"/>
     </row>
     <row r="168" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A168" s="133"/>
+      <c r="A168" s="136"/>
       <c r="B168" s="119" t="s">
         <v>560</v>
       </c>
       <c r="C168" s="119"/>
     </row>
     <row r="169" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A169" s="131">
+      <c r="A169" s="134">
         <v>44654</v>
       </c>
       <c r="B169" s="8" t="s">
@@ -13376,21 +13393,21 @@
       <c r="C169" s="8"/>
     </row>
     <row r="170" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A170" s="132"/>
+      <c r="A170" s="135"/>
       <c r="B170" s="4" t="s">
         <v>564</v>
       </c>
       <c r="C170" s="4"/>
     </row>
     <row r="171" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A171" s="133"/>
+      <c r="A171" s="136"/>
       <c r="B171" s="120" t="s">
         <v>565</v>
       </c>
       <c r="C171" s="120"/>
     </row>
     <row r="172" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A172" s="131">
+      <c r="A172" s="134">
         <v>44655</v>
       </c>
       <c r="B172" s="8" t="s">
@@ -13399,21 +13416,21 @@
       <c r="C172" s="8"/>
     </row>
     <row r="173" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A173" s="132"/>
+      <c r="A173" s="135"/>
       <c r="B173" s="4" t="s">
         <v>483</v>
       </c>
       <c r="C173" s="4"/>
     </row>
     <row r="174" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A174" s="133"/>
+      <c r="A174" s="136"/>
       <c r="B174" s="121" t="s">
         <v>573</v>
       </c>
       <c r="C174" s="121"/>
     </row>
     <row r="175" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A175" s="131">
+      <c r="A175" s="134">
         <v>44656</v>
       </c>
       <c r="B175" s="8" t="s">
@@ -13422,21 +13439,21 @@
       <c r="C175" s="8"/>
     </row>
     <row r="176" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A176" s="132"/>
+      <c r="A176" s="135"/>
       <c r="B176" s="4" t="s">
         <v>576</v>
       </c>
       <c r="C176" s="4"/>
     </row>
     <row r="177" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A177" s="133"/>
+      <c r="A177" s="136"/>
       <c r="B177" s="122" t="s">
         <v>514</v>
       </c>
       <c r="C177" s="122"/>
     </row>
     <row r="178" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A178" s="131">
+      <c r="A178" s="134">
         <v>44657</v>
       </c>
       <c r="B178" s="8" t="s">
@@ -13445,28 +13462,28 @@
       <c r="C178" s="8"/>
     </row>
     <row r="179" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A179" s="132"/>
+      <c r="A179" s="135"/>
       <c r="B179" s="4" t="s">
         <v>578</v>
       </c>
       <c r="C179" s="4"/>
     </row>
     <row r="180" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A180" s="132"/>
+      <c r="A180" s="135"/>
       <c r="B180" s="4" t="s">
         <v>579</v>
       </c>
       <c r="C180" s="4"/>
     </row>
     <row r="181" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A181" s="133"/>
+      <c r="A181" s="136"/>
       <c r="B181" s="123" t="s">
         <v>580</v>
       </c>
       <c r="C181" s="123"/>
     </row>
     <row r="182" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A182" s="131">
+      <c r="A182" s="134">
         <v>44658</v>
       </c>
       <c r="B182" s="8" t="s">
@@ -13475,28 +13492,28 @@
       <c r="C182" s="8"/>
     </row>
     <row r="183" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A183" s="132"/>
+      <c r="A183" s="135"/>
       <c r="B183" s="4" t="s">
         <v>583</v>
       </c>
       <c r="C183" s="4"/>
     </row>
     <row r="184" spans="1:3" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A184" s="132"/>
+      <c r="A184" s="135"/>
       <c r="B184" s="4" t="s">
         <v>584</v>
       </c>
       <c r="C184" s="4"/>
     </row>
     <row r="185" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A185" s="133"/>
+      <c r="A185" s="136"/>
       <c r="B185" s="124" t="s">
         <v>585</v>
       </c>
       <c r="C185" s="124"/>
     </row>
     <row r="186" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A186" s="131">
+      <c r="A186" s="134">
         <v>44659</v>
       </c>
       <c r="B186" s="8" t="s">
@@ -13505,14 +13522,14 @@
       <c r="C186" s="8"/>
     </row>
     <row r="187" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A187" s="133"/>
+      <c r="A187" s="136"/>
       <c r="B187" s="126" t="s">
         <v>592</v>
       </c>
       <c r="C187" s="126"/>
     </row>
     <row r="188" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A188" s="131">
+      <c r="A188" s="134">
         <v>44660</v>
       </c>
       <c r="B188" s="8" t="s">
@@ -13521,7 +13538,7 @@
       <c r="C188" s="8"/>
     </row>
     <row r="189" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A189" s="133"/>
+      <c r="A189" s="136"/>
       <c r="B189" s="127" t="s">
         <v>597</v>
       </c>
@@ -13573,7 +13590,7 @@
       <c r="C194" s="12"/>
     </row>
     <row r="195" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A195" s="131">
+      <c r="A195" s="134">
         <v>44666</v>
       </c>
       <c r="B195" s="8" t="s">
@@ -13582,21 +13599,27 @@
       <c r="C195" s="8"/>
     </row>
     <row r="196" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A196" s="133"/>
+      <c r="A196" s="136"/>
       <c r="B196" s="130" t="s">
         <v>609</v>
       </c>
       <c r="C196" s="130"/>
     </row>
-    <row r="197" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A197" s="28"/>
-      <c r="B197" s="3"/>
-      <c r="C197" s="3"/>
-    </row>
-    <row r="198" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A198" s="28"/>
-      <c r="B198" s="3"/>
-      <c r="C198" s="3"/>
+    <row r="197" spans="1:3" s="9" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A197" s="131">
+        <v>44671</v>
+      </c>
+      <c r="B197" s="8" t="s">
+        <v>610</v>
+      </c>
+      <c r="C197" s="8"/>
+    </row>
+    <row r="198" spans="1:3" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A198" s="132"/>
+      <c r="B198" s="133" t="s">
+        <v>611</v>
+      </c>
+      <c r="C198" s="133"/>
     </row>
     <row r="199" spans="1:3" ht="20.399999999999999" x14ac:dyDescent="0.3">
       <c r="A199" s="28"/>
@@ -13818,6 +13841,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="A186:A187"/>
+    <mergeCell ref="A129:A130"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="A188:A189"/>
+    <mergeCell ref="A123:A126"/>
+    <mergeCell ref="A182:A185"/>
+    <mergeCell ref="A175:A177"/>
+    <mergeCell ref="A147:A148"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="A153:A155"/>
+    <mergeCell ref="A156:A158"/>
+    <mergeCell ref="A166:A168"/>
+    <mergeCell ref="A162:A165"/>
+    <mergeCell ref="A159:A161"/>
+    <mergeCell ref="A149:A152"/>
+    <mergeCell ref="A172:A174"/>
+    <mergeCell ref="A169:A171"/>
+    <mergeCell ref="A178:A181"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A131:A133"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A90:A93"/>
+    <mergeCell ref="A86:A89"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="A77:A83"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A121:A122"/>
     <mergeCell ref="A195:A196"/>
     <mergeCell ref="A98:A99"/>
     <mergeCell ref="A96:A97"/>
@@ -13834,53 +13904,6 @@
     <mergeCell ref="A104:A105"/>
     <mergeCell ref="A111:A112"/>
     <mergeCell ref="A113:A114"/>
-    <mergeCell ref="A131:A133"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="A90:A93"/>
-    <mergeCell ref="A86:A89"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="A77:A83"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A182:A185"/>
-    <mergeCell ref="A175:A177"/>
-    <mergeCell ref="A147:A148"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="A153:A155"/>
-    <mergeCell ref="A156:A158"/>
-    <mergeCell ref="A166:A168"/>
-    <mergeCell ref="A162:A165"/>
-    <mergeCell ref="A159:A161"/>
-    <mergeCell ref="A149:A152"/>
-    <mergeCell ref="A172:A174"/>
-    <mergeCell ref="A169:A171"/>
-    <mergeCell ref="A178:A181"/>
-    <mergeCell ref="A186:A187"/>
-    <mergeCell ref="A129:A130"/>
-    <mergeCell ref="A127:A128"/>
-    <mergeCell ref="A188:A189"/>
-    <mergeCell ref="A123:A126"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13928,7 +13951,7 @@
       <c r="L1" s="1"/>
     </row>
     <row r="2" spans="1:17" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="131">
+      <c r="A2" s="134">
         <v>44623</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -13936,19 +13959,19 @@
       </c>
     </row>
     <row r="3" spans="1:17" s="5" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A3" s="132"/>
+      <c r="A3" s="135"/>
       <c r="B3" s="4" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="4" spans="1:17" s="7" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A4" s="133"/>
+      <c r="A4" s="136"/>
       <c r="B4" s="83" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="131">
+      <c r="A5" s="134">
         <v>44624</v>
       </c>
       <c r="B5" s="31" t="s">
@@ -13956,13 +13979,13 @@
       </c>
     </row>
     <row r="6" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="132"/>
+      <c r="A6" s="135"/>
       <c r="B6" s="52" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="7" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="133"/>
+      <c r="A7" s="136"/>
       <c r="B7" s="54" t="s">
         <v>378</v>
       </c>
@@ -13976,7 +13999,7 @@
       </c>
     </row>
     <row r="9" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="131">
+      <c r="A9" s="134">
         <v>44628</v>
       </c>
       <c r="B9" s="31"/>
@@ -13999,7 +14022,7 @@
       <c r="Q9" s="31"/>
     </row>
     <row r="10" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="133"/>
+      <c r="A10" s="136"/>
       <c r="B10" s="54"/>
       <c r="C10" s="54" t="s">
         <v>403</v>
@@ -14020,7 +14043,7 @@
       <c r="Q10" s="54"/>
     </row>
     <row r="11" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="131">
+      <c r="A11" s="134">
         <v>44630</v>
       </c>
       <c r="B11" s="31"/>
@@ -14043,7 +14066,7 @@
       <c r="Q11" s="31"/>
     </row>
     <row r="12" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="132"/>
+      <c r="A12" s="135"/>
       <c r="B12" s="52"/>
       <c r="C12" s="52" t="s">
         <v>417</v>
@@ -14064,7 +14087,7 @@
       <c r="Q12" s="52"/>
     </row>
     <row r="13" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="133"/>
+      <c r="A13" s="136"/>
       <c r="B13" s="54"/>
       <c r="C13" s="54" t="s">
         <v>418</v>
@@ -14085,7 +14108,7 @@
       <c r="Q13" s="54"/>
     </row>
     <row r="14" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="131">
+      <c r="A14" s="134">
         <v>44633</v>
       </c>
       <c r="B14" s="31"/>
@@ -14108,7 +14131,7 @@
       <c r="Q14" s="31"/>
     </row>
     <row r="15" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="132"/>
+      <c r="A15" s="135"/>
       <c r="B15" s="52"/>
       <c r="C15" s="52" t="s">
         <v>435</v>
@@ -14129,7 +14152,7 @@
       <c r="Q15" s="52"/>
     </row>
     <row r="16" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="132"/>
+      <c r="A16" s="135"/>
       <c r="B16" s="52"/>
       <c r="C16" s="52" t="s">
         <v>436</v>
@@ -14150,7 +14173,7 @@
       <c r="Q16" s="52"/>
     </row>
     <row r="17" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="133"/>
+      <c r="A17" s="136"/>
       <c r="B17" s="54"/>
       <c r="C17" s="54" t="s">
         <v>437</v>
@@ -14171,7 +14194,7 @@
       <c r="Q17" s="54"/>
     </row>
     <row r="18" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="131">
+      <c r="A18" s="134">
         <v>44634</v>
       </c>
       <c r="B18" s="31"/>
@@ -14194,7 +14217,7 @@
       <c r="Q18" s="31"/>
     </row>
     <row r="19" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="132"/>
+      <c r="A19" s="135"/>
       <c r="B19" s="52"/>
       <c r="C19" s="52" t="s">
         <v>441</v>
@@ -14215,7 +14238,7 @@
       <c r="Q19" s="52"/>
     </row>
     <row r="20" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="132"/>
+      <c r="A20" s="135"/>
       <c r="B20" s="52"/>
       <c r="C20" s="52" t="s">
         <v>442</v>
@@ -14236,7 +14259,7 @@
       <c r="Q20" s="52"/>
     </row>
     <row r="21" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="133"/>
+      <c r="A21" s="136"/>
       <c r="B21" s="54"/>
       <c r="C21" s="54" t="s">
         <v>443</v>
@@ -14257,7 +14280,7 @@
       <c r="Q21" s="54"/>
     </row>
     <row r="22" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="131">
+      <c r="A22" s="134">
         <v>44636</v>
       </c>
       <c r="B22" s="31"/>
@@ -14280,7 +14303,7 @@
       <c r="Q22" s="31"/>
     </row>
     <row r="23" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="133"/>
+      <c r="A23" s="136"/>
       <c r="B23" s="54"/>
       <c r="C23" s="54" t="s">
         <v>462</v>
@@ -14301,7 +14324,7 @@
       <c r="Q23" s="54"/>
     </row>
     <row r="24" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="131">
+      <c r="A24" s="134">
         <v>44639</v>
       </c>
       <c r="B24" s="31"/>
@@ -14324,7 +14347,7 @@
       <c r="Q24" s="31"/>
     </row>
     <row r="25" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="133"/>
+      <c r="A25" s="136"/>
       <c r="B25" s="54"/>
       <c r="C25" s="54" t="s">
         <v>473</v>
@@ -14345,7 +14368,7 @@
       <c r="Q25" s="54"/>
     </row>
     <row r="26" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="131">
+      <c r="A26" s="134">
         <v>44641</v>
       </c>
       <c r="B26" s="31" t="s">
@@ -14368,7 +14391,7 @@
       <c r="Q26" s="31"/>
     </row>
     <row r="27" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="132"/>
+      <c r="A27" s="135"/>
       <c r="B27" s="52" t="s">
         <v>489</v>
       </c>
@@ -14389,7 +14412,7 @@
       <c r="Q27" s="52"/>
     </row>
     <row r="28" spans="1:17" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="132"/>
+      <c r="A28" s="135"/>
       <c r="B28" s="52" t="s">
         <v>490</v>
       </c>
@@ -14410,7 +14433,7 @@
       <c r="Q28" s="52"/>
     </row>
     <row r="29" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="133"/>
+      <c r="A29" s="136"/>
       <c r="B29" s="54" t="s">
         <v>491</v>
       </c>
@@ -14454,7 +14477,7 @@
       <c r="Q30" s="90"/>
     </row>
     <row r="31" spans="1:17" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="131">
+      <c r="A31" s="134">
         <v>44658</v>
       </c>
       <c r="B31" s="31"/>
@@ -14477,7 +14500,7 @@
       <c r="Q31" s="31"/>
     </row>
     <row r="32" spans="1:17" s="7" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="133"/>
+      <c r="A32" s="136"/>
       <c r="B32" s="54"/>
       <c r="C32" s="54"/>
       <c r="D32" s="54" t="s">
@@ -17340,16 +17363,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A17"/>
     <mergeCell ref="A31:A32"/>
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
There are some bugs in IDEA Git, thus I can't push my JavaSE notes to GitHub...
</commit_message>
<xml_diff>
--- a/学习记录.xlsx
+++ b/学习记录.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\不怕晒的铃铛\Desktop\学习资料\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D751527A-25FD-4A24-88FA-2E56F586270E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D894503-90E1-4A63-8883-E45DADAA4CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11295,11 +11295,50 @@
     </row>
   </sheetData>
   <mergeCells count="65">
-    <mergeCell ref="A245:A247"/>
-    <mergeCell ref="A243:A244"/>
-    <mergeCell ref="A239:A242"/>
-    <mergeCell ref="A217:A218"/>
-    <mergeCell ref="A219:A224"/>
+    <mergeCell ref="A154:A156"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A232:A237"/>
+    <mergeCell ref="A229:A230"/>
+    <mergeCell ref="A225:A228"/>
+    <mergeCell ref="A213:A216"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="A72:A75"/>
+    <mergeCell ref="A124:A129"/>
+    <mergeCell ref="A179:A182"/>
+    <mergeCell ref="A176:A178"/>
+    <mergeCell ref="A130:A133"/>
+    <mergeCell ref="A120:A121"/>
+    <mergeCell ref="A135:A136"/>
+    <mergeCell ref="A162:A164"/>
+    <mergeCell ref="A144:A148"/>
+    <mergeCell ref="A78:A81"/>
+    <mergeCell ref="A111:A117"/>
+    <mergeCell ref="A67:A69"/>
+    <mergeCell ref="A87:A94"/>
+    <mergeCell ref="A85:A86"/>
+    <mergeCell ref="A82:A84"/>
+    <mergeCell ref="A98:A103"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A183:A185"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A149:A150"/>
+    <mergeCell ref="A151:A153"/>
+    <mergeCell ref="A157:A158"/>
+    <mergeCell ref="A159:A161"/>
+    <mergeCell ref="A54:A55"/>
+    <mergeCell ref="A104:A110"/>
+    <mergeCell ref="A95:A97"/>
+    <mergeCell ref="A118:A119"/>
     <mergeCell ref="A210:A212"/>
     <mergeCell ref="A50:A53"/>
     <mergeCell ref="A63:A66"/>
@@ -11316,50 +11355,11 @@
     <mergeCell ref="A205:A206"/>
     <mergeCell ref="A201:A203"/>
     <mergeCell ref="A192:A194"/>
-    <mergeCell ref="A183:A185"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="A35:A39"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A149:A150"/>
-    <mergeCell ref="A151:A153"/>
-    <mergeCell ref="A157:A158"/>
-    <mergeCell ref="A159:A161"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="A104:A110"/>
-    <mergeCell ref="A95:A97"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A78:A81"/>
-    <mergeCell ref="A111:A117"/>
-    <mergeCell ref="A67:A69"/>
-    <mergeCell ref="A87:A94"/>
-    <mergeCell ref="A85:A86"/>
-    <mergeCell ref="A82:A84"/>
-    <mergeCell ref="A98:A103"/>
-    <mergeCell ref="A154:A156"/>
-    <mergeCell ref="A44:A49"/>
-    <mergeCell ref="A232:A237"/>
-    <mergeCell ref="A229:A230"/>
-    <mergeCell ref="A225:A228"/>
-    <mergeCell ref="A213:A216"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="A72:A75"/>
-    <mergeCell ref="A124:A129"/>
-    <mergeCell ref="A179:A182"/>
-    <mergeCell ref="A176:A178"/>
-    <mergeCell ref="A130:A133"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="A135:A136"/>
-    <mergeCell ref="A162:A164"/>
-    <mergeCell ref="A144:A148"/>
+    <mergeCell ref="A245:A247"/>
+    <mergeCell ref="A243:A244"/>
+    <mergeCell ref="A239:A242"/>
+    <mergeCell ref="A217:A218"/>
+    <mergeCell ref="A219:A224"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12070,7 +12070,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B191" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B196" sqref="B196"/>
+      <selection pane="bottomRight" activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.8" x14ac:dyDescent="0.4"/>
@@ -13841,6 +13841,53 @@
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="A111:A112"/>
+    <mergeCell ref="A113:A114"/>
+    <mergeCell ref="A57:A60"/>
+    <mergeCell ref="A121:A122"/>
+    <mergeCell ref="A195:A196"/>
+    <mergeCell ref="A98:A99"/>
+    <mergeCell ref="A96:A97"/>
+    <mergeCell ref="A109:A110"/>
+    <mergeCell ref="A102:A103"/>
+    <mergeCell ref="A144:A145"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="A100:A101"/>
+    <mergeCell ref="A134:A136"/>
+    <mergeCell ref="A119:A120"/>
+    <mergeCell ref="A117:A118"/>
+    <mergeCell ref="A115:A116"/>
+    <mergeCell ref="A107:A108"/>
+    <mergeCell ref="A104:A105"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="A84:A85"/>
+    <mergeCell ref="A61:A63"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A36:A40"/>
+    <mergeCell ref="A27:A33"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="A172:A174"/>
+    <mergeCell ref="A169:A171"/>
+    <mergeCell ref="A178:A181"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A7:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A43:A46"/>
+    <mergeCell ref="A131:A133"/>
+    <mergeCell ref="A53:A56"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="A90:A93"/>
+    <mergeCell ref="A86:A89"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="A77:A83"/>
     <mergeCell ref="A186:A187"/>
     <mergeCell ref="A129:A130"/>
     <mergeCell ref="A127:A128"/>
@@ -13857,53 +13904,6 @@
     <mergeCell ref="A162:A165"/>
     <mergeCell ref="A159:A161"/>
     <mergeCell ref="A149:A152"/>
-    <mergeCell ref="A172:A174"/>
-    <mergeCell ref="A169:A171"/>
-    <mergeCell ref="A178:A181"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="A7:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A43:A46"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A36:A40"/>
-    <mergeCell ref="A27:A33"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="A131:A133"/>
-    <mergeCell ref="A53:A56"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="A90:A93"/>
-    <mergeCell ref="A86:A89"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="A77:A83"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="A61:A63"/>
-    <mergeCell ref="A57:A60"/>
-    <mergeCell ref="A121:A122"/>
-    <mergeCell ref="A195:A196"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="A109:A110"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="A144:A145"/>
-    <mergeCell ref="A141:A143"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="A134:A136"/>
-    <mergeCell ref="A119:A120"/>
-    <mergeCell ref="A117:A118"/>
-    <mergeCell ref="A115:A116"/>
-    <mergeCell ref="A107:A108"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="A111:A112"/>
-    <mergeCell ref="A113:A114"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17363,16 +17363,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A18:A21"/>
     <mergeCell ref="A2:A4"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A18:A21"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>